<commit_message>
internal changelog on xlsx, fixed typo
</commit_message>
<xml_diff>
--- a/BigAssTableOfLenses.xlsx
+++ b/BigAssTableOfLenses.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brand\Optics\Olaf\Software\Olaf-Optical-Testing-Software\Matlab\Support Scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brand\Optics\Olaf\Software\BigAssTableOfLenses\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8925" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8925"/>
   </bookViews>
   <sheets>
     <sheet name="LensTable" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1626" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1627" uniqueCount="481">
   <si>
     <t>Manufacture</t>
   </si>
@@ -1464,10 +1464,10 @@
     <t>100-400mm f/5-6.3 DG OS HSM Contemporary</t>
   </si>
   <si>
-    <t>100-100</t>
-  </si>
-  <si>
     <t>Added Fuji 18-55 &amp; 55-140 cine lenses and sigma 14mm f/1.8, 135mm f/1.8, 24-70 Art, and 100-400 contemporary, standardized zoom format</t>
+  </si>
+  <si>
+    <t>Correct typo on sigma 100-400mm efl</t>
   </si>
 </sst>
 </file>
@@ -1877,8 +1877,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M324"/>
   <sheetViews>
-    <sheetView topLeftCell="A301" workbookViewId="0">
-      <selection activeCell="B325" sqref="B325"/>
+    <sheetView tabSelected="1" topLeftCell="A313" workbookViewId="0">
+      <selection activeCell="D321" sqref="D321"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15498,7 +15498,7 @@
         <v>6.3</v>
       </c>
       <c r="I324" s="4" t="s">
-        <v>479</v>
+        <v>407</v>
       </c>
       <c r="J324" s="4" t="s">
         <v>182</v>
@@ -15524,10 +15524,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15804,6 +15804,14 @@
         <v>42788</v>
       </c>
       <c r="B35" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <v>42831</v>
+      </c>
+      <c r="B36" t="s">
         <v>480</v>
       </c>
     </row>

</xml_diff>

<commit_message>
+new Sony lenses + Fuji GFX + Hasselblad X1D
</commit_message>
<xml_diff>
--- a/BigAssTableOfLenses.xlsx
+++ b/BigAssTableOfLenses.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1943" uniqueCount="491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2010" uniqueCount="509">
   <si>
     <t>Manufacture</t>
   </si>
@@ -1498,6 +1498,60 @@
   </si>
   <si>
     <t>Index</t>
+  </si>
+  <si>
+    <t>FE 12-24mm f/4 G</t>
+  </si>
+  <si>
+    <t>FE 16-35mm f/2.8 GM</t>
+  </si>
+  <si>
+    <t>FE 100-400mm f/4.5-5.6 GM OSS</t>
+  </si>
+  <si>
+    <t>Laowa 15mm f/2 FE Zero-D</t>
+  </si>
+  <si>
+    <t>Laowa 7.5mm f/2 MFT Zero-D</t>
+  </si>
+  <si>
+    <t>7.5</t>
+  </si>
+  <si>
+    <t>Add Sony FE 16-35, 12-24, 100-400, Laowa 15mm f/2, Laowa 7.5mm f/2, Fuji GFX, Hasselblad XD</t>
+  </si>
+  <si>
+    <t>GF 63mm f/2.8 R WR</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>Crop Medium Format Digital</t>
+  </si>
+  <si>
+    <t>GF 120mm f/4 R LM OIS WR</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>GF 32-64mm f/4 R LM WR</t>
+  </si>
+  <si>
+    <t>32-64</t>
+  </si>
+  <si>
+    <t>GF 45mm f/2.8 R WR</t>
+  </si>
+  <si>
+    <t>Hasselblad</t>
+  </si>
+  <si>
+    <t>XCD 45mm f/3.5</t>
+  </si>
+  <si>
+    <t>XCD 90mm f/3.2</t>
   </si>
 </sst>
 </file>
@@ -1583,10 +1637,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O322" totalsRowShown="0">
-  <autoFilter ref="A1:O322"/>
-  <sortState ref="A2:M318">
-    <sortCondition ref="A1:A318"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O333" totalsRowShown="0">
+  <autoFilter ref="A1:O333"/>
+  <sortState ref="A2:O327">
+    <sortCondition ref="O1:O327"/>
   </sortState>
   <tableColumns count="15">
     <tableColumn id="1" name="Manufacture"/>
@@ -1907,10 +1961,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:O322"/>
+  <dimension ref="A1:O333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A296" workbookViewId="0">
-      <selection activeCell="O316" sqref="O316"/>
+    <sheetView tabSelected="1" topLeftCell="A311" workbookViewId="0">
+      <selection activeCell="A334" sqref="A334"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14518,7 +14572,7 @@
       <c r="B262" t="s">
         <v>165</v>
       </c>
-      <c r="C262">
+      <c r="C262" s="1">
         <v>2015</v>
       </c>
       <c r="D262">
@@ -14527,7 +14581,7 @@
       <c r="E262">
         <v>394</v>
       </c>
-      <c r="F262">
+      <c r="F262" s="1">
         <f>2.83*25.4</f>
         <v>71.881999999999991</v>
       </c>
@@ -14806,7 +14860,7 @@
       <c r="B268" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="C268">
+      <c r="C268" s="1">
         <v>2015</v>
       </c>
       <c r="D268">
@@ -14949,7 +15003,7 @@
       <c r="B271" t="s">
         <v>144</v>
       </c>
-      <c r="C271">
+      <c r="C271" s="1">
         <v>2009</v>
       </c>
       <c r="D271">
@@ -14998,7 +15052,7 @@
       <c r="B272" t="s">
         <v>153</v>
       </c>
-      <c r="C272">
+      <c r="C272" s="1">
         <v>2015</v>
       </c>
       <c r="D272">
@@ -15141,7 +15195,7 @@
       <c r="B275" t="s">
         <v>143</v>
       </c>
-      <c r="C275">
+      <c r="C275" s="1">
         <v>2006</v>
       </c>
       <c r="D275">
@@ -15190,7 +15244,7 @@
       <c r="B276" t="s">
         <v>145</v>
       </c>
-      <c r="C276">
+      <c r="C276" s="1">
         <v>2010</v>
       </c>
       <c r="D276">
@@ -15239,7 +15293,7 @@
       <c r="B277" t="s">
         <v>156</v>
       </c>
-      <c r="C277">
+      <c r="C277" s="1">
         <v>2015</v>
       </c>
       <c r="D277">
@@ -15288,7 +15342,7 @@
       <c r="B278" t="s">
         <v>164</v>
       </c>
-      <c r="C278">
+      <c r="C278" s="1">
         <v>2014</v>
       </c>
       <c r="D278">
@@ -15337,7 +15391,7 @@
       <c r="B279" t="s">
         <v>214</v>
       </c>
-      <c r="C279">
+      <c r="C279" s="1">
         <v>2014</v>
       </c>
       <c r="D279">
@@ -15431,7 +15485,7 @@
       <c r="B281" t="s">
         <v>215</v>
       </c>
-      <c r="C281">
+      <c r="C281" s="1">
         <v>2005</v>
       </c>
       <c r="D281">
@@ -15670,7 +15724,7 @@
       <c r="B286" t="s">
         <v>157</v>
       </c>
-      <c r="C286">
+      <c r="C286" s="1">
         <v>2015</v>
       </c>
       <c r="D286">
@@ -17412,6 +17466,513 @@
       </c>
       <c r="O322" s="1">
         <v>321</v>
+      </c>
+    </row>
+    <row r="323" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A323" t="s">
+        <v>168</v>
+      </c>
+      <c r="B323" t="s">
+        <v>491</v>
+      </c>
+      <c r="C323">
+        <v>2017</v>
+      </c>
+      <c r="D323">
+        <v>1698</v>
+      </c>
+      <c r="E323">
+        <v>565</v>
+      </c>
+      <c r="F323">
+        <v>116.84</v>
+      </c>
+      <c r="G323" s="2">
+        <v>88.9</v>
+      </c>
+      <c r="H323" s="1">
+        <v>4</v>
+      </c>
+      <c r="I323" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="J323" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="K323">
+        <v>0</v>
+      </c>
+      <c r="L323">
+        <v>0</v>
+      </c>
+      <c r="M323" t="s">
+        <v>286</v>
+      </c>
+      <c r="N323" t="s">
+        <v>477</v>
+      </c>
+      <c r="O323">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="324" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A324" t="s">
+        <v>168</v>
+      </c>
+      <c r="B324" t="s">
+        <v>492</v>
+      </c>
+      <c r="C324">
+        <v>2017</v>
+      </c>
+      <c r="D324">
+        <v>2198</v>
+      </c>
+      <c r="E324">
+        <v>680</v>
+      </c>
+      <c r="F324">
+        <v>121.6</v>
+      </c>
+      <c r="G324" s="2">
+        <v>88.5</v>
+      </c>
+      <c r="H324" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="I324" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="J324" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="K324">
+        <v>0</v>
+      </c>
+      <c r="L324">
+        <v>0</v>
+      </c>
+      <c r="M324" t="s">
+        <v>286</v>
+      </c>
+      <c r="N324" t="s">
+        <v>477</v>
+      </c>
+      <c r="O324">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="325" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A325" t="s">
+        <v>168</v>
+      </c>
+      <c r="B325" t="s">
+        <v>493</v>
+      </c>
+      <c r="C325">
+        <v>2017</v>
+      </c>
+      <c r="D325">
+        <v>2498</v>
+      </c>
+      <c r="E325">
+        <v>1395</v>
+      </c>
+      <c r="F325">
+        <v>205</v>
+      </c>
+      <c r="G325" s="2">
+        <v>93.9</v>
+      </c>
+      <c r="H325" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="I325" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="J325" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="K325">
+        <v>1</v>
+      </c>
+      <c r="L325">
+        <v>0</v>
+      </c>
+      <c r="M325" t="s">
+        <v>286</v>
+      </c>
+      <c r="N325" t="s">
+        <v>484</v>
+      </c>
+      <c r="O325">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="326" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A326" t="s">
+        <v>265</v>
+      </c>
+      <c r="B326" t="s">
+        <v>494</v>
+      </c>
+      <c r="C326">
+        <v>2017</v>
+      </c>
+      <c r="D326" s="5"/>
+      <c r="E326">
+        <v>500</v>
+      </c>
+      <c r="F326">
+        <v>82</v>
+      </c>
+      <c r="G326" s="2">
+        <v>66</v>
+      </c>
+      <c r="H326" s="1">
+        <v>2</v>
+      </c>
+      <c r="I326" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="J326" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="K326">
+        <v>0</v>
+      </c>
+      <c r="L326">
+        <v>0</v>
+      </c>
+      <c r="M326" t="s">
+        <v>286</v>
+      </c>
+      <c r="N326" t="s">
+        <v>477</v>
+      </c>
+      <c r="O326">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="327" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A327" t="s">
+        <v>265</v>
+      </c>
+      <c r="B327" t="s">
+        <v>495</v>
+      </c>
+      <c r="C327">
+        <v>2017</v>
+      </c>
+      <c r="D327">
+        <v>499</v>
+      </c>
+      <c r="E327">
+        <v>170</v>
+      </c>
+      <c r="F327">
+        <v>55</v>
+      </c>
+      <c r="G327" s="2">
+        <v>50</v>
+      </c>
+      <c r="H327" s="1">
+        <v>2</v>
+      </c>
+      <c r="I327" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="J327" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="K327">
+        <v>0</v>
+      </c>
+      <c r="L327">
+        <v>0</v>
+      </c>
+      <c r="M327" t="s">
+        <v>294</v>
+      </c>
+      <c r="N327" t="s">
+        <v>477</v>
+      </c>
+      <c r="O327">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="328" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A328" t="s">
+        <v>379</v>
+      </c>
+      <c r="B328" t="s">
+        <v>498</v>
+      </c>
+      <c r="C328">
+        <v>2017</v>
+      </c>
+      <c r="D328">
+        <v>1499</v>
+      </c>
+      <c r="E328">
+        <v>405</v>
+      </c>
+      <c r="F328">
+        <v>71</v>
+      </c>
+      <c r="G328" s="2">
+        <v>84</v>
+      </c>
+      <c r="H328" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="I328" s="4" t="s">
+        <v>499</v>
+      </c>
+      <c r="J328" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="K328">
+        <v>0</v>
+      </c>
+      <c r="L328">
+        <v>0</v>
+      </c>
+      <c r="M328" t="s">
+        <v>500</v>
+      </c>
+      <c r="N328" t="s">
+        <v>480</v>
+      </c>
+      <c r="O328">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="329" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A329" t="s">
+        <v>379</v>
+      </c>
+      <c r="B329" t="s">
+        <v>501</v>
+      </c>
+      <c r="C329">
+        <v>2017</v>
+      </c>
+      <c r="D329">
+        <v>2699</v>
+      </c>
+      <c r="E329">
+        <v>980</v>
+      </c>
+      <c r="F329">
+        <v>152.5</v>
+      </c>
+      <c r="G329" s="2">
+        <v>89.2</v>
+      </c>
+      <c r="H329" s="1">
+        <v>4</v>
+      </c>
+      <c r="I329" s="4" t="s">
+        <v>502</v>
+      </c>
+      <c r="J329" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="K329">
+        <v>1</v>
+      </c>
+      <c r="L329">
+        <v>0</v>
+      </c>
+      <c r="M329" t="s">
+        <v>500</v>
+      </c>
+      <c r="N329" t="s">
+        <v>482</v>
+      </c>
+      <c r="O329">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="330" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A330" t="s">
+        <v>379</v>
+      </c>
+      <c r="B330" t="s">
+        <v>503</v>
+      </c>
+      <c r="C330">
+        <v>2017</v>
+      </c>
+      <c r="D330">
+        <v>229</v>
+      </c>
+      <c r="E330">
+        <v>875</v>
+      </c>
+      <c r="F330">
+        <v>116</v>
+      </c>
+      <c r="G330" s="2">
+        <v>92.6</v>
+      </c>
+      <c r="H330" s="1">
+        <v>4</v>
+      </c>
+      <c r="I330" s="4" t="s">
+        <v>504</v>
+      </c>
+      <c r="J330" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="K330">
+        <v>0</v>
+      </c>
+      <c r="L330">
+        <v>0</v>
+      </c>
+      <c r="M330" t="s">
+        <v>500</v>
+      </c>
+      <c r="N330" t="s">
+        <v>479</v>
+      </c>
+      <c r="O330">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="331" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A331" t="s">
+        <v>379</v>
+      </c>
+      <c r="B331" t="s">
+        <v>505</v>
+      </c>
+      <c r="C331">
+        <v>2017</v>
+      </c>
+      <c r="D331" s="5"/>
+      <c r="E331" s="5"/>
+      <c r="F331" s="5"/>
+      <c r="G331" s="6"/>
+      <c r="H331" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="I331" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="J331" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="K331">
+        <v>0</v>
+      </c>
+      <c r="L331">
+        <v>0</v>
+      </c>
+      <c r="M331" t="s">
+        <v>500</v>
+      </c>
+      <c r="N331" t="s">
+        <v>480</v>
+      </c>
+      <c r="O331">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="332" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A332" t="s">
+        <v>506</v>
+      </c>
+      <c r="B332" t="s">
+        <v>507</v>
+      </c>
+      <c r="C332">
+        <v>2016</v>
+      </c>
+      <c r="D332">
+        <v>2695</v>
+      </c>
+      <c r="E332">
+        <v>417</v>
+      </c>
+      <c r="F332">
+        <v>75</v>
+      </c>
+      <c r="G332" s="2">
+        <v>77</v>
+      </c>
+      <c r="H332" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="I332" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="J332" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="K332">
+        <v>0</v>
+      </c>
+      <c r="L332">
+        <v>0</v>
+      </c>
+      <c r="M332" t="s">
+        <v>500</v>
+      </c>
+      <c r="N332" t="s">
+        <v>480</v>
+      </c>
+      <c r="O332">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="333" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A333" t="s">
+        <v>506</v>
+      </c>
+      <c r="B333" t="s">
+        <v>508</v>
+      </c>
+      <c r="C333">
+        <v>2016</v>
+      </c>
+      <c r="D333">
+        <v>3195</v>
+      </c>
+      <c r="E333">
+        <v>619</v>
+      </c>
+      <c r="F333">
+        <v>100</v>
+      </c>
+      <c r="G333" s="2">
+        <v>77</v>
+      </c>
+      <c r="H333" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="I333" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="J333" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="K333">
+        <v>0</v>
+      </c>
+      <c r="L333">
+        <v>0</v>
+      </c>
+      <c r="M333" t="s">
+        <v>500</v>
+      </c>
+      <c r="N333" t="s">
+        <v>482</v>
+      </c>
+      <c r="O333">
+        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -17425,10 +17986,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17732,6 +18293,14 @@
         <v>489</v>
       </c>
     </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="3">
+        <v>42874</v>
+      </c>
+      <c r="B39" t="s">
+        <v>497</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Removed duplicate CN-E 18-80 and updated changelog
</commit_message>
<xml_diff>
--- a/BigAssTableOfLenses.xlsx
+++ b/BigAssTableOfLenses.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brand\Optics\Olaf\Software\BigAssTableOfLenses\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Markus\Desktop\BATOL\BigAssTableOfLenses\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8928"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8928" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LensTable" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2338" uniqueCount="612">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2338" uniqueCount="614">
   <si>
     <t>Manufacture</t>
   </si>
@@ -1861,6 +1861,12 @@
   </si>
   <si>
     <t>Correct metadata on CN-E 18-80, 70-200, 14.5-60, and 30-300</t>
+  </si>
+  <si>
+    <t>Added Angenieux Cine, Schneider Xenon and Cine-Xenar III, Sigma Cine Primes, Fujifilm Cabrio Premier, Tokina Vista Cines. Rows 322-380</t>
+  </si>
+  <si>
+    <t>Removed duplicate CN-E 18-80</t>
   </si>
 </sst>
 </file>
@@ -1954,8 +1960,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O398" totalsRowShown="0">
-  <autoFilter ref="A1:O398"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O397" totalsRowShown="0">
+  <autoFilter ref="A1:O397"/>
   <sortState ref="A2:M314">
     <sortCondition ref="A1:A314"/>
   </sortState>
@@ -2278,29 +2284,29 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:O398"/>
+  <dimension ref="A1:O397"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A256" workbookViewId="0">
-      <selection activeCell="D235" sqref="D235"/>
+    <sheetView topLeftCell="A376" workbookViewId="0">
+      <selection activeCell="D400" sqref="D400"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="8.109375" customWidth="1"/>
-    <col min="2" max="2" width="37.88671875" customWidth="1"/>
-    <col min="3" max="3" width="5.44140625" customWidth="1"/>
-    <col min="4" max="4" width="6.44140625" customWidth="1"/>
-    <col min="5" max="5" width="8.21875" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.109375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="5.88671875" style="4" customWidth="1"/>
-    <col min="11" max="11" width="10.21875" customWidth="1"/>
+    <col min="1" max="1" width="8.1015625" customWidth="1"/>
+    <col min="2" max="2" width="37.89453125" customWidth="1"/>
+    <col min="3" max="3" width="5.41796875" customWidth="1"/>
+    <col min="4" max="4" width="6.41796875" customWidth="1"/>
+    <col min="5" max="5" width="8.20703125" customWidth="1"/>
+    <col min="7" max="7" width="8.68359375" customWidth="1"/>
+    <col min="8" max="8" width="12.41796875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.1015625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="5.89453125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="10.20703125" customWidth="1"/>
     <col min="12" max="12" width="9" customWidth="1"/>
-    <col min="13" max="13" width="11.6640625" customWidth="1"/>
+    <col min="13" max="13" width="11.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2347,7 +2353,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -2396,7 +2402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -2445,7 +2451,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -2494,7 +2500,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -2543,7 +2549,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -2592,7 +2598,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -2641,7 +2647,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -2690,7 +2696,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2739,7 +2745,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2788,7 +2794,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -2837,7 +2843,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -2886,7 +2892,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -2935,7 +2941,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -2984,7 +2990,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
@@ -3033,7 +3039,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
@@ -3082,7 +3088,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
@@ -3131,7 +3137,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
@@ -3180,7 +3186,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -3229,7 +3235,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
@@ -3278,7 +3284,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
@@ -3327,7 +3333,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
@@ -3376,7 +3382,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
@@ -3425,7 +3431,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
@@ -3474,7 +3480,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
@@ -3523,7 +3529,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
@@ -3572,7 +3578,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
@@ -3621,7 +3627,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1" t="s">
         <v>7</v>
       </c>
@@ -3670,7 +3676,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="1" t="s">
         <v>7</v>
       </c>
@@ -3719,7 +3725,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1" t="s">
         <v>7</v>
       </c>
@@ -3768,7 +3774,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="1" t="s">
         <v>7</v>
       </c>
@@ -3817,7 +3823,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="1" t="s">
         <v>7</v>
       </c>
@@ -3866,7 +3872,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
@@ -3915,7 +3921,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="1" t="s">
         <v>7</v>
       </c>
@@ -3964,7 +3970,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="1" t="s">
         <v>7</v>
       </c>
@@ -4013,7 +4019,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="1" t="s">
         <v>7</v>
       </c>
@@ -4062,7 +4068,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="1" t="s">
         <v>7</v>
       </c>
@@ -4111,7 +4117,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -4160,7 +4166,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -4209,7 +4215,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -4258,7 +4264,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>7</v>
       </c>
@@ -4307,7 +4313,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>7</v>
       </c>
@@ -4356,7 +4362,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>7</v>
       </c>
@@ -4405,7 +4411,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -4452,7 +4458,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>7</v>
       </c>
@@ -4501,7 +4507,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
         <v>7</v>
       </c>
@@ -4550,7 +4556,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
         <v>7</v>
       </c>
@@ -4599,7 +4605,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
         <v>7</v>
       </c>
@@ -4648,7 +4654,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
         <v>7</v>
       </c>
@@ -4697,7 +4703,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
         <v>7</v>
       </c>
@@ -4746,7 +4752,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
         <v>7</v>
       </c>
@@ -4795,7 +4801,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -4844,7 +4850,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
         <v>7</v>
       </c>
@@ -4893,7 +4899,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
         <v>7</v>
       </c>
@@ -4942,7 +4948,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
         <v>7</v>
       </c>
@@ -4991,7 +4997,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="1" t="s">
         <v>7</v>
       </c>
@@ -5040,7 +5046,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="1" t="s">
         <v>7</v>
       </c>
@@ -5089,7 +5095,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="1" t="s">
         <v>7</v>
       </c>
@@ -5138,7 +5144,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="1" t="s">
         <v>7</v>
       </c>
@@ -5187,7 +5193,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="1" t="s">
         <v>7</v>
       </c>
@@ -5236,7 +5242,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="1" t="s">
         <v>7</v>
       </c>
@@ -5283,7 +5289,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="1" t="s">
         <v>7</v>
       </c>
@@ -5332,7 +5338,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="1" t="s">
         <v>7</v>
       </c>
@@ -5379,7 +5385,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="1" t="s">
         <v>7</v>
       </c>
@@ -5426,7 +5432,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="1" t="s">
         <v>7</v>
       </c>
@@ -5473,7 +5479,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="1" t="s">
         <v>7</v>
       </c>
@@ -5520,7 +5526,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="1" t="s">
         <v>7</v>
       </c>
@@ -5567,7 +5573,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="1" t="s">
         <v>378</v>
       </c>
@@ -5614,7 +5620,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="1" t="s">
         <v>378</v>
       </c>
@@ -5661,7 +5667,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="1" t="s">
         <v>378</v>
       </c>
@@ -5708,7 +5714,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="1" t="s">
         <v>378</v>
       </c>
@@ -5755,7 +5761,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="1" t="s">
         <v>378</v>
       </c>
@@ -5802,7 +5808,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="1" t="s">
         <v>378</v>
       </c>
@@ -5849,7 +5855,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="1" t="s">
         <v>378</v>
       </c>
@@ -5896,7 +5902,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="1" t="s">
         <v>378</v>
       </c>
@@ -5943,7 +5949,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="1" t="s">
         <v>378</v>
       </c>
@@ -5990,7 +5996,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="1" t="s">
         <v>378</v>
       </c>
@@ -6037,7 +6043,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="1" t="s">
         <v>378</v>
       </c>
@@ -6084,7 +6090,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="1" t="s">
         <v>378</v>
       </c>
@@ -6131,7 +6137,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="1" t="s">
         <v>378</v>
       </c>
@@ -6178,7 +6184,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="1" t="s">
         <v>378</v>
       </c>
@@ -6225,7 +6231,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="1" t="s">
         <v>378</v>
       </c>
@@ -6272,7 +6278,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="1" t="s">
         <v>378</v>
       </c>
@@ -6319,7 +6325,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="1" t="s">
         <v>378</v>
       </c>
@@ -6366,7 +6372,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="1" t="s">
         <v>378</v>
       </c>
@@ -6413,7 +6419,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="1" t="s">
         <v>378</v>
       </c>
@@ -6460,7 +6466,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="1" t="s">
         <v>378</v>
       </c>
@@ -6507,7 +6513,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="1" t="s">
         <v>378</v>
       </c>
@@ -6551,7 +6557,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="1" t="s">
         <v>294</v>
       </c>
@@ -6600,7 +6606,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="1" t="s">
         <v>429</v>
       </c>
@@ -6647,7 +6653,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="1" t="s">
         <v>429</v>
       </c>
@@ -6694,7 +6700,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="1" t="s">
         <v>233</v>
       </c>
@@ -6741,7 +6747,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="1" t="s">
         <v>233</v>
       </c>
@@ -6788,7 +6794,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="1" t="s">
         <v>233</v>
       </c>
@@ -6835,7 +6841,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="1" t="s">
         <v>233</v>
       </c>
@@ -6882,7 +6888,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="1" t="s">
         <v>233</v>
       </c>
@@ -6929,7 +6935,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="1" t="s">
         <v>233</v>
       </c>
@@ -6976,7 +6982,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="1" t="s">
         <v>233</v>
       </c>
@@ -7025,7 +7031,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="1" t="s">
         <v>233</v>
       </c>
@@ -7075,7 +7081,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="1" t="s">
         <v>233</v>
       </c>
@@ -7124,7 +7130,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="1" t="s">
         <v>233</v>
       </c>
@@ -7171,7 +7177,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" t="s">
         <v>233</v>
       </c>
@@ -7218,7 +7224,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" t="s">
         <v>233</v>
       </c>
@@ -7265,7 +7271,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" t="s">
         <v>233</v>
       </c>
@@ -7312,7 +7318,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
         <v>233</v>
       </c>
@@ -7359,7 +7365,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="s">
         <v>233</v>
       </c>
@@ -7406,7 +7412,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="s">
         <v>233</v>
       </c>
@@ -7456,7 +7462,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" t="s">
         <v>233</v>
       </c>
@@ -7503,7 +7509,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" t="s">
         <v>233</v>
       </c>
@@ -7550,7 +7556,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" t="s">
         <v>233</v>
       </c>
@@ -7597,7 +7603,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" t="s">
         <v>233</v>
       </c>
@@ -7644,7 +7650,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" t="s">
         <v>233</v>
       </c>
@@ -7691,7 +7697,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" t="s">
         <v>233</v>
       </c>
@@ -7738,7 +7744,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" t="s">
         <v>233</v>
       </c>
@@ -7785,7 +7791,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" t="s">
         <v>233</v>
       </c>
@@ -7832,7 +7838,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" t="s">
         <v>233</v>
       </c>
@@ -7882,7 +7888,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" t="s">
         <v>233</v>
       </c>
@@ -7932,7 +7938,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" t="s">
         <v>233</v>
       </c>
@@ -7979,7 +7985,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" t="s">
         <v>233</v>
       </c>
@@ -8026,7 +8032,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" t="s">
         <v>233</v>
       </c>
@@ -8073,7 +8079,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" t="s">
         <v>296</v>
       </c>
@@ -8122,7 +8128,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" t="s">
         <v>296</v>
       </c>
@@ -8171,7 +8177,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" t="s">
         <v>296</v>
       </c>
@@ -8220,7 +8226,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" t="s">
         <v>59</v>
       </c>
@@ -8269,7 +8275,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" t="s">
         <v>59</v>
       </c>
@@ -8318,7 +8324,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" t="s">
         <v>59</v>
       </c>
@@ -8367,7 +8373,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" t="s">
         <v>59</v>
       </c>
@@ -8416,7 +8422,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" t="s">
         <v>59</v>
       </c>
@@ -8465,7 +8471,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" t="s">
         <v>59</v>
       </c>
@@ -8514,7 +8520,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" t="s">
         <v>59</v>
       </c>
@@ -8563,7 +8569,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" t="s">
         <v>59</v>
       </c>
@@ -8612,7 +8618,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" t="s">
         <v>59</v>
       </c>
@@ -8661,7 +8667,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" t="s">
         <v>59</v>
       </c>
@@ -8710,7 +8716,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" t="s">
         <v>59</v>
       </c>
@@ -8759,7 +8765,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" t="s">
         <v>59</v>
       </c>
@@ -8808,7 +8814,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" t="s">
         <v>59</v>
       </c>
@@ -8857,7 +8863,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" t="s">
         <v>59</v>
       </c>
@@ -8906,7 +8912,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" t="s">
         <v>59</v>
       </c>
@@ -8955,7 +8961,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" t="s">
         <v>59</v>
       </c>
@@ -9005,7 +9011,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" t="s">
         <v>59</v>
       </c>
@@ -9054,7 +9060,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" t="s">
         <v>59</v>
       </c>
@@ -9103,7 +9109,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="142" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="1" t="s">
         <v>59</v>
       </c>
@@ -9152,7 +9158,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="1" t="s">
         <v>59</v>
       </c>
@@ -9201,7 +9207,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="1" t="s">
         <v>59</v>
       </c>
@@ -9250,7 +9256,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="145" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="1" t="s">
         <v>59</v>
       </c>
@@ -9299,7 +9305,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="1" t="s">
         <v>59</v>
       </c>
@@ -9348,7 +9354,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" t="s">
         <v>59</v>
       </c>
@@ -9397,7 +9403,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" t="s">
         <v>59</v>
       </c>
@@ -9446,7 +9452,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" t="s">
         <v>59</v>
       </c>
@@ -9495,7 +9501,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" t="s">
         <v>59</v>
       </c>
@@ -9544,7 +9550,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" t="s">
         <v>59</v>
       </c>
@@ -9593,7 +9599,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" t="s">
         <v>59</v>
       </c>
@@ -9642,7 +9648,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" t="s">
         <v>59</v>
       </c>
@@ -9691,7 +9697,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" t="s">
         <v>59</v>
       </c>
@@ -9740,7 +9746,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="155" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" t="s">
         <v>59</v>
       </c>
@@ -9789,7 +9795,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" t="s">
         <v>59</v>
       </c>
@@ -9836,7 +9842,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="157" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" t="s">
         <v>59</v>
       </c>
@@ -9883,7 +9889,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="158" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" t="s">
         <v>59</v>
       </c>
@@ -9930,7 +9936,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" t="s">
         <v>59</v>
       </c>
@@ -9977,7 +9983,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="160" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" t="s">
         <v>59</v>
       </c>
@@ -10024,7 +10030,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="161" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" t="s">
         <v>371</v>
       </c>
@@ -10071,7 +10077,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="162" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" t="s">
         <v>371</v>
       </c>
@@ -10118,7 +10124,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="163" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" t="s">
         <v>371</v>
       </c>
@@ -10165,7 +10171,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="164" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" t="s">
         <v>438</v>
       </c>
@@ -10212,7 +10218,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="165" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" t="s">
         <v>438</v>
       </c>
@@ -10259,7 +10265,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="166" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" t="s">
         <v>438</v>
       </c>
@@ -10306,7 +10312,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="167" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" t="s">
         <v>100</v>
       </c>
@@ -10355,7 +10361,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="168" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" s="1" t="s">
         <v>100</v>
       </c>
@@ -10402,7 +10408,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="169" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" t="s">
         <v>100</v>
       </c>
@@ -10452,7 +10458,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="170" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" t="s">
         <v>100</v>
       </c>
@@ -10499,7 +10505,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="171" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" t="s">
         <v>100</v>
       </c>
@@ -10548,7 +10554,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="172" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" t="s">
         <v>100</v>
       </c>
@@ -10595,7 +10601,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="173" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" t="s">
         <v>100</v>
       </c>
@@ -10644,7 +10650,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="174" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" t="s">
         <v>100</v>
       </c>
@@ -10691,7 +10697,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="175" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" t="s">
         <v>100</v>
       </c>
@@ -10740,7 +10746,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="176" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" t="s">
         <v>100</v>
       </c>
@@ -10787,7 +10793,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="177" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" t="s">
         <v>100</v>
       </c>
@@ -10834,7 +10840,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="178" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" t="s">
         <v>100</v>
       </c>
@@ -10881,7 +10887,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="179" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" t="s">
         <v>219</v>
       </c>
@@ -10930,7 +10936,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="180" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" t="s">
         <v>219</v>
       </c>
@@ -10979,7 +10985,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="181" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" t="s">
         <v>219</v>
       </c>
@@ -11028,7 +11034,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="182" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" t="s">
         <v>101</v>
       </c>
@@ -11077,7 +11083,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="183" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" t="s">
         <v>101</v>
       </c>
@@ -11126,7 +11132,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="184" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" t="s">
         <v>101</v>
       </c>
@@ -11175,7 +11181,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="185" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" t="s">
         <v>101</v>
       </c>
@@ -11224,7 +11230,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="186" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" t="s">
         <v>101</v>
       </c>
@@ -11273,7 +11279,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="187" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A187" t="s">
         <v>101</v>
       </c>
@@ -11322,7 +11328,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="188" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A188" t="s">
         <v>101</v>
       </c>
@@ -11371,7 +11377,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="189" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A189" t="s">
         <v>101</v>
       </c>
@@ -11420,7 +11426,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="190" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A190" t="s">
         <v>101</v>
       </c>
@@ -11469,7 +11475,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="191" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A191" t="s">
         <v>101</v>
       </c>
@@ -11518,7 +11524,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="192" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A192" t="s">
         <v>101</v>
       </c>
@@ -11567,7 +11573,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="193" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A193" t="s">
         <v>101</v>
       </c>
@@ -11614,7 +11620,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="194" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A194" t="s">
         <v>101</v>
       </c>
@@ -11661,7 +11667,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="195" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A195" t="s">
         <v>101</v>
       </c>
@@ -11705,7 +11711,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="196" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A196" t="s">
         <v>101</v>
       </c>
@@ -11752,7 +11758,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="197" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A197" t="s">
         <v>101</v>
       </c>
@@ -11799,7 +11805,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="198" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A198" t="s">
         <v>101</v>
       </c>
@@ -11846,7 +11852,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="199" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A199" t="s">
         <v>167</v>
       </c>
@@ -11895,7 +11901,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="200" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A200" t="s">
         <v>167</v>
       </c>
@@ -11944,7 +11950,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="201" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A201" t="s">
         <v>167</v>
       </c>
@@ -11993,7 +11999,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="202" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A202" t="s">
         <v>167</v>
       </c>
@@ -12042,7 +12048,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="203" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A203" t="s">
         <v>167</v>
       </c>
@@ -12091,7 +12097,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="204" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A204" t="s">
         <v>167</v>
       </c>
@@ -12140,7 +12146,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="205" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A205" t="s">
         <v>167</v>
       </c>
@@ -12190,7 +12196,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="206" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A206" t="s">
         <v>167</v>
       </c>
@@ -12239,7 +12245,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="207" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A207" t="s">
         <v>167</v>
       </c>
@@ -12288,7 +12294,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="208" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A208" t="s">
         <v>167</v>
       </c>
@@ -12337,7 +12343,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="209" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A209" t="s">
         <v>167</v>
       </c>
@@ -12386,7 +12392,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="210" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A210" t="s">
         <v>167</v>
       </c>
@@ -12435,7 +12441,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="211" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A211" t="s">
         <v>167</v>
       </c>
@@ -12484,7 +12490,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="212" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A212" t="s">
         <v>167</v>
       </c>
@@ -12533,7 +12539,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="213" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A213" t="s">
         <v>167</v>
       </c>
@@ -12582,7 +12588,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="214" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A214" t="s">
         <v>167</v>
       </c>
@@ -12629,7 +12635,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="215" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A215" t="s">
         <v>183</v>
       </c>
@@ -12678,7 +12684,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="216" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A216" t="s">
         <v>183</v>
       </c>
@@ -12727,7 +12733,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="217" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A217" t="s">
         <v>183</v>
       </c>
@@ -12776,7 +12782,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="218" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A218" t="s">
         <v>183</v>
       </c>
@@ -12825,7 +12831,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="219" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A219" t="s">
         <v>183</v>
       </c>
@@ -12874,7 +12880,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="220" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A220" t="s">
         <v>183</v>
       </c>
@@ -12923,7 +12929,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="221" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A221" t="s">
         <v>183</v>
       </c>
@@ -12972,7 +12978,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="222" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A222" t="s">
         <v>183</v>
       </c>
@@ -13021,7 +13027,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="223" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A223" t="s">
         <v>183</v>
       </c>
@@ -13070,7 +13076,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="224" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A224" t="s">
         <v>183</v>
       </c>
@@ -13117,7 +13123,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="225" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A225" s="1" t="s">
         <v>183</v>
       </c>
@@ -13164,7 +13170,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="226" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A226" s="1" t="s">
         <v>183</v>
       </c>
@@ -13211,7 +13217,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="227" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A227" t="s">
         <v>192</v>
       </c>
@@ -13260,7 +13266,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="228" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A228" t="s">
         <v>192</v>
       </c>
@@ -13309,7 +13315,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="229" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A229" t="s">
         <v>192</v>
       </c>
@@ -13358,7 +13364,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="230" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A230" t="s">
         <v>192</v>
       </c>
@@ -13407,7 +13413,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="231" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A231" t="s">
         <v>192</v>
       </c>
@@ -13456,7 +13462,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="232" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A232" t="s">
         <v>192</v>
       </c>
@@ -13503,7 +13509,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="233" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A233" t="s">
         <v>264</v>
       </c>
@@ -13550,7 +13556,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="234" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A234" s="1" t="s">
         <v>264</v>
       </c>
@@ -13597,7 +13603,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="235" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A235" s="1" t="s">
         <v>264</v>
       </c>
@@ -13644,7 +13650,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="236" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A236" s="1" t="s">
         <v>264</v>
       </c>
@@ -13691,7 +13697,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="237" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A237" s="1" t="s">
         <v>221</v>
       </c>
@@ -13740,7 +13746,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="238" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A238" s="1" t="s">
         <v>221</v>
       </c>
@@ -13787,7 +13793,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="239" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A239" s="1" t="s">
         <v>221</v>
       </c>
@@ -13834,7 +13840,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="240" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A240" s="1" t="s">
         <v>221</v>
       </c>
@@ -13883,7 +13889,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="241" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A241" s="1" t="s">
         <v>221</v>
       </c>
@@ -13930,7 +13936,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="242" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A242" s="1" t="s">
         <v>221</v>
       </c>
@@ -13977,7 +13983,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="243" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A243" s="1" t="s">
         <v>221</v>
       </c>
@@ -14024,7 +14030,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="244" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A244" s="1" t="s">
         <v>221</v>
       </c>
@@ -14073,7 +14079,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="245" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A245" s="1" t="s">
         <v>221</v>
       </c>
@@ -14120,7 +14126,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="246" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A246" s="1" t="s">
         <v>221</v>
       </c>
@@ -14167,7 +14173,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="247" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A247" t="s">
         <v>221</v>
       </c>
@@ -14214,7 +14220,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="248" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A248" t="s">
         <v>221</v>
       </c>
@@ -14261,7 +14267,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="249" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A249" t="s">
         <v>221</v>
       </c>
@@ -14308,7 +14314,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="250" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A250" t="s">
         <v>221</v>
       </c>
@@ -14357,7 +14363,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="251" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A251" t="s">
         <v>221</v>
       </c>
@@ -14404,7 +14410,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="252" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A252" s="1" t="s">
         <v>221</v>
       </c>
@@ -14451,7 +14457,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="253" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A253" s="1" t="s">
         <v>221</v>
       </c>
@@ -14498,7 +14504,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="254" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A254" t="s">
         <v>133</v>
       </c>
@@ -14547,7 +14553,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="255" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A255" t="s">
         <v>133</v>
       </c>
@@ -14594,7 +14600,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="256" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A256" t="s">
         <v>133</v>
       </c>
@@ -14641,7 +14647,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="257" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A257" t="s">
         <v>133</v>
       </c>
@@ -14690,7 +14696,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="258" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A258" t="s">
         <v>133</v>
       </c>
@@ -14737,7 +14743,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="259" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A259" t="s">
         <v>133</v>
       </c>
@@ -14784,7 +14790,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="260" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A260" t="s">
         <v>133</v>
       </c>
@@ -14833,7 +14839,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="261" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A261" t="s">
         <v>133</v>
       </c>
@@ -14882,7 +14888,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="262" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A262" t="s">
         <v>133</v>
       </c>
@@ -14931,7 +14937,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="263" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A263" t="s">
         <v>133</v>
       </c>
@@ -14978,7 +14984,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="264" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A264" t="s">
         <v>133</v>
       </c>
@@ -15025,7 +15031,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="265" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A265" t="s">
         <v>133</v>
       </c>
@@ -15072,7 +15078,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="266" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A266" t="s">
         <v>133</v>
       </c>
@@ -15121,7 +15127,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="267" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A267" t="s">
         <v>133</v>
       </c>
@@ -15170,7 +15176,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="268" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A268" s="1" t="s">
         <v>133</v>
       </c>
@@ -15219,7 +15225,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="269" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A269" s="1" t="s">
         <v>133</v>
       </c>
@@ -15266,7 +15272,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="270" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A270" t="s">
         <v>133</v>
       </c>
@@ -15313,7 +15319,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="271" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A271" t="s">
         <v>133</v>
       </c>
@@ -15362,7 +15368,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="272" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A272" t="s">
         <v>133</v>
       </c>
@@ -15411,7 +15417,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="273" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A273" t="s">
         <v>133</v>
       </c>
@@ -15458,7 +15464,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="274" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A274" t="s">
         <v>133</v>
       </c>
@@ -15505,7 +15511,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="275" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A275" t="s">
         <v>133</v>
       </c>
@@ -15554,7 +15560,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="276" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A276" t="s">
         <v>133</v>
       </c>
@@ -15603,7 +15609,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="277" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A277" t="s">
         <v>133</v>
       </c>
@@ -15652,7 +15658,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="278" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A278" t="s">
         <v>133</v>
       </c>
@@ -15701,7 +15707,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="279" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A279" t="s">
         <v>133</v>
       </c>
@@ -15748,7 +15754,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="280" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A280" t="s">
         <v>133</v>
       </c>
@@ -15795,7 +15801,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="281" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A281" t="s">
         <v>133</v>
       </c>
@@ -15842,7 +15848,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="282" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A282" t="s">
         <v>133</v>
       </c>
@@ -15889,7 +15895,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="283" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A283" t="s">
         <v>133</v>
       </c>
@@ -15936,7 +15942,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="284" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A284" t="s">
         <v>133</v>
       </c>
@@ -15985,7 +15991,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="285" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A285" t="s">
         <v>133</v>
       </c>
@@ -16034,7 +16040,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="286" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A286" t="s">
         <v>133</v>
       </c>
@@ -16083,7 +16089,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="287" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A287" t="s">
         <v>133</v>
       </c>
@@ -16132,7 +16138,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="288" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A288" t="s">
         <v>133</v>
       </c>
@@ -16181,7 +16187,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="289" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A289" t="s">
         <v>133</v>
       </c>
@@ -16228,7 +16234,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="290" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A290" t="s">
         <v>133</v>
       </c>
@@ -16275,7 +16281,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="291" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A291" t="s">
         <v>133</v>
       </c>
@@ -16322,7 +16328,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="292" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A292" t="s">
         <v>133</v>
       </c>
@@ -16369,7 +16375,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="293" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A293" t="s">
         <v>133</v>
       </c>
@@ -16416,7 +16422,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="294" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A294" t="s">
         <v>133</v>
       </c>
@@ -16465,7 +16471,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="295" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A295" t="s">
         <v>133</v>
       </c>
@@ -16514,7 +16520,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="296" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A296" t="s">
         <v>133</v>
       </c>
@@ -16563,7 +16569,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="297" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A297" t="s">
         <v>133</v>
       </c>
@@ -16612,7 +16618,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="298" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A298" t="s">
         <v>133</v>
       </c>
@@ -16661,7 +16667,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="299" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A299" t="s">
         <v>133</v>
       </c>
@@ -16708,7 +16714,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="300" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A300" t="s">
         <v>133</v>
       </c>
@@ -16755,7 +16761,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="301" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A301" t="s">
         <v>133</v>
       </c>
@@ -16802,7 +16808,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="302" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A302" t="s">
         <v>133</v>
       </c>
@@ -16851,7 +16857,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="303" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A303" t="s">
         <v>133</v>
       </c>
@@ -16900,7 +16906,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="304" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A304" t="s">
         <v>133</v>
       </c>
@@ -16947,7 +16953,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="305" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A305" t="s">
         <v>133</v>
       </c>
@@ -16996,7 +17002,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="306" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A306" t="s">
         <v>133</v>
       </c>
@@ -17043,7 +17049,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="307" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A307" t="s">
         <v>133</v>
       </c>
@@ -17090,7 +17096,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="308" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A308" t="s">
         <v>133</v>
       </c>
@@ -17137,7 +17143,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="309" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A309" t="s">
         <v>133</v>
       </c>
@@ -17184,7 +17190,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="310" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A310" t="s">
         <v>133</v>
       </c>
@@ -17231,7 +17237,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="311" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A311" t="s">
         <v>133</v>
       </c>
@@ -17278,7 +17284,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="312" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A312" t="s">
         <v>133</v>
       </c>
@@ -17325,7 +17331,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="313" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A313" t="s">
         <v>133</v>
       </c>
@@ -17372,7 +17378,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="314" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A314" t="s">
         <v>133</v>
       </c>
@@ -17419,7 +17425,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="315" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A315" t="s">
         <v>378</v>
       </c>
@@ -17466,7 +17472,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="316" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A316" t="s">
         <v>378</v>
       </c>
@@ -17513,7 +17519,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="317" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A317" t="s">
         <v>101</v>
       </c>
@@ -17558,7 +17564,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="318" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A318" t="s">
         <v>101</v>
       </c>
@@ -17603,7 +17609,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="319" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A319" t="s">
         <v>101</v>
       </c>
@@ -17646,7 +17652,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="320" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A320" t="s">
         <v>101</v>
       </c>
@@ -17691,7 +17697,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="321" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A321" t="s">
         <v>7</v>
       </c>
@@ -17738,7 +17744,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="322" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A322" t="s">
         <v>219</v>
       </c>
@@ -17781,7 +17787,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="323" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A323" t="s">
         <v>219</v>
       </c>
@@ -17824,7 +17830,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="324" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A324" t="s">
         <v>219</v>
       </c>
@@ -17867,7 +17873,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="325" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A325" t="s">
         <v>101</v>
       </c>
@@ -17910,7 +17916,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="326" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A326" t="s">
         <v>192</v>
       </c>
@@ -17953,7 +17959,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="327" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A327" t="s">
         <v>7</v>
       </c>
@@ -17996,7 +18002,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="328" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A328" t="s">
         <v>7</v>
       </c>
@@ -18043,7 +18049,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="329" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A329" t="s">
         <v>7</v>
       </c>
@@ -18090,7 +18096,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="330" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A330" t="s">
         <v>7</v>
       </c>
@@ -18137,7 +18143,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="331" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A331" t="s">
         <v>7</v>
       </c>
@@ -18182,7 +18188,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="332" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A332" t="s">
         <v>219</v>
       </c>
@@ -18225,7 +18231,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="333" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A333" t="s">
         <v>219</v>
       </c>
@@ -18268,7 +18274,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="334" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A334" t="s">
         <v>219</v>
       </c>
@@ -18311,7 +18317,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="335" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A335" t="s">
         <v>219</v>
       </c>
@@ -18354,7 +18360,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="336" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A336" t="s">
         <v>219</v>
       </c>
@@ -18397,7 +18403,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="337" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A337" t="s">
         <v>219</v>
       </c>
@@ -18440,7 +18446,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="338" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A338" t="s">
         <v>505</v>
       </c>
@@ -18485,7 +18491,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="339" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A339" t="s">
         <v>505</v>
       </c>
@@ -18528,7 +18534,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="340" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A340" t="s">
         <v>505</v>
       </c>
@@ -18571,7 +18577,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="341" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A341" t="s">
         <v>505</v>
       </c>
@@ -18614,7 +18620,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="342" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A342" t="s">
         <v>505</v>
       </c>
@@ -18657,7 +18663,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="343" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A343" t="s">
         <v>505</v>
       </c>
@@ -18700,7 +18706,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="344" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A344" t="s">
         <v>505</v>
       </c>
@@ -18743,7 +18749,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="345" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A345" t="s">
         <v>505</v>
       </c>
@@ -18786,7 +18792,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="346" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A346" t="s">
         <v>505</v>
       </c>
@@ -18829,7 +18835,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="347" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A347" t="s">
         <v>505</v>
       </c>
@@ -18872,7 +18878,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="348" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A348" t="s">
         <v>505</v>
       </c>
@@ -18915,7 +18921,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="349" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A349" t="s">
         <v>505</v>
       </c>
@@ -18958,7 +18964,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="350" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A350" t="s">
         <v>505</v>
       </c>
@@ -19001,7 +19007,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="351" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A351" t="s">
         <v>505</v>
       </c>
@@ -19044,7 +19050,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="352" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A352" t="s">
         <v>505</v>
       </c>
@@ -19087,7 +19093,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="353" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A353" t="s">
         <v>505</v>
       </c>
@@ -19130,7 +19136,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="354" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A354" t="s">
         <v>505</v>
       </c>
@@ -19173,7 +19179,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="355" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A355" t="s">
         <v>378</v>
       </c>
@@ -19218,7 +19224,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="356" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A356" t="s">
         <v>378</v>
       </c>
@@ -19263,7 +19269,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="357" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A357" t="s">
         <v>378</v>
       </c>
@@ -19308,7 +19314,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="358" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A358" t="s">
         <v>378</v>
       </c>
@@ -19353,7 +19359,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="359" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A359" t="s">
         <v>378</v>
       </c>
@@ -19398,7 +19404,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="360" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A360" t="s">
         <v>378</v>
       </c>
@@ -19443,7 +19449,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="361" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A361" t="s">
         <v>378</v>
       </c>
@@ -19488,7 +19494,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="362" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A362" t="s">
         <v>378</v>
       </c>
@@ -19533,7 +19539,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="363" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A363" t="s">
         <v>378</v>
       </c>
@@ -19578,7 +19584,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="364" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A364" t="s">
         <v>101</v>
       </c>
@@ -19621,7 +19627,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="365" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A365" t="s">
         <v>101</v>
       </c>
@@ -19666,7 +19672,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="366" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A366" t="s">
         <v>101</v>
       </c>
@@ -19711,7 +19717,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="367" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A367" t="s">
         <v>101</v>
       </c>
@@ -19756,7 +19762,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="368" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A368" t="s">
         <v>101</v>
       </c>
@@ -19801,7 +19807,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="369" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A369" t="s">
         <v>101</v>
       </c>
@@ -19846,7 +19852,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="370" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A370" t="s">
         <v>101</v>
       </c>
@@ -19891,7 +19897,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="371" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A371" t="s">
         <v>101</v>
       </c>
@@ -19936,7 +19942,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="372" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A372" t="s">
         <v>192</v>
       </c>
@@ -19981,7 +19987,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="373" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A373" t="s">
         <v>192</v>
       </c>
@@ -20026,7 +20032,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="374" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A374" t="s">
         <v>192</v>
       </c>
@@ -20071,7 +20077,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="375" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A375" t="s">
         <v>192</v>
       </c>
@@ -20116,7 +20122,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="376" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A376" t="s">
         <v>192</v>
       </c>
@@ -20159,7 +20165,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="377" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A377" t="s">
         <v>192</v>
       </c>
@@ -20204,7 +20210,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="378" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A378" t="s">
         <v>192</v>
       </c>
@@ -20249,7 +20255,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="379" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A379" t="s">
         <v>133</v>
       </c>
@@ -20294,7 +20300,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="380" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A380" t="s">
         <v>7</v>
       </c>
@@ -20339,7 +20345,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="381" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A381" t="s">
         <v>432</v>
       </c>
@@ -20384,7 +20390,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="382" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A382" t="s">
         <v>432</v>
       </c>
@@ -20429,7 +20435,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="383" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A383" t="s">
         <v>432</v>
       </c>
@@ -20474,7 +20480,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="384" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A384" t="s">
         <v>432</v>
       </c>
@@ -20519,7 +20525,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="385" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A385" s="8" t="s">
         <v>183</v>
       </c>
@@ -20566,7 +20572,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="386" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A386" s="8" t="s">
         <v>133</v>
       </c>
@@ -20613,7 +20619,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="387" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A387" s="8" t="s">
         <v>167</v>
       </c>
@@ -20660,7 +20666,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="388" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A388" s="8" t="s">
         <v>167</v>
       </c>
@@ -20707,7 +20713,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="389" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A389" s="8" t="s">
         <v>167</v>
       </c>
@@ -20754,7 +20760,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="390" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A390" s="8" t="s">
         <v>264</v>
       </c>
@@ -20799,7 +20805,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="391" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A391" s="8" t="s">
         <v>264</v>
       </c>
@@ -20846,7 +20852,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="392" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A392" s="8" t="s">
         <v>378</v>
       </c>
@@ -20893,7 +20899,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="393" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A393" s="8" t="s">
         <v>378</v>
       </c>
@@ -20940,7 +20946,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="394" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A394" s="8" t="s">
         <v>378</v>
       </c>
@@ -20987,7 +20993,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="395" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A395" s="8" t="s">
         <v>378</v>
       </c>
@@ -21026,7 +21032,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="396" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A396" s="8" t="s">
         <v>605</v>
       </c>
@@ -21073,7 +21079,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="397" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A397" s="8" t="s">
         <v>605</v>
       </c>
@@ -21119,17 +21125,6 @@
       <c r="O397" s="8">
         <v>396</v>
       </c>
-    </row>
-    <row r="398" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A398" t="s">
-        <v>7</v>
-      </c>
-      <c r="B398" t="s">
-        <v>492</v>
-      </c>
-      <c r="G398" s="9"/>
-      <c r="I398" s="10"/>
-      <c r="J398" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21142,23 +21137,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3">
         <v>42361</v>
       </c>
@@ -21166,7 +21161,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3">
         <v>42369</v>
       </c>
@@ -21174,7 +21169,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3">
         <v>42371</v>
       </c>
@@ -21182,7 +21177,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3">
         <v>42372</v>
       </c>
@@ -21190,7 +21185,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3">
         <v>42373</v>
       </c>
@@ -21198,7 +21193,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3">
         <v>42382</v>
       </c>
@@ -21206,7 +21201,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3">
         <v>42385</v>
       </c>
@@ -21214,7 +21209,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3">
         <v>42387</v>
       </c>
@@ -21222,7 +21217,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3">
         <v>42388</v>
       </c>
@@ -21230,7 +21225,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3">
         <v>42390</v>
       </c>
@@ -21238,7 +21233,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3">
         <v>42391</v>
       </c>
@@ -21246,7 +21241,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3">
         <v>42400</v>
       </c>
@@ -21254,7 +21249,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="3">
         <v>42414</v>
       </c>
@@ -21262,7 +21257,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="3">
         <v>42432</v>
       </c>
@@ -21273,7 +21268,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3">
         <v>42435</v>
       </c>
@@ -21281,7 +21276,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="3">
         <v>42436</v>
       </c>
@@ -21289,7 +21284,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="3">
         <v>42441</v>
       </c>
@@ -21297,7 +21292,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="3">
         <v>42445</v>
       </c>
@@ -21305,7 +21300,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="3">
         <v>42453</v>
       </c>
@@ -21313,7 +21308,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="3">
         <v>42456</v>
       </c>
@@ -21321,7 +21316,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="3">
         <v>42457</v>
       </c>
@@ -21329,7 +21324,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="3">
         <v>42458</v>
       </c>
@@ -21337,7 +21332,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="3">
         <v>42464</v>
       </c>
@@ -21345,7 +21340,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="3">
         <v>42510</v>
       </c>
@@ -21353,7 +21348,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="3">
         <v>42515</v>
       </c>
@@ -21361,7 +21356,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="3">
         <v>42560</v>
       </c>
@@ -21369,7 +21364,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="3">
         <v>42565</v>
       </c>
@@ -21377,7 +21372,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="3">
         <v>42576</v>
       </c>
@@ -21385,7 +21380,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="3">
         <v>42590</v>
       </c>
@@ -21393,7 +21388,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="3">
         <v>42593</v>
       </c>
@@ -21401,7 +21396,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="3">
         <v>42598</v>
       </c>
@@ -21409,7 +21404,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="3">
         <v>42665</v>
       </c>
@@ -21417,7 +21412,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="3">
         <v>42788</v>
       </c>
@@ -21425,7 +21420,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="3">
         <v>42831</v>
       </c>
@@ -21433,7 +21428,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="14">
         <v>42833</v>
       </c>
@@ -21441,7 +21436,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="14">
         <v>42833</v>
       </c>
@@ -21449,7 +21444,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="14">
         <v>42874</v>
       </c>
@@ -21457,12 +21452,28 @@
         <v>610</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="14">
+        <v>42876</v>
+      </c>
+      <c r="B40" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="14">
         <v>42878</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>611</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="14">
+        <v>42878</v>
+      </c>
+      <c r="B42" t="s">
+        <v>613</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Sont FE 85mm f/1.8
</commit_message>
<xml_diff>
--- a/BigAssTableOfLenses.xlsx
+++ b/BigAssTableOfLenses.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Markus\Desktop\BATOL\BigAssTableOfLenses\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Markus\Desktop\olaff\Olaf-Optical-Testing-Software\Matlab\Support Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8928" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8928"/>
   </bookViews>
   <sheets>
     <sheet name="LensTable" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2338" uniqueCount="614">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2344" uniqueCount="616">
   <si>
     <t>Manufacture</t>
   </si>
@@ -1867,6 +1867,12 @@
   </si>
   <si>
     <t>Removed duplicate CN-E 18-80</t>
+  </si>
+  <si>
+    <t>FE 85mm f/1.8</t>
+  </si>
+  <si>
+    <t>Added Sony FE 85mm f/1.8</t>
   </si>
 </sst>
 </file>
@@ -1960,8 +1966,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O397" totalsRowShown="0">
-  <autoFilter ref="A1:O397"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O398" totalsRowShown="0">
+  <autoFilter ref="A1:O398"/>
   <sortState ref="A2:M314">
     <sortCondition ref="A1:A314"/>
   </sortState>
@@ -2284,10 +2290,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:O397"/>
+  <dimension ref="A1:O398"/>
   <sheetViews>
-    <sheetView topLeftCell="A376" workbookViewId="0">
-      <selection activeCell="D400" sqref="D400"/>
+    <sheetView tabSelected="1" topLeftCell="A376" workbookViewId="0">
+      <selection activeCell="K403" sqref="K403"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -21126,6 +21132,51 @@
         <v>396</v>
       </c>
     </row>
+    <row r="398" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A398" t="s">
+        <v>167</v>
+      </c>
+      <c r="B398" t="s">
+        <v>614</v>
+      </c>
+      <c r="C398">
+        <v>2017</v>
+      </c>
+      <c r="D398">
+        <v>598</v>
+      </c>
+      <c r="E398">
+        <v>371</v>
+      </c>
+      <c r="F398">
+        <v>82</v>
+      </c>
+      <c r="G398" s="9">
+        <v>78</v>
+      </c>
+      <c r="H398" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="I398" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="J398" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="K398">
+        <v>0</v>
+      </c>
+      <c r="L398">
+        <v>0</v>
+      </c>
+      <c r="M398" t="s">
+        <v>285</v>
+      </c>
+      <c r="N398" s="11"/>
+      <c r="O398">
+        <v>397</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -21137,10 +21188,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -21476,6 +21527,14 @@
         <v>613</v>
       </c>
     </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="14">
+        <v>42891</v>
+      </c>
+      <c r="B43" t="s">
+        <v>615</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert "Added Sont FE 85mm f/1.8"
This reverts commit 665478b84f321c46ac71fcc651dc1dc3b2d449b3.
</commit_message>
<xml_diff>
--- a/BigAssTableOfLenses.xlsx
+++ b/BigAssTableOfLenses.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Markus\Desktop\olaff\Olaf-Optical-Testing-Software\Matlab\Support Scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Markus\Desktop\BATOL\BigAssTableOfLenses\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8928"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8928" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LensTable" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2344" uniqueCount="616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2338" uniqueCount="614">
   <si>
     <t>Manufacture</t>
   </si>
@@ -1867,12 +1867,6 @@
   </si>
   <si>
     <t>Removed duplicate CN-E 18-80</t>
-  </si>
-  <si>
-    <t>FE 85mm f/1.8</t>
-  </si>
-  <si>
-    <t>Added Sony FE 85mm f/1.8</t>
   </si>
 </sst>
 </file>
@@ -1966,8 +1960,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O398" totalsRowShown="0">
-  <autoFilter ref="A1:O398"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O397" totalsRowShown="0">
+  <autoFilter ref="A1:O397"/>
   <sortState ref="A2:M314">
     <sortCondition ref="A1:A314"/>
   </sortState>
@@ -2290,10 +2284,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:O398"/>
+  <dimension ref="A1:O397"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A376" workbookViewId="0">
-      <selection activeCell="K403" sqref="K403"/>
+    <sheetView topLeftCell="A376" workbookViewId="0">
+      <selection activeCell="D400" sqref="D400"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -21132,51 +21126,6 @@
         <v>396</v>
       </c>
     </row>
-    <row r="398" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A398" t="s">
-        <v>167</v>
-      </c>
-      <c r="B398" t="s">
-        <v>614</v>
-      </c>
-      <c r="C398">
-        <v>2017</v>
-      </c>
-      <c r="D398">
-        <v>598</v>
-      </c>
-      <c r="E398">
-        <v>371</v>
-      </c>
-      <c r="F398">
-        <v>82</v>
-      </c>
-      <c r="G398" s="9">
-        <v>78</v>
-      </c>
-      <c r="H398" s="1">
-        <v>1.8</v>
-      </c>
-      <c r="I398" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="J398" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="K398">
-        <v>0</v>
-      </c>
-      <c r="L398">
-        <v>0</v>
-      </c>
-      <c r="M398" t="s">
-        <v>285</v>
-      </c>
-      <c r="N398" s="11"/>
-      <c r="O398">
-        <v>397</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -21188,10 +21137,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -21527,14 +21476,6 @@
         <v>613</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="14">
-        <v>42891</v>
-      </c>
-      <c r="B43" t="s">
-        <v>615</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Sony FE 85mm f/1.8
</commit_message>
<xml_diff>
--- a/BigAssTableOfLenses.xlsx
+++ b/BigAssTableOfLenses.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brand\Optics\Olaf\Software\BigAssTableOfLenses\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Markus\Desktop\BATOL\BigAssTableOfLenses\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8928" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8928"/>
   </bookViews>
   <sheets>
     <sheet name="LensTable" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3008" uniqueCount="633">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3014" uniqueCount="635">
   <si>
     <t>Manufacture</t>
   </si>
@@ -1924,6 +1924,12 @@
   </si>
   <si>
     <t>New Designed in and Made In columns (needs substantial additions).  Variety for CN-E 14.5-45mm, Format for Angenieux Lenses</t>
+  </si>
+  <si>
+    <t>FE 85mm f/1.8</t>
+  </si>
+  <si>
+    <t>Added Sony FE 85mm f/1.8</t>
   </si>
 </sst>
 </file>
@@ -2016,8 +2022,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q402" totalsRowShown="0">
-  <autoFilter ref="A1:Q402">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q403" totalsRowShown="0">
+  <autoFilter ref="A1:Q403">
     <filterColumn colId="11">
       <filters>
         <filter val="0"/>
@@ -2348,30 +2354,30 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q402"/>
+  <dimension ref="A1:Q403"/>
   <sheetViews>
-    <sheetView topLeftCell="A389" workbookViewId="0">
-      <selection activeCell="O396" sqref="O396"/>
+    <sheetView tabSelected="1" topLeftCell="A321" workbookViewId="0">
+      <selection activeCell="B406" sqref="B406"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="8.109375" customWidth="1"/>
-    <col min="2" max="2" width="37.88671875" customWidth="1"/>
-    <col min="3" max="3" width="5.44140625" customWidth="1"/>
-    <col min="4" max="4" width="6.44140625" customWidth="1"/>
-    <col min="5" max="5" width="8.21875" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.109375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="5.88671875" style="4" customWidth="1"/>
-    <col min="11" max="11" width="10.21875" customWidth="1"/>
+    <col min="1" max="1" width="8.1015625" customWidth="1"/>
+    <col min="2" max="2" width="37.89453125" customWidth="1"/>
+    <col min="3" max="3" width="5.41796875" customWidth="1"/>
+    <col min="4" max="4" width="6.41796875" customWidth="1"/>
+    <col min="5" max="5" width="8.20703125" customWidth="1"/>
+    <col min="7" max="7" width="8.68359375" customWidth="1"/>
+    <col min="8" max="8" width="12.41796875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.1015625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="5.89453125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="10.20703125" customWidth="1"/>
     <col min="12" max="12" width="9" customWidth="1"/>
-    <col min="13" max="13" width="11.6640625" customWidth="1"/>
-    <col min="15" max="16" width="8.88671875" style="12"/>
+    <col min="13" max="13" width="11.68359375" customWidth="1"/>
+    <col min="15" max="16" width="8.89453125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2424,7 +2430,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -2479,7 +2485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -2534,7 +2540,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -2589,7 +2595,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -2644,7 +2650,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -2699,7 +2705,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -2754,7 +2760,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -2809,7 +2815,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2864,7 +2870,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2919,7 +2925,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -2974,7 +2980,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -3029,7 +3035,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -3084,7 +3090,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -3139,7 +3145,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
@@ -3194,7 +3200,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
@@ -3249,7 +3255,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
@@ -3304,7 +3310,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
@@ -3359,7 +3365,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -3414,7 +3420,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
@@ -3469,7 +3475,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
@@ -3524,7 +3530,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
@@ -3579,7 +3585,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
@@ -3634,7 +3640,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
@@ -3689,7 +3695,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
@@ -3744,7 +3750,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
@@ -3799,7 +3805,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
@@ -3854,7 +3860,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1" t="s">
         <v>7</v>
       </c>
@@ -3909,7 +3915,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="1" t="s">
         <v>7</v>
       </c>
@@ -3964,7 +3970,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1" t="s">
         <v>7</v>
       </c>
@@ -4019,7 +4025,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="1" t="s">
         <v>7</v>
       </c>
@@ -4074,7 +4080,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="1" t="s">
         <v>7</v>
       </c>
@@ -4129,7 +4135,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
@@ -4184,7 +4190,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="1" t="s">
         <v>7</v>
       </c>
@@ -4239,7 +4245,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="1" t="s">
         <v>7</v>
       </c>
@@ -4294,7 +4300,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="1" t="s">
         <v>7</v>
       </c>
@@ -4349,7 +4355,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="1" t="s">
         <v>7</v>
       </c>
@@ -4404,7 +4410,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -4459,7 +4465,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -4514,7 +4520,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -4569,7 +4575,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>7</v>
       </c>
@@ -4624,7 +4630,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>7</v>
       </c>
@@ -4679,7 +4685,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>7</v>
       </c>
@@ -4734,7 +4740,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -4787,7 +4793,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>7</v>
       </c>
@@ -4842,7 +4848,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
         <v>7</v>
       </c>
@@ -4897,7 +4903,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
         <v>7</v>
       </c>
@@ -4952,7 +4958,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
         <v>7</v>
       </c>
@@ -5007,7 +5013,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
         <v>7</v>
       </c>
@@ -5062,7 +5068,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
         <v>7</v>
       </c>
@@ -5117,7 +5123,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
         <v>7</v>
       </c>
@@ -5172,7 +5178,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -5227,7 +5233,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
         <v>7</v>
       </c>
@@ -5282,7 +5288,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
         <v>7</v>
       </c>
@@ -5337,7 +5343,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
         <v>7</v>
       </c>
@@ -5392,7 +5398,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="1" t="s">
         <v>7</v>
       </c>
@@ -5447,7 +5453,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="1" t="s">
         <v>7</v>
       </c>
@@ -5502,7 +5508,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="1" t="s">
         <v>7</v>
       </c>
@@ -5557,7 +5563,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="1" t="s">
         <v>7</v>
       </c>
@@ -5612,7 +5618,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="1" t="s">
         <v>7</v>
       </c>
@@ -5667,7 +5673,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="1" t="s">
         <v>7</v>
       </c>
@@ -5720,7 +5726,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="1" t="s">
         <v>7</v>
       </c>
@@ -5775,7 +5781,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="1" t="s">
         <v>7</v>
       </c>
@@ -5828,7 +5834,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="1" t="s">
         <v>7</v>
       </c>
@@ -5881,7 +5887,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="1" t="s">
         <v>7</v>
       </c>
@@ -5934,7 +5940,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="1" t="s">
         <v>7</v>
       </c>
@@ -5987,7 +5993,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="1" t="s">
         <v>7</v>
       </c>
@@ -6040,7 +6046,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="1" t="s">
         <v>378</v>
       </c>
@@ -6093,7 +6099,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="1" t="s">
         <v>378</v>
       </c>
@@ -6146,7 +6152,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="1" t="s">
         <v>378</v>
       </c>
@@ -6199,7 +6205,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="1" t="s">
         <v>378</v>
       </c>
@@ -6252,7 +6258,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="1" t="s">
         <v>378</v>
       </c>
@@ -6305,7 +6311,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="1" t="s">
         <v>378</v>
       </c>
@@ -6358,7 +6364,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="1" t="s">
         <v>378</v>
       </c>
@@ -6411,7 +6417,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="1" t="s">
         <v>378</v>
       </c>
@@ -6464,7 +6470,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="1" t="s">
         <v>378</v>
       </c>
@@ -6517,7 +6523,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="1" t="s">
         <v>378</v>
       </c>
@@ -6570,7 +6576,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="1" t="s">
         <v>378</v>
       </c>
@@ -6623,7 +6629,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="1" t="s">
         <v>378</v>
       </c>
@@ -6676,7 +6682,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="1" t="s">
         <v>378</v>
       </c>
@@ -6729,7 +6735,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="1" t="s">
         <v>378</v>
       </c>
@@ -6782,7 +6788,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="1" t="s">
         <v>378</v>
       </c>
@@ -6835,7 +6841,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="1" t="s">
         <v>378</v>
       </c>
@@ -6888,7 +6894,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="1" t="s">
         <v>378</v>
       </c>
@@ -6941,7 +6947,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="1" t="s">
         <v>378</v>
       </c>
@@ -6994,7 +7000,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="1" t="s">
         <v>378</v>
       </c>
@@ -7047,7 +7053,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="1" t="s">
         <v>378</v>
       </c>
@@ -7100,7 +7106,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="1" t="s">
         <v>378</v>
       </c>
@@ -7150,7 +7156,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="1" t="s">
         <v>294</v>
       </c>
@@ -7199,7 +7205,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="1" t="s">
         <v>429</v>
       </c>
@@ -7246,7 +7252,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="1" t="s">
         <v>429</v>
       </c>
@@ -7293,7 +7299,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="1" t="s">
         <v>233</v>
       </c>
@@ -7346,7 +7352,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="1" t="s">
         <v>233</v>
       </c>
@@ -7399,7 +7405,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="1" t="s">
         <v>233</v>
       </c>
@@ -7452,7 +7458,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="1" t="s">
         <v>233</v>
       </c>
@@ -7505,7 +7511,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="1" t="s">
         <v>233</v>
       </c>
@@ -7558,7 +7564,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="1" t="s">
         <v>233</v>
       </c>
@@ -7611,7 +7617,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="1" t="s">
         <v>233</v>
       </c>
@@ -7666,7 +7672,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="1" t="s">
         <v>233</v>
       </c>
@@ -7722,7 +7728,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="1" t="s">
         <v>233</v>
       </c>
@@ -7777,7 +7783,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="1" t="s">
         <v>233</v>
       </c>
@@ -7830,7 +7836,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" t="s">
         <v>233</v>
       </c>
@@ -7883,7 +7889,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" t="s">
         <v>233</v>
       </c>
@@ -7936,7 +7942,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" t="s">
         <v>233</v>
       </c>
@@ -7989,7 +7995,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
         <v>233</v>
       </c>
@@ -8042,7 +8048,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="s">
         <v>233</v>
       </c>
@@ -8095,7 +8101,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="s">
         <v>233</v>
       </c>
@@ -8151,7 +8157,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" t="s">
         <v>233</v>
       </c>
@@ -8204,7 +8210,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" t="s">
         <v>233</v>
       </c>
@@ -8257,7 +8263,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" t="s">
         <v>233</v>
       </c>
@@ -8310,7 +8316,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" t="s">
         <v>233</v>
       </c>
@@ -8363,7 +8369,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" t="s">
         <v>233</v>
       </c>
@@ -8416,7 +8422,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" t="s">
         <v>233</v>
       </c>
@@ -8469,7 +8475,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" t="s">
         <v>233</v>
       </c>
@@ -8522,7 +8528,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" t="s">
         <v>233</v>
       </c>
@@ -8575,7 +8581,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" t="s">
         <v>233</v>
       </c>
@@ -8631,7 +8637,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" t="s">
         <v>233</v>
       </c>
@@ -8687,7 +8693,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" t="s">
         <v>233</v>
       </c>
@@ -8740,7 +8746,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" t="s">
         <v>233</v>
       </c>
@@ -8793,7 +8799,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" t="s">
         <v>233</v>
       </c>
@@ -8846,7 +8852,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" t="s">
         <v>296</v>
       </c>
@@ -8901,7 +8907,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" t="s">
         <v>296</v>
       </c>
@@ -8956,7 +8962,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" t="s">
         <v>296</v>
       </c>
@@ -9011,7 +9017,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" t="s">
         <v>59</v>
       </c>
@@ -9063,7 +9069,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" t="s">
         <v>59</v>
       </c>
@@ -9115,7 +9121,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" t="s">
         <v>59</v>
       </c>
@@ -9167,7 +9173,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" t="s">
         <v>59</v>
       </c>
@@ -9219,7 +9225,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" t="s">
         <v>59</v>
       </c>
@@ -9271,7 +9277,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" t="s">
         <v>59</v>
       </c>
@@ -9323,7 +9329,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" t="s">
         <v>59</v>
       </c>
@@ -9375,7 +9381,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" t="s">
         <v>59</v>
       </c>
@@ -9427,7 +9433,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" t="s">
         <v>59</v>
       </c>
@@ -9479,7 +9485,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" t="s">
         <v>59</v>
       </c>
@@ -9531,7 +9537,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" t="s">
         <v>59</v>
       </c>
@@ -9583,7 +9589,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" t="s">
         <v>59</v>
       </c>
@@ -9635,7 +9641,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" t="s">
         <v>59</v>
       </c>
@@ -9687,7 +9693,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" t="s">
         <v>59</v>
       </c>
@@ -9739,7 +9745,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" t="s">
         <v>59</v>
       </c>
@@ -9791,7 +9797,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" t="s">
         <v>59</v>
       </c>
@@ -9844,7 +9850,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" t="s">
         <v>59</v>
       </c>
@@ -9896,7 +9902,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" t="s">
         <v>59</v>
       </c>
@@ -9948,7 +9954,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="142" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="1" t="s">
         <v>59</v>
       </c>
@@ -10001,7 +10007,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="1" t="s">
         <v>59</v>
       </c>
@@ -10054,7 +10060,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="1" t="s">
         <v>59</v>
       </c>
@@ -10107,7 +10113,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="145" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="1" t="s">
         <v>59</v>
       </c>
@@ -10160,7 +10166,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="1" t="s">
         <v>59</v>
       </c>
@@ -10213,7 +10219,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" t="s">
         <v>59</v>
       </c>
@@ -10265,7 +10271,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" t="s">
         <v>59</v>
       </c>
@@ -10317,7 +10323,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" t="s">
         <v>59</v>
       </c>
@@ -10369,7 +10375,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" t="s">
         <v>59</v>
       </c>
@@ -10421,7 +10427,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" t="s">
         <v>59</v>
       </c>
@@ -10473,7 +10479,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" t="s">
         <v>59</v>
       </c>
@@ -10525,7 +10531,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" t="s">
         <v>59</v>
       </c>
@@ -10577,7 +10583,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" t="s">
         <v>59</v>
       </c>
@@ -10629,7 +10635,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" t="s">
         <v>59</v>
       </c>
@@ -10681,7 +10687,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" t="s">
         <v>59</v>
       </c>
@@ -10731,7 +10737,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" t="s">
         <v>59</v>
       </c>
@@ -10781,7 +10787,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" t="s">
         <v>59</v>
       </c>
@@ -10831,7 +10837,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" t="s">
         <v>59</v>
       </c>
@@ -10881,7 +10887,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" t="s">
         <v>59</v>
       </c>
@@ -10931,7 +10937,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="161" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" t="s">
         <v>371</v>
       </c>
@@ -10981,7 +10987,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="162" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" t="s">
         <v>371</v>
       </c>
@@ -11031,7 +11037,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="163" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" t="s">
         <v>371</v>
       </c>
@@ -11081,7 +11087,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="164" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" t="s">
         <v>438</v>
       </c>
@@ -11131,7 +11137,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="165" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" t="s">
         <v>438</v>
       </c>
@@ -11181,7 +11187,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="166" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" t="s">
         <v>438</v>
       </c>
@@ -11231,7 +11237,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="167" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" t="s">
         <v>100</v>
       </c>
@@ -11280,7 +11286,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="168" spans="1:17" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:17" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" s="1" t="s">
         <v>100</v>
       </c>
@@ -11329,7 +11335,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="169" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" t="s">
         <v>100</v>
       </c>
@@ -11379,7 +11385,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="170" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" t="s">
         <v>100</v>
       </c>
@@ -11426,7 +11432,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="171" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" t="s">
         <v>100</v>
       </c>
@@ -11475,7 +11481,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="172" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" t="s">
         <v>100</v>
       </c>
@@ -11522,7 +11528,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="173" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" t="s">
         <v>100</v>
       </c>
@@ -11571,7 +11577,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="174" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" t="s">
         <v>100</v>
       </c>
@@ -11618,7 +11624,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="175" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" t="s">
         <v>100</v>
       </c>
@@ -11667,7 +11673,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="176" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" t="s">
         <v>100</v>
       </c>
@@ -11714,7 +11720,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="177" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" t="s">
         <v>100</v>
       </c>
@@ -11761,7 +11767,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="178" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" t="s">
         <v>100</v>
       </c>
@@ -11808,7 +11814,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="179" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" t="s">
         <v>219</v>
       </c>
@@ -11863,7 +11869,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="180" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" t="s">
         <v>219</v>
       </c>
@@ -11918,7 +11924,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="181" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" t="s">
         <v>219</v>
       </c>
@@ -11973,7 +11979,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="182" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" t="s">
         <v>101</v>
       </c>
@@ -12025,7 +12031,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="183" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" t="s">
         <v>101</v>
       </c>
@@ -12077,7 +12083,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="184" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" t="s">
         <v>101</v>
       </c>
@@ -12129,7 +12135,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="185" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" t="s">
         <v>101</v>
       </c>
@@ -12181,7 +12187,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="186" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" t="s">
         <v>101</v>
       </c>
@@ -12233,7 +12239,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="187" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A187" t="s">
         <v>101</v>
       </c>
@@ -12285,7 +12291,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="188" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A188" t="s">
         <v>101</v>
       </c>
@@ -12337,7 +12343,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="189" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A189" t="s">
         <v>101</v>
       </c>
@@ -12389,7 +12395,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="190" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A190" t="s">
         <v>101</v>
       </c>
@@ -12441,7 +12447,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="191" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A191" t="s">
         <v>101</v>
       </c>
@@ -12493,7 +12499,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="192" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A192" t="s">
         <v>101</v>
       </c>
@@ -12545,7 +12551,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="193" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A193" t="s">
         <v>101</v>
       </c>
@@ -12595,7 +12601,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="194" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A194" t="s">
         <v>101</v>
       </c>
@@ -12645,7 +12651,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="195" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A195" t="s">
         <v>101</v>
       </c>
@@ -12692,7 +12698,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="196" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A196" t="s">
         <v>101</v>
       </c>
@@ -12742,7 +12748,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="197" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A197" t="s">
         <v>101</v>
       </c>
@@ -12792,7 +12798,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="198" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A198" t="s">
         <v>101</v>
       </c>
@@ -12842,7 +12848,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="199" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A199" t="s">
         <v>167</v>
       </c>
@@ -12894,7 +12900,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="200" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A200" t="s">
         <v>167</v>
       </c>
@@ -12946,7 +12952,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="201" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A201" t="s">
         <v>167</v>
       </c>
@@ -12998,7 +13004,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="202" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A202" t="s">
         <v>167</v>
       </c>
@@ -13050,7 +13056,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="203" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A203" t="s">
         <v>167</v>
       </c>
@@ -13102,7 +13108,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="204" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A204" t="s">
         <v>167</v>
       </c>
@@ -13154,7 +13160,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="205" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A205" t="s">
         <v>167</v>
       </c>
@@ -13207,7 +13213,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="206" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A206" t="s">
         <v>167</v>
       </c>
@@ -13259,7 +13265,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="207" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A207" t="s">
         <v>167</v>
       </c>
@@ -13311,7 +13317,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="208" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A208" t="s">
         <v>167</v>
       </c>
@@ -13363,7 +13369,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="209" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A209" t="s">
         <v>167</v>
       </c>
@@ -13415,7 +13421,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="210" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A210" t="s">
         <v>167</v>
       </c>
@@ -13467,7 +13473,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="211" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A211" t="s">
         <v>167</v>
       </c>
@@ -13519,7 +13525,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="212" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A212" t="s">
         <v>167</v>
       </c>
@@ -13571,7 +13577,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="213" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A213" t="s">
         <v>167</v>
       </c>
@@ -13623,7 +13629,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="214" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A214" t="s">
         <v>167</v>
       </c>
@@ -13673,7 +13679,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="215" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A215" t="s">
         <v>183</v>
       </c>
@@ -13725,7 +13731,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="216" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A216" t="s">
         <v>183</v>
       </c>
@@ -13777,7 +13783,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="217" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A217" t="s">
         <v>183</v>
       </c>
@@ -13829,7 +13835,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="218" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A218" t="s">
         <v>183</v>
       </c>
@@ -13881,7 +13887,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="219" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A219" t="s">
         <v>183</v>
       </c>
@@ -13933,7 +13939,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="220" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A220" t="s">
         <v>183</v>
       </c>
@@ -13985,7 +13991,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="221" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A221" t="s">
         <v>183</v>
       </c>
@@ -14037,7 +14043,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="222" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A222" t="s">
         <v>183</v>
       </c>
@@ -14089,7 +14095,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="223" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A223" t="s">
         <v>183</v>
       </c>
@@ -14141,7 +14147,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="224" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A224" t="s">
         <v>183</v>
       </c>
@@ -14191,7 +14197,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="225" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A225" s="1" t="s">
         <v>183</v>
       </c>
@@ -14241,7 +14247,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="226" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A226" s="1" t="s">
         <v>183</v>
       </c>
@@ -14291,7 +14297,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="227" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A227" t="s">
         <v>192</v>
       </c>
@@ -14343,7 +14349,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="228" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A228" t="s">
         <v>192</v>
       </c>
@@ -14395,7 +14401,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="229" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A229" t="s">
         <v>192</v>
       </c>
@@ -14447,7 +14453,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="230" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A230" t="s">
         <v>192</v>
       </c>
@@ -14499,7 +14505,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="231" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A231" t="s">
         <v>192</v>
       </c>
@@ -14551,7 +14557,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="232" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A232" t="s">
         <v>192</v>
       </c>
@@ -14601,7 +14607,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="233" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A233" t="s">
         <v>264</v>
       </c>
@@ -14654,7 +14660,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="234" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A234" s="1" t="s">
         <v>264</v>
       </c>
@@ -14707,7 +14713,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="235" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A235" s="1" t="s">
         <v>264</v>
       </c>
@@ -14760,7 +14766,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="236" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A236" s="1" t="s">
         <v>264</v>
       </c>
@@ -14813,7 +14819,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="237" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A237" s="1" t="s">
         <v>221</v>
       </c>
@@ -14862,7 +14868,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="238" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A238" s="1" t="s">
         <v>221</v>
       </c>
@@ -14909,7 +14915,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="239" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A239" s="1" t="s">
         <v>221</v>
       </c>
@@ -14956,7 +14962,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="240" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A240" s="1" t="s">
         <v>221</v>
       </c>
@@ -15005,7 +15011,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="241" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A241" s="1" t="s">
         <v>221</v>
       </c>
@@ -15052,7 +15058,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="242" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A242" s="1" t="s">
         <v>221</v>
       </c>
@@ -15099,7 +15105,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="243" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A243" s="1" t="s">
         <v>221</v>
       </c>
@@ -15146,7 +15152,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="244" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A244" s="1" t="s">
         <v>221</v>
       </c>
@@ -15195,7 +15201,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="245" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A245" s="1" t="s">
         <v>221</v>
       </c>
@@ -15242,7 +15248,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="246" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A246" s="1" t="s">
         <v>221</v>
       </c>
@@ -15289,7 +15295,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="247" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A247" t="s">
         <v>221</v>
       </c>
@@ -15336,7 +15342,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="248" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A248" t="s">
         <v>221</v>
       </c>
@@ -15383,7 +15389,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="249" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A249" t="s">
         <v>221</v>
       </c>
@@ -15430,7 +15436,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="250" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A250" t="s">
         <v>221</v>
       </c>
@@ -15479,7 +15485,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="251" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A251" t="s">
         <v>221</v>
       </c>
@@ -15526,7 +15532,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="252" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A252" s="1" t="s">
         <v>221</v>
       </c>
@@ -15573,7 +15579,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="253" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A253" s="1" t="s">
         <v>221</v>
       </c>
@@ -15620,7 +15626,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="254" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A254" t="s">
         <v>133</v>
       </c>
@@ -15675,7 +15681,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="255" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A255" t="s">
         <v>133</v>
       </c>
@@ -15728,7 +15734,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="256" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A256" t="s">
         <v>133</v>
       </c>
@@ -15781,7 +15787,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="257" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A257" t="s">
         <v>133</v>
       </c>
@@ -15836,7 +15842,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="258" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A258" t="s">
         <v>133</v>
       </c>
@@ -15889,7 +15895,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="259" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A259" t="s">
         <v>133</v>
       </c>
@@ -15942,7 +15948,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="260" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A260" t="s">
         <v>133</v>
       </c>
@@ -15997,7 +16003,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="261" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A261" t="s">
         <v>133</v>
       </c>
@@ -16052,7 +16058,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="262" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A262" t="s">
         <v>133</v>
       </c>
@@ -16107,7 +16113,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="263" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A263" t="s">
         <v>133</v>
       </c>
@@ -16160,7 +16166,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="264" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A264" t="s">
         <v>133</v>
       </c>
@@ -16213,7 +16219,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="265" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A265" t="s">
         <v>133</v>
       </c>
@@ -16266,7 +16272,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="266" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A266" t="s">
         <v>133</v>
       </c>
@@ -16321,7 +16327,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="267" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A267" t="s">
         <v>133</v>
       </c>
@@ -16376,7 +16382,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="268" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A268" s="1" t="s">
         <v>133</v>
       </c>
@@ -16431,7 +16437,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="269" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A269" s="1" t="s">
         <v>133</v>
       </c>
@@ -16484,7 +16490,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="270" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A270" t="s">
         <v>133</v>
       </c>
@@ -16537,7 +16543,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="271" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A271" t="s">
         <v>133</v>
       </c>
@@ -16592,7 +16598,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="272" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A272" t="s">
         <v>133</v>
       </c>
@@ -16647,7 +16653,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="273" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A273" t="s">
         <v>133</v>
       </c>
@@ -16700,7 +16706,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="274" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A274" t="s">
         <v>133</v>
       </c>
@@ -16753,7 +16759,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="275" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A275" t="s">
         <v>133</v>
       </c>
@@ -16808,7 +16814,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="276" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A276" t="s">
         <v>133</v>
       </c>
@@ -16863,7 +16869,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="277" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A277" t="s">
         <v>133</v>
       </c>
@@ -16918,7 +16924,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="278" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A278" t="s">
         <v>133</v>
       </c>
@@ -16973,7 +16979,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="279" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A279" t="s">
         <v>133</v>
       </c>
@@ -17026,7 +17032,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="280" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A280" t="s">
         <v>133</v>
       </c>
@@ -17079,7 +17085,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="281" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A281" t="s">
         <v>133</v>
       </c>
@@ -17132,7 +17138,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="282" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A282" t="s">
         <v>133</v>
       </c>
@@ -17185,7 +17191,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="283" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A283" t="s">
         <v>133</v>
       </c>
@@ -17238,7 +17244,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="284" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A284" t="s">
         <v>133</v>
       </c>
@@ -17293,7 +17299,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="285" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A285" t="s">
         <v>133</v>
       </c>
@@ -17348,7 +17354,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="286" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A286" t="s">
         <v>133</v>
       </c>
@@ -17403,7 +17409,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="287" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A287" t="s">
         <v>133</v>
       </c>
@@ -17458,7 +17464,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="288" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A288" t="s">
         <v>133</v>
       </c>
@@ -17513,7 +17519,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="289" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A289" t="s">
         <v>133</v>
       </c>
@@ -17566,7 +17572,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="290" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A290" t="s">
         <v>133</v>
       </c>
@@ -17619,7 +17625,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="291" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A291" t="s">
         <v>133</v>
       </c>
@@ -17672,7 +17678,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="292" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A292" t="s">
         <v>133</v>
       </c>
@@ -17725,7 +17731,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="293" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A293" t="s">
         <v>133</v>
       </c>
@@ -17778,7 +17784,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="294" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A294" t="s">
         <v>133</v>
       </c>
@@ -17833,7 +17839,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="295" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A295" t="s">
         <v>133</v>
       </c>
@@ -17888,7 +17894,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="296" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A296" t="s">
         <v>133</v>
       </c>
@@ -17943,7 +17949,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="297" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A297" t="s">
         <v>133</v>
       </c>
@@ -17998,7 +18004,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="298" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A298" t="s">
         <v>133</v>
       </c>
@@ -18053,7 +18059,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="299" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A299" t="s">
         <v>133</v>
       </c>
@@ -18106,7 +18112,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="300" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A300" t="s">
         <v>133</v>
       </c>
@@ -18159,7 +18165,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="301" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A301" t="s">
         <v>133</v>
       </c>
@@ -18212,7 +18218,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="302" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A302" t="s">
         <v>133</v>
       </c>
@@ -18267,7 +18273,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="303" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A303" t="s">
         <v>133</v>
       </c>
@@ -18322,7 +18328,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="304" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A304" t="s">
         <v>133</v>
       </c>
@@ -18375,7 +18381,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="305" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A305" t="s">
         <v>133</v>
       </c>
@@ -18430,7 +18436,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="306" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A306" t="s">
         <v>133</v>
       </c>
@@ -18483,7 +18489,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="307" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A307" t="s">
         <v>133</v>
       </c>
@@ -18536,7 +18542,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="308" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A308" t="s">
         <v>133</v>
       </c>
@@ -18589,7 +18595,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="309" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A309" t="s">
         <v>133</v>
       </c>
@@ -18642,7 +18648,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="310" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A310" t="s">
         <v>133</v>
       </c>
@@ -18695,7 +18701,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="311" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A311" t="s">
         <v>133</v>
       </c>
@@ -18748,7 +18754,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="312" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A312" t="s">
         <v>133</v>
       </c>
@@ -18801,7 +18807,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="313" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A313" t="s">
         <v>133</v>
       </c>
@@ -18854,7 +18860,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="314" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A314" t="s">
         <v>133</v>
       </c>
@@ -18907,7 +18913,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="315" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A315" t="s">
         <v>378</v>
       </c>
@@ -18960,7 +18966,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="316" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A316" t="s">
         <v>378</v>
       </c>
@@ -19013,7 +19019,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="317" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A317" t="s">
         <v>101</v>
       </c>
@@ -19061,7 +19067,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="318" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A318" t="s">
         <v>101</v>
       </c>
@@ -19109,7 +19115,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="319" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A319" t="s">
         <v>101</v>
       </c>
@@ -19155,7 +19161,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="320" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A320" t="s">
         <v>101</v>
       </c>
@@ -19203,7 +19209,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="321" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A321" t="s">
         <v>7</v>
       </c>
@@ -19256,7 +19262,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="322" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A322" t="s">
         <v>219</v>
       </c>
@@ -19305,7 +19311,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="323" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A323" t="s">
         <v>219</v>
       </c>
@@ -19354,7 +19360,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="324" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A324" t="s">
         <v>219</v>
       </c>
@@ -19403,7 +19409,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="325" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A325" t="s">
         <v>101</v>
       </c>
@@ -19450,7 +19456,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="326" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A326" t="s">
         <v>192</v>
       </c>
@@ -19497,7 +19503,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="327" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A327" t="s">
         <v>7</v>
       </c>
@@ -19546,7 +19552,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="328" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A328" t="s">
         <v>7</v>
       </c>
@@ -19599,7 +19605,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="329" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A329" t="s">
         <v>7</v>
       </c>
@@ -19652,7 +19658,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="330" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A330" t="s">
         <v>7</v>
       </c>
@@ -19705,7 +19711,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="331" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A331" t="s">
         <v>7</v>
       </c>
@@ -19758,7 +19764,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="332" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A332" t="s">
         <v>219</v>
       </c>
@@ -19807,7 +19813,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="333" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A333" t="s">
         <v>219</v>
       </c>
@@ -19856,7 +19862,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="334" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A334" t="s">
         <v>219</v>
       </c>
@@ -19905,7 +19911,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="335" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A335" t="s">
         <v>219</v>
       </c>
@@ -19954,7 +19960,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="336" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A336" t="s">
         <v>219</v>
       </c>
@@ -20003,7 +20009,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="337" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A337" t="s">
         <v>219</v>
       </c>
@@ -20052,7 +20058,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="338" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A338" t="s">
         <v>505</v>
       </c>
@@ -20103,7 +20109,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="339" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A339" t="s">
         <v>505</v>
       </c>
@@ -20152,7 +20158,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="340" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A340" t="s">
         <v>505</v>
       </c>
@@ -20201,7 +20207,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="341" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A341" t="s">
         <v>505</v>
       </c>
@@ -20250,7 +20256,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="342" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A342" t="s">
         <v>505</v>
       </c>
@@ -20299,7 +20305,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="343" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A343" t="s">
         <v>505</v>
       </c>
@@ -20348,7 +20354,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="344" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A344" t="s">
         <v>505</v>
       </c>
@@ -20397,7 +20403,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="345" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A345" t="s">
         <v>505</v>
       </c>
@@ -20446,7 +20452,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="346" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A346" t="s">
         <v>505</v>
       </c>
@@ -20495,7 +20501,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="347" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A347" t="s">
         <v>505</v>
       </c>
@@ -20544,7 +20550,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="348" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A348" t="s">
         <v>505</v>
       </c>
@@ -20593,7 +20599,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="349" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A349" t="s">
         <v>505</v>
       </c>
@@ -20642,7 +20648,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="350" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A350" t="s">
         <v>505</v>
       </c>
@@ -20691,7 +20697,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="351" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A351" t="s">
         <v>505</v>
       </c>
@@ -20740,7 +20746,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="352" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A352" t="s">
         <v>505</v>
       </c>
@@ -20789,7 +20795,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="353" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A353" t="s">
         <v>505</v>
       </c>
@@ -20838,7 +20844,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="354" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A354" t="s">
         <v>505</v>
       </c>
@@ -20887,7 +20893,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="355" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A355" t="s">
         <v>378</v>
       </c>
@@ -20940,7 +20946,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="356" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A356" t="s">
         <v>378</v>
       </c>
@@ -20993,7 +20999,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="357" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A357" t="s">
         <v>378</v>
       </c>
@@ -21046,7 +21052,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="358" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A358" t="s">
         <v>378</v>
       </c>
@@ -21099,7 +21105,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="359" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A359" t="s">
         <v>378</v>
       </c>
@@ -21152,7 +21158,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="360" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A360" t="s">
         <v>378</v>
       </c>
@@ -21205,7 +21211,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="361" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A361" t="s">
         <v>378</v>
       </c>
@@ -21258,7 +21264,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="362" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A362" t="s">
         <v>378</v>
       </c>
@@ -21311,7 +21317,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="363" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A363" t="s">
         <v>378</v>
       </c>
@@ -21364,7 +21370,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="364" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A364" t="s">
         <v>101</v>
       </c>
@@ -21414,7 +21420,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="365" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A365" t="s">
         <v>101</v>
       </c>
@@ -21464,7 +21470,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="366" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A366" t="s">
         <v>101</v>
       </c>
@@ -21514,7 +21520,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="367" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A367" t="s">
         <v>101</v>
       </c>
@@ -21564,7 +21570,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="368" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A368" t="s">
         <v>101</v>
       </c>
@@ -21614,7 +21620,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="369" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A369" t="s">
         <v>101</v>
       </c>
@@ -21664,7 +21670,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="370" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A370" t="s">
         <v>101</v>
       </c>
@@ -21714,7 +21720,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="371" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A371" t="s">
         <v>101</v>
       </c>
@@ -21764,7 +21770,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="372" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A372" t="s">
         <v>192</v>
       </c>
@@ -21814,7 +21820,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="373" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A373" t="s">
         <v>192</v>
       </c>
@@ -21864,7 +21870,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="374" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A374" t="s">
         <v>192</v>
       </c>
@@ -21914,7 +21920,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="375" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A375" t="s">
         <v>192</v>
       </c>
@@ -21964,7 +21970,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="376" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A376" t="s">
         <v>192</v>
       </c>
@@ -22012,7 +22018,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="377" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A377" t="s">
         <v>192</v>
       </c>
@@ -22062,7 +22068,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="378" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A378" t="s">
         <v>192</v>
       </c>
@@ -22112,7 +22118,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="379" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A379" t="s">
         <v>133</v>
       </c>
@@ -22165,7 +22171,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="380" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A380" t="s">
         <v>7</v>
       </c>
@@ -22218,7 +22224,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="381" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A381" t="s">
         <v>432</v>
       </c>
@@ -22265,7 +22271,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="382" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A382" t="s">
         <v>432</v>
       </c>
@@ -22312,7 +22318,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="383" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A383" t="s">
         <v>432</v>
       </c>
@@ -22359,7 +22365,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="384" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A384" t="s">
         <v>432</v>
       </c>
@@ -22406,7 +22412,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="385" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A385" s="7" t="s">
         <v>183</v>
       </c>
@@ -22456,7 +22462,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="386" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A386" s="7" t="s">
         <v>133</v>
       </c>
@@ -22506,7 +22512,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="387" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A387" s="7" t="s">
         <v>167</v>
       </c>
@@ -22556,7 +22562,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="388" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A388" s="7" t="s">
         <v>167</v>
       </c>
@@ -22606,7 +22612,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="389" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A389" s="7" t="s">
         <v>167</v>
       </c>
@@ -22656,7 +22662,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="390" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A390" s="7" t="s">
         <v>264</v>
       </c>
@@ -22707,7 +22713,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="391" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A391" s="7" t="s">
         <v>264</v>
       </c>
@@ -22760,7 +22766,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="392" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A392" s="7" t="s">
         <v>378</v>
       </c>
@@ -22813,7 +22819,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="393" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A393" s="7" t="s">
         <v>378</v>
       </c>
@@ -22866,7 +22872,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="394" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A394" s="7" t="s">
         <v>378</v>
       </c>
@@ -22919,7 +22925,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="395" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A395" s="7" t="s">
         <v>378</v>
       </c>
@@ -22964,7 +22970,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="396" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A396" s="7" t="s">
         <v>604</v>
       </c>
@@ -23011,7 +23017,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="397" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A397" s="7" t="s">
         <v>604</v>
       </c>
@@ -23058,7 +23064,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="398" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A398" t="s">
         <v>615</v>
       </c>
@@ -23111,7 +23117,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="399" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A399" t="s">
         <v>615</v>
       </c>
@@ -23160,7 +23166,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="400" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A400" t="s">
         <v>59</v>
       </c>
@@ -23210,7 +23216,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="401" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A401" t="s">
         <v>59</v>
       </c>
@@ -23260,7 +23266,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="402" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A402" t="s">
         <v>59</v>
       </c>
@@ -23308,6 +23314,50 @@
       </c>
       <c r="Q402">
         <v>401</v>
+      </c>
+    </row>
+    <row r="403" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A403" t="s">
+        <v>167</v>
+      </c>
+      <c r="B403" t="s">
+        <v>633</v>
+      </c>
+      <c r="C403">
+        <v>2017</v>
+      </c>
+      <c r="D403">
+        <v>598</v>
+      </c>
+      <c r="E403">
+        <v>371</v>
+      </c>
+      <c r="F403">
+        <v>82</v>
+      </c>
+      <c r="G403" s="8">
+        <v>78</v>
+      </c>
+      <c r="H403" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="I403" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="J403" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="K403">
+        <v>0</v>
+      </c>
+      <c r="L403">
+        <v>0</v>
+      </c>
+      <c r="M403" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q403">
+        <v>402</v>
       </c>
     </row>
   </sheetData>
@@ -23321,23 +23371,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="P38" sqref="P38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3">
         <v>42361</v>
       </c>
@@ -23345,7 +23395,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3">
         <v>42369</v>
       </c>
@@ -23353,7 +23403,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3">
         <v>42371</v>
       </c>
@@ -23361,7 +23411,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3">
         <v>42372</v>
       </c>
@@ -23369,7 +23419,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3">
         <v>42373</v>
       </c>
@@ -23377,7 +23427,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3">
         <v>42382</v>
       </c>
@@ -23385,7 +23435,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3">
         <v>42385</v>
       </c>
@@ -23393,7 +23443,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3">
         <v>42387</v>
       </c>
@@ -23401,7 +23451,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3">
         <v>42388</v>
       </c>
@@ -23409,7 +23459,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3">
         <v>42390</v>
       </c>
@@ -23417,7 +23467,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3">
         <v>42391</v>
       </c>
@@ -23425,7 +23475,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3">
         <v>42400</v>
       </c>
@@ -23433,7 +23483,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="3">
         <v>42414</v>
       </c>
@@ -23441,7 +23491,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="3">
         <v>42432</v>
       </c>
@@ -23452,7 +23502,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3">
         <v>42435</v>
       </c>
@@ -23460,7 +23510,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="3">
         <v>42436</v>
       </c>
@@ -23468,7 +23518,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="3">
         <v>42441</v>
       </c>
@@ -23476,7 +23526,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="3">
         <v>42445</v>
       </c>
@@ -23484,7 +23534,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="3">
         <v>42453</v>
       </c>
@@ -23492,7 +23542,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="3">
         <v>42456</v>
       </c>
@@ -23500,7 +23550,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="3">
         <v>42457</v>
       </c>
@@ -23508,7 +23558,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="3">
         <v>42458</v>
       </c>
@@ -23516,7 +23566,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="3">
         <v>42464</v>
       </c>
@@ -23524,7 +23574,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="3">
         <v>42510</v>
       </c>
@@ -23532,7 +23582,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="3">
         <v>42515</v>
       </c>
@@ -23540,7 +23590,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="3">
         <v>42560</v>
       </c>
@@ -23548,7 +23598,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="3">
         <v>42565</v>
       </c>
@@ -23556,7 +23606,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="3">
         <v>42576</v>
       </c>
@@ -23564,7 +23614,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="3">
         <v>42590</v>
       </c>
@@ -23572,7 +23622,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="3">
         <v>42593</v>
       </c>
@@ -23580,7 +23630,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="3">
         <v>42598</v>
       </c>
@@ -23588,7 +23638,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="3">
         <v>42665</v>
       </c>
@@ -23596,7 +23646,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="3">
         <v>42788</v>
       </c>
@@ -23604,7 +23654,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="3">
         <v>42831</v>
       </c>
@@ -23612,7 +23662,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="13">
         <v>42833</v>
       </c>
@@ -23620,7 +23670,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="13">
         <v>42833</v>
       </c>
@@ -23628,7 +23678,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="13">
         <v>42874</v>
       </c>
@@ -23636,7 +23686,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="13">
         <v>42876</v>
       </c>
@@ -23644,7 +23694,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="13">
         <v>42878</v>
       </c>
@@ -23652,7 +23702,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="13">
         <v>42878</v>
       </c>
@@ -23660,7 +23710,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="13">
         <v>42879</v>
       </c>
@@ -23668,7 +23718,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="13">
         <v>42884</v>
       </c>
@@ -23676,7 +23726,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="13">
         <v>42887</v>
       </c>
@@ -23684,12 +23734,20 @@
         <v>624</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="13">
         <v>42887</v>
       </c>
       <c r="B46" t="s">
         <v>632</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="13">
+        <v>42891</v>
+      </c>
+      <c r="B47" t="s">
+        <v>634</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Prices for new sigma lenses
</commit_message>
<xml_diff>
--- a/BigAssTableOfLenses.xlsx
+++ b/BigAssTableOfLenses.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Markus\Desktop\BATOL\BigAssTableOfLenses\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brand\Optics\Olaf\Software\BigAssTableOfLenses\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8928"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8928" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LensTable" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3014" uniqueCount="635">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3015" uniqueCount="636">
   <si>
     <t>Manufacture</t>
   </si>
@@ -1930,6 +1930,9 @@
   </si>
   <si>
     <t>Added Sony FE 85mm f/1.8</t>
+  </si>
+  <si>
+    <t>Prices for new Sigma lenses</t>
   </si>
 </sst>
 </file>
@@ -2356,28 +2359,28 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Q403"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A321" workbookViewId="0">
-      <selection activeCell="B406" sqref="B406"/>
+    <sheetView topLeftCell="A295" workbookViewId="0">
+      <selection activeCell="D320" sqref="D320"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.1015625" customWidth="1"/>
-    <col min="2" max="2" width="37.89453125" customWidth="1"/>
-    <col min="3" max="3" width="5.41796875" customWidth="1"/>
-    <col min="4" max="4" width="6.41796875" customWidth="1"/>
-    <col min="5" max="5" width="8.20703125" customWidth="1"/>
-    <col min="7" max="7" width="8.68359375" customWidth="1"/>
-    <col min="8" max="8" width="12.41796875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.1015625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="5.89453125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="10.20703125" customWidth="1"/>
+    <col min="1" max="1" width="8.109375" customWidth="1"/>
+    <col min="2" max="2" width="37.88671875" customWidth="1"/>
+    <col min="3" max="3" width="5.44140625" customWidth="1"/>
+    <col min="4" max="4" width="6.44140625" customWidth="1"/>
+    <col min="5" max="5" width="8.21875" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.109375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="5.88671875" style="4" customWidth="1"/>
+    <col min="11" max="11" width="10.21875" customWidth="1"/>
     <col min="12" max="12" width="9" customWidth="1"/>
-    <col min="13" max="13" width="11.68359375" customWidth="1"/>
-    <col min="15" max="16" width="8.89453125" style="12"/>
+    <col min="13" max="13" width="11.6640625" customWidth="1"/>
+    <col min="15" max="16" width="8.88671875" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2430,7 +2433,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -2485,7 +2488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -2540,7 +2543,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -2595,7 +2598,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -2650,7 +2653,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -2705,7 +2708,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -2760,7 +2763,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -2815,7 +2818,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2870,7 +2873,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2925,7 +2928,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -2980,7 +2983,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -3035,7 +3038,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -3090,7 +3093,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -3145,7 +3148,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
@@ -3200,7 +3203,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
@@ -3255,7 +3258,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
@@ -3310,7 +3313,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
@@ -3365,7 +3368,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -3420,7 +3423,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
@@ -3475,7 +3478,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
@@ -3530,7 +3533,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
@@ -3585,7 +3588,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
@@ -3640,7 +3643,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
@@ -3695,7 +3698,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
@@ -3750,7 +3753,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
@@ -3805,7 +3808,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
@@ -3860,7 +3863,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>7</v>
       </c>
@@ -3915,7 +3918,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>7</v>
       </c>
@@ -3970,7 +3973,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>7</v>
       </c>
@@ -4025,7 +4028,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>7</v>
       </c>
@@ -4080,7 +4083,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>7</v>
       </c>
@@ -4135,7 +4138,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
@@ -4190,7 +4193,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>7</v>
       </c>
@@ -4245,7 +4248,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>7</v>
       </c>
@@ -4300,7 +4303,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>7</v>
       </c>
@@ -4355,7 +4358,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>7</v>
       </c>
@@ -4410,7 +4413,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -4465,7 +4468,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -4520,7 +4523,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -4575,7 +4578,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>7</v>
       </c>
@@ -4630,7 +4633,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>7</v>
       </c>
@@ -4685,7 +4688,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>7</v>
       </c>
@@ -4740,7 +4743,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -4793,7 +4796,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>7</v>
       </c>
@@ -4848,7 +4851,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>7</v>
       </c>
@@ -4903,7 +4906,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>7</v>
       </c>
@@ -4958,7 +4961,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>7</v>
       </c>
@@ -5013,7 +5016,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>7</v>
       </c>
@@ -5068,7 +5071,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>7</v>
       </c>
@@ -5123,7 +5126,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>7</v>
       </c>
@@ -5178,7 +5181,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -5233,7 +5236,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>7</v>
       </c>
@@ -5288,7 +5291,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>7</v>
       </c>
@@ -5343,7 +5346,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>7</v>
       </c>
@@ -5398,7 +5401,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>7</v>
       </c>
@@ -5453,7 +5456,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>7</v>
       </c>
@@ -5508,7 +5511,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>7</v>
       </c>
@@ -5563,7 +5566,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>7</v>
       </c>
@@ -5618,7 +5621,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>7</v>
       </c>
@@ -5673,7 +5676,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>7</v>
       </c>
@@ -5726,7 +5729,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>7</v>
       </c>
@@ -5781,7 +5784,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>7</v>
       </c>
@@ -5834,7 +5837,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>7</v>
       </c>
@@ -5887,7 +5890,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>7</v>
       </c>
@@ -5940,7 +5943,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>7</v>
       </c>
@@ -5993,7 +5996,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>7</v>
       </c>
@@ -6046,7 +6049,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>378</v>
       </c>
@@ -6099,7 +6102,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>378</v>
       </c>
@@ -6152,7 +6155,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>378</v>
       </c>
@@ -6205,7 +6208,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>378</v>
       </c>
@@ -6258,7 +6261,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>378</v>
       </c>
@@ -6311,7 +6314,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>378</v>
       </c>
@@ -6364,7 +6367,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>378</v>
       </c>
@@ -6417,7 +6420,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>378</v>
       </c>
@@ -6470,7 +6473,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>378</v>
       </c>
@@ -6523,7 +6526,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>378</v>
       </c>
@@ -6576,7 +6579,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>378</v>
       </c>
@@ -6629,7 +6632,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>378</v>
       </c>
@@ -6682,7 +6685,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>378</v>
       </c>
@@ -6735,7 +6738,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>378</v>
       </c>
@@ -6788,7 +6791,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>378</v>
       </c>
@@ -6841,7 +6844,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>378</v>
       </c>
@@ -6894,7 +6897,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>378</v>
       </c>
@@ -6947,7 +6950,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>378</v>
       </c>
@@ -7000,7 +7003,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>378</v>
       </c>
@@ -7053,7 +7056,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>378</v>
       </c>
@@ -7106,7 +7109,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>378</v>
       </c>
@@ -7156,7 +7159,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>294</v>
       </c>
@@ -7205,7 +7208,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>429</v>
       </c>
@@ -7252,7 +7255,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>429</v>
       </c>
@@ -7299,7 +7302,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>233</v>
       </c>
@@ -7352,7 +7355,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>233</v>
       </c>
@@ -7405,7 +7408,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>233</v>
       </c>
@@ -7458,7 +7461,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>233</v>
       </c>
@@ -7511,7 +7514,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>233</v>
       </c>
@@ -7564,7 +7567,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>233</v>
       </c>
@@ -7617,7 +7620,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>233</v>
       </c>
@@ -7672,7 +7675,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>233</v>
       </c>
@@ -7728,7 +7731,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>233</v>
       </c>
@@ -7783,7 +7786,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>233</v>
       </c>
@@ -7836,7 +7839,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>233</v>
       </c>
@@ -7889,7 +7892,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>233</v>
       </c>
@@ -7942,7 +7945,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>233</v>
       </c>
@@ -7995,7 +7998,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>233</v>
       </c>
@@ -8048,7 +8051,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>233</v>
       </c>
@@ -8101,7 +8104,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>233</v>
       </c>
@@ -8157,7 +8160,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>233</v>
       </c>
@@ -8210,7 +8213,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>233</v>
       </c>
@@ -8263,7 +8266,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>233</v>
       </c>
@@ -8316,7 +8319,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>233</v>
       </c>
@@ -8369,7 +8372,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>233</v>
       </c>
@@ -8422,7 +8425,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>233</v>
       </c>
@@ -8475,7 +8478,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>233</v>
       </c>
@@ -8528,7 +8531,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>233</v>
       </c>
@@ -8581,7 +8584,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>233</v>
       </c>
@@ -8637,7 +8640,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>233</v>
       </c>
@@ -8693,7 +8696,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>233</v>
       </c>
@@ -8746,7 +8749,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>233</v>
       </c>
@@ -8799,7 +8802,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>233</v>
       </c>
@@ -8852,7 +8855,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>296</v>
       </c>
@@ -8907,7 +8910,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>296</v>
       </c>
@@ -8962,7 +8965,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>296</v>
       </c>
@@ -9017,7 +9020,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>59</v>
       </c>
@@ -9069,7 +9072,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>59</v>
       </c>
@@ -9121,7 +9124,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>59</v>
       </c>
@@ -9173,7 +9176,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>59</v>
       </c>
@@ -9225,7 +9228,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>59</v>
       </c>
@@ -9277,7 +9280,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>59</v>
       </c>
@@ -9329,7 +9332,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>59</v>
       </c>
@@ -9381,7 +9384,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>59</v>
       </c>
@@ -9433,7 +9436,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>59</v>
       </c>
@@ -9485,7 +9488,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>59</v>
       </c>
@@ -9537,7 +9540,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>59</v>
       </c>
@@ -9589,7 +9592,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>59</v>
       </c>
@@ -9641,7 +9644,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>59</v>
       </c>
@@ -9693,7 +9696,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>59</v>
       </c>
@@ -9745,7 +9748,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>59</v>
       </c>
@@ -9797,7 +9800,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>59</v>
       </c>
@@ -9850,7 +9853,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>59</v>
       </c>
@@ -9902,7 +9905,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>59</v>
       </c>
@@ -9954,7 +9957,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="142" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>59</v>
       </c>
@@ -10007,7 +10010,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>59</v>
       </c>
@@ -10060,7 +10063,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>59</v>
       </c>
@@ -10113,7 +10116,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="145" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>59</v>
       </c>
@@ -10166,7 +10169,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>59</v>
       </c>
@@ -10219,7 +10222,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>59</v>
       </c>
@@ -10271,7 +10274,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>59</v>
       </c>
@@ -10323,7 +10326,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="149" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>59</v>
       </c>
@@ -10375,7 +10378,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>59</v>
       </c>
@@ -10427,7 +10430,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>59</v>
       </c>
@@ -10479,7 +10482,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>59</v>
       </c>
@@ -10531,7 +10534,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="153" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>59</v>
       </c>
@@ -10583,7 +10586,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="154" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>59</v>
       </c>
@@ -10635,7 +10638,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="155" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>59</v>
       </c>
@@ -10687,7 +10690,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>59</v>
       </c>
@@ -10737,7 +10740,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>59</v>
       </c>
@@ -10787,7 +10790,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>59</v>
       </c>
@@ -10837,7 +10840,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>59</v>
       </c>
@@ -10887,7 +10890,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>59</v>
       </c>
@@ -10937,7 +10940,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="161" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>371</v>
       </c>
@@ -10987,7 +10990,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="162" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>371</v>
       </c>
@@ -11037,7 +11040,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="163" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="163" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>371</v>
       </c>
@@ -11087,7 +11090,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="164" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="164" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>438</v>
       </c>
@@ -11137,7 +11140,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="165" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>438</v>
       </c>
@@ -11187,7 +11190,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="166" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="166" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>438</v>
       </c>
@@ -11237,7 +11240,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="167" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="167" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>100</v>
       </c>
@@ -11286,7 +11289,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="168" spans="1:17" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="168" spans="1:17" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>100</v>
       </c>
@@ -11335,7 +11338,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="169" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="169" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>100</v>
       </c>
@@ -11385,7 +11388,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="170" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="170" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>100</v>
       </c>
@@ -11432,7 +11435,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="171" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="171" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>100</v>
       </c>
@@ -11481,7 +11484,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="172" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="172" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>100</v>
       </c>
@@ -11528,7 +11531,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="173" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="173" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>100</v>
       </c>
@@ -11577,7 +11580,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="174" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="174" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>100</v>
       </c>
@@ -11624,7 +11627,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="175" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="175" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>100</v>
       </c>
@@ -11673,7 +11676,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="176" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="176" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>100</v>
       </c>
@@ -11720,7 +11723,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="177" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>100</v>
       </c>
@@ -11767,7 +11770,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="178" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="178" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>100</v>
       </c>
@@ -11814,7 +11817,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="179" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="179" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>219</v>
       </c>
@@ -11869,7 +11872,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="180" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="180" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>219</v>
       </c>
@@ -11924,7 +11927,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="181" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="181" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>219</v>
       </c>
@@ -11979,7 +11982,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="182" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="182" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>101</v>
       </c>
@@ -12031,7 +12034,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="183" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="183" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>101</v>
       </c>
@@ -12083,7 +12086,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="184" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="184" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>101</v>
       </c>
@@ -12135,7 +12138,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="185" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="185" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>101</v>
       </c>
@@ -12187,7 +12190,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="186" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="186" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>101</v>
       </c>
@@ -12239,7 +12242,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="187" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="187" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>101</v>
       </c>
@@ -12291,7 +12294,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="188" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="188" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>101</v>
       </c>
@@ -12343,7 +12346,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="189" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="189" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>101</v>
       </c>
@@ -12395,7 +12398,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="190" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="190" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>101</v>
       </c>
@@ -12447,7 +12450,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="191" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="191" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>101</v>
       </c>
@@ -12499,7 +12502,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="192" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="192" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>101</v>
       </c>
@@ -12551,7 +12554,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="193" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="193" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>101</v>
       </c>
@@ -12601,7 +12604,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="194" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="194" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>101</v>
       </c>
@@ -12651,7 +12654,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="195" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="195" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>101</v>
       </c>
@@ -12698,7 +12701,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="196" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="196" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>101</v>
       </c>
@@ -12748,7 +12751,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="197" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="197" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>101</v>
       </c>
@@ -12798,7 +12801,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="198" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="198" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>101</v>
       </c>
@@ -12848,7 +12851,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="199" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="199" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>167</v>
       </c>
@@ -12900,7 +12903,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="200" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="200" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>167</v>
       </c>
@@ -12952,7 +12955,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="201" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="201" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>167</v>
       </c>
@@ -13004,7 +13007,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="202" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="202" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>167</v>
       </c>
@@ -13056,7 +13059,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="203" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="203" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>167</v>
       </c>
@@ -13108,7 +13111,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="204" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="204" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>167</v>
       </c>
@@ -13160,7 +13163,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="205" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="205" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>167</v>
       </c>
@@ -13213,7 +13216,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="206" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="206" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>167</v>
       </c>
@@ -13265,7 +13268,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="207" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="207" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>167</v>
       </c>
@@ -13317,7 +13320,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="208" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="208" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>167</v>
       </c>
@@ -13369,7 +13372,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="209" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="209" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>167</v>
       </c>
@@ -13421,7 +13424,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="210" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="210" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>167</v>
       </c>
@@ -13473,7 +13476,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="211" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="211" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>167</v>
       </c>
@@ -13525,7 +13528,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="212" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="212" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>167</v>
       </c>
@@ -13577,7 +13580,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="213" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="213" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>167</v>
       </c>
@@ -13629,7 +13632,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="214" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="214" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>167</v>
       </c>
@@ -13679,7 +13682,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="215" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="215" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>183</v>
       </c>
@@ -13731,7 +13734,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="216" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="216" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>183</v>
       </c>
@@ -13783,7 +13786,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="217" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="217" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>183</v>
       </c>
@@ -13835,7 +13838,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="218" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="218" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>183</v>
       </c>
@@ -13887,7 +13890,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="219" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="219" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>183</v>
       </c>
@@ -13939,7 +13942,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="220" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="220" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>183</v>
       </c>
@@ -13991,7 +13994,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="221" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="221" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>183</v>
       </c>
@@ -14043,7 +14046,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="222" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="222" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>183</v>
       </c>
@@ -14095,7 +14098,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="223" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="223" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>183</v>
       </c>
@@ -14147,7 +14150,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="224" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="224" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>183</v>
       </c>
@@ -14197,7 +14200,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="225" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="225" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A225" s="1" t="s">
         <v>183</v>
       </c>
@@ -14247,7 +14250,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="226" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="226" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A226" s="1" t="s">
         <v>183</v>
       </c>
@@ -14297,7 +14300,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="227" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="227" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>192</v>
       </c>
@@ -14349,7 +14352,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="228" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="228" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>192</v>
       </c>
@@ -14401,7 +14404,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="229" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="229" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>192</v>
       </c>
@@ -14453,7 +14456,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="230" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="230" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>192</v>
       </c>
@@ -14505,7 +14508,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="231" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="231" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>192</v>
       </c>
@@ -14557,7 +14560,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="232" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="232" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>192</v>
       </c>
@@ -14607,7 +14610,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="233" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="233" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>264</v>
       </c>
@@ -14660,7 +14663,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="234" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="234" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A234" s="1" t="s">
         <v>264</v>
       </c>
@@ -14713,7 +14716,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="235" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="235" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A235" s="1" t="s">
         <v>264</v>
       </c>
@@ -14766,7 +14769,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="236" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="236" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A236" s="1" t="s">
         <v>264</v>
       </c>
@@ -14819,7 +14822,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="237" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="237" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A237" s="1" t="s">
         <v>221</v>
       </c>
@@ -14868,7 +14871,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="238" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="238" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A238" s="1" t="s">
         <v>221</v>
       </c>
@@ -14915,7 +14918,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="239" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="239" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A239" s="1" t="s">
         <v>221</v>
       </c>
@@ -14962,7 +14965,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="240" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="240" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A240" s="1" t="s">
         <v>221</v>
       </c>
@@ -15011,7 +15014,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="241" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="241" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A241" s="1" t="s">
         <v>221</v>
       </c>
@@ -15058,7 +15061,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="242" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="242" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A242" s="1" t="s">
         <v>221</v>
       </c>
@@ -15105,7 +15108,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="243" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="243" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A243" s="1" t="s">
         <v>221</v>
       </c>
@@ -15152,7 +15155,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="244" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="244" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A244" s="1" t="s">
         <v>221</v>
       </c>
@@ -15201,7 +15204,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="245" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="245" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A245" s="1" t="s">
         <v>221</v>
       </c>
@@ -15248,7 +15251,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="246" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="246" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A246" s="1" t="s">
         <v>221</v>
       </c>
@@ -15295,7 +15298,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="247" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="247" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>221</v>
       </c>
@@ -15342,7 +15345,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="248" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="248" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>221</v>
       </c>
@@ -15389,7 +15392,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="249" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="249" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>221</v>
       </c>
@@ -15436,7 +15439,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="250" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="250" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>221</v>
       </c>
@@ -15485,7 +15488,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="251" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="251" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>221</v>
       </c>
@@ -15532,7 +15535,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="252" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="252" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A252" s="1" t="s">
         <v>221</v>
       </c>
@@ -15579,7 +15582,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="253" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="253" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A253" s="1" t="s">
         <v>221</v>
       </c>
@@ -15626,7 +15629,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="254" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="254" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>133</v>
       </c>
@@ -15681,7 +15684,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="255" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="255" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>133</v>
       </c>
@@ -15734,7 +15737,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="256" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="256" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>133</v>
       </c>
@@ -15787,7 +15790,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="257" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="257" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>133</v>
       </c>
@@ -15842,7 +15845,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="258" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="258" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>133</v>
       </c>
@@ -15895,7 +15898,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="259" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="259" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>133</v>
       </c>
@@ -15948,7 +15951,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="260" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="260" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>133</v>
       </c>
@@ -16003,7 +16006,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="261" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="261" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>133</v>
       </c>
@@ -16058,7 +16061,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="262" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="262" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>133</v>
       </c>
@@ -16113,7 +16116,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="263" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="263" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>133</v>
       </c>
@@ -16166,7 +16169,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="264" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="264" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>133</v>
       </c>
@@ -16219,7 +16222,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="265" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="265" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>133</v>
       </c>
@@ -16272,7 +16275,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="266" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="266" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>133</v>
       </c>
@@ -16327,7 +16330,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="267" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="267" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>133</v>
       </c>
@@ -16382,7 +16385,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="268" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="268" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A268" s="1" t="s">
         <v>133</v>
       </c>
@@ -16437,7 +16440,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="269" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="269" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A269" s="1" t="s">
         <v>133</v>
       </c>
@@ -16490,7 +16493,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="270" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="270" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>133</v>
       </c>
@@ -16543,7 +16546,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="271" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="271" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>133</v>
       </c>
@@ -16598,7 +16601,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="272" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="272" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>133</v>
       </c>
@@ -16653,7 +16656,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="273" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="273" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>133</v>
       </c>
@@ -16706,7 +16709,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="274" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="274" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>133</v>
       </c>
@@ -16759,7 +16762,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="275" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="275" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>133</v>
       </c>
@@ -16814,7 +16817,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="276" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="276" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>133</v>
       </c>
@@ -16869,7 +16872,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="277" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="277" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>133</v>
       </c>
@@ -16924,7 +16927,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="278" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="278" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>133</v>
       </c>
@@ -16979,7 +16982,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="279" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="279" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>133</v>
       </c>
@@ -17032,7 +17035,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="280" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="280" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>133</v>
       </c>
@@ -17085,7 +17088,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="281" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="281" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>133</v>
       </c>
@@ -17138,7 +17141,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="282" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="282" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>133</v>
       </c>
@@ -17191,7 +17194,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="283" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="283" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>133</v>
       </c>
@@ -17244,7 +17247,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="284" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="284" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>133</v>
       </c>
@@ -17299,7 +17302,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="285" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="285" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>133</v>
       </c>
@@ -17354,7 +17357,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="286" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="286" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>133</v>
       </c>
@@ -17409,7 +17412,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="287" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="287" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>133</v>
       </c>
@@ -17464,7 +17467,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="288" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="288" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>133</v>
       </c>
@@ -17519,7 +17522,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="289" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="289" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>133</v>
       </c>
@@ -17572,7 +17575,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="290" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="290" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>133</v>
       </c>
@@ -17625,7 +17628,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="291" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="291" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>133</v>
       </c>
@@ -17678,7 +17681,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="292" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="292" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>133</v>
       </c>
@@ -17731,7 +17734,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="293" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="293" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>133</v>
       </c>
@@ -17784,7 +17787,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="294" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="294" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>133</v>
       </c>
@@ -17839,7 +17842,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="295" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="295" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>133</v>
       </c>
@@ -17894,7 +17897,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="296" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="296" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>133</v>
       </c>
@@ -17949,7 +17952,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="297" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="297" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>133</v>
       </c>
@@ -18004,7 +18007,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="298" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="298" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>133</v>
       </c>
@@ -18059,7 +18062,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="299" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="299" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>133</v>
       </c>
@@ -18112,7 +18115,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="300" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="300" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>133</v>
       </c>
@@ -18165,7 +18168,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="301" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="301" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>133</v>
       </c>
@@ -18218,7 +18221,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="302" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="302" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>133</v>
       </c>
@@ -18273,7 +18276,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="303" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="303" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>133</v>
       </c>
@@ -18328,7 +18331,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="304" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="304" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>133</v>
       </c>
@@ -18381,7 +18384,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="305" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="305" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>133</v>
       </c>
@@ -18436,7 +18439,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="306" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="306" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>133</v>
       </c>
@@ -18489,7 +18492,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="307" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="307" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>133</v>
       </c>
@@ -18542,7 +18545,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="308" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="308" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>133</v>
       </c>
@@ -18595,7 +18598,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="309" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="309" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>133</v>
       </c>
@@ -18648,7 +18651,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="310" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="310" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>133</v>
       </c>
@@ -18701,7 +18704,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="311" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="311" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>133</v>
       </c>
@@ -18754,7 +18757,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="312" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="312" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>133</v>
       </c>
@@ -18807,7 +18810,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="313" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="313" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>133</v>
       </c>
@@ -18860,7 +18863,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="314" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="314" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>133</v>
       </c>
@@ -18913,7 +18916,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="315" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="315" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>378</v>
       </c>
@@ -18966,7 +18969,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="316" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="316" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>378</v>
       </c>
@@ -19019,7 +19022,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="317" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="317" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>101</v>
       </c>
@@ -19029,7 +19032,9 @@
       <c r="C317" s="12">
         <v>2017</v>
       </c>
-      <c r="D317" s="10"/>
+      <c r="D317" s="12">
+        <v>1599</v>
+      </c>
       <c r="E317">
         <v>1170</v>
       </c>
@@ -19067,7 +19072,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="318" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="318" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>101</v>
       </c>
@@ -19077,7 +19082,9 @@
       <c r="C318">
         <v>2017</v>
       </c>
-      <c r="D318" s="10"/>
+      <c r="D318" s="12">
+        <v>1399</v>
+      </c>
       <c r="E318">
         <v>1130</v>
       </c>
@@ -19115,7 +19122,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="319" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="319" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>101</v>
       </c>
@@ -19125,7 +19132,9 @@
       <c r="C319">
         <v>2017</v>
       </c>
-      <c r="D319" s="10"/>
+      <c r="D319" s="12">
+        <v>1299</v>
+      </c>
       <c r="E319" s="10"/>
       <c r="F319">
         <v>107.6</v>
@@ -19161,7 +19170,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="320" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="320" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>101</v>
       </c>
@@ -19171,7 +19180,9 @@
       <c r="C320">
         <v>2017</v>
       </c>
-      <c r="D320" s="10"/>
+      <c r="D320" s="12">
+        <v>799</v>
+      </c>
       <c r="E320">
         <v>1160</v>
       </c>
@@ -19209,7 +19220,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="321" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="321" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>7</v>
       </c>
@@ -19262,7 +19273,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="322" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="322" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>219</v>
       </c>
@@ -19311,7 +19322,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="323" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="323" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>219</v>
       </c>
@@ -19360,7 +19371,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="324" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="324" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>219</v>
       </c>
@@ -19409,7 +19420,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="325" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="325" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>101</v>
       </c>
@@ -19456,7 +19467,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="326" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="326" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>192</v>
       </c>
@@ -19503,7 +19514,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="327" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="327" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>7</v>
       </c>
@@ -19552,7 +19563,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="328" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="328" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>7</v>
       </c>
@@ -19605,7 +19616,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="329" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="329" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>7</v>
       </c>
@@ -19658,7 +19669,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="330" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="330" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>7</v>
       </c>
@@ -19711,7 +19722,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="331" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="331" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>7</v>
       </c>
@@ -19764,7 +19775,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="332" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="332" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>219</v>
       </c>
@@ -19813,7 +19824,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="333" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="333" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>219</v>
       </c>
@@ -19862,7 +19873,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="334" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="334" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>219</v>
       </c>
@@ -19911,7 +19922,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="335" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="335" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>219</v>
       </c>
@@ -19960,7 +19971,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="336" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="336" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>219</v>
       </c>
@@ -20009,7 +20020,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="337" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="337" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>219</v>
       </c>
@@ -20058,7 +20069,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="338" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="338" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
         <v>505</v>
       </c>
@@ -20109,7 +20120,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="339" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="339" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
         <v>505</v>
       </c>
@@ -20158,7 +20169,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="340" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="340" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
         <v>505</v>
       </c>
@@ -20207,7 +20218,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="341" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="341" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>505</v>
       </c>
@@ -20256,7 +20267,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="342" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="342" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
         <v>505</v>
       </c>
@@ -20305,7 +20316,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="343" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="343" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
         <v>505</v>
       </c>
@@ -20354,7 +20365,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="344" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="344" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
         <v>505</v>
       </c>
@@ -20403,7 +20414,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="345" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="345" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
         <v>505</v>
       </c>
@@ -20452,7 +20463,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="346" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="346" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
         <v>505</v>
       </c>
@@ -20501,7 +20512,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="347" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="347" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
         <v>505</v>
       </c>
@@ -20550,7 +20561,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="348" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="348" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
         <v>505</v>
       </c>
@@ -20599,7 +20610,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="349" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="349" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
         <v>505</v>
       </c>
@@ -20648,7 +20659,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="350" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="350" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
         <v>505</v>
       </c>
@@ -20697,7 +20708,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="351" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="351" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
         <v>505</v>
       </c>
@@ -20746,7 +20757,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="352" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="352" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
         <v>505</v>
       </c>
@@ -20795,7 +20806,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="353" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="353" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
         <v>505</v>
       </c>
@@ -20844,7 +20855,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="354" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="354" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
         <v>505</v>
       </c>
@@ -20893,7 +20904,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="355" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="355" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
         <v>378</v>
       </c>
@@ -20946,7 +20957,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="356" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="356" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
         <v>378</v>
       </c>
@@ -20999,7 +21010,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="357" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="357" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
         <v>378</v>
       </c>
@@ -21052,7 +21063,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="358" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="358" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
         <v>378</v>
       </c>
@@ -21105,7 +21116,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="359" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="359" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
         <v>378</v>
       </c>
@@ -21158,7 +21169,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="360" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="360" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
         <v>378</v>
       </c>
@@ -21211,7 +21222,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="361" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="361" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
         <v>378</v>
       </c>
@@ -21264,7 +21275,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="362" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="362" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
         <v>378</v>
       </c>
@@ -21317,7 +21328,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="363" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="363" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
         <v>378</v>
       </c>
@@ -21370,7 +21381,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="364" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="364" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
         <v>101</v>
       </c>
@@ -21420,7 +21431,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="365" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="365" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
         <v>101</v>
       </c>
@@ -21470,7 +21481,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="366" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="366" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
         <v>101</v>
       </c>
@@ -21520,7 +21531,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="367" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="367" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
         <v>101</v>
       </c>
@@ -21570,7 +21581,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="368" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="368" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
         <v>101</v>
       </c>
@@ -21620,7 +21631,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="369" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="369" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
         <v>101</v>
       </c>
@@ -21670,7 +21681,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="370" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="370" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
         <v>101</v>
       </c>
@@ -21720,7 +21731,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="371" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="371" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
         <v>101</v>
       </c>
@@ -21770,7 +21781,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="372" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="372" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
         <v>192</v>
       </c>
@@ -21820,7 +21831,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="373" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="373" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
         <v>192</v>
       </c>
@@ -21870,7 +21881,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="374" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="374" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
         <v>192</v>
       </c>
@@ -21920,7 +21931,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="375" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="375" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
         <v>192</v>
       </c>
@@ -21970,7 +21981,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="376" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="376" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
         <v>192</v>
       </c>
@@ -22018,7 +22029,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="377" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="377" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
         <v>192</v>
       </c>
@@ -22068,7 +22079,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="378" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="378" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
         <v>192</v>
       </c>
@@ -22118,7 +22129,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="379" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="379" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A379" t="s">
         <v>133</v>
       </c>
@@ -22171,7 +22182,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="380" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="380" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A380" t="s">
         <v>7</v>
       </c>
@@ -22224,7 +22235,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="381" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="381" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A381" t="s">
         <v>432</v>
       </c>
@@ -22271,7 +22282,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="382" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="382" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A382" t="s">
         <v>432</v>
       </c>
@@ -22318,7 +22329,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="383" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="383" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A383" t="s">
         <v>432</v>
       </c>
@@ -22365,7 +22376,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="384" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="384" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A384" t="s">
         <v>432</v>
       </c>
@@ -22412,7 +22423,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="385" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="385" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A385" s="7" t="s">
         <v>183</v>
       </c>
@@ -22462,7 +22473,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="386" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="386" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A386" s="7" t="s">
         <v>133</v>
       </c>
@@ -22512,7 +22523,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="387" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="387" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A387" s="7" t="s">
         <v>167</v>
       </c>
@@ -22562,7 +22573,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="388" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="388" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A388" s="7" t="s">
         <v>167</v>
       </c>
@@ -22612,7 +22623,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="389" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="389" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A389" s="7" t="s">
         <v>167</v>
       </c>
@@ -22662,7 +22673,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="390" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="390" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A390" s="7" t="s">
         <v>264</v>
       </c>
@@ -22713,7 +22724,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="391" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="391" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A391" s="7" t="s">
         <v>264</v>
       </c>
@@ -22766,7 +22777,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="392" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="392" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A392" s="7" t="s">
         <v>378</v>
       </c>
@@ -22819,7 +22830,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="393" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="393" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A393" s="7" t="s">
         <v>378</v>
       </c>
@@ -22872,7 +22883,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="394" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="394" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A394" s="7" t="s">
         <v>378</v>
       </c>
@@ -22925,7 +22936,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="395" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="395" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A395" s="7" t="s">
         <v>378</v>
       </c>
@@ -22970,7 +22981,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="396" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="396" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A396" s="7" t="s">
         <v>604</v>
       </c>
@@ -23017,7 +23028,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="397" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="397" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A397" s="7" t="s">
         <v>604</v>
       </c>
@@ -23064,7 +23075,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="398" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="398" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A398" t="s">
         <v>615</v>
       </c>
@@ -23117,7 +23128,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="399" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="399" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A399" t="s">
         <v>615</v>
       </c>
@@ -23166,7 +23177,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="400" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="400" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A400" t="s">
         <v>59</v>
       </c>
@@ -23216,7 +23227,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="401" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="401" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A401" t="s">
         <v>59</v>
       </c>
@@ -23266,7 +23277,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="402" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="402" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A402" t="s">
         <v>59</v>
       </c>
@@ -23316,7 +23327,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="403" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="403" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A403" t="s">
         <v>167</v>
       </c>
@@ -23371,23 +23382,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="P38" sqref="P38"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.68359375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>42361</v>
       </c>
@@ -23395,7 +23406,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>42369</v>
       </c>
@@ -23403,7 +23414,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>42371</v>
       </c>
@@ -23411,7 +23422,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>42372</v>
       </c>
@@ -23419,7 +23430,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>42373</v>
       </c>
@@ -23427,7 +23438,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>42382</v>
       </c>
@@ -23435,7 +23446,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>42385</v>
       </c>
@@ -23443,7 +23454,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>42387</v>
       </c>
@@ -23451,7 +23462,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>42388</v>
       </c>
@@ -23459,7 +23470,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>42390</v>
       </c>
@@ -23467,7 +23478,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>42391</v>
       </c>
@@ -23475,7 +23486,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>42400</v>
       </c>
@@ -23483,7 +23494,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>42414</v>
       </c>
@@ -23491,7 +23502,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>42432</v>
       </c>
@@ -23502,7 +23513,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>42435</v>
       </c>
@@ -23510,7 +23521,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>42436</v>
       </c>
@@ -23518,7 +23529,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>42441</v>
       </c>
@@ -23526,7 +23537,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>42445</v>
       </c>
@@ -23534,7 +23545,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>42453</v>
       </c>
@@ -23542,7 +23553,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>42456</v>
       </c>
@@ -23550,7 +23561,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>42457</v>
       </c>
@@ -23558,7 +23569,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>42458</v>
       </c>
@@ -23566,7 +23577,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>42464</v>
       </c>
@@ -23574,7 +23585,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>42510</v>
       </c>
@@ -23582,7 +23593,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>42515</v>
       </c>
@@ -23590,7 +23601,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>42560</v>
       </c>
@@ -23598,7 +23609,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>42565</v>
       </c>
@@ -23606,7 +23617,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>42576</v>
       </c>
@@ -23614,7 +23625,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>42590</v>
       </c>
@@ -23622,7 +23633,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>42593</v>
       </c>
@@ -23630,7 +23641,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>42598</v>
       </c>
@@ -23638,7 +23649,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>42665</v>
       </c>
@@ -23646,7 +23657,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>42788</v>
       </c>
@@ -23654,7 +23665,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>42831</v>
       </c>
@@ -23662,7 +23673,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="13">
         <v>42833</v>
       </c>
@@ -23670,7 +23681,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="13">
         <v>42833</v>
       </c>
@@ -23678,7 +23689,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="13">
         <v>42874</v>
       </c>
@@ -23686,7 +23697,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="13">
         <v>42876</v>
       </c>
@@ -23694,7 +23705,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="13">
         <v>42878</v>
       </c>
@@ -23702,7 +23713,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="13">
         <v>42878</v>
       </c>
@@ -23710,7 +23721,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="13">
         <v>42879</v>
       </c>
@@ -23718,7 +23729,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="13">
         <v>42884</v>
       </c>
@@ -23726,7 +23737,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="13">
         <v>42887</v>
       </c>
@@ -23734,7 +23745,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="13">
         <v>42887</v>
       </c>
@@ -23742,12 +23753,20 @@
         <v>632</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="13">
         <v>42891</v>
       </c>
       <c r="B47" t="s">
         <v>634</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="13">
+        <v>42901</v>
+      </c>
+      <c r="B48" t="s">
+        <v>635</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Zeiss CP.3 lenses
</commit_message>
<xml_diff>
--- a/BigAssTableOfLenses.xlsx
+++ b/BigAssTableOfLenses.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3014" uniqueCount="635">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3085" uniqueCount="650">
   <si>
     <t>Manufacture</t>
   </si>
@@ -1930,6 +1930,51 @@
   </si>
   <si>
     <t>Added Sony FE 85mm f/1.8</t>
+  </si>
+  <si>
+    <t>CP.3 XD 135mm T2.1 Compact Prime</t>
+  </si>
+  <si>
+    <t>CP.3 25mm T2.1 Compact Prime</t>
+  </si>
+  <si>
+    <t>CP.3 35mm T2.1 Compact Prime</t>
+  </si>
+  <si>
+    <t>CP.3 50mm T2.1 Compact Prime</t>
+  </si>
+  <si>
+    <t>CP.3 85mm T2.1 Compact Prime</t>
+  </si>
+  <si>
+    <t>CP.3 XD 100mm T2.1 Compact Prime</t>
+  </si>
+  <si>
+    <t>CP.3 XD 15mm T2.9 Compact Prime</t>
+  </si>
+  <si>
+    <t>CP.3 XD 18mm T2.9 Compact Prime</t>
+  </si>
+  <si>
+    <t>CP.3 XD 21mm T2.9 Compact Prime</t>
+  </si>
+  <si>
+    <t>CP.3 XD 25mm T2.1 Compact Prime</t>
+  </si>
+  <si>
+    <t>CP.3 XD 28mm T2.1 Compact Prime</t>
+  </si>
+  <si>
+    <t>CP.3 XD 35mm T2.1 Compact Prime</t>
+  </si>
+  <si>
+    <t>CP.3 XD 50mm T2.1 Compact Prime</t>
+  </si>
+  <si>
+    <t>CP.3 XD 85mm T2.1 Compact Prime</t>
+  </si>
+  <si>
+    <t>Added Zeiss CP.3 lenses</t>
   </si>
 </sst>
 </file>
@@ -2022,8 +2067,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q403" totalsRowShown="0">
-  <autoFilter ref="A1:Q403">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q417" totalsRowShown="0">
+  <autoFilter ref="A1:Q417">
     <filterColumn colId="11">
       <filters>
         <filter val="0"/>
@@ -2354,10 +2399,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q403"/>
+  <dimension ref="A1:Q417"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A321" workbookViewId="0">
-      <selection activeCell="B406" sqref="B406"/>
+    <sheetView tabSelected="1" topLeftCell="A398" workbookViewId="0">
+      <selection activeCell="B419" sqref="B419"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -18165,7 +18210,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="301" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="301" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A301" t="s">
         <v>133</v>
       </c>
@@ -18273,7 +18318,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="303" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="303" spans="1:17" ht="24.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A303" t="s">
         <v>133</v>
       </c>
@@ -18328,7 +18373,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="304" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="304" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A304" t="s">
         <v>133</v>
       </c>
@@ -18381,7 +18426,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="305" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="305" spans="1:17" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A305" t="s">
         <v>133</v>
       </c>
@@ -18436,7 +18481,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="306" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="306" spans="1:17" ht="15.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A306" t="s">
         <v>133</v>
       </c>
@@ -18489,7 +18534,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="307" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="307" spans="1:17" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A307" t="s">
         <v>133</v>
       </c>
@@ -18542,7 +18587,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="308" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="308" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A308" t="s">
         <v>133</v>
       </c>
@@ -18595,7 +18640,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="309" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="309" spans="1:17" ht="16.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A309" t="s">
         <v>133</v>
       </c>
@@ -23358,6 +23403,622 @@
       </c>
       <c r="Q403">
         <v>402</v>
+      </c>
+    </row>
+    <row r="404" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A404" t="s">
+        <v>133</v>
+      </c>
+      <c r="B404" t="s">
+        <v>635</v>
+      </c>
+      <c r="C404">
+        <v>2017</v>
+      </c>
+      <c r="D404">
+        <v>7490</v>
+      </c>
+      <c r="E404">
+        <v>1150</v>
+      </c>
+      <c r="F404">
+        <v>126.5</v>
+      </c>
+      <c r="G404" s="8">
+        <v>95</v>
+      </c>
+      <c r="H404" s="1">
+        <v>2</v>
+      </c>
+      <c r="I404" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="J404" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="K404">
+        <v>0</v>
+      </c>
+      <c r="L404">
+        <v>1</v>
+      </c>
+      <c r="M404" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q404">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="405" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A405" t="s">
+        <v>133</v>
+      </c>
+      <c r="B405" t="s">
+        <v>636</v>
+      </c>
+      <c r="C405">
+        <v>2017</v>
+      </c>
+      <c r="D405">
+        <v>4390</v>
+      </c>
+      <c r="E405">
+        <v>820</v>
+      </c>
+      <c r="F405">
+        <v>83.7</v>
+      </c>
+      <c r="G405" s="8">
+        <v>95</v>
+      </c>
+      <c r="H405" s="1">
+        <v>2</v>
+      </c>
+      <c r="I405" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="J405" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="K405">
+        <v>0</v>
+      </c>
+      <c r="L405">
+        <v>1</v>
+      </c>
+      <c r="M405" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q405">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="406" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A406" t="s">
+        <v>133</v>
+      </c>
+      <c r="B406" t="s">
+        <v>637</v>
+      </c>
+      <c r="C406">
+        <v>2017</v>
+      </c>
+      <c r="D406">
+        <v>4390</v>
+      </c>
+      <c r="E406">
+        <v>800</v>
+      </c>
+      <c r="F406">
+        <v>83.7</v>
+      </c>
+      <c r="G406" s="8">
+        <v>95</v>
+      </c>
+      <c r="H406" s="1">
+        <v>2</v>
+      </c>
+      <c r="I406" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="J406" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="K406">
+        <v>0</v>
+      </c>
+      <c r="L406">
+        <v>1</v>
+      </c>
+      <c r="M406" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q406">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="407" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A407" t="s">
+        <v>133</v>
+      </c>
+      <c r="B407" t="s">
+        <v>638</v>
+      </c>
+      <c r="C407">
+        <v>2017</v>
+      </c>
+      <c r="D407">
+        <v>4390</v>
+      </c>
+      <c r="E407">
+        <v>770</v>
+      </c>
+      <c r="F407">
+        <v>83.7</v>
+      </c>
+      <c r="G407" s="8">
+        <v>95</v>
+      </c>
+      <c r="H407" s="1">
+        <v>2</v>
+      </c>
+      <c r="I407" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="J407" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="K407">
+        <v>0</v>
+      </c>
+      <c r="L407">
+        <v>1</v>
+      </c>
+      <c r="M407" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q407">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="408" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A408" t="s">
+        <v>133</v>
+      </c>
+      <c r="B408" t="s">
+        <v>639</v>
+      </c>
+      <c r="C408">
+        <v>2017</v>
+      </c>
+      <c r="D408">
+        <v>4390</v>
+      </c>
+      <c r="E408">
+        <v>880</v>
+      </c>
+      <c r="F408">
+        <v>83.7</v>
+      </c>
+      <c r="G408" s="8">
+        <v>95</v>
+      </c>
+      <c r="H408" s="1">
+        <v>2</v>
+      </c>
+      <c r="I408" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="J408" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="K408">
+        <v>0</v>
+      </c>
+      <c r="L408">
+        <v>1</v>
+      </c>
+      <c r="M408" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q408">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="409" spans="1:17" ht="22.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A409" t="s">
+        <v>133</v>
+      </c>
+      <c r="B409" t="s">
+        <v>640</v>
+      </c>
+      <c r="C409">
+        <v>2017</v>
+      </c>
+      <c r="D409">
+        <v>6690</v>
+      </c>
+      <c r="E409">
+        <v>1010</v>
+      </c>
+      <c r="F409">
+        <v>126.5</v>
+      </c>
+      <c r="G409" s="8">
+        <v>95</v>
+      </c>
+      <c r="H409" s="1">
+        <v>2</v>
+      </c>
+      <c r="I409" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="J409" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="K409">
+        <v>0</v>
+      </c>
+      <c r="L409">
+        <v>1</v>
+      </c>
+      <c r="M409" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q409">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="410" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A410" t="s">
+        <v>133</v>
+      </c>
+      <c r="B410" t="s">
+        <v>641</v>
+      </c>
+      <c r="C410">
+        <v>2017</v>
+      </c>
+      <c r="D410">
+        <v>7490</v>
+      </c>
+      <c r="E410">
+        <v>870</v>
+      </c>
+      <c r="F410">
+        <v>83.7</v>
+      </c>
+      <c r="G410" s="8">
+        <v>95</v>
+      </c>
+      <c r="H410" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="I410" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="J410" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="K410">
+        <v>0</v>
+      </c>
+      <c r="L410">
+        <v>1</v>
+      </c>
+      <c r="M410" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q410">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="411" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A411" t="s">
+        <v>133</v>
+      </c>
+      <c r="B411" t="s">
+        <v>642</v>
+      </c>
+      <c r="C411">
+        <v>2017</v>
+      </c>
+      <c r="D411">
+        <v>6690</v>
+      </c>
+      <c r="E411">
+        <v>860</v>
+      </c>
+      <c r="F411">
+        <v>83.7</v>
+      </c>
+      <c r="G411" s="8">
+        <v>95</v>
+      </c>
+      <c r="H411" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="I411" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="J411" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="K411">
+        <v>0</v>
+      </c>
+      <c r="L411">
+        <v>1</v>
+      </c>
+      <c r="M411" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q411">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="412" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A412" t="s">
+        <v>133</v>
+      </c>
+      <c r="B412" t="s">
+        <v>643</v>
+      </c>
+      <c r="C412">
+        <v>2017</v>
+      </c>
+      <c r="D412">
+        <v>5790</v>
+      </c>
+      <c r="E412">
+        <v>820</v>
+      </c>
+      <c r="F412">
+        <v>83.7</v>
+      </c>
+      <c r="G412" s="8">
+        <v>95</v>
+      </c>
+      <c r="H412" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="I412" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="J412" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="K412">
+        <v>0</v>
+      </c>
+      <c r="L412">
+        <v>1</v>
+      </c>
+      <c r="M412" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q412">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="413" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A413" t="s">
+        <v>133</v>
+      </c>
+      <c r="B413" t="s">
+        <v>644</v>
+      </c>
+      <c r="C413">
+        <v>2017</v>
+      </c>
+      <c r="D413">
+        <v>5790</v>
+      </c>
+      <c r="E413">
+        <v>820</v>
+      </c>
+      <c r="F413">
+        <v>83.7</v>
+      </c>
+      <c r="G413" s="8">
+        <v>95</v>
+      </c>
+      <c r="H413" s="1">
+        <v>2</v>
+      </c>
+      <c r="I413" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="J413" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="K413">
+        <v>0</v>
+      </c>
+      <c r="L413">
+        <v>1</v>
+      </c>
+      <c r="M413" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q413">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="414" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A414" t="s">
+        <v>133</v>
+      </c>
+      <c r="B414" t="s">
+        <v>645</v>
+      </c>
+      <c r="C414">
+        <v>2017</v>
+      </c>
+      <c r="D414">
+        <v>5790</v>
+      </c>
+      <c r="E414">
+        <v>840</v>
+      </c>
+      <c r="F414">
+        <v>83.7</v>
+      </c>
+      <c r="G414" s="8">
+        <v>95</v>
+      </c>
+      <c r="H414" s="1">
+        <v>2</v>
+      </c>
+      <c r="I414" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="J414" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="K414">
+        <v>0</v>
+      </c>
+      <c r="L414">
+        <v>1</v>
+      </c>
+      <c r="M414" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q414">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="415" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A415" t="s">
+        <v>133</v>
+      </c>
+      <c r="B415" t="s">
+        <v>646</v>
+      </c>
+      <c r="C415">
+        <v>2017</v>
+      </c>
+      <c r="D415">
+        <v>5790</v>
+      </c>
+      <c r="E415">
+        <v>800</v>
+      </c>
+      <c r="F415">
+        <v>83.7</v>
+      </c>
+      <c r="G415" s="8">
+        <v>95</v>
+      </c>
+      <c r="H415" s="1">
+        <v>2</v>
+      </c>
+      <c r="I415" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="J415" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="K415">
+        <v>0</v>
+      </c>
+      <c r="L415">
+        <v>1</v>
+      </c>
+      <c r="M415" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q415">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="416" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A416" t="s">
+        <v>133</v>
+      </c>
+      <c r="B416" t="s">
+        <v>647</v>
+      </c>
+      <c r="C416">
+        <v>2017</v>
+      </c>
+      <c r="D416">
+        <v>5790</v>
+      </c>
+      <c r="E416">
+        <v>770</v>
+      </c>
+      <c r="F416">
+        <v>83.7</v>
+      </c>
+      <c r="G416" s="8">
+        <v>95</v>
+      </c>
+      <c r="H416" s="1">
+        <v>2</v>
+      </c>
+      <c r="I416" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="J416" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="K416">
+        <v>0</v>
+      </c>
+      <c r="L416">
+        <v>1</v>
+      </c>
+      <c r="M416" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q416">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="417" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A417" t="s">
+        <v>133</v>
+      </c>
+      <c r="B417" t="s">
+        <v>648</v>
+      </c>
+      <c r="C417">
+        <v>2017</v>
+      </c>
+      <c r="D417">
+        <v>5790</v>
+      </c>
+      <c r="E417">
+        <v>880</v>
+      </c>
+      <c r="F417">
+        <v>83.7</v>
+      </c>
+      <c r="G417" s="8">
+        <v>95</v>
+      </c>
+      <c r="H417" s="1">
+        <v>2</v>
+      </c>
+      <c r="I417" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="J417" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="K417">
+        <v>0</v>
+      </c>
+      <c r="L417">
+        <v>1</v>
+      </c>
+      <c r="M417" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q417">
+        <v>416</v>
       </c>
     </row>
   </sheetData>
@@ -23371,10 +24032,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="P38" sqref="P38"/>
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -23750,6 +24411,14 @@
         <v>634</v>
       </c>
     </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="13">
+        <v>42910</v>
+      </c>
+      <c r="B48" t="s">
+        <v>649</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert "Added Zeiss CP.3 lenses"
This reverts commit e4ca3da016414be210a51f7dd9d12e3cc7ea1249.
</commit_message>
<xml_diff>
--- a/BigAssTableOfLenses.xlsx
+++ b/BigAssTableOfLenses.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3085" uniqueCount="650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3014" uniqueCount="635">
   <si>
     <t>Manufacture</t>
   </si>
@@ -1930,51 +1930,6 @@
   </si>
   <si>
     <t>Added Sony FE 85mm f/1.8</t>
-  </si>
-  <si>
-    <t>CP.3 XD 135mm T2.1 Compact Prime</t>
-  </si>
-  <si>
-    <t>CP.3 25mm T2.1 Compact Prime</t>
-  </si>
-  <si>
-    <t>CP.3 35mm T2.1 Compact Prime</t>
-  </si>
-  <si>
-    <t>CP.3 50mm T2.1 Compact Prime</t>
-  </si>
-  <si>
-    <t>CP.3 85mm T2.1 Compact Prime</t>
-  </si>
-  <si>
-    <t>CP.3 XD 100mm T2.1 Compact Prime</t>
-  </si>
-  <si>
-    <t>CP.3 XD 15mm T2.9 Compact Prime</t>
-  </si>
-  <si>
-    <t>CP.3 XD 18mm T2.9 Compact Prime</t>
-  </si>
-  <si>
-    <t>CP.3 XD 21mm T2.9 Compact Prime</t>
-  </si>
-  <si>
-    <t>CP.3 XD 25mm T2.1 Compact Prime</t>
-  </si>
-  <si>
-    <t>CP.3 XD 28mm T2.1 Compact Prime</t>
-  </si>
-  <si>
-    <t>CP.3 XD 35mm T2.1 Compact Prime</t>
-  </si>
-  <si>
-    <t>CP.3 XD 50mm T2.1 Compact Prime</t>
-  </si>
-  <si>
-    <t>CP.3 XD 85mm T2.1 Compact Prime</t>
-  </si>
-  <si>
-    <t>Added Zeiss CP.3 lenses</t>
   </si>
 </sst>
 </file>
@@ -2067,8 +2022,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q417" totalsRowShown="0">
-  <autoFilter ref="A1:Q417">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q403" totalsRowShown="0">
+  <autoFilter ref="A1:Q403">
     <filterColumn colId="11">
       <filters>
         <filter val="0"/>
@@ -2399,10 +2354,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q417"/>
+  <dimension ref="A1:Q403"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A398" workbookViewId="0">
-      <selection activeCell="B419" sqref="B419"/>
+    <sheetView tabSelected="1" topLeftCell="A321" workbookViewId="0">
+      <selection activeCell="B406" sqref="B406"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -18210,7 +18165,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="301" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="301" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A301" t="s">
         <v>133</v>
       </c>
@@ -18318,7 +18273,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="303" spans="1:17" ht="24.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="303" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A303" t="s">
         <v>133</v>
       </c>
@@ -18373,7 +18328,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="304" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="304" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A304" t="s">
         <v>133</v>
       </c>
@@ -18426,7 +18381,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="305" spans="1:17" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="305" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A305" t="s">
         <v>133</v>
       </c>
@@ -18481,7 +18436,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="306" spans="1:17" ht="15.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="306" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A306" t="s">
         <v>133</v>
       </c>
@@ -18534,7 +18489,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="307" spans="1:17" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="307" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A307" t="s">
         <v>133</v>
       </c>
@@ -18587,7 +18542,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="308" spans="1:17" ht="12.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="308" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A308" t="s">
         <v>133</v>
       </c>
@@ -18640,7 +18595,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="309" spans="1:17" ht="16.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="309" spans="1:17" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A309" t="s">
         <v>133</v>
       </c>
@@ -23403,622 +23358,6 @@
       </c>
       <c r="Q403">
         <v>402</v>
-      </c>
-    </row>
-    <row r="404" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A404" t="s">
-        <v>133</v>
-      </c>
-      <c r="B404" t="s">
-        <v>635</v>
-      </c>
-      <c r="C404">
-        <v>2017</v>
-      </c>
-      <c r="D404">
-        <v>7490</v>
-      </c>
-      <c r="E404">
-        <v>1150</v>
-      </c>
-      <c r="F404">
-        <v>126.5</v>
-      </c>
-      <c r="G404" s="8">
-        <v>95</v>
-      </c>
-      <c r="H404" s="1">
-        <v>2</v>
-      </c>
-      <c r="I404" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="J404" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="K404">
-        <v>0</v>
-      </c>
-      <c r="L404">
-        <v>1</v>
-      </c>
-      <c r="M404" t="s">
-        <v>285</v>
-      </c>
-      <c r="Q404">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="405" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A405" t="s">
-        <v>133</v>
-      </c>
-      <c r="B405" t="s">
-        <v>636</v>
-      </c>
-      <c r="C405">
-        <v>2017</v>
-      </c>
-      <c r="D405">
-        <v>4390</v>
-      </c>
-      <c r="E405">
-        <v>820</v>
-      </c>
-      <c r="F405">
-        <v>83.7</v>
-      </c>
-      <c r="G405" s="8">
-        <v>95</v>
-      </c>
-      <c r="H405" s="1">
-        <v>2</v>
-      </c>
-      <c r="I405" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="J405" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="K405">
-        <v>0</v>
-      </c>
-      <c r="L405">
-        <v>1</v>
-      </c>
-      <c r="M405" t="s">
-        <v>285</v>
-      </c>
-      <c r="Q405">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="406" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A406" t="s">
-        <v>133</v>
-      </c>
-      <c r="B406" t="s">
-        <v>637</v>
-      </c>
-      <c r="C406">
-        <v>2017</v>
-      </c>
-      <c r="D406">
-        <v>4390</v>
-      </c>
-      <c r="E406">
-        <v>800</v>
-      </c>
-      <c r="F406">
-        <v>83.7</v>
-      </c>
-      <c r="G406" s="8">
-        <v>95</v>
-      </c>
-      <c r="H406" s="1">
-        <v>2</v>
-      </c>
-      <c r="I406" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="J406" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="K406">
-        <v>0</v>
-      </c>
-      <c r="L406">
-        <v>1</v>
-      </c>
-      <c r="M406" t="s">
-        <v>285</v>
-      </c>
-      <c r="Q406">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="407" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A407" t="s">
-        <v>133</v>
-      </c>
-      <c r="B407" t="s">
-        <v>638</v>
-      </c>
-      <c r="C407">
-        <v>2017</v>
-      </c>
-      <c r="D407">
-        <v>4390</v>
-      </c>
-      <c r="E407">
-        <v>770</v>
-      </c>
-      <c r="F407">
-        <v>83.7</v>
-      </c>
-      <c r="G407" s="8">
-        <v>95</v>
-      </c>
-      <c r="H407" s="1">
-        <v>2</v>
-      </c>
-      <c r="I407" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="J407" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="K407">
-        <v>0</v>
-      </c>
-      <c r="L407">
-        <v>1</v>
-      </c>
-      <c r="M407" t="s">
-        <v>285</v>
-      </c>
-      <c r="Q407">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="408" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A408" t="s">
-        <v>133</v>
-      </c>
-      <c r="B408" t="s">
-        <v>639</v>
-      </c>
-      <c r="C408">
-        <v>2017</v>
-      </c>
-      <c r="D408">
-        <v>4390</v>
-      </c>
-      <c r="E408">
-        <v>880</v>
-      </c>
-      <c r="F408">
-        <v>83.7</v>
-      </c>
-      <c r="G408" s="8">
-        <v>95</v>
-      </c>
-      <c r="H408" s="1">
-        <v>2</v>
-      </c>
-      <c r="I408" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="J408" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="K408">
-        <v>0</v>
-      </c>
-      <c r="L408">
-        <v>1</v>
-      </c>
-      <c r="M408" t="s">
-        <v>285</v>
-      </c>
-      <c r="Q408">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="409" spans="1:17" ht="22.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A409" t="s">
-        <v>133</v>
-      </c>
-      <c r="B409" t="s">
-        <v>640</v>
-      </c>
-      <c r="C409">
-        <v>2017</v>
-      </c>
-      <c r="D409">
-        <v>6690</v>
-      </c>
-      <c r="E409">
-        <v>1010</v>
-      </c>
-      <c r="F409">
-        <v>126.5</v>
-      </c>
-      <c r="G409" s="8">
-        <v>95</v>
-      </c>
-      <c r="H409" s="1">
-        <v>2</v>
-      </c>
-      <c r="I409" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="J409" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="K409">
-        <v>0</v>
-      </c>
-      <c r="L409">
-        <v>1</v>
-      </c>
-      <c r="M409" t="s">
-        <v>285</v>
-      </c>
-      <c r="Q409">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="410" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A410" t="s">
-        <v>133</v>
-      </c>
-      <c r="B410" t="s">
-        <v>641</v>
-      </c>
-      <c r="C410">
-        <v>2017</v>
-      </c>
-      <c r="D410">
-        <v>7490</v>
-      </c>
-      <c r="E410">
-        <v>870</v>
-      </c>
-      <c r="F410">
-        <v>83.7</v>
-      </c>
-      <c r="G410" s="8">
-        <v>95</v>
-      </c>
-      <c r="H410" s="1">
-        <v>2.8</v>
-      </c>
-      <c r="I410" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="J410" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="K410">
-        <v>0</v>
-      </c>
-      <c r="L410">
-        <v>1</v>
-      </c>
-      <c r="M410" t="s">
-        <v>285</v>
-      </c>
-      <c r="Q410">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="411" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A411" t="s">
-        <v>133</v>
-      </c>
-      <c r="B411" t="s">
-        <v>642</v>
-      </c>
-      <c r="C411">
-        <v>2017</v>
-      </c>
-      <c r="D411">
-        <v>6690</v>
-      </c>
-      <c r="E411">
-        <v>860</v>
-      </c>
-      <c r="F411">
-        <v>83.7</v>
-      </c>
-      <c r="G411" s="8">
-        <v>95</v>
-      </c>
-      <c r="H411" s="1">
-        <v>2.8</v>
-      </c>
-      <c r="I411" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="J411" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="K411">
-        <v>0</v>
-      </c>
-      <c r="L411">
-        <v>1</v>
-      </c>
-      <c r="M411" t="s">
-        <v>285</v>
-      </c>
-      <c r="Q411">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="412" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A412" t="s">
-        <v>133</v>
-      </c>
-      <c r="B412" t="s">
-        <v>643</v>
-      </c>
-      <c r="C412">
-        <v>2017</v>
-      </c>
-      <c r="D412">
-        <v>5790</v>
-      </c>
-      <c r="E412">
-        <v>820</v>
-      </c>
-      <c r="F412">
-        <v>83.7</v>
-      </c>
-      <c r="G412" s="8">
-        <v>95</v>
-      </c>
-      <c r="H412" s="1">
-        <v>2.8</v>
-      </c>
-      <c r="I412" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="J412" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="K412">
-        <v>0</v>
-      </c>
-      <c r="L412">
-        <v>1</v>
-      </c>
-      <c r="M412" t="s">
-        <v>285</v>
-      </c>
-      <c r="Q412">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="413" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A413" t="s">
-        <v>133</v>
-      </c>
-      <c r="B413" t="s">
-        <v>644</v>
-      </c>
-      <c r="C413">
-        <v>2017</v>
-      </c>
-      <c r="D413">
-        <v>5790</v>
-      </c>
-      <c r="E413">
-        <v>820</v>
-      </c>
-      <c r="F413">
-        <v>83.7</v>
-      </c>
-      <c r="G413" s="8">
-        <v>95</v>
-      </c>
-      <c r="H413" s="1">
-        <v>2</v>
-      </c>
-      <c r="I413" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="J413" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="K413">
-        <v>0</v>
-      </c>
-      <c r="L413">
-        <v>1</v>
-      </c>
-      <c r="M413" t="s">
-        <v>285</v>
-      </c>
-      <c r="Q413">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="414" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A414" t="s">
-        <v>133</v>
-      </c>
-      <c r="B414" t="s">
-        <v>645</v>
-      </c>
-      <c r="C414">
-        <v>2017</v>
-      </c>
-      <c r="D414">
-        <v>5790</v>
-      </c>
-      <c r="E414">
-        <v>840</v>
-      </c>
-      <c r="F414">
-        <v>83.7</v>
-      </c>
-      <c r="G414" s="8">
-        <v>95</v>
-      </c>
-      <c r="H414" s="1">
-        <v>2</v>
-      </c>
-      <c r="I414" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="J414" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="K414">
-        <v>0</v>
-      </c>
-      <c r="L414">
-        <v>1</v>
-      </c>
-      <c r="M414" t="s">
-        <v>285</v>
-      </c>
-      <c r="Q414">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="415" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A415" t="s">
-        <v>133</v>
-      </c>
-      <c r="B415" t="s">
-        <v>646</v>
-      </c>
-      <c r="C415">
-        <v>2017</v>
-      </c>
-      <c r="D415">
-        <v>5790</v>
-      </c>
-      <c r="E415">
-        <v>800</v>
-      </c>
-      <c r="F415">
-        <v>83.7</v>
-      </c>
-      <c r="G415" s="8">
-        <v>95</v>
-      </c>
-      <c r="H415" s="1">
-        <v>2</v>
-      </c>
-      <c r="I415" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="J415" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="K415">
-        <v>0</v>
-      </c>
-      <c r="L415">
-        <v>1</v>
-      </c>
-      <c r="M415" t="s">
-        <v>285</v>
-      </c>
-      <c r="Q415">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="416" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A416" t="s">
-        <v>133</v>
-      </c>
-      <c r="B416" t="s">
-        <v>647</v>
-      </c>
-      <c r="C416">
-        <v>2017</v>
-      </c>
-      <c r="D416">
-        <v>5790</v>
-      </c>
-      <c r="E416">
-        <v>770</v>
-      </c>
-      <c r="F416">
-        <v>83.7</v>
-      </c>
-      <c r="G416" s="8">
-        <v>95</v>
-      </c>
-      <c r="H416" s="1">
-        <v>2</v>
-      </c>
-      <c r="I416" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="J416" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="K416">
-        <v>0</v>
-      </c>
-      <c r="L416">
-        <v>1</v>
-      </c>
-      <c r="M416" t="s">
-        <v>285</v>
-      </c>
-      <c r="Q416">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="417" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A417" t="s">
-        <v>133</v>
-      </c>
-      <c r="B417" t="s">
-        <v>648</v>
-      </c>
-      <c r="C417">
-        <v>2017</v>
-      </c>
-      <c r="D417">
-        <v>5790</v>
-      </c>
-      <c r="E417">
-        <v>880</v>
-      </c>
-      <c r="F417">
-        <v>83.7</v>
-      </c>
-      <c r="G417" s="8">
-        <v>95</v>
-      </c>
-      <c r="H417" s="1">
-        <v>2</v>
-      </c>
-      <c r="I417" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="J417" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="K417">
-        <v>0</v>
-      </c>
-      <c r="L417">
-        <v>1</v>
-      </c>
-      <c r="M417" t="s">
-        <v>285</v>
-      </c>
-      <c r="Q417">
-        <v>416</v>
       </c>
     </row>
   </sheetData>
@@ -24032,10 +23371,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+      <selection activeCell="P38" sqref="P38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -24411,14 +23750,6 @@
         <v>634</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="13">
-        <v>42910</v>
-      </c>
-      <c r="B48" t="s">
-        <v>649</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
+ lensbaby velvet 85
</commit_message>
<xml_diff>
--- a/BigAssTableOfLenses.xlsx
+++ b/BigAssTableOfLenses.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Markus\Desktop\BATOL\BigAssTableOfLenses\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brand\Optics\Olaf\Software\BigAssTableOfLenses\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8928"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8928" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LensTable" sheetId="1" r:id="rId1"/>
     <sheet name="Changelog" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3169" uniqueCount="657">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3105" uniqueCount="645">
   <si>
     <t>Manufacture</t>
   </si>
@@ -1953,49 +1953,13 @@
     <t>Cine lens metadata</t>
   </si>
   <si>
-    <t>CP.3 XD 135mm T2.1 Compact Prime</t>
-  </si>
-  <si>
-    <t>CP.3 25mm T2.1 Compact Prime</t>
-  </si>
-  <si>
-    <t>CP.3 35mm T2.1 Compact Prime</t>
-  </si>
-  <si>
-    <t>CP.3 50mm T2.1 Compact Prime</t>
-  </si>
-  <si>
-    <t>CP.3 85mm T2.1 Compact Prime</t>
-  </si>
-  <si>
-    <t>CP.3 XD 100mm T2.1 Compact Prime</t>
-  </si>
-  <si>
-    <t>CP.3 XD 15mm T2.9 Compact Prime</t>
-  </si>
-  <si>
-    <t>CP.3 XD 18mm T2.9 Compact Prime</t>
-  </si>
-  <si>
-    <t>CP.3 XD 21mm T2.9 Compact Prime</t>
-  </si>
-  <si>
-    <t>CP.3 XD 25mm T2.1 Compact Prime</t>
-  </si>
-  <si>
-    <t>CP.3 XD 28mm T2.1 Compact Prime</t>
-  </si>
-  <si>
-    <t>CP.3 XD 35mm T2.1 Compact Prime</t>
-  </si>
-  <si>
-    <t>CP.3 XD 50mm T2.1 Compact Prime</t>
-  </si>
-  <si>
-    <t>CP.3 XD 85mm T2.1 Compact Prime</t>
-  </si>
-  <si>
-    <t>Added CP.3 lenses</t>
+    <t>Lensbaby</t>
+  </si>
+  <si>
+    <t>Velvet 85mm f/1.8</t>
+  </si>
+  <si>
+    <t>Lensbaby Velvet 85mm added</t>
   </si>
 </sst>
 </file>
@@ -2088,8 +2052,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q419" totalsRowShown="0">
-  <autoFilter ref="A1:Q419"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q406" totalsRowShown="0">
+  <autoFilter ref="A1:Q406"/>
   <sortState ref="A2:Q403">
     <sortCondition ref="Q1:Q403"/>
   </sortState>
@@ -2414,30 +2378,30 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q419"/>
+  <dimension ref="A1:Q406"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A394" workbookViewId="0">
-      <selection activeCell="Q422" sqref="Q422"/>
+    <sheetView topLeftCell="A346" workbookViewId="0">
+      <selection activeCell="H407" sqref="H407"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.1015625" customWidth="1"/>
-    <col min="2" max="2" width="37.89453125" customWidth="1"/>
-    <col min="3" max="3" width="5.41796875" customWidth="1"/>
-    <col min="4" max="4" width="6.41796875" customWidth="1"/>
-    <col min="5" max="5" width="8.20703125" customWidth="1"/>
-    <col min="7" max="7" width="8.68359375" customWidth="1"/>
-    <col min="8" max="8" width="12.41796875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.1015625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="5.89453125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="10.20703125" customWidth="1"/>
+    <col min="1" max="1" width="8.109375" customWidth="1"/>
+    <col min="2" max="2" width="37.88671875" customWidth="1"/>
+    <col min="3" max="3" width="5.44140625" customWidth="1"/>
+    <col min="4" max="4" width="6.44140625" customWidth="1"/>
+    <col min="5" max="5" width="8.21875" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.109375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="5.88671875" style="4" customWidth="1"/>
+    <col min="11" max="11" width="10.21875" customWidth="1"/>
     <col min="12" max="12" width="9" customWidth="1"/>
-    <col min="13" max="13" width="11.68359375" customWidth="1"/>
-    <col min="15" max="16" width="8.89453125" style="12"/>
+    <col min="13" max="13" width="11.6640625" customWidth="1"/>
+    <col min="15" max="16" width="8.88671875" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2490,7 +2454,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -2545,7 +2509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -2600,7 +2564,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -2655,7 +2619,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -2710,7 +2674,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -2765,7 +2729,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -2820,7 +2784,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -2875,7 +2839,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2930,7 +2894,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2985,7 +2949,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -3040,7 +3004,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -3095,7 +3059,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -3150,7 +3114,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -3205,7 +3169,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
@@ -3260,7 +3224,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
@@ -3315,7 +3279,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
@@ -3370,7 +3334,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
@@ -3425,7 +3389,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -3480,7 +3444,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
@@ -3535,7 +3499,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
@@ -3590,7 +3554,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
@@ -3645,7 +3609,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
@@ -3700,7 +3664,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
@@ -3755,7 +3719,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
@@ -3810,7 +3774,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
@@ -3865,7 +3829,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
@@ -3920,7 +3884,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>7</v>
       </c>
@@ -3975,7 +3939,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>7</v>
       </c>
@@ -4030,7 +3994,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>7</v>
       </c>
@@ -4085,7 +4049,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>7</v>
       </c>
@@ -4140,7 +4104,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>7</v>
       </c>
@@ -4195,7 +4159,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
@@ -4250,7 +4214,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>7</v>
       </c>
@@ -4305,7 +4269,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>7</v>
       </c>
@@ -4360,7 +4324,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>7</v>
       </c>
@@ -4415,7 +4379,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>7</v>
       </c>
@@ -4470,7 +4434,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -4525,7 +4489,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -4580,7 +4544,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -4635,7 +4599,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>7</v>
       </c>
@@ -4690,7 +4654,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>7</v>
       </c>
@@ -4745,7 +4709,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>7</v>
       </c>
@@ -4800,7 +4764,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -4853,7 +4817,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>7</v>
       </c>
@@ -4908,7 +4872,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>7</v>
       </c>
@@ -4963,7 +4927,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>7</v>
       </c>
@@ -5018,7 +4982,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>7</v>
       </c>
@@ -5073,7 +5037,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>7</v>
       </c>
@@ -5128,7 +5092,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>7</v>
       </c>
@@ -5183,7 +5147,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>7</v>
       </c>
@@ -5238,7 +5202,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -5293,7 +5257,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>7</v>
       </c>
@@ -5348,7 +5312,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>7</v>
       </c>
@@ -5403,7 +5367,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>7</v>
       </c>
@@ -5458,7 +5422,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>7</v>
       </c>
@@ -5513,7 +5477,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>7</v>
       </c>
@@ -5568,7 +5532,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>7</v>
       </c>
@@ -5623,7 +5587,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>7</v>
       </c>
@@ -5678,7 +5642,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>7</v>
       </c>
@@ -5733,7 +5697,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>7</v>
       </c>
@@ -5786,7 +5750,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>7</v>
       </c>
@@ -5841,7 +5805,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>7</v>
       </c>
@@ -5894,7 +5858,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>7</v>
       </c>
@@ -5947,7 +5911,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>7</v>
       </c>
@@ -6000,7 +5964,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>7</v>
       </c>
@@ -6053,7 +6017,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>7</v>
       </c>
@@ -6106,7 +6070,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>377</v>
       </c>
@@ -6159,7 +6123,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>377</v>
       </c>
@@ -6212,7 +6176,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>377</v>
       </c>
@@ -6265,7 +6229,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>377</v>
       </c>
@@ -6318,7 +6282,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>377</v>
       </c>
@@ -6371,7 +6335,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>377</v>
       </c>
@@ -6424,7 +6388,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>377</v>
       </c>
@@ -6477,7 +6441,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>377</v>
       </c>
@@ -6530,7 +6494,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>377</v>
       </c>
@@ -6583,7 +6547,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>377</v>
       </c>
@@ -6636,7 +6600,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>377</v>
       </c>
@@ -6689,7 +6653,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>377</v>
       </c>
@@ -6742,7 +6706,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>377</v>
       </c>
@@ -6795,7 +6759,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>377</v>
       </c>
@@ -6848,7 +6812,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>377</v>
       </c>
@@ -6901,7 +6865,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>377</v>
       </c>
@@ -6954,7 +6918,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>377</v>
       </c>
@@ -7007,7 +6971,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>377</v>
       </c>
@@ -7060,7 +7024,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>377</v>
       </c>
@@ -7113,7 +7077,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>377</v>
       </c>
@@ -7166,7 +7130,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>377</v>
       </c>
@@ -7216,7 +7180,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>293</v>
       </c>
@@ -7268,7 +7232,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>428</v>
       </c>
@@ -7315,7 +7279,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>428</v>
       </c>
@@ -7362,7 +7326,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>232</v>
       </c>
@@ -7415,7 +7379,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>232</v>
       </c>
@@ -7468,7 +7432,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>232</v>
       </c>
@@ -7521,7 +7485,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>232</v>
       </c>
@@ -7574,7 +7538,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>232</v>
       </c>
@@ -7627,7 +7591,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>232</v>
       </c>
@@ -7680,7 +7644,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>232</v>
       </c>
@@ -7735,7 +7699,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>232</v>
       </c>
@@ -7791,7 +7755,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>232</v>
       </c>
@@ -7846,7 +7810,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>232</v>
       </c>
@@ -7899,7 +7863,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>232</v>
       </c>
@@ -7952,7 +7916,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>232</v>
       </c>
@@ -8005,7 +7969,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>232</v>
       </c>
@@ -8058,7 +8022,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>232</v>
       </c>
@@ -8111,7 +8075,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>232</v>
       </c>
@@ -8164,7 +8128,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>232</v>
       </c>
@@ -8220,7 +8184,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>232</v>
       </c>
@@ -8273,7 +8237,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>232</v>
       </c>
@@ -8326,7 +8290,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>232</v>
       </c>
@@ -8379,7 +8343,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>232</v>
       </c>
@@ -8432,7 +8396,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>232</v>
       </c>
@@ -8485,7 +8449,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>232</v>
       </c>
@@ -8538,7 +8502,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>232</v>
       </c>
@@ -8591,7 +8555,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>232</v>
       </c>
@@ -8644,7 +8608,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>232</v>
       </c>
@@ -8700,7 +8664,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>232</v>
       </c>
@@ -8756,7 +8720,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>232</v>
       </c>
@@ -8809,7 +8773,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>232</v>
       </c>
@@ -8862,7 +8826,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>232</v>
       </c>
@@ -8915,7 +8879,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>295</v>
       </c>
@@ -8970,7 +8934,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>295</v>
       </c>
@@ -9025,7 +8989,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>295</v>
       </c>
@@ -9080,7 +9044,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>59</v>
       </c>
@@ -9132,7 +9096,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>59</v>
       </c>
@@ -9184,7 +9148,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>59</v>
       </c>
@@ -9236,7 +9200,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>59</v>
       </c>
@@ -9288,7 +9252,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>59</v>
       </c>
@@ -9340,7 +9304,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>59</v>
       </c>
@@ -9392,7 +9356,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>59</v>
       </c>
@@ -9444,7 +9408,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>59</v>
       </c>
@@ -9496,7 +9460,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>59</v>
       </c>
@@ -9548,7 +9512,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>59</v>
       </c>
@@ -9600,7 +9564,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>59</v>
       </c>
@@ -9652,7 +9616,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>59</v>
       </c>
@@ -9704,7 +9668,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>59</v>
       </c>
@@ -9756,7 +9720,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>59</v>
       </c>
@@ -9808,7 +9772,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>59</v>
       </c>
@@ -9860,7 +9824,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>59</v>
       </c>
@@ -9913,7 +9877,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>59</v>
       </c>
@@ -9965,7 +9929,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>59</v>
       </c>
@@ -10017,7 +9981,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="142" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>59</v>
       </c>
@@ -10070,7 +10034,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>59</v>
       </c>
@@ -10123,7 +10087,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>59</v>
       </c>
@@ -10176,7 +10140,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="145" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>59</v>
       </c>
@@ -10229,7 +10193,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>59</v>
       </c>
@@ -10282,7 +10246,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>59</v>
       </c>
@@ -10334,7 +10298,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>59</v>
       </c>
@@ -10386,7 +10350,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="149" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>59</v>
       </c>
@@ -10438,7 +10402,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>59</v>
       </c>
@@ -10490,7 +10454,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>59</v>
       </c>
@@ -10542,7 +10506,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>59</v>
       </c>
@@ -10594,7 +10558,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="153" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>59</v>
       </c>
@@ -10646,7 +10610,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="154" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>59</v>
       </c>
@@ -10698,7 +10662,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="155" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>59</v>
       </c>
@@ -10750,7 +10714,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>59</v>
       </c>
@@ -10800,7 +10764,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>59</v>
       </c>
@@ -10850,7 +10814,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>59</v>
       </c>
@@ -10900,7 +10864,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>59</v>
       </c>
@@ -10950,7 +10914,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>59</v>
       </c>
@@ -11000,7 +10964,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="161" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>370</v>
       </c>
@@ -11050,7 +11014,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="162" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>370</v>
       </c>
@@ -11100,7 +11064,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="163" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="163" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>370</v>
       </c>
@@ -11150,7 +11114,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="164" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="164" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>437</v>
       </c>
@@ -11200,7 +11164,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="165" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>437</v>
       </c>
@@ -11250,7 +11214,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="166" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="166" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>437</v>
       </c>
@@ -11300,7 +11264,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="167" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="167" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>431</v>
       </c>
@@ -11355,7 +11319,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="168" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="168" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>431</v>
       </c>
@@ -11408,7 +11372,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="169" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="169" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>431</v>
       </c>
@@ -11464,7 +11428,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="170" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="170" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>431</v>
       </c>
@@ -11517,7 +11481,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="171" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="171" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>431</v>
       </c>
@@ -11572,7 +11536,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="172" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="172" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A172" s="12" t="s">
         <v>431</v>
       </c>
@@ -11625,7 +11589,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="173" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="173" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A173" s="12" t="s">
         <v>431</v>
       </c>
@@ -11680,7 +11644,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="174" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="174" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A174" s="12" t="s">
         <v>431</v>
       </c>
@@ -11733,7 +11697,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="175" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="175" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A175" s="12" t="s">
         <v>431</v>
       </c>
@@ -11788,7 +11752,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="176" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="176" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A176" s="12" t="s">
         <v>431</v>
       </c>
@@ -11841,7 +11805,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="177" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A177" s="12" t="s">
         <v>431</v>
       </c>
@@ -11894,7 +11858,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="178" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="178" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A178" s="12" t="s">
         <v>431</v>
       </c>
@@ -11947,7 +11911,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="179" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="179" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>218</v>
       </c>
@@ -12002,7 +11966,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="180" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="180" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>218</v>
       </c>
@@ -12057,7 +12021,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="181" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="181" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>218</v>
       </c>
@@ -12112,7 +12076,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="182" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="182" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>100</v>
       </c>
@@ -12164,7 +12128,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="183" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="183" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>100</v>
       </c>
@@ -12216,7 +12180,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="184" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="184" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>100</v>
       </c>
@@ -12268,7 +12232,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="185" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="185" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>100</v>
       </c>
@@ -12320,7 +12284,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="186" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="186" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>100</v>
       </c>
@@ -12372,7 +12336,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="187" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="187" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>100</v>
       </c>
@@ -12424,7 +12388,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="188" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="188" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>100</v>
       </c>
@@ -12476,7 +12440,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="189" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="189" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>100</v>
       </c>
@@ -12528,7 +12492,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="190" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="190" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>100</v>
       </c>
@@ -12580,7 +12544,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="191" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="191" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>100</v>
       </c>
@@ -12632,7 +12596,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="192" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="192" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>100</v>
       </c>
@@ -12684,7 +12648,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="193" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="193" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>100</v>
       </c>
@@ -12734,7 +12698,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="194" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="194" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>100</v>
       </c>
@@ -12784,7 +12748,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="195" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="195" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>100</v>
       </c>
@@ -12831,7 +12795,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="196" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="196" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>100</v>
       </c>
@@ -12881,7 +12845,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="197" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="197" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>100</v>
       </c>
@@ -12931,7 +12895,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="198" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="198" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>100</v>
       </c>
@@ -12981,7 +12945,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="199" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="199" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>166</v>
       </c>
@@ -13033,7 +12997,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="200" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="200" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>166</v>
       </c>
@@ -13085,7 +13049,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="201" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="201" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>166</v>
       </c>
@@ -13137,7 +13101,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="202" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="202" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>166</v>
       </c>
@@ -13189,7 +13153,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="203" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="203" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>166</v>
       </c>
@@ -13241,7 +13205,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="204" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="204" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>166</v>
       </c>
@@ -13293,7 +13257,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="205" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="205" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>166</v>
       </c>
@@ -13346,7 +13310,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="206" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="206" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>166</v>
       </c>
@@ -13398,7 +13362,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="207" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="207" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>166</v>
       </c>
@@ -13450,7 +13414,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="208" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="208" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>166</v>
       </c>
@@ -13502,7 +13466,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="209" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="209" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>166</v>
       </c>
@@ -13554,7 +13518,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="210" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="210" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>166</v>
       </c>
@@ -13606,7 +13570,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="211" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="211" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>166</v>
       </c>
@@ -13658,7 +13622,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="212" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="212" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>166</v>
       </c>
@@ -13710,7 +13674,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="213" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="213" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>166</v>
       </c>
@@ -13762,7 +13726,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="214" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="214" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>166</v>
       </c>
@@ -13812,7 +13776,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="215" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="215" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>182</v>
       </c>
@@ -13864,7 +13828,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="216" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="216" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>182</v>
       </c>
@@ -13916,7 +13880,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="217" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="217" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>182</v>
       </c>
@@ -13968,7 +13932,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="218" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="218" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>182</v>
       </c>
@@ -14020,7 +13984,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="219" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="219" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>182</v>
       </c>
@@ -14072,7 +14036,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="220" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="220" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>182</v>
       </c>
@@ -14124,7 +14088,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="221" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="221" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>182</v>
       </c>
@@ -14176,7 +14140,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="222" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="222" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>182</v>
       </c>
@@ -14228,7 +14192,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="223" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="223" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>182</v>
       </c>
@@ -14280,7 +14244,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="224" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="224" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>182</v>
       </c>
@@ -14330,7 +14294,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="225" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="225" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A225" s="1" t="s">
         <v>182</v>
       </c>
@@ -14380,7 +14344,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="226" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="226" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A226" s="1" t="s">
         <v>182</v>
       </c>
@@ -14430,7 +14394,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="227" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="227" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>191</v>
       </c>
@@ -14482,7 +14446,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="228" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="228" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>191</v>
       </c>
@@ -14534,7 +14498,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="229" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="229" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>191</v>
       </c>
@@ -14586,7 +14550,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="230" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="230" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>191</v>
       </c>
@@ -14638,7 +14602,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="231" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="231" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>191</v>
       </c>
@@ -14690,7 +14654,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="232" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="232" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>191</v>
       </c>
@@ -14740,7 +14704,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="233" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="233" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>263</v>
       </c>
@@ -14793,7 +14757,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="234" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="234" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A234" s="1" t="s">
         <v>263</v>
       </c>
@@ -14846,7 +14810,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="235" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="235" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A235" s="1" t="s">
         <v>263</v>
       </c>
@@ -14899,7 +14863,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="236" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="236" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A236" s="1" t="s">
         <v>263</v>
       </c>
@@ -14952,7 +14916,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="237" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="237" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A237" s="1" t="s">
         <v>220</v>
       </c>
@@ -15001,7 +14965,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="238" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="238" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A238" s="1" t="s">
         <v>220</v>
       </c>
@@ -15048,7 +15012,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="239" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="239" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A239" s="1" t="s">
         <v>220</v>
       </c>
@@ -15095,7 +15059,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="240" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="240" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A240" s="1" t="s">
         <v>220</v>
       </c>
@@ -15144,7 +15108,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="241" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="241" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A241" s="1" t="s">
         <v>220</v>
       </c>
@@ -15191,7 +15155,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="242" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="242" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A242" s="1" t="s">
         <v>220</v>
       </c>
@@ -15238,7 +15202,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="243" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="243" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A243" s="1" t="s">
         <v>220</v>
       </c>
@@ -15285,7 +15249,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="244" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="244" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A244" s="1" t="s">
         <v>220</v>
       </c>
@@ -15334,7 +15298,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="245" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="245" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A245" s="1" t="s">
         <v>220</v>
       </c>
@@ -15381,7 +15345,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="246" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="246" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A246" s="1" t="s">
         <v>220</v>
       </c>
@@ -15428,7 +15392,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="247" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="247" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>220</v>
       </c>
@@ -15475,7 +15439,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="248" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="248" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>220</v>
       </c>
@@ -15522,7 +15486,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="249" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="249" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>220</v>
       </c>
@@ -15569,7 +15533,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="250" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="250" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>220</v>
       </c>
@@ -15618,7 +15582,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="251" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="251" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>220</v>
       </c>
@@ -15665,7 +15629,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="252" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="252" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A252" s="1" t="s">
         <v>220</v>
       </c>
@@ -15712,7 +15676,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="253" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="253" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A253" s="1" t="s">
         <v>220</v>
       </c>
@@ -15759,7 +15723,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="254" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="254" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>132</v>
       </c>
@@ -15814,7 +15778,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="255" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="255" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>132</v>
       </c>
@@ -15867,7 +15831,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="256" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="256" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>132</v>
       </c>
@@ -15920,7 +15884,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="257" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="257" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>132</v>
       </c>
@@ -15975,7 +15939,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="258" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="258" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>132</v>
       </c>
@@ -16028,7 +15992,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="259" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="259" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>132</v>
       </c>
@@ -16081,7 +16045,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="260" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="260" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>132</v>
       </c>
@@ -16136,7 +16100,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="261" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="261" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>132</v>
       </c>
@@ -16191,7 +16155,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="262" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="262" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>132</v>
       </c>
@@ -16246,7 +16210,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="263" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="263" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>132</v>
       </c>
@@ -16299,7 +16263,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="264" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="264" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>132</v>
       </c>
@@ -16352,7 +16316,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="265" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="265" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>132</v>
       </c>
@@ -16405,7 +16369,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="266" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="266" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>132</v>
       </c>
@@ -16460,7 +16424,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="267" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="267" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>132</v>
       </c>
@@ -16515,7 +16479,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="268" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="268" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A268" s="1" t="s">
         <v>132</v>
       </c>
@@ -16570,7 +16534,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="269" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="269" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A269" s="1" t="s">
         <v>132</v>
       </c>
@@ -16623,7 +16587,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="270" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="270" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>132</v>
       </c>
@@ -16676,7 +16640,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="271" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="271" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>132</v>
       </c>
@@ -16731,7 +16695,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="272" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="272" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>132</v>
       </c>
@@ -16786,7 +16750,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="273" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="273" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>132</v>
       </c>
@@ -16839,7 +16803,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="274" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="274" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>132</v>
       </c>
@@ -16892,7 +16856,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="275" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="275" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>132</v>
       </c>
@@ -16947,7 +16911,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="276" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="276" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>132</v>
       </c>
@@ -17002,7 +16966,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="277" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="277" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>132</v>
       </c>
@@ -17057,7 +17021,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="278" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="278" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>132</v>
       </c>
@@ -17112,7 +17076,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="279" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="279" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>132</v>
       </c>
@@ -17165,7 +17129,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="280" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="280" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>132</v>
       </c>
@@ -17218,7 +17182,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="281" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="281" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>132</v>
       </c>
@@ -17271,7 +17235,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="282" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="282" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>132</v>
       </c>
@@ -17324,7 +17288,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="283" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="283" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>132</v>
       </c>
@@ -17377,7 +17341,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="284" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="284" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>132</v>
       </c>
@@ -17432,7 +17396,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="285" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="285" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>132</v>
       </c>
@@ -17487,7 +17451,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="286" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="286" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>132</v>
       </c>
@@ -17542,7 +17506,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="287" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="287" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>132</v>
       </c>
@@ -17597,7 +17561,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="288" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="288" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>132</v>
       </c>
@@ -17652,7 +17616,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="289" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="289" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>132</v>
       </c>
@@ -17705,7 +17669,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="290" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="290" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>132</v>
       </c>
@@ -17758,7 +17722,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="291" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="291" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>132</v>
       </c>
@@ -17811,7 +17775,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="292" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="292" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>132</v>
       </c>
@@ -17864,7 +17828,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="293" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="293" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>132</v>
       </c>
@@ -17917,7 +17881,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="294" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="294" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>132</v>
       </c>
@@ -17972,7 +17936,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="295" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="295" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>132</v>
       </c>
@@ -18027,7 +17991,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="296" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="296" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>132</v>
       </c>
@@ -18082,7 +18046,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="297" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="297" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>132</v>
       </c>
@@ -18137,7 +18101,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="298" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="298" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>132</v>
       </c>
@@ -18192,7 +18156,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="299" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="299" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>132</v>
       </c>
@@ -18245,7 +18209,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="300" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="300" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>132</v>
       </c>
@@ -18298,7 +18262,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="301" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="301" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>132</v>
       </c>
@@ -18351,7 +18315,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="302" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="302" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>132</v>
       </c>
@@ -18406,7 +18370,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="303" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="303" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>132</v>
       </c>
@@ -18461,7 +18425,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="304" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="304" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>132</v>
       </c>
@@ -18514,7 +18478,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="305" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="305" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>132</v>
       </c>
@@ -18569,7 +18533,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="306" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="306" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>132</v>
       </c>
@@ -18622,7 +18586,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="307" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="307" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>132</v>
       </c>
@@ -18675,7 +18639,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="308" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="308" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>132</v>
       </c>
@@ -18728,7 +18692,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="309" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="309" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>132</v>
       </c>
@@ -18781,7 +18745,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="310" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="310" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>132</v>
       </c>
@@ -18834,7 +18798,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="311" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="311" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>132</v>
       </c>
@@ -18887,7 +18851,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="312" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="312" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>132</v>
       </c>
@@ -18940,7 +18904,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="313" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="313" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>132</v>
       </c>
@@ -18993,7 +18957,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="314" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="314" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>132</v>
       </c>
@@ -19046,7 +19010,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="315" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="315" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>377</v>
       </c>
@@ -19099,7 +19063,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="316" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="316" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>377</v>
       </c>
@@ -19152,7 +19116,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="317" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="317" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>100</v>
       </c>
@@ -19202,7 +19166,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="318" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="318" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>100</v>
       </c>
@@ -19252,7 +19216,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="319" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="319" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>100</v>
       </c>
@@ -19300,7 +19264,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="320" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="320" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>100</v>
       </c>
@@ -19350,7 +19314,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="321" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="321" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>7</v>
       </c>
@@ -19403,7 +19367,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="322" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="322" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>218</v>
       </c>
@@ -19454,7 +19418,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="323" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="323" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>218</v>
       </c>
@@ -19505,7 +19469,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="324" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="324" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>218</v>
       </c>
@@ -19556,7 +19520,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="325" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="325" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>100</v>
       </c>
@@ -19605,7 +19569,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="326" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="326" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>191</v>
       </c>
@@ -19656,7 +19620,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="327" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="327" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>7</v>
       </c>
@@ -19705,7 +19669,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="328" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="328" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>7</v>
       </c>
@@ -19758,7 +19722,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="329" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="329" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>7</v>
       </c>
@@ -19811,7 +19775,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="330" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="330" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>7</v>
       </c>
@@ -19864,7 +19828,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="331" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="331" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>7</v>
       </c>
@@ -19917,7 +19881,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="332" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="332" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>218</v>
       </c>
@@ -19968,7 +19932,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="333" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="333" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>218</v>
       </c>
@@ -20019,7 +19983,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="334" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="334" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>218</v>
       </c>
@@ -20070,7 +20034,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="335" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="335" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>218</v>
       </c>
@@ -20121,7 +20085,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="336" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="336" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>218</v>
       </c>
@@ -20172,7 +20136,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="337" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="337" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>218</v>
       </c>
@@ -20223,7 +20187,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="338" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="338" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
         <v>504</v>
       </c>
@@ -20276,7 +20240,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="339" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="339" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
         <v>504</v>
       </c>
@@ -20327,7 +20291,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="340" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="340" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
         <v>504</v>
       </c>
@@ -20378,7 +20342,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="341" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="341" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>504</v>
       </c>
@@ -20429,7 +20393,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="342" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="342" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
         <v>504</v>
       </c>
@@ -20480,7 +20444,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="343" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="343" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
         <v>504</v>
       </c>
@@ -20531,7 +20495,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="344" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="344" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
         <v>504</v>
       </c>
@@ -20582,7 +20546,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="345" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="345" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
         <v>504</v>
       </c>
@@ -20633,7 +20597,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="346" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="346" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
         <v>504</v>
       </c>
@@ -20684,7 +20648,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="347" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="347" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
         <v>504</v>
       </c>
@@ -20735,7 +20699,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="348" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="348" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
         <v>504</v>
       </c>
@@ -20786,7 +20750,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="349" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="349" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
         <v>504</v>
       </c>
@@ -20837,7 +20801,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="350" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="350" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
         <v>504</v>
       </c>
@@ -20888,7 +20852,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="351" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="351" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
         <v>504</v>
       </c>
@@ -20939,7 +20903,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="352" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="352" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
         <v>504</v>
       </c>
@@ -20990,7 +20954,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="353" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="353" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
         <v>504</v>
       </c>
@@ -21041,7 +21005,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="354" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="354" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
         <v>504</v>
       </c>
@@ -21092,7 +21056,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="355" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="355" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
         <v>377</v>
       </c>
@@ -21145,7 +21109,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="356" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="356" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
         <v>377</v>
       </c>
@@ -21198,7 +21162,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="357" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="357" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
         <v>377</v>
       </c>
@@ -21251,7 +21215,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="358" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="358" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
         <v>377</v>
       </c>
@@ -21304,7 +21268,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="359" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="359" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
         <v>377</v>
       </c>
@@ -21357,7 +21321,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="360" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="360" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
         <v>377</v>
       </c>
@@ -21410,7 +21374,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="361" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="361" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
         <v>377</v>
       </c>
@@ -21463,7 +21427,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="362" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="362" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
         <v>377</v>
       </c>
@@ -21516,7 +21480,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="363" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="363" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
         <v>377</v>
       </c>
@@ -21569,7 +21533,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="364" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="364" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
         <v>100</v>
       </c>
@@ -21619,7 +21583,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="365" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="365" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
         <v>100</v>
       </c>
@@ -21669,7 +21633,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="366" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="366" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
         <v>100</v>
       </c>
@@ -21719,7 +21683,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="367" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="367" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
         <v>100</v>
       </c>
@@ -21769,7 +21733,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="368" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="368" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
         <v>100</v>
       </c>
@@ -21819,7 +21783,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="369" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="369" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
         <v>100</v>
       </c>
@@ -21869,7 +21833,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="370" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="370" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
         <v>100</v>
       </c>
@@ -21919,7 +21883,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="371" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="371" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
         <v>100</v>
       </c>
@@ -21969,7 +21933,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="372" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="372" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
         <v>191</v>
       </c>
@@ -22019,7 +21983,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="373" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="373" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
         <v>191</v>
       </c>
@@ -22069,7 +22033,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="374" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="374" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
         <v>191</v>
       </c>
@@ -22119,7 +22083,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="375" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="375" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
         <v>191</v>
       </c>
@@ -22169,7 +22133,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="376" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="376" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
         <v>191</v>
       </c>
@@ -22217,7 +22181,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="377" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="377" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
         <v>191</v>
       </c>
@@ -22267,7 +22231,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="378" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="378" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
         <v>191</v>
       </c>
@@ -22317,7 +22281,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="379" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="379" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A379" t="s">
         <v>132</v>
       </c>
@@ -22370,7 +22334,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="380" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="380" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A380" t="s">
         <v>7</v>
       </c>
@@ -22423,7 +22387,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="381" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="381" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A381" t="s">
         <v>431</v>
       </c>
@@ -22476,7 +22440,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="382" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="382" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A382" t="s">
         <v>431</v>
       </c>
@@ -22529,7 +22493,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="383" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="383" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A383" t="s">
         <v>431</v>
       </c>
@@ -22582,7 +22546,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="384" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="384" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A384" t="s">
         <v>431</v>
       </c>
@@ -22635,7 +22599,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="385" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="385" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A385" s="7" t="s">
         <v>182</v>
       </c>
@@ -22685,7 +22649,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="386" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="386" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A386" s="7" t="s">
         <v>132</v>
       </c>
@@ -22738,7 +22702,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="387" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="387" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A387" s="7" t="s">
         <v>166</v>
       </c>
@@ -22788,7 +22752,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="388" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="388" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A388" s="7" t="s">
         <v>166</v>
       </c>
@@ -22838,7 +22802,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="389" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="389" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A389" s="7" t="s">
         <v>166</v>
       </c>
@@ -22888,7 +22852,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="390" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="390" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A390" s="7" t="s">
         <v>263</v>
       </c>
@@ -22939,7 +22903,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="391" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="391" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A391" s="7" t="s">
         <v>263</v>
       </c>
@@ -22992,7 +22956,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="392" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="392" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A392" s="7" t="s">
         <v>377</v>
       </c>
@@ -23045,7 +23009,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="393" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="393" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A393" s="7" t="s">
         <v>377</v>
       </c>
@@ -23098,7 +23062,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="394" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="394" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A394" s="7" t="s">
         <v>377</v>
       </c>
@@ -23151,7 +23115,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="395" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="395" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A395" s="7" t="s">
         <v>377</v>
       </c>
@@ -23196,7 +23160,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="396" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="396" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A396" s="7" t="s">
         <v>603</v>
       </c>
@@ -23243,7 +23207,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="397" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="397" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A397" s="7" t="s">
         <v>603</v>
       </c>
@@ -23290,7 +23254,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="398" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="398" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A398" t="s">
         <v>614</v>
       </c>
@@ -23343,7 +23307,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="399" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="399" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A399" t="s">
         <v>614</v>
       </c>
@@ -23392,7 +23356,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="400" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="400" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A400" t="s">
         <v>59</v>
       </c>
@@ -23442,7 +23406,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="401" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="401" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A401" t="s">
         <v>59</v>
       </c>
@@ -23492,7 +23456,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="402" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="402" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A402" t="s">
         <v>59</v>
       </c>
@@ -23542,7 +23506,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="403" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="403" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A403" t="s">
         <v>166</v>
       </c>
@@ -23592,7 +23556,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="404" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="404" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A404" t="s">
         <v>182</v>
       </c>
@@ -23634,7 +23598,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="405" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="405" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A405" t="s">
         <v>182</v>
       </c>
@@ -23687,33 +23651,33 @@
         <v>404</v>
       </c>
     </row>
-    <row r="406" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="406" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A406" t="s">
-        <v>132</v>
+        <v>642</v>
       </c>
       <c r="B406" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="C406">
         <v>2017</v>
       </c>
       <c r="D406">
-        <v>7490</v>
+        <v>499.95</v>
       </c>
       <c r="E406">
-        <v>1150</v>
+        <v>530.13610000000006</v>
       </c>
       <c r="F406">
-        <v>126.5</v>
+        <v>89</v>
       </c>
       <c r="G406" s="8">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="H406" s="1">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="I406" s="9" t="s">
-        <v>125</v>
+        <v>77</v>
       </c>
       <c r="J406" s="9" t="s">
         <v>179</v>
@@ -23722,585 +23686,18 @@
         <v>0</v>
       </c>
       <c r="L406">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M406" t="s">
         <v>284</v>
       </c>
+      <c r="N406" t="s">
+        <v>583</v>
+      </c>
+      <c r="O406" s="10"/>
+      <c r="P406" s="10"/>
       <c r="Q406">
         <v>405</v>
-      </c>
-    </row>
-    <row r="407" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A407" t="s">
-        <v>132</v>
-      </c>
-      <c r="B407" t="s">
-        <v>643</v>
-      </c>
-      <c r="C407">
-        <v>2017</v>
-      </c>
-      <c r="D407">
-        <v>4390</v>
-      </c>
-      <c r="E407">
-        <v>820</v>
-      </c>
-      <c r="F407">
-        <v>83.7</v>
-      </c>
-      <c r="G407" s="8">
-        <v>95</v>
-      </c>
-      <c r="H407" s="1">
-        <v>2</v>
-      </c>
-      <c r="I407" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="J407" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="K407">
-        <v>0</v>
-      </c>
-      <c r="L407">
-        <v>1</v>
-      </c>
-      <c r="M407" t="s">
-        <v>284</v>
-      </c>
-      <c r="Q407" s="12">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="408" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A408" t="s">
-        <v>132</v>
-      </c>
-      <c r="B408" t="s">
-        <v>644</v>
-      </c>
-      <c r="C408">
-        <v>2017</v>
-      </c>
-      <c r="D408">
-        <v>4390</v>
-      </c>
-      <c r="E408">
-        <v>800</v>
-      </c>
-      <c r="F408">
-        <v>83.7</v>
-      </c>
-      <c r="G408" s="8">
-        <v>95</v>
-      </c>
-      <c r="H408" s="1">
-        <v>2</v>
-      </c>
-      <c r="I408" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="J408" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="K408">
-        <v>0</v>
-      </c>
-      <c r="L408">
-        <v>1</v>
-      </c>
-      <c r="M408" t="s">
-        <v>284</v>
-      </c>
-      <c r="Q408" s="12">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="409" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A409" t="s">
-        <v>132</v>
-      </c>
-      <c r="B409" t="s">
-        <v>645</v>
-      </c>
-      <c r="C409">
-        <v>2017</v>
-      </c>
-      <c r="D409">
-        <v>4390</v>
-      </c>
-      <c r="E409">
-        <v>770</v>
-      </c>
-      <c r="F409">
-        <v>83.7</v>
-      </c>
-      <c r="G409" s="8">
-        <v>95</v>
-      </c>
-      <c r="H409" s="1">
-        <v>2</v>
-      </c>
-      <c r="I409" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="J409" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="K409">
-        <v>0</v>
-      </c>
-      <c r="L409">
-        <v>1</v>
-      </c>
-      <c r="M409" t="s">
-        <v>284</v>
-      </c>
-      <c r="Q409" s="12">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="410" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A410" t="s">
-        <v>132</v>
-      </c>
-      <c r="B410" t="s">
-        <v>646</v>
-      </c>
-      <c r="C410">
-        <v>2017</v>
-      </c>
-      <c r="D410">
-        <v>4390</v>
-      </c>
-      <c r="E410">
-        <v>880</v>
-      </c>
-      <c r="F410">
-        <v>83.7</v>
-      </c>
-      <c r="G410" s="8">
-        <v>95</v>
-      </c>
-      <c r="H410" s="1">
-        <v>2</v>
-      </c>
-      <c r="I410" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="J410" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="K410">
-        <v>0</v>
-      </c>
-      <c r="L410">
-        <v>1</v>
-      </c>
-      <c r="M410" t="s">
-        <v>284</v>
-      </c>
-      <c r="Q410" s="12">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="411" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A411" t="s">
-        <v>132</v>
-      </c>
-      <c r="B411" t="s">
-        <v>647</v>
-      </c>
-      <c r="C411">
-        <v>2017</v>
-      </c>
-      <c r="D411">
-        <v>6690</v>
-      </c>
-      <c r="E411">
-        <v>1010</v>
-      </c>
-      <c r="F411">
-        <v>126.5</v>
-      </c>
-      <c r="G411" s="8">
-        <v>95</v>
-      </c>
-      <c r="H411" s="1">
-        <v>2</v>
-      </c>
-      <c r="I411" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="J411" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="K411">
-        <v>0</v>
-      </c>
-      <c r="L411">
-        <v>1</v>
-      </c>
-      <c r="M411" t="s">
-        <v>284</v>
-      </c>
-      <c r="Q411" s="12">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="412" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A412" t="s">
-        <v>132</v>
-      </c>
-      <c r="B412" t="s">
-        <v>648</v>
-      </c>
-      <c r="C412">
-        <v>2017</v>
-      </c>
-      <c r="D412">
-        <v>7490</v>
-      </c>
-      <c r="E412">
-        <v>870</v>
-      </c>
-      <c r="F412">
-        <v>83.7</v>
-      </c>
-      <c r="G412" s="8">
-        <v>95</v>
-      </c>
-      <c r="H412" s="1">
-        <v>2.8</v>
-      </c>
-      <c r="I412" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="J412" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="K412">
-        <v>0</v>
-      </c>
-      <c r="L412">
-        <v>1</v>
-      </c>
-      <c r="M412" t="s">
-        <v>284</v>
-      </c>
-      <c r="Q412" s="12">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="413" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A413" t="s">
-        <v>132</v>
-      </c>
-      <c r="B413" t="s">
-        <v>649</v>
-      </c>
-      <c r="C413">
-        <v>2017</v>
-      </c>
-      <c r="D413">
-        <v>6690</v>
-      </c>
-      <c r="E413">
-        <v>860</v>
-      </c>
-      <c r="F413">
-        <v>83.7</v>
-      </c>
-      <c r="G413" s="8">
-        <v>95</v>
-      </c>
-      <c r="H413" s="1">
-        <v>2.8</v>
-      </c>
-      <c r="I413" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="J413" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="K413">
-        <v>0</v>
-      </c>
-      <c r="L413">
-        <v>1</v>
-      </c>
-      <c r="M413" t="s">
-        <v>284</v>
-      </c>
-      <c r="Q413" s="12">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="414" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A414" t="s">
-        <v>132</v>
-      </c>
-      <c r="B414" t="s">
-        <v>650</v>
-      </c>
-      <c r="C414">
-        <v>2017</v>
-      </c>
-      <c r="D414">
-        <v>5790</v>
-      </c>
-      <c r="E414">
-        <v>820</v>
-      </c>
-      <c r="F414">
-        <v>83.7</v>
-      </c>
-      <c r="G414" s="8">
-        <v>95</v>
-      </c>
-      <c r="H414" s="1">
-        <v>2.8</v>
-      </c>
-      <c r="I414" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="J414" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="K414">
-        <v>0</v>
-      </c>
-      <c r="L414">
-        <v>1</v>
-      </c>
-      <c r="M414" t="s">
-        <v>284</v>
-      </c>
-      <c r="Q414" s="12">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="415" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A415" t="s">
-        <v>132</v>
-      </c>
-      <c r="B415" t="s">
-        <v>651</v>
-      </c>
-      <c r="C415">
-        <v>2017</v>
-      </c>
-      <c r="D415">
-        <v>5790</v>
-      </c>
-      <c r="E415">
-        <v>820</v>
-      </c>
-      <c r="F415">
-        <v>83.7</v>
-      </c>
-      <c r="G415" s="8">
-        <v>95</v>
-      </c>
-      <c r="H415" s="1">
-        <v>2</v>
-      </c>
-      <c r="I415" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="J415" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="K415">
-        <v>0</v>
-      </c>
-      <c r="L415">
-        <v>1</v>
-      </c>
-      <c r="M415" t="s">
-        <v>284</v>
-      </c>
-      <c r="Q415" s="12">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="416" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A416" t="s">
-        <v>132</v>
-      </c>
-      <c r="B416" t="s">
-        <v>652</v>
-      </c>
-      <c r="C416">
-        <v>2017</v>
-      </c>
-      <c r="D416">
-        <v>5790</v>
-      </c>
-      <c r="E416">
-        <v>840</v>
-      </c>
-      <c r="F416">
-        <v>83.7</v>
-      </c>
-      <c r="G416" s="8">
-        <v>95</v>
-      </c>
-      <c r="H416" s="1">
-        <v>2</v>
-      </c>
-      <c r="I416" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="J416" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="K416">
-        <v>0</v>
-      </c>
-      <c r="L416">
-        <v>1</v>
-      </c>
-      <c r="M416" t="s">
-        <v>284</v>
-      </c>
-      <c r="Q416" s="12">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="417" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A417" t="s">
-        <v>132</v>
-      </c>
-      <c r="B417" t="s">
-        <v>653</v>
-      </c>
-      <c r="C417">
-        <v>2017</v>
-      </c>
-      <c r="D417">
-        <v>5790</v>
-      </c>
-      <c r="E417">
-        <v>800</v>
-      </c>
-      <c r="F417">
-        <v>83.7</v>
-      </c>
-      <c r="G417" s="8">
-        <v>95</v>
-      </c>
-      <c r="H417" s="1">
-        <v>2</v>
-      </c>
-      <c r="I417" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="J417" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="K417">
-        <v>0</v>
-      </c>
-      <c r="L417">
-        <v>1</v>
-      </c>
-      <c r="M417" t="s">
-        <v>284</v>
-      </c>
-      <c r="Q417" s="12">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="418" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A418" t="s">
-        <v>132</v>
-      </c>
-      <c r="B418" t="s">
-        <v>654</v>
-      </c>
-      <c r="C418">
-        <v>2017</v>
-      </c>
-      <c r="D418">
-        <v>5790</v>
-      </c>
-      <c r="E418">
-        <v>770</v>
-      </c>
-      <c r="F418">
-        <v>83.7</v>
-      </c>
-      <c r="G418" s="8">
-        <v>95</v>
-      </c>
-      <c r="H418" s="1">
-        <v>2</v>
-      </c>
-      <c r="I418" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="J418" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="K418">
-        <v>0</v>
-      </c>
-      <c r="L418">
-        <v>1</v>
-      </c>
-      <c r="M418" t="s">
-        <v>284</v>
-      </c>
-      <c r="Q418" s="12">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="419" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A419" t="s">
-        <v>132</v>
-      </c>
-      <c r="B419" t="s">
-        <v>655</v>
-      </c>
-      <c r="C419">
-        <v>2017</v>
-      </c>
-      <c r="D419">
-        <v>5790</v>
-      </c>
-      <c r="E419">
-        <v>880</v>
-      </c>
-      <c r="F419">
-        <v>83.7</v>
-      </c>
-      <c r="G419" s="8">
-        <v>95</v>
-      </c>
-      <c r="H419" s="1">
-        <v>2</v>
-      </c>
-      <c r="I419" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="J419" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="K419">
-        <v>0</v>
-      </c>
-      <c r="L419">
-        <v>1</v>
-      </c>
-      <c r="M419" t="s">
-        <v>284</v>
-      </c>
-      <c r="Q419" s="12">
-        <v>418</v>
       </c>
     </row>
   </sheetData>
@@ -24316,21 +23713,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.68359375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>42361</v>
       </c>
@@ -24338,7 +23735,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>42369</v>
       </c>
@@ -24346,7 +23743,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>42371</v>
       </c>
@@ -24354,7 +23751,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>42372</v>
       </c>
@@ -24362,7 +23759,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>42373</v>
       </c>
@@ -24370,7 +23767,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>42382</v>
       </c>
@@ -24378,7 +23775,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>42385</v>
       </c>
@@ -24386,7 +23783,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>42387</v>
       </c>
@@ -24394,7 +23791,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>42388</v>
       </c>
@@ -24402,7 +23799,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>42390</v>
       </c>
@@ -24410,7 +23807,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>42391</v>
       </c>
@@ -24418,7 +23815,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>42400</v>
       </c>
@@ -24426,7 +23823,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>42414</v>
       </c>
@@ -24434,7 +23831,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>42432</v>
       </c>
@@ -24445,7 +23842,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>42435</v>
       </c>
@@ -24453,7 +23850,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>42436</v>
       </c>
@@ -24461,7 +23858,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>42441</v>
       </c>
@@ -24469,7 +23866,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>42445</v>
       </c>
@@ -24477,7 +23874,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>42453</v>
       </c>
@@ -24485,7 +23882,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>42456</v>
       </c>
@@ -24493,7 +23890,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>42457</v>
       </c>
@@ -24501,7 +23898,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>42458</v>
       </c>
@@ -24509,7 +23906,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>42464</v>
       </c>
@@ -24517,7 +23914,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>42510</v>
       </c>
@@ -24525,7 +23922,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>42515</v>
       </c>
@@ -24533,7 +23930,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>42560</v>
       </c>
@@ -24541,7 +23938,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>42565</v>
       </c>
@@ -24549,7 +23946,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>42576</v>
       </c>
@@ -24557,7 +23954,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>42590</v>
       </c>
@@ -24565,7 +23962,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>42593</v>
       </c>
@@ -24573,7 +23970,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>42598</v>
       </c>
@@ -24581,7 +23978,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>42665</v>
       </c>
@@ -24589,7 +23986,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>42788</v>
       </c>
@@ -24597,7 +23994,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>42831</v>
       </c>
@@ -24605,7 +24002,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="13">
         <v>42833</v>
       </c>
@@ -24613,7 +24010,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="13">
         <v>42833</v>
       </c>
@@ -24621,7 +24018,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="13">
         <v>42874</v>
       </c>
@@ -24629,7 +24026,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="13">
         <v>42876</v>
       </c>
@@ -24637,7 +24034,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="13">
         <v>42878</v>
       </c>
@@ -24645,7 +24042,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="13">
         <v>42878</v>
       </c>
@@ -24653,7 +24050,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="13">
         <v>42879</v>
       </c>
@@ -24661,7 +24058,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="13">
         <v>42884</v>
       </c>
@@ -24669,7 +24066,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="13">
         <v>42887</v>
       </c>
@@ -24677,7 +24074,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="13">
         <v>42887</v>
       </c>
@@ -24685,7 +24082,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="13">
         <v>42891</v>
       </c>
@@ -24693,7 +24090,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="13">
         <v>42901</v>
       </c>
@@ -24701,7 +24098,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="13">
         <v>42908</v>
       </c>
@@ -24709,7 +24106,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="13">
         <v>42909</v>
       </c>
@@ -24717,7 +24114,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="13">
         <v>42910</v>
       </c>
@@ -24725,12 +24122,12 @@
         <v>641</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="13">
-        <v>42910</v>
+        <v>42913</v>
       </c>
       <c r="B52" t="s">
-        <v>656</v>
+        <v>644</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
+CP.3, +GF 23mm, GF 110mm
</commit_message>
<xml_diff>
--- a/BigAssTableOfLenses.xlsx
+++ b/BigAssTableOfLenses.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8928" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8928"/>
   </bookViews>
   <sheets>
     <sheet name="LensTable" sheetId="1" r:id="rId1"/>
     <sheet name="Changelog" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3105" uniqueCount="645">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3192" uniqueCount="658">
   <si>
     <t>Manufacture</t>
   </si>
@@ -1960,6 +1960,45 @@
   </si>
   <si>
     <t>Lensbaby Velvet 85mm added</t>
+  </si>
+  <si>
+    <t>CP.3 XD 100mm T2.1 Compact Prime</t>
+  </si>
+  <si>
+    <t>CP.3 XD 15mm T2.9 Compact Prime</t>
+  </si>
+  <si>
+    <t>CP.3 XD 18mm T2.9 Compact Prime</t>
+  </si>
+  <si>
+    <t>CP.3 XD 21mm T2.9 Compact Prime</t>
+  </si>
+  <si>
+    <t>CP.3 XD 25mm T2.1 Compact Prime</t>
+  </si>
+  <si>
+    <t>CP.3 XD 28mm T2.1 Compact Prime</t>
+  </si>
+  <si>
+    <t>CP.3 XD 35mm T2.1 Compact Prime</t>
+  </si>
+  <si>
+    <t>CP.3 XD 50mm T2.1 Compact Prime</t>
+  </si>
+  <si>
+    <t>CP.3 XD 85mm T2.1 Compact Prime</t>
+  </si>
+  <si>
+    <t>GF 23mm f/4 R LM WR</t>
+  </si>
+  <si>
+    <t>GF 110mm f/2 R LM WR</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>Restore CP.3 lenses, + GF 23mm and GF 110mm</t>
   </si>
 </sst>
 </file>
@@ -1995,7 +2034,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -2003,12 +2042,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2023,6 +2077,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -2052,8 +2107,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q406" totalsRowShown="0">
-  <autoFilter ref="A1:Q406"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q417" totalsRowShown="0">
+  <autoFilter ref="A1:Q417"/>
   <sortState ref="A2:Q403">
     <sortCondition ref="Q1:Q403"/>
   </sortState>
@@ -2378,10 +2433,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q406"/>
+  <dimension ref="A1:Q417"/>
   <sheetViews>
-    <sheetView topLeftCell="A346" workbookViewId="0">
-      <selection activeCell="H407" sqref="H407"/>
+    <sheetView tabSelected="1" topLeftCell="A399" workbookViewId="0">
+      <selection activeCell="E417" sqref="E417"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7228,6 +7283,7 @@
       <c r="O89" s="12" t="s">
         <v>629</v>
       </c>
+      <c r="P89" s="10"/>
       <c r="Q89" s="6">
         <v>88</v>
       </c>
@@ -7275,6 +7331,8 @@
       <c r="N90" s="6" t="s">
         <v>578</v>
       </c>
+      <c r="O90" s="10"/>
+      <c r="P90" s="10"/>
       <c r="Q90" s="6">
         <v>89</v>
       </c>
@@ -7322,6 +7380,8 @@
       <c r="N91" s="6" t="s">
         <v>578</v>
       </c>
+      <c r="O91" s="10"/>
+      <c r="P91" s="10"/>
       <c r="Q91" s="6">
         <v>90</v>
       </c>
@@ -9092,6 +9152,7 @@
       <c r="O124" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P124" s="10"/>
       <c r="Q124" s="6">
         <v>123</v>
       </c>
@@ -9144,6 +9205,7 @@
       <c r="O125" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P125" s="10"/>
       <c r="Q125" s="6">
         <v>124</v>
       </c>
@@ -9196,6 +9258,7 @@
       <c r="O126" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P126" s="10"/>
       <c r="Q126" s="6">
         <v>125</v>
       </c>
@@ -9248,6 +9311,7 @@
       <c r="O127" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P127" s="10"/>
       <c r="Q127" s="6">
         <v>126</v>
       </c>
@@ -9300,6 +9364,7 @@
       <c r="O128" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P128" s="10"/>
       <c r="Q128" s="6">
         <v>127</v>
       </c>
@@ -9352,6 +9417,7 @@
       <c r="O129" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P129" s="10"/>
       <c r="Q129" s="6">
         <v>128</v>
       </c>
@@ -9404,6 +9470,7 @@
       <c r="O130" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P130" s="10"/>
       <c r="Q130" s="6">
         <v>129</v>
       </c>
@@ -9456,6 +9523,7 @@
       <c r="O131" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P131" s="10"/>
       <c r="Q131" s="6">
         <v>130</v>
       </c>
@@ -9508,6 +9576,7 @@
       <c r="O132" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P132" s="10"/>
       <c r="Q132" s="6">
         <v>131</v>
       </c>
@@ -9560,6 +9629,7 @@
       <c r="O133" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P133" s="10"/>
       <c r="Q133" s="6">
         <v>132</v>
       </c>
@@ -9612,6 +9682,7 @@
       <c r="O134" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P134" s="10"/>
       <c r="Q134" s="6">
         <v>133</v>
       </c>
@@ -9664,6 +9735,7 @@
       <c r="O135" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P135" s="10"/>
       <c r="Q135" s="6">
         <v>134</v>
       </c>
@@ -9716,6 +9788,7 @@
       <c r="O136" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P136" s="10"/>
       <c r="Q136" s="6">
         <v>135</v>
       </c>
@@ -9768,6 +9841,7 @@
       <c r="O137" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P137" s="10"/>
       <c r="Q137" s="6">
         <v>136</v>
       </c>
@@ -9820,6 +9894,7 @@
       <c r="O138" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P138" s="10"/>
       <c r="Q138" s="6">
         <v>137</v>
       </c>
@@ -9873,6 +9948,7 @@
       <c r="O139" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P139" s="10"/>
       <c r="Q139" s="6">
         <v>138</v>
       </c>
@@ -9925,6 +10001,7 @@
       <c r="O140" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P140" s="10"/>
       <c r="Q140" s="6">
         <v>139</v>
       </c>
@@ -9977,6 +10054,7 @@
       <c r="O141" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P141" s="10"/>
       <c r="Q141" s="6">
         <v>140</v>
       </c>
@@ -10029,7 +10107,7 @@
       <c r="O142" s="12" t="s">
         <v>626</v>
       </c>
-      <c r="P142" s="12"/>
+      <c r="P142" s="10"/>
       <c r="Q142" s="6">
         <v>141</v>
       </c>
@@ -10082,7 +10160,7 @@
       <c r="O143" s="12" t="s">
         <v>626</v>
       </c>
-      <c r="P143" s="12"/>
+      <c r="P143" s="10"/>
       <c r="Q143" s="6">
         <v>142</v>
       </c>
@@ -10135,7 +10213,7 @@
       <c r="O144" s="12" t="s">
         <v>626</v>
       </c>
-      <c r="P144" s="12"/>
+      <c r="P144" s="10"/>
       <c r="Q144" s="6">
         <v>143</v>
       </c>
@@ -10188,7 +10266,7 @@
       <c r="O145" s="12" t="s">
         <v>626</v>
       </c>
-      <c r="P145" s="12"/>
+      <c r="P145" s="10"/>
       <c r="Q145" s="6">
         <v>144</v>
       </c>
@@ -10241,7 +10319,7 @@
       <c r="O146" s="12" t="s">
         <v>626</v>
       </c>
-      <c r="P146" s="12"/>
+      <c r="P146" s="10"/>
       <c r="Q146" s="6">
         <v>145</v>
       </c>
@@ -10294,6 +10372,7 @@
       <c r="O147" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P147" s="10"/>
       <c r="Q147" s="6">
         <v>146</v>
       </c>
@@ -10346,6 +10425,7 @@
       <c r="O148" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P148" s="10"/>
       <c r="Q148" s="6">
         <v>147</v>
       </c>
@@ -10398,6 +10478,7 @@
       <c r="O149" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P149" s="10"/>
       <c r="Q149" s="6">
         <v>148</v>
       </c>
@@ -10450,6 +10531,7 @@
       <c r="O150" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P150" s="10"/>
       <c r="Q150" s="6">
         <v>149</v>
       </c>
@@ -10502,6 +10584,7 @@
       <c r="O151" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P151" s="10"/>
       <c r="Q151" s="6">
         <v>150</v>
       </c>
@@ -10554,6 +10637,7 @@
       <c r="O152" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P152" s="10"/>
       <c r="Q152" s="6">
         <v>151</v>
       </c>
@@ -10606,6 +10690,7 @@
       <c r="O153" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P153" s="10"/>
       <c r="Q153" s="6">
         <v>152</v>
       </c>
@@ -10658,6 +10743,7 @@
       <c r="O154" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P154" s="10"/>
       <c r="Q154" s="6">
         <v>153</v>
       </c>
@@ -10710,6 +10796,7 @@
       <c r="O155" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P155" s="10"/>
       <c r="Q155" s="6">
         <v>154</v>
       </c>
@@ -10760,6 +10847,7 @@
       <c r="O156" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P156" s="10"/>
       <c r="Q156" s="6">
         <v>155</v>
       </c>
@@ -10810,6 +10898,7 @@
       <c r="O157" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P157" s="10"/>
       <c r="Q157" s="6">
         <v>156</v>
       </c>
@@ -10860,6 +10949,7 @@
       <c r="O158" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P158" s="10"/>
       <c r="Q158" s="6">
         <v>157</v>
       </c>
@@ -10910,6 +11000,7 @@
       <c r="O159" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P159" s="10"/>
       <c r="Q159" s="6">
         <v>158</v>
       </c>
@@ -10960,6 +11051,7 @@
       <c r="O160" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P160" s="10"/>
       <c r="Q160" s="6">
         <v>159</v>
       </c>
@@ -11010,6 +11102,7 @@
       <c r="O161" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P161" s="10"/>
       <c r="Q161" s="6">
         <v>160</v>
       </c>
@@ -11060,6 +11153,7 @@
       <c r="O162" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P162" s="10"/>
       <c r="Q162" s="6">
         <v>161</v>
       </c>
@@ -11110,6 +11204,7 @@
       <c r="O163" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P163" s="10"/>
       <c r="Q163" s="6">
         <v>162</v>
       </c>
@@ -11160,6 +11255,7 @@
       <c r="O164" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P164" s="10"/>
       <c r="Q164" s="6">
         <v>163</v>
       </c>
@@ -11210,6 +11306,7 @@
       <c r="O165" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P165" s="10"/>
       <c r="Q165" s="6">
         <v>164</v>
       </c>
@@ -11260,6 +11357,7 @@
       <c r="O166" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P166" s="10"/>
       <c r="Q166" s="6">
         <v>165</v>
       </c>
@@ -12124,6 +12222,7 @@
       <c r="O182" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P182" s="10"/>
       <c r="Q182" s="6">
         <v>181</v>
       </c>
@@ -12176,6 +12275,7 @@
       <c r="O183" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P183" s="10"/>
       <c r="Q183" s="6">
         <v>182</v>
       </c>
@@ -12228,6 +12328,7 @@
       <c r="O184" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P184" s="10"/>
       <c r="Q184" s="6">
         <v>183</v>
       </c>
@@ -12280,6 +12381,7 @@
       <c r="O185" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P185" s="10"/>
       <c r="Q185" s="6">
         <v>184</v>
       </c>
@@ -12332,6 +12434,7 @@
       <c r="O186" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P186" s="10"/>
       <c r="Q186" s="6">
         <v>185</v>
       </c>
@@ -12384,6 +12487,7 @@
       <c r="O187" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P187" s="10"/>
       <c r="Q187" s="6">
         <v>186</v>
       </c>
@@ -12436,6 +12540,7 @@
       <c r="O188" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P188" s="10"/>
       <c r="Q188" s="6">
         <v>187</v>
       </c>
@@ -12488,6 +12593,7 @@
       <c r="O189" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P189" s="10"/>
       <c r="Q189" s="6">
         <v>188</v>
       </c>
@@ -12540,6 +12646,7 @@
       <c r="O190" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P190" s="10"/>
       <c r="Q190" s="6">
         <v>189</v>
       </c>
@@ -12592,6 +12699,7 @@
       <c r="O191" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P191" s="10"/>
       <c r="Q191" s="6">
         <v>190</v>
       </c>
@@ -12644,6 +12752,7 @@
       <c r="O192" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P192" s="10"/>
       <c r="Q192" s="6">
         <v>191</v>
       </c>
@@ -12694,6 +12803,7 @@
       <c r="O193" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P193" s="10"/>
       <c r="Q193" s="6">
         <v>192</v>
       </c>
@@ -12744,6 +12854,7 @@
       <c r="O194" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P194" s="10"/>
       <c r="Q194" s="6">
         <v>193</v>
       </c>
@@ -12791,6 +12902,7 @@
       <c r="O195" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P195" s="10"/>
       <c r="Q195" s="6">
         <v>194</v>
       </c>
@@ -12841,6 +12953,7 @@
       <c r="O196" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P196" s="10"/>
       <c r="Q196" s="6">
         <v>195</v>
       </c>
@@ -12891,6 +13004,7 @@
       <c r="O197" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P197" s="10"/>
       <c r="Q197" s="6">
         <v>196</v>
       </c>
@@ -12941,6 +13055,7 @@
       <c r="O198" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P198" s="10"/>
       <c r="Q198" s="6">
         <v>197</v>
       </c>
@@ -12993,6 +13108,7 @@
       <c r="O199" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P199" s="10"/>
       <c r="Q199" s="6">
         <v>198</v>
       </c>
@@ -13045,6 +13161,7 @@
       <c r="O200" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P200" s="10"/>
       <c r="Q200" s="6">
         <v>199</v>
       </c>
@@ -13097,6 +13214,7 @@
       <c r="O201" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P201" s="10"/>
       <c r="Q201" s="6">
         <v>200</v>
       </c>
@@ -13149,6 +13267,7 @@
       <c r="O202" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P202" s="10"/>
       <c r="Q202" s="6">
         <v>201</v>
       </c>
@@ -13201,6 +13320,7 @@
       <c r="O203" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P203" s="10"/>
       <c r="Q203" s="6">
         <v>202</v>
       </c>
@@ -13253,6 +13373,7 @@
       <c r="O204" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P204" s="10"/>
       <c r="Q204" s="6">
         <v>203</v>
       </c>
@@ -13306,6 +13427,7 @@
       <c r="O205" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P205" s="10"/>
       <c r="Q205" s="6">
         <v>204</v>
       </c>
@@ -13358,6 +13480,7 @@
       <c r="O206" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P206" s="10"/>
       <c r="Q206" s="6">
         <v>205</v>
       </c>
@@ -13410,6 +13533,7 @@
       <c r="O207" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P207" s="10"/>
       <c r="Q207" s="6">
         <v>206</v>
       </c>
@@ -13462,6 +13586,7 @@
       <c r="O208" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P208" s="10"/>
       <c r="Q208" s="6">
         <v>207</v>
       </c>
@@ -13514,6 +13639,7 @@
       <c r="O209" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P209" s="10"/>
       <c r="Q209" s="6">
         <v>208</v>
       </c>
@@ -13566,6 +13692,7 @@
       <c r="O210" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P210" s="10"/>
       <c r="Q210" s="6">
         <v>209</v>
       </c>
@@ -13618,6 +13745,7 @@
       <c r="O211" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P211" s="10"/>
       <c r="Q211" s="6">
         <v>210</v>
       </c>
@@ -13670,6 +13798,7 @@
       <c r="O212" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P212" s="10"/>
       <c r="Q212" s="6">
         <v>211</v>
       </c>
@@ -13722,6 +13851,7 @@
       <c r="O213" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P213" s="10"/>
       <c r="Q213" s="6">
         <v>212</v>
       </c>
@@ -13772,6 +13902,7 @@
       <c r="O214" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P214" s="10"/>
       <c r="Q214" s="6">
         <v>213</v>
       </c>
@@ -13824,6 +13955,7 @@
       <c r="O215" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P215" s="10"/>
       <c r="Q215" s="6">
         <v>214</v>
       </c>
@@ -13876,6 +14008,7 @@
       <c r="O216" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P216" s="10"/>
       <c r="Q216" s="6">
         <v>215</v>
       </c>
@@ -13928,6 +14061,7 @@
       <c r="O217" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P217" s="10"/>
       <c r="Q217" s="6">
         <v>216</v>
       </c>
@@ -13980,6 +14114,7 @@
       <c r="O218" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P218" s="10"/>
       <c r="Q218" s="6">
         <v>217</v>
       </c>
@@ -14032,6 +14167,7 @@
       <c r="O219" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P219" s="10"/>
       <c r="Q219" s="6">
         <v>218</v>
       </c>
@@ -14084,6 +14220,7 @@
       <c r="O220" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P220" s="10"/>
       <c r="Q220" s="6">
         <v>219</v>
       </c>
@@ -14136,6 +14273,7 @@
       <c r="O221" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P221" s="10"/>
       <c r="Q221" s="6">
         <v>220</v>
       </c>
@@ -14188,6 +14326,7 @@
       <c r="O222" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P222" s="10"/>
       <c r="Q222" s="6">
         <v>221</v>
       </c>
@@ -14240,6 +14379,7 @@
       <c r="O223" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P223" s="10"/>
       <c r="Q223" s="6">
         <v>222</v>
       </c>
@@ -14290,6 +14430,7 @@
       <c r="O224" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P224" s="10"/>
       <c r="Q224" s="6">
         <v>223</v>
       </c>
@@ -14340,6 +14481,7 @@
       <c r="O225" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P225" s="10"/>
       <c r="Q225" s="6">
         <v>224</v>
       </c>
@@ -14390,6 +14532,7 @@
       <c r="O226" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P226" s="10"/>
       <c r="Q226" s="6">
         <v>225</v>
       </c>
@@ -14442,6 +14585,7 @@
       <c r="O227" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P227" s="10"/>
       <c r="Q227" s="6">
         <v>226</v>
       </c>
@@ -14494,6 +14638,7 @@
       <c r="O228" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P228" s="10"/>
       <c r="Q228" s="6">
         <v>227</v>
       </c>
@@ -14546,6 +14691,7 @@
       <c r="O229" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P229" s="10"/>
       <c r="Q229" s="6">
         <v>228</v>
       </c>
@@ -14598,6 +14744,7 @@
       <c r="O230" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P230" s="10"/>
       <c r="Q230" s="6">
         <v>229</v>
       </c>
@@ -14650,6 +14797,7 @@
       <c r="O231" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P231" s="10"/>
       <c r="Q231" s="6">
         <v>230</v>
       </c>
@@ -14700,6 +14848,7 @@
       <c r="O232" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P232" s="10"/>
       <c r="Q232" s="6">
         <v>231</v>
       </c>
@@ -14961,6 +15110,8 @@
       <c r="N237" s="6" t="s">
         <v>578</v>
       </c>
+      <c r="O237" s="14"/>
+      <c r="P237" s="14"/>
       <c r="Q237" s="6">
         <v>236</v>
       </c>
@@ -15008,6 +15159,8 @@
       <c r="N238" s="6" t="s">
         <v>578</v>
       </c>
+      <c r="O238" s="14"/>
+      <c r="P238" s="14"/>
       <c r="Q238" s="6">
         <v>237</v>
       </c>
@@ -15055,6 +15208,8 @@
       <c r="N239" s="6" t="s">
         <v>578</v>
       </c>
+      <c r="O239" s="14"/>
+      <c r="P239" s="14"/>
       <c r="Q239" s="6">
         <v>238</v>
       </c>
@@ -15104,6 +15259,8 @@
       <c r="N240" s="6" t="s">
         <v>580</v>
       </c>
+      <c r="O240" s="14"/>
+      <c r="P240" s="14"/>
       <c r="Q240" s="6">
         <v>239</v>
       </c>
@@ -15151,6 +15308,8 @@
       <c r="N241" s="6" t="s">
         <v>580</v>
       </c>
+      <c r="O241" s="14"/>
+      <c r="P241" s="14"/>
       <c r="Q241" s="6">
         <v>240</v>
       </c>
@@ -15198,6 +15357,8 @@
       <c r="N242" s="6" t="s">
         <v>580</v>
       </c>
+      <c r="O242" s="14"/>
+      <c r="P242" s="14"/>
       <c r="Q242" s="6">
         <v>241</v>
       </c>
@@ -15245,6 +15406,8 @@
       <c r="N243" s="6" t="s">
         <v>580</v>
       </c>
+      <c r="O243" s="14"/>
+      <c r="P243" s="14"/>
       <c r="Q243" s="6">
         <v>242</v>
       </c>
@@ -15294,6 +15457,8 @@
       <c r="N244" s="6" t="s">
         <v>581</v>
       </c>
+      <c r="O244" s="14"/>
+      <c r="P244" s="14"/>
       <c r="Q244" s="6">
         <v>243</v>
       </c>
@@ -15341,6 +15506,8 @@
       <c r="N245" s="6" t="s">
         <v>580</v>
       </c>
+      <c r="O245" s="14"/>
+      <c r="P245" s="14"/>
       <c r="Q245" s="6">
         <v>244</v>
       </c>
@@ -15388,6 +15555,8 @@
       <c r="N246" s="6" t="s">
         <v>580</v>
       </c>
+      <c r="O246" s="14"/>
+      <c r="P246" s="14"/>
       <c r="Q246" s="6">
         <v>245</v>
       </c>
@@ -15435,6 +15604,8 @@
       <c r="N247" s="6" t="s">
         <v>580</v>
       </c>
+      <c r="O247" s="14"/>
+      <c r="P247" s="14"/>
       <c r="Q247" s="6">
         <v>246</v>
       </c>
@@ -15482,6 +15653,8 @@
       <c r="N248" s="6" t="s">
         <v>580</v>
       </c>
+      <c r="O248" s="14"/>
+      <c r="P248" s="14"/>
       <c r="Q248" s="6">
         <v>247</v>
       </c>
@@ -15529,6 +15702,8 @@
       <c r="N249" s="6" t="s">
         <v>581</v>
       </c>
+      <c r="O249" s="14"/>
+      <c r="P249" s="14"/>
       <c r="Q249" s="6">
         <v>248</v>
       </c>
@@ -15578,6 +15753,8 @@
       <c r="N250" s="6" t="s">
         <v>583</v>
       </c>
+      <c r="O250" s="14"/>
+      <c r="P250" s="14"/>
       <c r="Q250" s="6">
         <v>249</v>
       </c>
@@ -15625,6 +15802,8 @@
       <c r="N251" s="6" t="s">
         <v>581</v>
       </c>
+      <c r="O251" s="14"/>
+      <c r="P251" s="14"/>
       <c r="Q251" s="6">
         <v>250</v>
       </c>
@@ -15672,6 +15851,8 @@
       <c r="N252" s="6" t="s">
         <v>581</v>
       </c>
+      <c r="O252" s="14"/>
+      <c r="P252" s="14"/>
       <c r="Q252" s="6">
         <v>251</v>
       </c>
@@ -15719,6 +15900,8 @@
       <c r="N253" s="6" t="s">
         <v>583</v>
       </c>
+      <c r="O253" s="14"/>
+      <c r="P253" s="14"/>
       <c r="Q253" s="6">
         <v>252</v>
       </c>
@@ -19162,6 +19345,7 @@
       <c r="O317" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P317" s="10"/>
       <c r="Q317" s="6">
         <v>316</v>
       </c>
@@ -19212,6 +19396,7 @@
       <c r="O318" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P318" s="10"/>
       <c r="Q318" s="6">
         <v>317</v>
       </c>
@@ -19260,6 +19445,7 @@
       <c r="O319" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P319" s="10"/>
       <c r="Q319" s="6">
         <v>318</v>
       </c>
@@ -19310,6 +19496,7 @@
       <c r="O320" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P320" s="10"/>
       <c r="Q320" s="6">
         <v>319</v>
       </c>
@@ -21579,6 +21766,7 @@
       <c r="O364" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P364" s="10"/>
       <c r="Q364" s="7">
         <v>363</v>
       </c>
@@ -21629,6 +21817,7 @@
       <c r="O365" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P365" s="10"/>
       <c r="Q365" s="7">
         <v>364</v>
       </c>
@@ -21679,6 +21868,7 @@
       <c r="O366" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P366" s="10"/>
       <c r="Q366" s="7">
         <v>365</v>
       </c>
@@ -21729,6 +21919,7 @@
       <c r="O367" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P367" s="10"/>
       <c r="Q367" s="7">
         <v>366</v>
       </c>
@@ -21779,6 +21970,7 @@
       <c r="O368" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P368" s="10"/>
       <c r="Q368" s="7">
         <v>367</v>
       </c>
@@ -21829,6 +22021,7 @@
       <c r="O369" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P369" s="10"/>
       <c r="Q369" s="7">
         <v>368</v>
       </c>
@@ -21879,6 +22072,7 @@
       <c r="O370" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P370" s="10"/>
       <c r="Q370" s="7">
         <v>369</v>
       </c>
@@ -21929,6 +22123,7 @@
       <c r="O371" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P371" s="10"/>
       <c r="Q371" s="7">
         <v>370</v>
       </c>
@@ -21979,6 +22174,7 @@
       <c r="O372" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P372" s="10"/>
       <c r="Q372" s="7">
         <v>371</v>
       </c>
@@ -22029,6 +22225,7 @@
       <c r="O373" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P373" s="10"/>
       <c r="Q373" s="7">
         <v>372</v>
       </c>
@@ -22079,6 +22276,7 @@
       <c r="O374" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P374" s="10"/>
       <c r="Q374" s="7">
         <v>373</v>
       </c>
@@ -22129,6 +22327,7 @@
       <c r="O375" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P375" s="10"/>
       <c r="Q375" s="7">
         <v>374</v>
       </c>
@@ -22177,6 +22376,7 @@
       <c r="O376" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P376" s="10"/>
       <c r="Q376" s="7">
         <v>375</v>
       </c>
@@ -22227,6 +22427,7 @@
       <c r="O377" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P377" s="10"/>
       <c r="Q377" s="7">
         <v>376</v>
       </c>
@@ -22277,6 +22478,7 @@
       <c r="O378" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P378" s="10"/>
       <c r="Q378" s="7">
         <v>377</v>
       </c>
@@ -22645,6 +22847,7 @@
       <c r="O385" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P385" s="10"/>
       <c r="Q385" s="7">
         <v>384</v>
       </c>
@@ -22748,6 +22951,7 @@
       <c r="O387" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P387" s="10"/>
       <c r="Q387" s="7">
         <v>386</v>
       </c>
@@ -22798,6 +23002,7 @@
       <c r="O388" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P388" s="10"/>
       <c r="Q388" s="7">
         <v>387</v>
       </c>
@@ -22848,6 +23053,7 @@
       <c r="O389" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P389" s="10"/>
       <c r="Q389" s="7">
         <v>388</v>
       </c>
@@ -23203,6 +23409,8 @@
       <c r="N396" s="12" t="s">
         <v>581</v>
       </c>
+      <c r="O396" s="10"/>
+      <c r="P396" s="10"/>
       <c r="Q396" s="7">
         <v>395</v>
       </c>
@@ -23250,6 +23458,8 @@
       <c r="N397" s="12" t="s">
         <v>583</v>
       </c>
+      <c r="O397" s="10"/>
+      <c r="P397" s="10"/>
       <c r="Q397" s="7">
         <v>396</v>
       </c>
@@ -23402,6 +23612,7 @@
       <c r="O400" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P400" s="10"/>
       <c r="Q400">
         <v>399</v>
       </c>
@@ -23452,6 +23663,7 @@
       <c r="O401" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P401" s="10"/>
       <c r="Q401">
         <v>400</v>
       </c>
@@ -23502,6 +23714,7 @@
       <c r="O402" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P402" s="10"/>
       <c r="Q402">
         <v>401</v>
       </c>
@@ -23552,6 +23765,7 @@
       <c r="O403" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P403" s="10"/>
       <c r="Q403">
         <v>402</v>
       </c>
@@ -23594,6 +23808,7 @@
       <c r="O404" s="12" t="s">
         <v>626</v>
       </c>
+      <c r="P404" s="10"/>
       <c r="Q404">
         <v>403</v>
       </c>
@@ -23698,6 +23913,584 @@
       <c r="P406" s="10"/>
       <c r="Q406">
         <v>405</v>
+      </c>
+    </row>
+    <row r="407" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A407" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B407" s="12" t="s">
+        <v>645</v>
+      </c>
+      <c r="C407" s="12">
+        <v>2017</v>
+      </c>
+      <c r="D407" s="12">
+        <v>6690</v>
+      </c>
+      <c r="E407" s="12">
+        <v>1010</v>
+      </c>
+      <c r="F407" s="12">
+        <v>126.5</v>
+      </c>
+      <c r="G407" s="8">
+        <v>95</v>
+      </c>
+      <c r="H407" s="12">
+        <v>2</v>
+      </c>
+      <c r="I407" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="J407" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="K407" s="12">
+        <v>0</v>
+      </c>
+      <c r="L407" s="12">
+        <v>1</v>
+      </c>
+      <c r="M407" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="N407" s="12" t="s">
+        <v>587</v>
+      </c>
+      <c r="O407" s="12" t="s">
+        <v>629</v>
+      </c>
+      <c r="P407" s="12" t="s">
+        <v>629</v>
+      </c>
+      <c r="Q407" s="12">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="408" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A408" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B408" s="12" t="s">
+        <v>646</v>
+      </c>
+      <c r="C408" s="12">
+        <v>2017</v>
+      </c>
+      <c r="D408" s="12">
+        <v>7490</v>
+      </c>
+      <c r="E408" s="12">
+        <v>870</v>
+      </c>
+      <c r="F408" s="12">
+        <v>83.7</v>
+      </c>
+      <c r="G408" s="8">
+        <v>95</v>
+      </c>
+      <c r="H408" s="12">
+        <v>2.8</v>
+      </c>
+      <c r="I408" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="J408" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="K408" s="12">
+        <v>0</v>
+      </c>
+      <c r="L408" s="12">
+        <v>1</v>
+      </c>
+      <c r="M408" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="N408" s="12" t="s">
+        <v>578</v>
+      </c>
+      <c r="O408" s="12" t="s">
+        <v>629</v>
+      </c>
+      <c r="P408" s="12" t="s">
+        <v>629</v>
+      </c>
+      <c r="Q408" s="12">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="409" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A409" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B409" s="12" t="s">
+        <v>647</v>
+      </c>
+      <c r="C409" s="12">
+        <v>2017</v>
+      </c>
+      <c r="D409" s="12">
+        <v>6690</v>
+      </c>
+      <c r="E409" s="12">
+        <v>860</v>
+      </c>
+      <c r="F409" s="12">
+        <v>83.7</v>
+      </c>
+      <c r="G409" s="8">
+        <v>95</v>
+      </c>
+      <c r="H409" s="12">
+        <v>2.8</v>
+      </c>
+      <c r="I409" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="J409" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="K409" s="12">
+        <v>0</v>
+      </c>
+      <c r="L409" s="12">
+        <v>1</v>
+      </c>
+      <c r="M409" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="N409" s="12" t="s">
+        <v>578</v>
+      </c>
+      <c r="O409" s="12" t="s">
+        <v>629</v>
+      </c>
+      <c r="P409" s="12" t="s">
+        <v>629</v>
+      </c>
+      <c r="Q409" s="12">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="410" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A410" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B410" s="12" t="s">
+        <v>648</v>
+      </c>
+      <c r="C410" s="12">
+        <v>2017</v>
+      </c>
+      <c r="D410" s="12">
+        <v>5790</v>
+      </c>
+      <c r="E410" s="12">
+        <v>820</v>
+      </c>
+      <c r="F410" s="12">
+        <v>83.7</v>
+      </c>
+      <c r="G410" s="8">
+        <v>95</v>
+      </c>
+      <c r="H410" s="12">
+        <v>2.8</v>
+      </c>
+      <c r="I410" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="J410" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="K410" s="12">
+        <v>0</v>
+      </c>
+      <c r="L410" s="12">
+        <v>1</v>
+      </c>
+      <c r="M410" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="N410" s="12" t="s">
+        <v>578</v>
+      </c>
+      <c r="O410" s="12" t="s">
+        <v>629</v>
+      </c>
+      <c r="P410" s="12" t="s">
+        <v>629</v>
+      </c>
+      <c r="Q410" s="12">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="411" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A411" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B411" s="12" t="s">
+        <v>649</v>
+      </c>
+      <c r="C411" s="12">
+        <v>2017</v>
+      </c>
+      <c r="D411" s="12">
+        <v>5790</v>
+      </c>
+      <c r="E411" s="12">
+        <v>820</v>
+      </c>
+      <c r="F411" s="12">
+        <v>83.7</v>
+      </c>
+      <c r="G411" s="8">
+        <v>95</v>
+      </c>
+      <c r="H411" s="12">
+        <v>2</v>
+      </c>
+      <c r="I411" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="J411" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="K411" s="12">
+        <v>0</v>
+      </c>
+      <c r="L411" s="12">
+        <v>1</v>
+      </c>
+      <c r="M411" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="N411" s="12" t="s">
+        <v>580</v>
+      </c>
+      <c r="O411" s="12" t="s">
+        <v>629</v>
+      </c>
+      <c r="P411" s="12" t="s">
+        <v>629</v>
+      </c>
+      <c r="Q411" s="12">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="412" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A412" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B412" s="12" t="s">
+        <v>650</v>
+      </c>
+      <c r="C412" s="12">
+        <v>2017</v>
+      </c>
+      <c r="D412" s="12">
+        <v>5790</v>
+      </c>
+      <c r="E412" s="12">
+        <v>840</v>
+      </c>
+      <c r="F412" s="12">
+        <v>83.7</v>
+      </c>
+      <c r="G412" s="8">
+        <v>95</v>
+      </c>
+      <c r="H412" s="12">
+        <v>2</v>
+      </c>
+      <c r="I412" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="J412" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="K412" s="12">
+        <v>0</v>
+      </c>
+      <c r="L412" s="12">
+        <v>1</v>
+      </c>
+      <c r="M412" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="N412" s="12" t="s">
+        <v>580</v>
+      </c>
+      <c r="O412" s="12" t="s">
+        <v>629</v>
+      </c>
+      <c r="P412" s="12" t="s">
+        <v>629</v>
+      </c>
+      <c r="Q412" s="12">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="413" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A413" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B413" s="12" t="s">
+        <v>651</v>
+      </c>
+      <c r="C413" s="12">
+        <v>2017</v>
+      </c>
+      <c r="D413" s="12">
+        <v>5790</v>
+      </c>
+      <c r="E413" s="12">
+        <v>800</v>
+      </c>
+      <c r="F413" s="12">
+        <v>83.7</v>
+      </c>
+      <c r="G413" s="8">
+        <v>95</v>
+      </c>
+      <c r="H413" s="12">
+        <v>2</v>
+      </c>
+      <c r="I413" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="J413" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="K413" s="12">
+        <v>0</v>
+      </c>
+      <c r="L413" s="12">
+        <v>1</v>
+      </c>
+      <c r="M413" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="N413" s="12" t="s">
+        <v>580</v>
+      </c>
+      <c r="O413" s="12" t="s">
+        <v>629</v>
+      </c>
+      <c r="P413" s="12" t="s">
+        <v>629</v>
+      </c>
+      <c r="Q413" s="12">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="414" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A414" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B414" s="12" t="s">
+        <v>652</v>
+      </c>
+      <c r="C414" s="12">
+        <v>2017</v>
+      </c>
+      <c r="D414" s="12">
+        <v>5790</v>
+      </c>
+      <c r="E414" s="12">
+        <v>770</v>
+      </c>
+      <c r="F414" s="12">
+        <v>83.7</v>
+      </c>
+      <c r="G414" s="8">
+        <v>95</v>
+      </c>
+      <c r="H414" s="12">
+        <v>2</v>
+      </c>
+      <c r="I414" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="J414" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="K414" s="12">
+        <v>0</v>
+      </c>
+      <c r="L414" s="12">
+        <v>1</v>
+      </c>
+      <c r="M414" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="N414" s="12" t="s">
+        <v>581</v>
+      </c>
+      <c r="O414" s="12" t="s">
+        <v>629</v>
+      </c>
+      <c r="P414" s="12" t="s">
+        <v>629</v>
+      </c>
+      <c r="Q414" s="12">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="415" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A415" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B415" s="12" t="s">
+        <v>653</v>
+      </c>
+      <c r="C415" s="12">
+        <v>2017</v>
+      </c>
+      <c r="D415" s="12">
+        <v>5790</v>
+      </c>
+      <c r="E415" s="12">
+        <v>880</v>
+      </c>
+      <c r="F415" s="12">
+        <v>83.7</v>
+      </c>
+      <c r="G415" s="8">
+        <v>95</v>
+      </c>
+      <c r="H415" s="12">
+        <v>2</v>
+      </c>
+      <c r="I415" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="J415" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="K415" s="12">
+        <v>0</v>
+      </c>
+      <c r="L415" s="12">
+        <v>1</v>
+      </c>
+      <c r="M415" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="N415" s="12" t="s">
+        <v>583</v>
+      </c>
+      <c r="O415" s="12" t="s">
+        <v>629</v>
+      </c>
+      <c r="P415" s="12" t="s">
+        <v>629</v>
+      </c>
+      <c r="Q415" s="12">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="416" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A416" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="B416" s="12" t="s">
+        <v>654</v>
+      </c>
+      <c r="C416" s="12">
+        <v>2017</v>
+      </c>
+      <c r="D416" s="12">
+        <v>2599</v>
+      </c>
+      <c r="E416" s="12">
+        <v>845</v>
+      </c>
+      <c r="F416" s="12">
+        <v>103</v>
+      </c>
+      <c r="G416" s="8">
+        <v>89.8</v>
+      </c>
+      <c r="H416" s="12">
+        <v>4</v>
+      </c>
+      <c r="I416" s="9" t="s">
+        <v>383</v>
+      </c>
+      <c r="J416" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="K416" s="12">
+        <v>0</v>
+      </c>
+      <c r="L416" s="12">
+        <v>0</v>
+      </c>
+      <c r="M416" s="12" t="s">
+        <v>597</v>
+      </c>
+      <c r="N416" s="12" t="s">
+        <v>578</v>
+      </c>
+      <c r="O416" s="12" t="s">
+        <v>626</v>
+      </c>
+      <c r="P416" s="10"/>
+      <c r="Q416" s="12">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="417" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A417" t="s">
+        <v>377</v>
+      </c>
+      <c r="B417" t="s">
+        <v>655</v>
+      </c>
+      <c r="C417">
+        <v>2017</v>
+      </c>
+      <c r="D417">
+        <v>2799</v>
+      </c>
+      <c r="E417">
+        <v>1010</v>
+      </c>
+      <c r="F417">
+        <v>125.5</v>
+      </c>
+      <c r="G417" s="8">
+        <v>94.3</v>
+      </c>
+      <c r="H417" s="1">
+        <v>2</v>
+      </c>
+      <c r="I417" s="9" t="s">
+        <v>656</v>
+      </c>
+      <c r="J417" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="K417">
+        <v>0</v>
+      </c>
+      <c r="L417">
+        <v>0</v>
+      </c>
+      <c r="M417" t="s">
+        <v>597</v>
+      </c>
+      <c r="N417" t="s">
+        <v>583</v>
+      </c>
+      <c r="O417" s="12" t="s">
+        <v>626</v>
+      </c>
+      <c r="Q417">
+        <v>416</v>
       </c>
     </row>
   </sheetData>
@@ -23711,10 +24504,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24130,6 +24923,14 @@
         <v>644</v>
       </c>
     </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" s="13">
+        <v>42914</v>
+      </c>
+      <c r="B53" t="s">
+        <v>657</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
+ Veydra + Tamron 24-70 G2 meta
</commit_message>
<xml_diff>
--- a/BigAssTableOfLenses.xlsx
+++ b/BigAssTableOfLenses.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8928"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8928" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LensTable" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3200" uniqueCount="659">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3244" uniqueCount="668">
   <si>
     <t>Manufacture</t>
   </si>
@@ -2002,6 +2002,33 @@
   </si>
   <si>
     <t>Milvus 35mm f/1.4 ZE</t>
+  </si>
+  <si>
+    <t>Veydra</t>
+  </si>
+  <si>
+    <t>12mm T2.2 Mini Prime</t>
+  </si>
+  <si>
+    <t>16mm T2.2 Mini Prime</t>
+  </si>
+  <si>
+    <t>25mm T2.2 Mini Prime</t>
+  </si>
+  <si>
+    <t>35mm T2.2 Mini Prime</t>
+  </si>
+  <si>
+    <t>50mm T2.2 Mini Prime</t>
+  </si>
+  <si>
+    <t>19mm T2.6 Mini Prime</t>
+  </si>
+  <si>
+    <t>85mm T2.2 Mini Prime</t>
+  </si>
+  <si>
+    <t>Veydra lenses, Tamron 24-70 G2 metadata</t>
   </si>
 </sst>
 </file>
@@ -2110,8 +2137,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q418" totalsRowShown="0">
-  <autoFilter ref="A1:Q418"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q425" totalsRowShown="0">
+  <autoFilter ref="A1:Q425"/>
   <sortState ref="A2:Q403">
     <sortCondition ref="Q1:Q403"/>
   </sortState>
@@ -2436,10 +2463,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q418"/>
+  <dimension ref="A1:Q425"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A417" workbookViewId="0">
-      <selection activeCell="Q417" sqref="Q417"/>
+    <sheetView topLeftCell="A339" workbookViewId="0">
+      <selection activeCell="O405" sqref="O405"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23783,10 +23810,18 @@
       <c r="C404">
         <v>2017</v>
       </c>
-      <c r="D404" s="10"/>
-      <c r="E404" s="10"/>
-      <c r="F404" s="10"/>
-      <c r="G404" s="11"/>
+      <c r="D404" s="12">
+        <v>1199</v>
+      </c>
+      <c r="E404" s="12">
+        <v>904</v>
+      </c>
+      <c r="F404" s="12">
+        <v>111.8</v>
+      </c>
+      <c r="G404" s="12">
+        <v>88.4</v>
+      </c>
       <c r="H404" s="1">
         <v>2.8</v>
       </c>
@@ -24548,6 +24583,329 @@
       </c>
       <c r="Q418">
         <v>417</v>
+      </c>
+    </row>
+    <row r="419" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A419" t="s">
+        <v>659</v>
+      </c>
+      <c r="B419" t="s">
+        <v>660</v>
+      </c>
+      <c r="C419" s="10">
+        <v>2014</v>
+      </c>
+      <c r="D419">
+        <v>999</v>
+      </c>
+      <c r="E419">
+        <v>544</v>
+      </c>
+      <c r="F419" s="10"/>
+      <c r="G419" s="8">
+        <v>80</v>
+      </c>
+      <c r="H419" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I419" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="J419" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="K419">
+        <v>0</v>
+      </c>
+      <c r="L419">
+        <v>1</v>
+      </c>
+      <c r="M419" t="s">
+        <v>292</v>
+      </c>
+      <c r="N419" t="s">
+        <v>580</v>
+      </c>
+      <c r="O419" s="12" t="s">
+        <v>628</v>
+      </c>
+      <c r="P419" s="10"/>
+      <c r="Q419">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="420" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A420" t="s">
+        <v>659</v>
+      </c>
+      <c r="B420" t="s">
+        <v>661</v>
+      </c>
+      <c r="C420" s="10">
+        <v>2014</v>
+      </c>
+      <c r="D420">
+        <v>999</v>
+      </c>
+      <c r="E420">
+        <v>546</v>
+      </c>
+      <c r="F420" s="10"/>
+      <c r="G420" s="8">
+        <v>80</v>
+      </c>
+      <c r="H420" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I420" s="9" t="s">
+        <v>380</v>
+      </c>
+      <c r="J420" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="K420">
+        <v>0</v>
+      </c>
+      <c r="L420">
+        <v>1</v>
+      </c>
+      <c r="M420" t="s">
+        <v>292</v>
+      </c>
+      <c r="O420" s="12" t="s">
+        <v>628</v>
+      </c>
+      <c r="P420" s="10"/>
+      <c r="Q420" s="12">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="421" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A421" s="12" t="s">
+        <v>659</v>
+      </c>
+      <c r="B421" s="12" t="s">
+        <v>665</v>
+      </c>
+      <c r="C421" s="12">
+        <v>2017</v>
+      </c>
+      <c r="D421" s="12">
+        <v>999</v>
+      </c>
+      <c r="E421" s="10"/>
+      <c r="F421" s="10"/>
+      <c r="G421" s="8">
+        <v>80</v>
+      </c>
+      <c r="H421" s="12">
+        <v>2.6</v>
+      </c>
+      <c r="I421" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="J421" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="K421" s="12">
+        <v>0</v>
+      </c>
+      <c r="L421" s="12">
+        <v>1</v>
+      </c>
+      <c r="M421" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="O421" s="12" t="s">
+        <v>628</v>
+      </c>
+      <c r="P421" s="10"/>
+      <c r="Q421" s="12">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="422" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A422" t="s">
+        <v>659</v>
+      </c>
+      <c r="B422" t="s">
+        <v>662</v>
+      </c>
+      <c r="C422" s="10">
+        <v>2014</v>
+      </c>
+      <c r="D422">
+        <v>899</v>
+      </c>
+      <c r="E422">
+        <v>500</v>
+      </c>
+      <c r="F422" s="10"/>
+      <c r="G422" s="8">
+        <v>80</v>
+      </c>
+      <c r="H422" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I422" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="J422" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="K422">
+        <v>0</v>
+      </c>
+      <c r="L422">
+        <v>1</v>
+      </c>
+      <c r="M422" t="s">
+        <v>292</v>
+      </c>
+      <c r="O422" s="12" t="s">
+        <v>628</v>
+      </c>
+      <c r="P422" s="10"/>
+      <c r="Q422" s="12">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="423" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A423" t="s">
+        <v>659</v>
+      </c>
+      <c r="B423" t="s">
+        <v>663</v>
+      </c>
+      <c r="C423" s="10">
+        <v>2014</v>
+      </c>
+      <c r="D423">
+        <v>799</v>
+      </c>
+      <c r="E423">
+        <v>473</v>
+      </c>
+      <c r="F423" s="10"/>
+      <c r="G423" s="8">
+        <v>80</v>
+      </c>
+      <c r="H423" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I423" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="J423" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="K423">
+        <v>0</v>
+      </c>
+      <c r="L423">
+        <v>1</v>
+      </c>
+      <c r="M423" t="s">
+        <v>292</v>
+      </c>
+      <c r="O423" s="12" t="s">
+        <v>628</v>
+      </c>
+      <c r="P423" s="10"/>
+      <c r="Q423" s="12">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="424" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A424" t="s">
+        <v>659</v>
+      </c>
+      <c r="B424" t="s">
+        <v>664</v>
+      </c>
+      <c r="C424" s="10">
+        <v>2014</v>
+      </c>
+      <c r="D424">
+        <v>799</v>
+      </c>
+      <c r="E424">
+        <v>461</v>
+      </c>
+      <c r="F424" s="10"/>
+      <c r="G424" s="8">
+        <v>80</v>
+      </c>
+      <c r="H424" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I424" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="J424" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="K424">
+        <v>0</v>
+      </c>
+      <c r="L424">
+        <v>1</v>
+      </c>
+      <c r="M424" t="s">
+        <v>292</v>
+      </c>
+      <c r="O424" s="12" t="s">
+        <v>628</v>
+      </c>
+      <c r="P424" s="10"/>
+      <c r="Q424" s="12">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="425" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A425" t="s">
+        <v>659</v>
+      </c>
+      <c r="B425" t="s">
+        <v>666</v>
+      </c>
+      <c r="C425">
+        <v>2015</v>
+      </c>
+      <c r="D425">
+        <v>999</v>
+      </c>
+      <c r="E425">
+        <v>770</v>
+      </c>
+      <c r="F425" s="10"/>
+      <c r="G425" s="8">
+        <v>80</v>
+      </c>
+      <c r="H425" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I425" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="J425" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="K425">
+        <v>0</v>
+      </c>
+      <c r="L425">
+        <v>1</v>
+      </c>
+      <c r="M425" t="s">
+        <v>292</v>
+      </c>
+      <c r="O425" s="12" t="s">
+        <v>628</v>
+      </c>
+      <c r="P425" s="10"/>
+      <c r="Q425">
+        <v>424</v>
       </c>
     </row>
   </sheetData>
@@ -24561,10 +24919,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24988,6 +25346,14 @@
         <v>657</v>
       </c>
     </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="13">
+        <v>42948</v>
+      </c>
+      <c r="B54" t="s">
+        <v>667</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
+ new canon lenses
</commit_message>
<xml_diff>
--- a/BigAssTableOfLenses.xlsx
+++ b/BigAssTableOfLenses.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Markus\Desktop\BATOL\BigAssTableOfLenses\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brand\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3245" uniqueCount="669">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3291" uniqueCount="673">
   <si>
     <t>Manufacture</t>
   </si>
@@ -2001,6 +2001,21 @@
     <t>Veydra lenses, Tamron 24-70 G2 metadata</t>
   </si>
   <si>
+    <t>New lenses from Canon</t>
+  </si>
+  <si>
+    <t>85mm f/1.4L IS USM</t>
+  </si>
+  <si>
+    <t>TS-E 50mm f/2.8L Macro</t>
+  </si>
+  <si>
+    <t>TS-E 90mm f/2.8L Macro</t>
+  </si>
+  <si>
+    <t>TS-E 135mm f/4L Macro</t>
+  </si>
+  <si>
     <t>Xeen 14mm T3.1</t>
   </si>
   <si>
@@ -2029,9 +2044,6 @@
   </si>
   <si>
     <t>Xenon FF 75mm T2.1</t>
-  </si>
-  <si>
-    <t>Removed slashes for old T#'s</t>
   </si>
 </sst>
 </file>
@@ -2140,8 +2152,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q425" totalsRowShown="0">
-  <autoFilter ref="A1:Q425"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q429" totalsRowShown="0">
+  <autoFilter ref="A1:Q429"/>
   <sortState ref="A2:Q403">
     <sortCondition ref="Q1:Q403"/>
   </sortState>
@@ -2466,30 +2478,30 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q425"/>
+  <dimension ref="A1:Q429"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A356" workbookViewId="0">
+      <selection activeCell="J367" sqref="J367"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.1015625" customWidth="1"/>
-    <col min="2" max="2" width="37.89453125" customWidth="1"/>
-    <col min="3" max="3" width="5.41796875" customWidth="1"/>
-    <col min="4" max="4" width="6.41796875" customWidth="1"/>
-    <col min="5" max="5" width="8.20703125" customWidth="1"/>
-    <col min="7" max="7" width="8.68359375" customWidth="1"/>
-    <col min="8" max="8" width="12.41796875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.1015625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="5.89453125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="10.20703125" customWidth="1"/>
+    <col min="1" max="1" width="8.109375" customWidth="1"/>
+    <col min="2" max="2" width="37.88671875" customWidth="1"/>
+    <col min="3" max="3" width="5.44140625" customWidth="1"/>
+    <col min="4" max="4" width="6.44140625" customWidth="1"/>
+    <col min="5" max="5" width="8.21875" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.109375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="5.88671875" style="4" customWidth="1"/>
+    <col min="11" max="11" width="10.21875" customWidth="1"/>
     <col min="12" max="12" width="9" customWidth="1"/>
-    <col min="13" max="13" width="11.68359375" customWidth="1"/>
-    <col min="15" max="16" width="8.89453125" style="12"/>
+    <col min="13" max="13" width="11.6640625" customWidth="1"/>
+    <col min="15" max="16" width="8.88671875" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2542,7 +2554,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -2597,7 +2609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -2652,7 +2664,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -2707,7 +2719,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -2762,7 +2774,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -2817,7 +2829,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -2872,7 +2884,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -2927,7 +2939,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2982,7 +2994,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -3037,7 +3049,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -3092,7 +3104,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -3147,7 +3159,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -3202,7 +3214,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -3257,7 +3269,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
@@ -3312,7 +3324,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
@@ -3367,7 +3379,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
@@ -3422,7 +3434,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
@@ -3477,7 +3489,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -3532,7 +3544,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
@@ -3587,7 +3599,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
@@ -3642,7 +3654,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
@@ -3697,7 +3709,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
@@ -3752,7 +3764,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
@@ -3807,7 +3819,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
@@ -3862,7 +3874,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
@@ -3917,7 +3929,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
@@ -3972,7 +3984,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>7</v>
       </c>
@@ -4027,7 +4039,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>7</v>
       </c>
@@ -4082,7 +4094,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>7</v>
       </c>
@@ -4137,7 +4149,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>7</v>
       </c>
@@ -4192,7 +4204,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>7</v>
       </c>
@@ -4247,7 +4259,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
@@ -4302,7 +4314,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>7</v>
       </c>
@@ -4357,7 +4369,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>7</v>
       </c>
@@ -4412,7 +4424,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>7</v>
       </c>
@@ -4467,7 +4479,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>7</v>
       </c>
@@ -4522,7 +4534,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -4577,7 +4589,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -4632,7 +4644,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -4687,7 +4699,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>7</v>
       </c>
@@ -4742,7 +4754,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>7</v>
       </c>
@@ -4797,7 +4809,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>7</v>
       </c>
@@ -4852,7 +4864,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -4905,7 +4917,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>7</v>
       </c>
@@ -4960,7 +4972,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>7</v>
       </c>
@@ -5015,7 +5027,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>7</v>
       </c>
@@ -5070,7 +5082,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>7</v>
       </c>
@@ -5125,7 +5137,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>7</v>
       </c>
@@ -5180,7 +5192,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>7</v>
       </c>
@@ -5235,7 +5247,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>7</v>
       </c>
@@ -5290,7 +5302,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -5345,7 +5357,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>7</v>
       </c>
@@ -5400,7 +5412,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>7</v>
       </c>
@@ -5455,7 +5467,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>7</v>
       </c>
@@ -5510,7 +5522,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>7</v>
       </c>
@@ -5565,7 +5577,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>7</v>
       </c>
@@ -5620,7 +5632,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>7</v>
       </c>
@@ -5675,7 +5687,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>7</v>
       </c>
@@ -5730,7 +5742,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>7</v>
       </c>
@@ -5785,7 +5797,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>7</v>
       </c>
@@ -5838,7 +5850,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>7</v>
       </c>
@@ -5893,7 +5905,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>7</v>
       </c>
@@ -5946,7 +5958,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>7</v>
       </c>
@@ -5999,7 +6011,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>7</v>
       </c>
@@ -6052,7 +6064,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>7</v>
       </c>
@@ -6105,7 +6117,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>7</v>
       </c>
@@ -6158,7 +6170,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>370</v>
       </c>
@@ -6211,7 +6223,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>370</v>
       </c>
@@ -6264,7 +6276,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>370</v>
       </c>
@@ -6317,7 +6329,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>370</v>
       </c>
@@ -6370,7 +6382,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>370</v>
       </c>
@@ -6423,7 +6435,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>370</v>
       </c>
@@ -6476,7 +6488,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>370</v>
       </c>
@@ -6529,7 +6541,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>370</v>
       </c>
@@ -6582,7 +6594,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>370</v>
       </c>
@@ -6635,7 +6647,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>370</v>
       </c>
@@ -6688,7 +6700,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>370</v>
       </c>
@@ -6741,7 +6753,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>370</v>
       </c>
@@ -6794,7 +6806,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>370</v>
       </c>
@@ -6847,7 +6859,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>370</v>
       </c>
@@ -6900,7 +6912,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>370</v>
       </c>
@@ -6953,7 +6965,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>370</v>
       </c>
@@ -7006,7 +7018,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>370</v>
       </c>
@@ -7059,7 +7071,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>370</v>
       </c>
@@ -7112,7 +7124,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>370</v>
       </c>
@@ -7165,7 +7177,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>370</v>
       </c>
@@ -7218,7 +7230,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>370</v>
       </c>
@@ -7268,7 +7280,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>287</v>
       </c>
@@ -7321,7 +7333,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>421</v>
       </c>
@@ -7370,7 +7382,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>421</v>
       </c>
@@ -7419,7 +7431,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>227</v>
       </c>
@@ -7472,7 +7484,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>227</v>
       </c>
@@ -7525,7 +7537,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>227</v>
       </c>
@@ -7578,7 +7590,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>227</v>
       </c>
@@ -7631,7 +7643,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>227</v>
       </c>
@@ -7684,7 +7696,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>227</v>
       </c>
@@ -7737,7 +7749,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>227</v>
       </c>
@@ -7792,7 +7804,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>227</v>
       </c>
@@ -7848,7 +7860,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>227</v>
       </c>
@@ -7903,7 +7915,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>227</v>
       </c>
@@ -7956,7 +7968,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>227</v>
       </c>
@@ -8009,7 +8021,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>227</v>
       </c>
@@ -8062,7 +8074,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>227</v>
       </c>
@@ -8115,7 +8127,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>227</v>
       </c>
@@ -8168,7 +8180,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>227</v>
       </c>
@@ -8221,7 +8233,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>227</v>
       </c>
@@ -8277,7 +8289,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>227</v>
       </c>
@@ -8330,7 +8342,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>227</v>
       </c>
@@ -8383,7 +8395,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>227</v>
       </c>
@@ -8436,7 +8448,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>227</v>
       </c>
@@ -8489,7 +8501,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>227</v>
       </c>
@@ -8542,7 +8554,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>227</v>
       </c>
@@ -8595,7 +8607,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>227</v>
       </c>
@@ -8648,7 +8660,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>227</v>
       </c>
@@ -8701,7 +8713,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>227</v>
       </c>
@@ -8757,7 +8769,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>227</v>
       </c>
@@ -8813,7 +8825,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>227</v>
       </c>
@@ -8866,7 +8878,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>227</v>
       </c>
@@ -8919,7 +8931,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>227</v>
       </c>
@@ -8972,7 +8984,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>289</v>
       </c>
@@ -9027,7 +9039,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>289</v>
       </c>
@@ -9082,7 +9094,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>289</v>
       </c>
@@ -9137,7 +9149,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>59</v>
       </c>
@@ -9190,7 +9202,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>59</v>
       </c>
@@ -9243,7 +9255,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>59</v>
       </c>
@@ -9296,7 +9308,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>59</v>
       </c>
@@ -9349,7 +9361,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>59</v>
       </c>
@@ -9402,7 +9414,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>59</v>
       </c>
@@ -9455,7 +9467,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>59</v>
       </c>
@@ -9508,7 +9520,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>59</v>
       </c>
@@ -9561,7 +9573,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>59</v>
       </c>
@@ -9614,7 +9626,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>59</v>
       </c>
@@ -9667,7 +9679,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>59</v>
       </c>
@@ -9720,7 +9732,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>59</v>
       </c>
@@ -9773,7 +9785,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>59</v>
       </c>
@@ -9826,7 +9838,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>59</v>
       </c>
@@ -9879,7 +9891,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>59</v>
       </c>
@@ -9932,7 +9944,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>59</v>
       </c>
@@ -9986,7 +9998,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>59</v>
       </c>
@@ -10039,7 +10051,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>59</v>
       </c>
@@ -10092,7 +10104,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="142" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>59</v>
       </c>
@@ -10145,7 +10157,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>59</v>
       </c>
@@ -10198,7 +10210,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>59</v>
       </c>
@@ -10251,7 +10263,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="145" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>59</v>
       </c>
@@ -10304,7 +10316,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>59</v>
       </c>
@@ -10357,7 +10369,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>59</v>
       </c>
@@ -10410,7 +10422,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>59</v>
       </c>
@@ -10463,7 +10475,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="149" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>59</v>
       </c>
@@ -10516,7 +10528,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>59</v>
       </c>
@@ -10569,7 +10581,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>59</v>
       </c>
@@ -10622,7 +10634,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>59</v>
       </c>
@@ -10675,7 +10687,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="153" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>59</v>
       </c>
@@ -10728,7 +10740,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="154" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>59</v>
       </c>
@@ -10781,7 +10793,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="155" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>59</v>
       </c>
@@ -10834,7 +10846,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>59</v>
       </c>
@@ -10885,7 +10897,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>59</v>
       </c>
@@ -10936,7 +10948,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>59</v>
       </c>
@@ -10987,7 +10999,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>59</v>
       </c>
@@ -11038,7 +11050,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>59</v>
       </c>
@@ -11089,7 +11101,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="161" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>363</v>
       </c>
@@ -11140,7 +11152,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="162" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>363</v>
       </c>
@@ -11191,7 +11203,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="163" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="163" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>363</v>
       </c>
@@ -11242,7 +11254,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="164" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="164" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>430</v>
       </c>
@@ -11293,7 +11305,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="165" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>430</v>
       </c>
@@ -11344,7 +11356,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="166" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="166" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>430</v>
       </c>
@@ -11395,7 +11407,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="167" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="167" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>424</v>
       </c>
@@ -11450,12 +11462,12 @@
         <v>166</v>
       </c>
     </row>
-    <row r="168" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="168" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>424</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>658</v>
+        <v>663</v>
       </c>
       <c r="C168" s="1">
         <v>2016</v>
@@ -11503,7 +11515,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="169" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="169" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>424</v>
       </c>
@@ -11559,12 +11571,12 @@
         <v>168</v>
       </c>
     </row>
-    <row r="170" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="170" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>424</v>
       </c>
       <c r="B170" t="s">
-        <v>659</v>
+        <v>664</v>
       </c>
       <c r="C170">
         <v>2015</v>
@@ -11612,7 +11624,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="171" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="171" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>424</v>
       </c>
@@ -11667,12 +11679,12 @@
         <v>170</v>
       </c>
     </row>
-    <row r="172" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="172" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A172" s="12" t="s">
         <v>424</v>
       </c>
       <c r="B172" t="s">
-        <v>660</v>
+        <v>665</v>
       </c>
       <c r="C172" s="12">
         <v>2016</v>
@@ -11720,7 +11732,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="173" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="173" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A173" s="12" t="s">
         <v>424</v>
       </c>
@@ -11775,12 +11787,12 @@
         <v>172</v>
       </c>
     </row>
-    <row r="174" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="174" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A174" s="12" t="s">
         <v>424</v>
       </c>
       <c r="B174" t="s">
-        <v>661</v>
+        <v>666</v>
       </c>
       <c r="C174">
         <v>2015</v>
@@ -11828,7 +11840,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="175" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="175" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A175" s="12" t="s">
         <v>424</v>
       </c>
@@ -11883,12 +11895,12 @@
         <v>174</v>
       </c>
     </row>
-    <row r="176" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="176" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A176" s="12" t="s">
         <v>424</v>
       </c>
       <c r="B176" t="s">
-        <v>662</v>
+        <v>667</v>
       </c>
       <c r="C176">
         <v>2015</v>
@@ -11936,7 +11948,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="177" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A177" s="12" t="s">
         <v>424</v>
       </c>
@@ -11989,12 +12001,12 @@
         <v>176</v>
       </c>
     </row>
-    <row r="178" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="178" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A178" s="12" t="s">
         <v>424</v>
       </c>
       <c r="B178" t="s">
-        <v>663</v>
+        <v>668</v>
       </c>
       <c r="C178">
         <v>2016</v>
@@ -12042,7 +12054,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="179" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="179" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>213</v>
       </c>
@@ -12097,7 +12109,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="180" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="180" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>213</v>
       </c>
@@ -12152,7 +12164,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="181" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="181" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>213</v>
       </c>
@@ -12207,7 +12219,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="182" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="182" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>100</v>
       </c>
@@ -12260,7 +12272,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="183" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="183" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>100</v>
       </c>
@@ -12313,7 +12325,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="184" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="184" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>100</v>
       </c>
@@ -12366,7 +12378,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="185" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="185" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>100</v>
       </c>
@@ -12419,7 +12431,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="186" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="186" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>100</v>
       </c>
@@ -12472,7 +12484,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="187" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="187" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>100</v>
       </c>
@@ -12525,7 +12537,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="188" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="188" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>100</v>
       </c>
@@ -12578,7 +12590,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="189" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="189" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>100</v>
       </c>
@@ -12631,7 +12643,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="190" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="190" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>100</v>
       </c>
@@ -12684,7 +12696,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="191" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="191" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>100</v>
       </c>
@@ -12737,7 +12749,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="192" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="192" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>100</v>
       </c>
@@ -12790,7 +12802,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="193" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="193" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>100</v>
       </c>
@@ -12841,7 +12853,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="194" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="194" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>100</v>
       </c>
@@ -12892,7 +12904,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="195" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="195" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>100</v>
       </c>
@@ -12940,7 +12952,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="196" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="196" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>100</v>
       </c>
@@ -12991,7 +13003,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="197" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="197" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>100</v>
       </c>
@@ -13042,7 +13054,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="198" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="198" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>100</v>
       </c>
@@ -13093,7 +13105,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="199" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="199" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>166</v>
       </c>
@@ -13146,7 +13158,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="200" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="200" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>166</v>
       </c>
@@ -13199,7 +13211,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="201" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="201" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>166</v>
       </c>
@@ -13252,7 +13264,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="202" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="202" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>166</v>
       </c>
@@ -13305,7 +13317,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="203" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="203" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>166</v>
       </c>
@@ -13358,7 +13370,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="204" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="204" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>166</v>
       </c>
@@ -13411,7 +13423,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="205" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="205" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>166</v>
       </c>
@@ -13465,7 +13477,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="206" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="206" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>166</v>
       </c>
@@ -13518,7 +13530,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="207" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="207" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>166</v>
       </c>
@@ -13571,7 +13583,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="208" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="208" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>166</v>
       </c>
@@ -13624,7 +13636,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="209" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="209" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>166</v>
       </c>
@@ -13677,7 +13689,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="210" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="210" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>166</v>
       </c>
@@ -13730,7 +13742,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="211" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="211" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>166</v>
       </c>
@@ -13783,7 +13795,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="212" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="212" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>166</v>
       </c>
@@ -13836,7 +13848,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="213" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="213" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>166</v>
       </c>
@@ -13889,7 +13901,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="214" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="214" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>166</v>
       </c>
@@ -13940,7 +13952,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="215" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="215" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>182</v>
       </c>
@@ -13993,7 +14005,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="216" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="216" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>182</v>
       </c>
@@ -14046,7 +14058,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="217" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="217" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>182</v>
       </c>
@@ -14099,7 +14111,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="218" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="218" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>182</v>
       </c>
@@ -14152,7 +14164,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="219" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="219" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>182</v>
       </c>
@@ -14205,7 +14217,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="220" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="220" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>182</v>
       </c>
@@ -14258,7 +14270,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="221" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="221" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>182</v>
       </c>
@@ -14311,7 +14323,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="222" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="222" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>182</v>
       </c>
@@ -14364,7 +14376,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="223" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="223" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>182</v>
       </c>
@@ -14417,7 +14429,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="224" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="224" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>182</v>
       </c>
@@ -14468,7 +14480,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="225" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="225" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A225" s="1" t="s">
         <v>182</v>
       </c>
@@ -14519,7 +14531,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="226" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="226" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A226" s="1" t="s">
         <v>182</v>
       </c>
@@ -14570,7 +14582,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="227" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="227" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>191</v>
       </c>
@@ -14623,7 +14635,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="228" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="228" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>191</v>
       </c>
@@ -14676,7 +14688,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="229" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="229" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>191</v>
       </c>
@@ -14729,7 +14741,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="230" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="230" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>191</v>
       </c>
@@ -14782,7 +14794,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="231" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="231" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>191</v>
       </c>
@@ -14835,7 +14847,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="232" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="232" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>191</v>
       </c>
@@ -14886,7 +14898,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="233" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="233" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>258</v>
       </c>
@@ -14939,7 +14951,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="234" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="234" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A234" s="1" t="s">
         <v>258</v>
       </c>
@@ -14992,12 +15004,12 @@
         <v>233</v>
       </c>
     </row>
-    <row r="235" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="235" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A235" s="1" t="s">
         <v>258</v>
       </c>
       <c r="B235" t="s">
-        <v>664</v>
+        <v>669</v>
       </c>
       <c r="C235" s="1">
         <v>2016</v>
@@ -15045,7 +15057,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="236" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="236" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A236" s="1" t="s">
         <v>258</v>
       </c>
@@ -15098,7 +15110,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="237" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="237" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A237" s="1" t="s">
         <v>215</v>
       </c>
@@ -15149,7 +15161,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="238" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="238" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A238" s="1" t="s">
         <v>215</v>
       </c>
@@ -15198,7 +15210,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="239" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="239" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A239" s="1" t="s">
         <v>215</v>
       </c>
@@ -15247,7 +15259,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="240" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="240" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A240" s="1" t="s">
         <v>215</v>
       </c>
@@ -15298,7 +15310,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="241" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="241" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A241" s="1" t="s">
         <v>215</v>
       </c>
@@ -15347,7 +15359,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="242" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="242" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A242" s="1" t="s">
         <v>215</v>
       </c>
@@ -15396,7 +15408,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="243" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="243" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A243" s="1" t="s">
         <v>215</v>
       </c>
@@ -15445,7 +15457,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="244" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="244" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A244" s="1" t="s">
         <v>215</v>
       </c>
@@ -15496,7 +15508,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="245" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="245" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A245" s="1" t="s">
         <v>215</v>
       </c>
@@ -15545,7 +15557,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="246" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="246" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A246" s="1" t="s">
         <v>215</v>
       </c>
@@ -15594,7 +15606,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="247" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="247" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>215</v>
       </c>
@@ -15643,7 +15655,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="248" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="248" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>215</v>
       </c>
@@ -15692,7 +15704,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="249" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="249" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>215</v>
       </c>
@@ -15741,7 +15753,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="250" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="250" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>215</v>
       </c>
@@ -15792,7 +15804,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="251" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="251" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>215</v>
       </c>
@@ -15841,7 +15853,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="252" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="252" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A252" s="1" t="s">
         <v>215</v>
       </c>
@@ -15890,7 +15902,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="253" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="253" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A253" s="1" t="s">
         <v>215</v>
       </c>
@@ -15939,7 +15951,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="254" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="254" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>132</v>
       </c>
@@ -15994,7 +16006,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="255" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="255" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>132</v>
       </c>
@@ -16047,7 +16059,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="256" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="256" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>132</v>
       </c>
@@ -16100,7 +16112,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="257" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="257" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>132</v>
       </c>
@@ -16155,7 +16167,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="258" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="258" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>132</v>
       </c>
@@ -16208,7 +16220,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="259" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="259" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>132</v>
       </c>
@@ -16261,7 +16273,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="260" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="260" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>132</v>
       </c>
@@ -16316,7 +16328,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="261" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="261" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>132</v>
       </c>
@@ -16371,7 +16383,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="262" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="262" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>132</v>
       </c>
@@ -16426,7 +16438,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="263" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="263" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>132</v>
       </c>
@@ -16479,7 +16491,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="264" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="264" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>132</v>
       </c>
@@ -16532,7 +16544,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="265" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="265" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>132</v>
       </c>
@@ -16585,7 +16597,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="266" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="266" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>132</v>
       </c>
@@ -16640,7 +16652,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="267" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="267" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>132</v>
       </c>
@@ -16695,7 +16707,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="268" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="268" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A268" s="1" t="s">
         <v>132</v>
       </c>
@@ -16750,7 +16762,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="269" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="269" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A269" s="1" t="s">
         <v>132</v>
       </c>
@@ -16803,7 +16815,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="270" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="270" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>132</v>
       </c>
@@ -16856,7 +16868,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="271" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="271" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>132</v>
       </c>
@@ -16911,7 +16923,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="272" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="272" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>132</v>
       </c>
@@ -16966,7 +16978,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="273" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="273" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>132</v>
       </c>
@@ -17019,7 +17031,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="274" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="274" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>132</v>
       </c>
@@ -17072,7 +17084,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="275" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="275" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>132</v>
       </c>
@@ -17127,7 +17139,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="276" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="276" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>132</v>
       </c>
@@ -17182,7 +17194,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="277" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="277" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>132</v>
       </c>
@@ -17237,7 +17249,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="278" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="278" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>132</v>
       </c>
@@ -17292,7 +17304,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="279" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="279" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>132</v>
       </c>
@@ -17345,7 +17357,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="280" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="280" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>132</v>
       </c>
@@ -17398,7 +17410,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="281" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="281" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>132</v>
       </c>
@@ -17451,7 +17463,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="282" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="282" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>132</v>
       </c>
@@ -17504,7 +17516,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="283" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="283" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>132</v>
       </c>
@@ -17557,7 +17569,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="284" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="284" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>132</v>
       </c>
@@ -17612,7 +17624,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="285" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="285" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>132</v>
       </c>
@@ -17667,7 +17679,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="286" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="286" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>132</v>
       </c>
@@ -17722,7 +17734,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="287" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="287" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>132</v>
       </c>
@@ -17777,7 +17789,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="288" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="288" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>132</v>
       </c>
@@ -17832,7 +17844,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="289" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="289" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>132</v>
       </c>
@@ -17885,7 +17897,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="290" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="290" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>132</v>
       </c>
@@ -17938,7 +17950,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="291" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="291" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>132</v>
       </c>
@@ -17991,7 +18003,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="292" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="292" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>132</v>
       </c>
@@ -18044,7 +18056,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="293" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="293" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>132</v>
       </c>
@@ -18097,7 +18109,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="294" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="294" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>132</v>
       </c>
@@ -18152,7 +18164,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="295" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="295" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>132</v>
       </c>
@@ -18207,7 +18219,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="296" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="296" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>132</v>
       </c>
@@ -18262,7 +18274,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="297" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="297" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>132</v>
       </c>
@@ -18317,7 +18329,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="298" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="298" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>132</v>
       </c>
@@ -18372,7 +18384,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="299" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="299" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>132</v>
       </c>
@@ -18425,7 +18437,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="300" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="300" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>132</v>
       </c>
@@ -18478,7 +18490,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="301" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="301" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>132</v>
       </c>
@@ -18531,7 +18543,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="302" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="302" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>132</v>
       </c>
@@ -18586,7 +18598,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="303" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="303" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>132</v>
       </c>
@@ -18641,7 +18653,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="304" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="304" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>132</v>
       </c>
@@ -18694,7 +18706,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="305" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="305" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>132</v>
       </c>
@@ -18749,7 +18761,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="306" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="306" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>132</v>
       </c>
@@ -18802,7 +18814,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="307" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="307" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>132</v>
       </c>
@@ -18855,7 +18867,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="308" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="308" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>132</v>
       </c>
@@ -18908,7 +18920,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="309" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="309" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>132</v>
       </c>
@@ -18961,7 +18973,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="310" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="310" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>132</v>
       </c>
@@ -19014,7 +19026,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="311" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="311" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>132</v>
       </c>
@@ -19067,7 +19079,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="312" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="312" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>132</v>
       </c>
@@ -19120,7 +19132,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="313" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="313" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>132</v>
       </c>
@@ -19173,7 +19185,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="314" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="314" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>132</v>
       </c>
@@ -19226,7 +19238,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="315" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="315" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>370</v>
       </c>
@@ -19279,7 +19291,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="316" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="316" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>370</v>
       </c>
@@ -19332,7 +19344,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="317" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="317" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>100</v>
       </c>
@@ -19383,7 +19395,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="318" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="318" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>100</v>
       </c>
@@ -19434,7 +19446,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="319" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="319" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>100</v>
       </c>
@@ -19483,7 +19495,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="320" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="320" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>100</v>
       </c>
@@ -19534,7 +19546,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="321" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="321" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>7</v>
       </c>
@@ -19587,12 +19599,12 @@
         <v>320</v>
       </c>
     </row>
-    <row r="322" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="322" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>213</v>
       </c>
       <c r="B322" t="s">
-        <v>665</v>
+        <v>670</v>
       </c>
       <c r="C322" s="10"/>
       <c r="D322">
@@ -19638,12 +19650,12 @@
         <v>321</v>
       </c>
     </row>
-    <row r="323" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="323" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>213</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>666</v>
+        <v>671</v>
       </c>
       <c r="C323" s="10"/>
       <c r="D323">
@@ -19689,12 +19701,12 @@
         <v>322</v>
       </c>
     </row>
-    <row r="324" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="324" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>213</v>
       </c>
       <c r="B324" s="1" t="s">
-        <v>667</v>
+        <v>672</v>
       </c>
       <c r="C324" s="10"/>
       <c r="D324">
@@ -19740,7 +19752,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="325" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="325" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>100</v>
       </c>
@@ -19789,7 +19801,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="326" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="326" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>191</v>
       </c>
@@ -19840,7 +19852,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="327" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="327" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>7</v>
       </c>
@@ -19889,7 +19901,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="328" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="328" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>7</v>
       </c>
@@ -19942,7 +19954,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="329" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="329" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>7</v>
       </c>
@@ -19995,7 +20007,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="330" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="330" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>7</v>
       </c>
@@ -20048,7 +20060,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="331" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="331" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>7</v>
       </c>
@@ -20101,7 +20113,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="332" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="332" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>213</v>
       </c>
@@ -20152,7 +20164,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="333" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="333" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>213</v>
       </c>
@@ -20203,7 +20215,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="334" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="334" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>213</v>
       </c>
@@ -20254,7 +20266,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="335" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="335" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>213</v>
       </c>
@@ -20305,7 +20317,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="336" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="336" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>213</v>
       </c>
@@ -20356,7 +20368,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="337" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="337" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>213</v>
       </c>
@@ -20407,7 +20419,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="338" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="338" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
         <v>494</v>
       </c>
@@ -20460,7 +20472,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="339" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="339" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
         <v>494</v>
       </c>
@@ -20511,7 +20523,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="340" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="340" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
         <v>494</v>
       </c>
@@ -20562,7 +20574,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="341" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="341" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>494</v>
       </c>
@@ -20613,7 +20625,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="342" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="342" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
         <v>494</v>
       </c>
@@ -20664,7 +20676,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="343" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="343" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
         <v>494</v>
       </c>
@@ -20715,7 +20727,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="344" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="344" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
         <v>494</v>
       </c>
@@ -20766,7 +20778,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="345" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="345" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
         <v>494</v>
       </c>
@@ -20817,7 +20829,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="346" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="346" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
         <v>494</v>
       </c>
@@ -20868,7 +20880,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="347" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="347" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
         <v>494</v>
       </c>
@@ -20919,7 +20931,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="348" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="348" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
         <v>494</v>
       </c>
@@ -20970,7 +20982,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="349" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="349" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
         <v>494</v>
       </c>
@@ -21021,7 +21033,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="350" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="350" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
         <v>494</v>
       </c>
@@ -21072,7 +21084,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="351" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="351" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
         <v>494</v>
       </c>
@@ -21123,7 +21135,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="352" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="352" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
         <v>494</v>
       </c>
@@ -21174,7 +21186,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="353" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="353" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
         <v>494</v>
       </c>
@@ -21225,7 +21237,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="354" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="354" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
         <v>494</v>
       </c>
@@ -21276,7 +21288,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="355" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="355" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
         <v>370</v>
       </c>
@@ -21329,7 +21341,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="356" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="356" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
         <v>370</v>
       </c>
@@ -21382,7 +21394,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="357" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="357" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
         <v>370</v>
       </c>
@@ -21435,7 +21447,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="358" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="358" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
         <v>370</v>
       </c>
@@ -21488,7 +21500,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="359" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="359" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
         <v>370</v>
       </c>
@@ -21541,7 +21553,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="360" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="360" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
         <v>370</v>
       </c>
@@ -21594,7 +21606,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="361" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="361" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
         <v>370</v>
       </c>
@@ -21647,7 +21659,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="362" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="362" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
         <v>370</v>
       </c>
@@ -21700,7 +21712,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="363" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="363" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
         <v>370</v>
       </c>
@@ -21753,7 +21765,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="364" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="364" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
         <v>100</v>
       </c>
@@ -21799,12 +21811,14 @@
       <c r="O364" s="12" t="s">
         <v>616</v>
       </c>
-      <c r="P364" s="10"/>
+      <c r="P364" s="12" t="s">
+        <v>616</v>
+      </c>
       <c r="Q364" s="7">
         <v>363</v>
       </c>
     </row>
-    <row r="365" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="365" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
         <v>100</v>
       </c>
@@ -21850,12 +21864,14 @@
       <c r="O365" s="12" t="s">
         <v>616</v>
       </c>
-      <c r="P365" s="10"/>
+      <c r="P365" s="12" t="s">
+        <v>616</v>
+      </c>
       <c r="Q365" s="7">
         <v>364</v>
       </c>
     </row>
-    <row r="366" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="366" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
         <v>100</v>
       </c>
@@ -21901,12 +21917,14 @@
       <c r="O366" s="12" t="s">
         <v>616</v>
       </c>
-      <c r="P366" s="10"/>
+      <c r="P366" s="12" t="s">
+        <v>616</v>
+      </c>
       <c r="Q366" s="7">
         <v>365</v>
       </c>
     </row>
-    <row r="367" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="367" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
         <v>100</v>
       </c>
@@ -21952,12 +21970,14 @@
       <c r="O367" s="12" t="s">
         <v>616</v>
       </c>
-      <c r="P367" s="10"/>
+      <c r="P367" s="12" t="s">
+        <v>616</v>
+      </c>
       <c r="Q367" s="7">
         <v>366</v>
       </c>
     </row>
-    <row r="368" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="368" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
         <v>100</v>
       </c>
@@ -22003,12 +22023,14 @@
       <c r="O368" s="12" t="s">
         <v>616</v>
       </c>
-      <c r="P368" s="10"/>
+      <c r="P368" s="12" t="s">
+        <v>616</v>
+      </c>
       <c r="Q368" s="7">
         <v>367</v>
       </c>
     </row>
-    <row r="369" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="369" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
         <v>100</v>
       </c>
@@ -22054,12 +22076,14 @@
       <c r="O369" s="12" t="s">
         <v>616</v>
       </c>
-      <c r="P369" s="10"/>
+      <c r="P369" s="12" t="s">
+        <v>616</v>
+      </c>
       <c r="Q369" s="7">
         <v>368</v>
       </c>
     </row>
-    <row r="370" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="370" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
         <v>100</v>
       </c>
@@ -22105,12 +22129,14 @@
       <c r="O370" s="12" t="s">
         <v>616</v>
       </c>
-      <c r="P370" s="10"/>
+      <c r="P370" s="12" t="s">
+        <v>616</v>
+      </c>
       <c r="Q370" s="7">
         <v>369</v>
       </c>
     </row>
-    <row r="371" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="371" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
         <v>100</v>
       </c>
@@ -22156,12 +22182,14 @@
       <c r="O371" s="12" t="s">
         <v>616</v>
       </c>
-      <c r="P371" s="10"/>
+      <c r="P371" s="12" t="s">
+        <v>616</v>
+      </c>
       <c r="Q371" s="7">
         <v>370</v>
       </c>
     </row>
-    <row r="372" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="372" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
         <v>191</v>
       </c>
@@ -22212,7 +22240,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="373" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="373" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
         <v>191</v>
       </c>
@@ -22263,7 +22291,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="374" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="374" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
         <v>191</v>
       </c>
@@ -22314,7 +22342,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="375" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="375" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
         <v>191</v>
       </c>
@@ -22365,7 +22393,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="376" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="376" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
         <v>191</v>
       </c>
@@ -22414,7 +22442,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="377" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="377" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
         <v>191</v>
       </c>
@@ -22465,7 +22493,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="378" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="378" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
         <v>191</v>
       </c>
@@ -22516,7 +22544,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="379" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="379" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A379" t="s">
         <v>132</v>
       </c>
@@ -22569,7 +22597,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="380" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="380" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A380" t="s">
         <v>7</v>
       </c>
@@ -22622,7 +22650,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="381" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="381" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A381" t="s">
         <v>424</v>
       </c>
@@ -22675,7 +22703,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="382" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="382" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A382" t="s">
         <v>424</v>
       </c>
@@ -22728,7 +22756,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="383" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="383" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A383" t="s">
         <v>424</v>
       </c>
@@ -22781,7 +22809,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="384" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="384" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A384" t="s">
         <v>424</v>
       </c>
@@ -22834,7 +22862,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="385" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="385" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A385" s="7" t="s">
         <v>182</v>
       </c>
@@ -22885,7 +22913,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="386" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="386" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A386" s="7" t="s">
         <v>132</v>
       </c>
@@ -22938,7 +22966,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="387" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="387" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A387" s="7" t="s">
         <v>166</v>
       </c>
@@ -22989,7 +23017,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="388" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="388" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A388" s="7" t="s">
         <v>166</v>
       </c>
@@ -23040,7 +23068,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="389" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="389" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A389" s="7" t="s">
         <v>166</v>
       </c>
@@ -23091,7 +23119,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="390" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="390" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A390" s="7" t="s">
         <v>258</v>
       </c>
@@ -23142,7 +23170,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="391" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="391" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A391" s="7" t="s">
         <v>258</v>
       </c>
@@ -23195,7 +23223,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="392" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="392" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A392" s="7" t="s">
         <v>370</v>
       </c>
@@ -23248,7 +23276,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="393" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="393" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A393" s="7" t="s">
         <v>370</v>
       </c>
@@ -23301,7 +23329,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="394" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="394" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A394" s="7" t="s">
         <v>370</v>
       </c>
@@ -23354,7 +23382,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="395" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="395" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A395" s="7" t="s">
         <v>370</v>
       </c>
@@ -23399,7 +23427,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="396" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="396" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A396" s="7" t="s">
         <v>593</v>
       </c>
@@ -23448,7 +23476,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="397" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="397" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A397" s="7" t="s">
         <v>593</v>
       </c>
@@ -23497,7 +23525,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="398" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="398" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A398" t="s">
         <v>604</v>
       </c>
@@ -23550,7 +23578,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="399" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="399" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A399" t="s">
         <v>604</v>
       </c>
@@ -23599,7 +23627,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="400" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="400" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A400" t="s">
         <v>59</v>
       </c>
@@ -23650,7 +23678,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="401" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="401" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A401" t="s">
         <v>59</v>
       </c>
@@ -23701,7 +23729,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="402" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="402" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A402" t="s">
         <v>59</v>
       </c>
@@ -23752,7 +23780,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="403" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="403" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A403" t="s">
         <v>166</v>
       </c>
@@ -23803,7 +23831,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="404" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="404" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A404" t="s">
         <v>182</v>
       </c>
@@ -23854,7 +23882,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="405" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="405" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A405" t="s">
         <v>182</v>
       </c>
@@ -23907,7 +23935,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="406" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="406" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A406" t="s">
         <v>632</v>
       </c>
@@ -23956,7 +23984,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="407" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="407" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A407" s="12" t="s">
         <v>132</v>
       </c>
@@ -24009,7 +24037,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="408" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="408" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A408" s="12" t="s">
         <v>132</v>
       </c>
@@ -24062,7 +24090,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="409" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="409" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A409" s="12" t="s">
         <v>132</v>
       </c>
@@ -24115,7 +24143,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="410" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="410" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A410" s="12" t="s">
         <v>132</v>
       </c>
@@ -24168,7 +24196,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="411" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="411" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A411" s="12" t="s">
         <v>132</v>
       </c>
@@ -24221,7 +24249,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="412" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="412" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A412" s="12" t="s">
         <v>132</v>
       </c>
@@ -24274,7 +24302,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="413" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="413" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A413" s="12" t="s">
         <v>132</v>
       </c>
@@ -24327,7 +24355,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="414" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="414" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A414" s="12" t="s">
         <v>132</v>
       </c>
@@ -24380,7 +24408,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="415" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="415" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A415" s="12" t="s">
         <v>132</v>
       </c>
@@ -24433,7 +24461,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="416" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="416" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A416" s="12" t="s">
         <v>370</v>
       </c>
@@ -24484,7 +24512,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="417" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="417" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A417" t="s">
         <v>370</v>
       </c>
@@ -24535,7 +24563,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="418" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="418" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A418" t="s">
         <v>132</v>
       </c>
@@ -24588,7 +24616,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="419" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="419" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A419" t="s">
         <v>649</v>
       </c>
@@ -24637,7 +24665,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="420" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="420" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A420" t="s">
         <v>649</v>
       </c>
@@ -24675,6 +24703,9 @@
       <c r="M420" t="s">
         <v>286</v>
       </c>
+      <c r="N420" t="s">
+        <v>570</v>
+      </c>
       <c r="O420" s="12" t="s">
         <v>618</v>
       </c>
@@ -24683,7 +24714,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="421" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="421" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A421" s="12" t="s">
         <v>649</v>
       </c>
@@ -24719,6 +24750,9 @@
       <c r="M421" s="12" t="s">
         <v>286</v>
       </c>
+      <c r="N421" s="12" t="s">
+        <v>571</v>
+      </c>
       <c r="O421" s="12" t="s">
         <v>618</v>
       </c>
@@ -24727,7 +24761,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="422" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="422" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A422" t="s">
         <v>649</v>
       </c>
@@ -24765,6 +24799,9 @@
       <c r="M422" t="s">
         <v>286</v>
       </c>
+      <c r="N422" t="s">
+        <v>571</v>
+      </c>
       <c r="O422" s="12" t="s">
         <v>618</v>
       </c>
@@ -24773,7 +24810,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="423" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="423" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A423" t="s">
         <v>649</v>
       </c>
@@ -24811,6 +24848,9 @@
       <c r="M423" t="s">
         <v>286</v>
       </c>
+      <c r="N423" t="s">
+        <v>573</v>
+      </c>
       <c r="O423" s="12" t="s">
         <v>618</v>
       </c>
@@ -24819,7 +24859,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="424" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="424" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A424" t="s">
         <v>649</v>
       </c>
@@ -24857,6 +24897,9 @@
       <c r="M424" t="s">
         <v>286</v>
       </c>
+      <c r="N424" t="s">
+        <v>574</v>
+      </c>
       <c r="O424" s="12" t="s">
         <v>618</v>
       </c>
@@ -24865,7 +24908,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="425" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="425" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A425" t="s">
         <v>649</v>
       </c>
@@ -24903,12 +24946,227 @@
       <c r="M425" t="s">
         <v>286</v>
       </c>
+      <c r="N425" t="s">
+        <v>577</v>
+      </c>
       <c r="O425" s="12" t="s">
         <v>618</v>
       </c>
       <c r="P425" s="10"/>
       <c r="Q425">
         <v>424</v>
+      </c>
+    </row>
+    <row r="426" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A426" t="s">
+        <v>7</v>
+      </c>
+      <c r="B426" t="s">
+        <v>659</v>
+      </c>
+      <c r="C426">
+        <v>2017</v>
+      </c>
+      <c r="D426">
+        <v>1599</v>
+      </c>
+      <c r="E426">
+        <v>950</v>
+      </c>
+      <c r="F426">
+        <v>105.4</v>
+      </c>
+      <c r="G426" s="8">
+        <v>88.6</v>
+      </c>
+      <c r="H426" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="I426" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="J426" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="K426">
+        <v>1</v>
+      </c>
+      <c r="L426">
+        <v>0</v>
+      </c>
+      <c r="M426" t="s">
+        <v>278</v>
+      </c>
+      <c r="N426" t="s">
+        <v>573</v>
+      </c>
+      <c r="O426" s="12" t="s">
+        <v>616</v>
+      </c>
+      <c r="P426" s="12" t="s">
+        <v>616</v>
+      </c>
+      <c r="Q426">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="427" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A427" t="s">
+        <v>7</v>
+      </c>
+      <c r="B427" t="s">
+        <v>660</v>
+      </c>
+      <c r="C427">
+        <v>2017</v>
+      </c>
+      <c r="D427">
+        <v>2199</v>
+      </c>
+      <c r="E427">
+        <v>945</v>
+      </c>
+      <c r="F427">
+        <v>114.9</v>
+      </c>
+      <c r="G427" s="8">
+        <v>86.9</v>
+      </c>
+      <c r="H427" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="I427" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="J427" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="K427">
+        <v>0</v>
+      </c>
+      <c r="L427">
+        <v>0</v>
+      </c>
+      <c r="M427" t="s">
+        <v>278</v>
+      </c>
+      <c r="N427" t="s">
+        <v>569</v>
+      </c>
+      <c r="O427" s="12" t="s">
+        <v>616</v>
+      </c>
+      <c r="P427" s="12" t="s">
+        <v>616</v>
+      </c>
+      <c r="Q427">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="428" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A428" t="s">
+        <v>7</v>
+      </c>
+      <c r="B428" t="s">
+        <v>661</v>
+      </c>
+      <c r="C428">
+        <v>2017</v>
+      </c>
+      <c r="D428">
+        <v>2199</v>
+      </c>
+      <c r="E428">
+        <v>915</v>
+      </c>
+      <c r="F428">
+        <v>116.5</v>
+      </c>
+      <c r="G428" s="8">
+        <v>86.9</v>
+      </c>
+      <c r="H428" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="I428" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="J428" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="K428">
+        <v>0</v>
+      </c>
+      <c r="L428">
+        <v>0</v>
+      </c>
+      <c r="M428" t="s">
+        <v>278</v>
+      </c>
+      <c r="N428" t="s">
+        <v>569</v>
+      </c>
+      <c r="O428" s="12" t="s">
+        <v>616</v>
+      </c>
+      <c r="P428" s="12" t="s">
+        <v>616</v>
+      </c>
+      <c r="Q428">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="429" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A429" t="s">
+        <v>7</v>
+      </c>
+      <c r="B429" t="s">
+        <v>662</v>
+      </c>
+      <c r="C429">
+        <v>2017</v>
+      </c>
+      <c r="D429">
+        <v>2199</v>
+      </c>
+      <c r="E429">
+        <v>1100</v>
+      </c>
+      <c r="F429">
+        <v>139.1</v>
+      </c>
+      <c r="G429" s="8">
+        <v>88.5</v>
+      </c>
+      <c r="H429" s="1">
+        <v>4</v>
+      </c>
+      <c r="I429" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="J429" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="K429">
+        <v>0</v>
+      </c>
+      <c r="L429">
+        <v>0</v>
+      </c>
+      <c r="M429" t="s">
+        <v>278</v>
+      </c>
+      <c r="N429" t="s">
+        <v>569</v>
+      </c>
+      <c r="O429" s="12" t="s">
+        <v>616</v>
+      </c>
+      <c r="P429" s="12" t="s">
+        <v>616</v>
+      </c>
+      <c r="Q429">
+        <v>428</v>
       </c>
     </row>
   </sheetData>
@@ -24925,20 +25183,20 @@
   <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.68359375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>42361</v>
       </c>
@@ -24946,7 +25204,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>42369</v>
       </c>
@@ -24954,7 +25212,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>42371</v>
       </c>
@@ -24962,7 +25220,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>42372</v>
       </c>
@@ -24970,7 +25228,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>42373</v>
       </c>
@@ -24978,7 +25236,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>42382</v>
       </c>
@@ -24986,7 +25244,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>42385</v>
       </c>
@@ -24994,7 +25252,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>42387</v>
       </c>
@@ -25002,7 +25260,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>42388</v>
       </c>
@@ -25010,7 +25268,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>42390</v>
       </c>
@@ -25018,7 +25276,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>42391</v>
       </c>
@@ -25026,7 +25284,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>42400</v>
       </c>
@@ -25034,7 +25292,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>42414</v>
       </c>
@@ -25042,7 +25300,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>42432</v>
       </c>
@@ -25053,7 +25311,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>42435</v>
       </c>
@@ -25061,7 +25319,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>42436</v>
       </c>
@@ -25069,7 +25327,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>42441</v>
       </c>
@@ -25077,7 +25335,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>42445</v>
       </c>
@@ -25085,7 +25343,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>42453</v>
       </c>
@@ -25093,7 +25351,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>42456</v>
       </c>
@@ -25101,7 +25359,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>42457</v>
       </c>
@@ -25109,7 +25367,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>42458</v>
       </c>
@@ -25117,7 +25375,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>42464</v>
       </c>
@@ -25125,7 +25383,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>42510</v>
       </c>
@@ -25133,7 +25391,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>42515</v>
       </c>
@@ -25141,7 +25399,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>42560</v>
       </c>
@@ -25149,7 +25407,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>42565</v>
       </c>
@@ -25157,7 +25415,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>42576</v>
       </c>
@@ -25165,7 +25423,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>42590</v>
       </c>
@@ -25173,7 +25431,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>42593</v>
       </c>
@@ -25181,7 +25439,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>42598</v>
       </c>
@@ -25189,7 +25447,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>42665</v>
       </c>
@@ -25197,7 +25455,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>42788</v>
       </c>
@@ -25205,7 +25463,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>42831</v>
       </c>
@@ -25213,7 +25471,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="13">
         <v>42833</v>
       </c>
@@ -25221,7 +25479,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="13">
         <v>42833</v>
       </c>
@@ -25229,7 +25487,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="13">
         <v>42874</v>
       </c>
@@ -25237,7 +25495,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="13">
         <v>42876</v>
       </c>
@@ -25245,7 +25503,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="13">
         <v>42878</v>
       </c>
@@ -25253,7 +25511,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="13">
         <v>42878</v>
       </c>
@@ -25261,7 +25519,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="13">
         <v>42879</v>
       </c>
@@ -25269,7 +25527,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="13">
         <v>42884</v>
       </c>
@@ -25277,7 +25535,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="13">
         <v>42887</v>
       </c>
@@ -25285,7 +25543,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="13">
         <v>42887</v>
       </c>
@@ -25293,7 +25551,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="13">
         <v>42891</v>
       </c>
@@ -25301,7 +25559,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="13">
         <v>42901</v>
       </c>
@@ -25309,7 +25567,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="13">
         <v>42908</v>
       </c>
@@ -25317,7 +25575,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="13">
         <v>42909</v>
       </c>
@@ -25325,7 +25583,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="13">
         <v>42910</v>
       </c>
@@ -25333,7 +25591,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="13">
         <v>42913</v>
       </c>
@@ -25341,7 +25599,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="13">
         <v>42914</v>
       </c>
@@ -25349,7 +25607,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="13">
         <v>42948</v>
       </c>
@@ -25357,12 +25615,12 @@
         <v>657</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="13">
-        <v>42952</v>
+        <v>42977</v>
       </c>
       <c r="B55" t="s">
-        <v>668</v>
+        <v>658</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Sigma 150mm APO Macro
</commit_message>
<xml_diff>
--- a/BigAssTableOfLenses.xlsx
+++ b/BigAssTableOfLenses.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Markus\Desktop\BATOL\BigAssTableOfLenses\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mbruggeman/Documents/MTFWServer/BigAssTableOfLenses/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8928"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16820"/>
   </bookViews>
   <sheets>
     <sheet name="LensTable" sheetId="1" r:id="rId1"/>
     <sheet name="Changelog" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3245" uniqueCount="669">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3253" uniqueCount="672">
   <si>
     <t>Manufacture</t>
   </si>
@@ -2032,12 +2038,21 @@
   </si>
   <si>
     <t>Removed slashes for old T#'s</t>
+  </si>
+  <si>
+    <t>Added Sigma 150mm APO Macro</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>150mm F2.8 EX DG OS HSM APO Macro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2140,8 +2155,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q425" totalsRowShown="0">
-  <autoFilter ref="A1:Q425"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q426" totalsRowShown="0">
+  <autoFilter ref="A1:Q426"/>
   <sortState ref="A2:Q403">
     <sortCondition ref="Q1:Q403"/>
   </sortState>
@@ -2465,31 +2480,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q425"/>
+  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:Q426"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A411" workbookViewId="0">
+      <selection activeCell="C427" sqref="C427"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.1015625" customWidth="1"/>
-    <col min="2" max="2" width="37.89453125" customWidth="1"/>
-    <col min="3" max="3" width="5.41796875" customWidth="1"/>
-    <col min="4" max="4" width="6.41796875" customWidth="1"/>
-    <col min="5" max="5" width="8.20703125" customWidth="1"/>
-    <col min="7" max="7" width="8.68359375" customWidth="1"/>
-    <col min="8" max="8" width="12.41796875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.1015625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="5.89453125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="10.20703125" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" customWidth="1"/>
+    <col min="2" max="2" width="37.83203125" customWidth="1"/>
+    <col min="3" max="3" width="5.5" customWidth="1"/>
+    <col min="4" max="4" width="6.5" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.1640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="5.83203125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="10.1640625" customWidth="1"/>
     <col min="12" max="12" width="9" customWidth="1"/>
-    <col min="13" max="13" width="11.68359375" customWidth="1"/>
-    <col min="15" max="16" width="8.89453125" style="12"/>
+    <col min="13" max="13" width="11.6640625" customWidth="1"/>
+    <col min="15" max="16" width="8.83203125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2542,7 +2557,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -2597,7 +2612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -2652,7 +2667,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -2707,7 +2722,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -2762,7 +2777,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -2817,7 +2832,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -2872,7 +2887,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -2927,7 +2942,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2982,7 +2997,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -3037,7 +3052,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -3092,7 +3107,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -3147,7 +3162,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -3202,7 +3217,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -3257,7 +3272,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
@@ -3312,7 +3327,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
@@ -3367,7 +3382,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
@@ -3422,7 +3437,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
@@ -3477,7 +3492,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -3532,7 +3547,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
@@ -3587,7 +3602,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
@@ -3642,7 +3657,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
@@ -3697,7 +3712,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
@@ -3752,7 +3767,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
@@ -3807,7 +3822,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
@@ -3862,7 +3877,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
@@ -3917,7 +3932,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
@@ -3972,7 +3987,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>7</v>
       </c>
@@ -4027,7 +4042,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>7</v>
       </c>
@@ -4082,7 +4097,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>7</v>
       </c>
@@ -4137,7 +4152,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>7</v>
       </c>
@@ -4192,7 +4207,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>7</v>
       </c>
@@ -4247,7 +4262,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
@@ -4302,7 +4317,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>7</v>
       </c>
@@ -4357,7 +4372,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>7</v>
       </c>
@@ -4412,7 +4427,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>7</v>
       </c>
@@ -4467,7 +4482,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>7</v>
       </c>
@@ -4522,7 +4537,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -4577,7 +4592,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -4632,7 +4647,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -4687,7 +4702,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>7</v>
       </c>
@@ -4742,7 +4757,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>7</v>
       </c>
@@ -4797,7 +4812,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>7</v>
       </c>
@@ -4852,7 +4867,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -4905,7 +4920,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>7</v>
       </c>
@@ -4960,7 +4975,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>7</v>
       </c>
@@ -5015,7 +5030,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>7</v>
       </c>
@@ -5070,7 +5085,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>7</v>
       </c>
@@ -5125,7 +5140,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>7</v>
       </c>
@@ -5180,7 +5195,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>7</v>
       </c>
@@ -5235,7 +5250,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>7</v>
       </c>
@@ -5290,7 +5305,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -5345,7 +5360,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>7</v>
       </c>
@@ -5400,7 +5415,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>7</v>
       </c>
@@ -5455,7 +5470,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>7</v>
       </c>
@@ -5510,7 +5525,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>7</v>
       </c>
@@ -5565,7 +5580,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>7</v>
       </c>
@@ -5620,7 +5635,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>7</v>
       </c>
@@ -5675,7 +5690,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>7</v>
       </c>
@@ -5730,7 +5745,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>7</v>
       </c>
@@ -5785,7 +5800,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>7</v>
       </c>
@@ -5838,7 +5853,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>7</v>
       </c>
@@ -5893,7 +5908,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>7</v>
       </c>
@@ -5946,7 +5961,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>7</v>
       </c>
@@ -5999,7 +6014,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>7</v>
       </c>
@@ -6052,7 +6067,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>7</v>
       </c>
@@ -6105,7 +6120,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>7</v>
       </c>
@@ -6158,7 +6173,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>370</v>
       </c>
@@ -6211,7 +6226,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>370</v>
       </c>
@@ -6264,7 +6279,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>370</v>
       </c>
@@ -6317,7 +6332,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>370</v>
       </c>
@@ -6370,7 +6385,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>370</v>
       </c>
@@ -6423,7 +6438,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>370</v>
       </c>
@@ -6476,7 +6491,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>370</v>
       </c>
@@ -6529,7 +6544,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>370</v>
       </c>
@@ -6582,7 +6597,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>370</v>
       </c>
@@ -6635,7 +6650,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>370</v>
       </c>
@@ -6688,7 +6703,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>370</v>
       </c>
@@ -6741,7 +6756,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>370</v>
       </c>
@@ -6794,7 +6809,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>370</v>
       </c>
@@ -6847,7 +6862,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>370</v>
       </c>
@@ -6900,7 +6915,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>370</v>
       </c>
@@ -6953,7 +6968,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>370</v>
       </c>
@@ -7006,7 +7021,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>370</v>
       </c>
@@ -7059,7 +7074,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>370</v>
       </c>
@@ -7112,7 +7127,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>370</v>
       </c>
@@ -7165,7 +7180,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>370</v>
       </c>
@@ -7218,7 +7233,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>370</v>
       </c>
@@ -7268,7 +7283,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>287</v>
       </c>
@@ -7321,7 +7336,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>421</v>
       </c>
@@ -7370,7 +7385,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>421</v>
       </c>
@@ -7419,7 +7434,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>227</v>
       </c>
@@ -7472,7 +7487,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>227</v>
       </c>
@@ -7525,7 +7540,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>227</v>
       </c>
@@ -7578,7 +7593,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>227</v>
       </c>
@@ -7631,7 +7646,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>227</v>
       </c>
@@ -7684,7 +7699,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>227</v>
       </c>
@@ -7737,7 +7752,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>227</v>
       </c>
@@ -7792,7 +7807,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>227</v>
       </c>
@@ -7848,7 +7863,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>227</v>
       </c>
@@ -7903,7 +7918,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>227</v>
       </c>
@@ -7956,7 +7971,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>227</v>
       </c>
@@ -8009,7 +8024,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>227</v>
       </c>
@@ -8062,7 +8077,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>227</v>
       </c>
@@ -8115,7 +8130,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>227</v>
       </c>
@@ -8168,7 +8183,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>227</v>
       </c>
@@ -8221,7 +8236,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>227</v>
       </c>
@@ -8277,7 +8292,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>227</v>
       </c>
@@ -8330,7 +8345,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>227</v>
       </c>
@@ -8383,7 +8398,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>227</v>
       </c>
@@ -8436,7 +8451,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>227</v>
       </c>
@@ -8489,7 +8504,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>227</v>
       </c>
@@ -8542,7 +8557,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>227</v>
       </c>
@@ -8595,7 +8610,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>227</v>
       </c>
@@ -8648,7 +8663,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>227</v>
       </c>
@@ -8701,7 +8716,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>227</v>
       </c>
@@ -8757,7 +8772,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>227</v>
       </c>
@@ -8813,7 +8828,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>227</v>
       </c>
@@ -8866,7 +8881,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>227</v>
       </c>
@@ -8919,7 +8934,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>227</v>
       </c>
@@ -8972,7 +8987,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>289</v>
       </c>
@@ -9027,7 +9042,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>289</v>
       </c>
@@ -9082,7 +9097,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>289</v>
       </c>
@@ -9137,7 +9152,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>59</v>
       </c>
@@ -9190,7 +9205,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>59</v>
       </c>
@@ -9243,7 +9258,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>59</v>
       </c>
@@ -9296,7 +9311,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>59</v>
       </c>
@@ -9349,7 +9364,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>59</v>
       </c>
@@ -9402,7 +9417,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>59</v>
       </c>
@@ -9455,7 +9470,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>59</v>
       </c>
@@ -9508,7 +9523,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>59</v>
       </c>
@@ -9561,7 +9576,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>59</v>
       </c>
@@ -9614,7 +9629,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>59</v>
       </c>
@@ -9667,7 +9682,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>59</v>
       </c>
@@ -9720,7 +9735,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>59</v>
       </c>
@@ -9773,7 +9788,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>59</v>
       </c>
@@ -9826,7 +9841,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>59</v>
       </c>
@@ -9879,7 +9894,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>59</v>
       </c>
@@ -9932,7 +9947,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>59</v>
       </c>
@@ -9986,7 +10001,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>59</v>
       </c>
@@ -10039,7 +10054,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>59</v>
       </c>
@@ -10092,7 +10107,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="142" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>59</v>
       </c>
@@ -10145,7 +10160,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>59</v>
       </c>
@@ -10198,7 +10213,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>59</v>
       </c>
@@ -10251,7 +10266,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="145" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>59</v>
       </c>
@@ -10304,7 +10319,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>59</v>
       </c>
@@ -10357,7 +10372,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>59</v>
       </c>
@@ -10410,7 +10425,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>59</v>
       </c>
@@ -10463,7 +10478,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="149" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>59</v>
       </c>
@@ -10516,7 +10531,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>59</v>
       </c>
@@ -10569,7 +10584,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>59</v>
       </c>
@@ -10622,7 +10637,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>59</v>
       </c>
@@ -10675,7 +10690,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="153" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>59</v>
       </c>
@@ -10728,7 +10743,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="154" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>59</v>
       </c>
@@ -10781,7 +10796,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="155" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>59</v>
       </c>
@@ -10834,7 +10849,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>59</v>
       </c>
@@ -10885,7 +10900,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>59</v>
       </c>
@@ -10936,7 +10951,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>59</v>
       </c>
@@ -10987,7 +11002,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>59</v>
       </c>
@@ -11038,7 +11053,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>59</v>
       </c>
@@ -11089,7 +11104,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="161" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>363</v>
       </c>
@@ -11140,7 +11155,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="162" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>363</v>
       </c>
@@ -11191,7 +11206,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="163" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="163" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>363</v>
       </c>
@@ -11242,7 +11257,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="164" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="164" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>430</v>
       </c>
@@ -11293,7 +11308,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="165" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>430</v>
       </c>
@@ -11344,7 +11359,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="166" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="166" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>430</v>
       </c>
@@ -11395,7 +11410,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="167" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="167" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>424</v>
       </c>
@@ -11450,7 +11465,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="168" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="168" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>424</v>
       </c>
@@ -11503,7 +11518,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="169" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="169" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>424</v>
       </c>
@@ -11559,7 +11574,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="170" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="170" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>424</v>
       </c>
@@ -11612,7 +11627,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="171" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="171" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>424</v>
       </c>
@@ -11667,7 +11682,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="172" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="172" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A172" s="12" t="s">
         <v>424</v>
       </c>
@@ -11720,7 +11735,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="173" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="173" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A173" s="12" t="s">
         <v>424</v>
       </c>
@@ -11775,7 +11790,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="174" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="174" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A174" s="12" t="s">
         <v>424</v>
       </c>
@@ -11828,7 +11843,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="175" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="175" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A175" s="12" t="s">
         <v>424</v>
       </c>
@@ -11883,7 +11898,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="176" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="176" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A176" s="12" t="s">
         <v>424</v>
       </c>
@@ -11936,7 +11951,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="177" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A177" s="12" t="s">
         <v>424</v>
       </c>
@@ -11989,7 +12004,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="178" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="178" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A178" s="12" t="s">
         <v>424</v>
       </c>
@@ -12042,7 +12057,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="179" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="179" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>213</v>
       </c>
@@ -12097,7 +12112,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="180" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="180" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>213</v>
       </c>
@@ -12152,7 +12167,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="181" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="181" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>213</v>
       </c>
@@ -12207,7 +12222,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="182" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="182" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>100</v>
       </c>
@@ -12260,7 +12275,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="183" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="183" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>100</v>
       </c>
@@ -12313,7 +12328,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="184" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="184" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>100</v>
       </c>
@@ -12366,7 +12381,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="185" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="185" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>100</v>
       </c>
@@ -12419,7 +12434,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="186" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="186" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>100</v>
       </c>
@@ -12472,7 +12487,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="187" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="187" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>100</v>
       </c>
@@ -12525,7 +12540,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="188" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="188" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>100</v>
       </c>
@@ -12578,7 +12593,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="189" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="189" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>100</v>
       </c>
@@ -12631,7 +12646,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="190" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="190" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>100</v>
       </c>
@@ -12684,7 +12699,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="191" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="191" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>100</v>
       </c>
@@ -12737,7 +12752,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="192" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="192" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>100</v>
       </c>
@@ -12790,7 +12805,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="193" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="193" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>100</v>
       </c>
@@ -12841,7 +12856,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="194" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="194" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>100</v>
       </c>
@@ -12892,7 +12907,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="195" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="195" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>100</v>
       </c>
@@ -12940,7 +12955,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="196" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="196" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>100</v>
       </c>
@@ -12991,7 +13006,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="197" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="197" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>100</v>
       </c>
@@ -13042,7 +13057,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="198" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="198" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>100</v>
       </c>
@@ -13093,7 +13108,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="199" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="199" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>166</v>
       </c>
@@ -13146,7 +13161,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="200" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="200" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>166</v>
       </c>
@@ -13199,7 +13214,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="201" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="201" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>166</v>
       </c>
@@ -13252,7 +13267,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="202" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="202" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>166</v>
       </c>
@@ -13305,7 +13320,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="203" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="203" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>166</v>
       </c>
@@ -13358,7 +13373,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="204" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="204" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>166</v>
       </c>
@@ -13411,7 +13426,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="205" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="205" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>166</v>
       </c>
@@ -13465,7 +13480,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="206" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="206" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>166</v>
       </c>
@@ -13518,7 +13533,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="207" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="207" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>166</v>
       </c>
@@ -13571,7 +13586,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="208" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="208" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>166</v>
       </c>
@@ -13624,7 +13639,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="209" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="209" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>166</v>
       </c>
@@ -13677,7 +13692,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="210" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="210" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>166</v>
       </c>
@@ -13730,7 +13745,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="211" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="211" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>166</v>
       </c>
@@ -13783,7 +13798,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="212" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="212" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>166</v>
       </c>
@@ -13836,7 +13851,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="213" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="213" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>166</v>
       </c>
@@ -13889,7 +13904,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="214" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="214" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>166</v>
       </c>
@@ -13940,7 +13955,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="215" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="215" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>182</v>
       </c>
@@ -13993,7 +14008,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="216" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="216" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>182</v>
       </c>
@@ -14046,7 +14061,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="217" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="217" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>182</v>
       </c>
@@ -14099,7 +14114,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="218" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="218" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>182</v>
       </c>
@@ -14152,7 +14167,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="219" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="219" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>182</v>
       </c>
@@ -14205,7 +14220,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="220" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="220" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>182</v>
       </c>
@@ -14258,7 +14273,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="221" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="221" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>182</v>
       </c>
@@ -14311,7 +14326,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="222" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="222" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>182</v>
       </c>
@@ -14364,7 +14379,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="223" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="223" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>182</v>
       </c>
@@ -14417,7 +14432,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="224" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="224" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>182</v>
       </c>
@@ -14468,7 +14483,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="225" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="225" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
         <v>182</v>
       </c>
@@ -14519,7 +14534,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="226" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="226" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
         <v>182</v>
       </c>
@@ -14570,7 +14585,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="227" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="227" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>191</v>
       </c>
@@ -14623,7 +14638,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="228" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="228" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>191</v>
       </c>
@@ -14676,7 +14691,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="229" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="229" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>191</v>
       </c>
@@ -14729,7 +14744,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="230" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="230" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>191</v>
       </c>
@@ -14782,7 +14797,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="231" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="231" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>191</v>
       </c>
@@ -14835,7 +14850,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="232" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="232" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>191</v>
       </c>
@@ -14886,7 +14901,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="233" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="233" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>258</v>
       </c>
@@ -14939,7 +14954,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="234" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="234" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
         <v>258</v>
       </c>
@@ -14992,7 +15007,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="235" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="235" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
         <v>258</v>
       </c>
@@ -15045,7 +15060,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="236" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="236" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A236" s="1" t="s">
         <v>258</v>
       </c>
@@ -15098,7 +15113,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="237" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="237" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A237" s="1" t="s">
         <v>215</v>
       </c>
@@ -15149,7 +15164,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="238" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="238" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
         <v>215</v>
       </c>
@@ -15198,7 +15213,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="239" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="239" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
         <v>215</v>
       </c>
@@ -15247,7 +15262,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="240" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="240" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A240" s="1" t="s">
         <v>215</v>
       </c>
@@ -15298,7 +15313,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="241" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="241" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A241" s="1" t="s">
         <v>215</v>
       </c>
@@ -15347,7 +15362,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="242" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="242" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A242" s="1" t="s">
         <v>215</v>
       </c>
@@ -15396,7 +15411,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="243" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="243" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A243" s="1" t="s">
         <v>215</v>
       </c>
@@ -15445,7 +15460,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="244" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="244" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A244" s="1" t="s">
         <v>215</v>
       </c>
@@ -15496,7 +15511,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="245" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="245" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A245" s="1" t="s">
         <v>215</v>
       </c>
@@ -15545,7 +15560,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="246" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="246" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A246" s="1" t="s">
         <v>215</v>
       </c>
@@ -15594,7 +15609,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="247" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="247" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>215</v>
       </c>
@@ -15643,7 +15658,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="248" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="248" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>215</v>
       </c>
@@ -15692,7 +15707,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="249" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="249" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>215</v>
       </c>
@@ -15741,7 +15756,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="250" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="250" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>215</v>
       </c>
@@ -15792,7 +15807,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="251" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="251" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>215</v>
       </c>
@@ -15841,7 +15856,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="252" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="252" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A252" s="1" t="s">
         <v>215</v>
       </c>
@@ -15890,7 +15905,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="253" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="253" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A253" s="1" t="s">
         <v>215</v>
       </c>
@@ -15939,7 +15954,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="254" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="254" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>132</v>
       </c>
@@ -15994,7 +16009,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="255" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="255" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>132</v>
       </c>
@@ -16047,7 +16062,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="256" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="256" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>132</v>
       </c>
@@ -16100,7 +16115,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="257" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="257" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>132</v>
       </c>
@@ -16155,7 +16170,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="258" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="258" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>132</v>
       </c>
@@ -16208,7 +16223,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="259" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="259" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>132</v>
       </c>
@@ -16261,7 +16276,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="260" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="260" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>132</v>
       </c>
@@ -16316,7 +16331,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="261" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="261" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>132</v>
       </c>
@@ -16371,7 +16386,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="262" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="262" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>132</v>
       </c>
@@ -16426,7 +16441,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="263" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="263" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>132</v>
       </c>
@@ -16479,7 +16494,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="264" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="264" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>132</v>
       </c>
@@ -16532,7 +16547,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="265" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="265" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>132</v>
       </c>
@@ -16585,7 +16600,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="266" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="266" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>132</v>
       </c>
@@ -16640,7 +16655,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="267" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="267" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>132</v>
       </c>
@@ -16695,7 +16710,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="268" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="268" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A268" s="1" t="s">
         <v>132</v>
       </c>
@@ -16750,7 +16765,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="269" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="269" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A269" s="1" t="s">
         <v>132</v>
       </c>
@@ -16803,7 +16818,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="270" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="270" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>132</v>
       </c>
@@ -16856,7 +16871,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="271" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="271" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>132</v>
       </c>
@@ -16911,7 +16926,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="272" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="272" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>132</v>
       </c>
@@ -16966,7 +16981,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="273" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="273" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>132</v>
       </c>
@@ -17019,7 +17034,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="274" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="274" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>132</v>
       </c>
@@ -17072,7 +17087,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="275" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="275" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>132</v>
       </c>
@@ -17127,7 +17142,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="276" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="276" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>132</v>
       </c>
@@ -17182,7 +17197,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="277" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="277" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>132</v>
       </c>
@@ -17237,7 +17252,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="278" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="278" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>132</v>
       </c>
@@ -17292,7 +17307,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="279" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="279" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>132</v>
       </c>
@@ -17345,7 +17360,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="280" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="280" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>132</v>
       </c>
@@ -17398,7 +17413,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="281" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="281" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>132</v>
       </c>
@@ -17451,7 +17466,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="282" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="282" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>132</v>
       </c>
@@ -17504,7 +17519,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="283" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="283" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>132</v>
       </c>
@@ -17557,7 +17572,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="284" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="284" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>132</v>
       </c>
@@ -17612,7 +17627,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="285" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="285" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>132</v>
       </c>
@@ -17667,7 +17682,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="286" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="286" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>132</v>
       </c>
@@ -17722,7 +17737,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="287" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="287" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>132</v>
       </c>
@@ -17777,7 +17792,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="288" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="288" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>132</v>
       </c>
@@ -17832,7 +17847,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="289" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="289" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>132</v>
       </c>
@@ -17885,7 +17900,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="290" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="290" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>132</v>
       </c>
@@ -17938,7 +17953,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="291" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="291" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>132</v>
       </c>
@@ -17991,7 +18006,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="292" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="292" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>132</v>
       </c>
@@ -18044,7 +18059,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="293" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="293" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>132</v>
       </c>
@@ -18097,7 +18112,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="294" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="294" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>132</v>
       </c>
@@ -18152,7 +18167,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="295" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="295" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>132</v>
       </c>
@@ -18207,7 +18222,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="296" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="296" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>132</v>
       </c>
@@ -18262,7 +18277,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="297" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="297" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>132</v>
       </c>
@@ -18317,7 +18332,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="298" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="298" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>132</v>
       </c>
@@ -18372,7 +18387,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="299" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="299" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>132</v>
       </c>
@@ -18425,7 +18440,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="300" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="300" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>132</v>
       </c>
@@ -18478,7 +18493,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="301" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="301" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>132</v>
       </c>
@@ -18531,7 +18546,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="302" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="302" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>132</v>
       </c>
@@ -18586,7 +18601,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="303" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="303" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>132</v>
       </c>
@@ -18641,7 +18656,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="304" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="304" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>132</v>
       </c>
@@ -18694,7 +18709,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="305" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="305" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>132</v>
       </c>
@@ -18749,7 +18764,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="306" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="306" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>132</v>
       </c>
@@ -18802,7 +18817,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="307" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="307" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>132</v>
       </c>
@@ -18855,7 +18870,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="308" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="308" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>132</v>
       </c>
@@ -18908,7 +18923,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="309" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="309" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>132</v>
       </c>
@@ -18961,7 +18976,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="310" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="310" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>132</v>
       </c>
@@ -19014,7 +19029,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="311" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="311" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>132</v>
       </c>
@@ -19067,7 +19082,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="312" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="312" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>132</v>
       </c>
@@ -19120,7 +19135,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="313" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="313" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>132</v>
       </c>
@@ -19173,7 +19188,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="314" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="314" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>132</v>
       </c>
@@ -19226,7 +19241,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="315" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="315" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>370</v>
       </c>
@@ -19279,7 +19294,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="316" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="316" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>370</v>
       </c>
@@ -19332,7 +19347,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="317" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="317" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>100</v>
       </c>
@@ -19383,7 +19398,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="318" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="318" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>100</v>
       </c>
@@ -19434,7 +19449,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="319" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="319" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>100</v>
       </c>
@@ -19483,7 +19498,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="320" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="320" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>100</v>
       </c>
@@ -19534,7 +19549,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="321" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="321" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>7</v>
       </c>
@@ -19587,7 +19602,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="322" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="322" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>213</v>
       </c>
@@ -19638,7 +19653,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="323" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="323" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>213</v>
       </c>
@@ -19689,7 +19704,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="324" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="324" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>213</v>
       </c>
@@ -19740,7 +19755,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="325" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="325" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>100</v>
       </c>
@@ -19789,7 +19804,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="326" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="326" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>191</v>
       </c>
@@ -19840,7 +19855,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="327" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="327" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>7</v>
       </c>
@@ -19889,7 +19904,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="328" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="328" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>7</v>
       </c>
@@ -19942,7 +19957,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="329" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="329" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>7</v>
       </c>
@@ -19995,7 +20010,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="330" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="330" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>7</v>
       </c>
@@ -20048,7 +20063,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="331" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="331" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>7</v>
       </c>
@@ -20101,7 +20116,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="332" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="332" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
         <v>213</v>
       </c>
@@ -20152,7 +20167,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="333" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="333" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
         <v>213</v>
       </c>
@@ -20203,7 +20218,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="334" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="334" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
         <v>213</v>
       </c>
@@ -20254,7 +20269,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="335" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="335" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
         <v>213</v>
       </c>
@@ -20305,7 +20320,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="336" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="336" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
         <v>213</v>
       </c>
@@ -20356,7 +20371,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="337" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="337" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
         <v>213</v>
       </c>
@@ -20407,7 +20422,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="338" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="338" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
         <v>494</v>
       </c>
@@ -20460,7 +20475,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="339" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="339" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
         <v>494</v>
       </c>
@@ -20511,7 +20526,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="340" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="340" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
         <v>494</v>
       </c>
@@ -20562,7 +20577,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="341" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="341" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
         <v>494</v>
       </c>
@@ -20613,7 +20628,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="342" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="342" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
         <v>494</v>
       </c>
@@ -20664,7 +20679,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="343" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="343" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
         <v>494</v>
       </c>
@@ -20715,7 +20730,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="344" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="344" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
         <v>494</v>
       </c>
@@ -20766,7 +20781,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="345" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="345" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
         <v>494</v>
       </c>
@@ -20817,7 +20832,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="346" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="346" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
         <v>494</v>
       </c>
@@ -20868,7 +20883,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="347" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="347" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
         <v>494</v>
       </c>
@@ -20919,7 +20934,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="348" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="348" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
         <v>494</v>
       </c>
@@ -20970,7 +20985,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="349" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="349" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
         <v>494</v>
       </c>
@@ -21021,7 +21036,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="350" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="350" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
         <v>494</v>
       </c>
@@ -21072,7 +21087,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="351" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="351" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
         <v>494</v>
       </c>
@@ -21123,7 +21138,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="352" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="352" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
         <v>494</v>
       </c>
@@ -21174,7 +21189,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="353" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="353" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
         <v>494</v>
       </c>
@@ -21225,7 +21240,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="354" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="354" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
         <v>494</v>
       </c>
@@ -21276,7 +21291,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="355" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="355" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
         <v>370</v>
       </c>
@@ -21329,7 +21344,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="356" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="356" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
         <v>370</v>
       </c>
@@ -21382,7 +21397,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="357" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="357" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
         <v>370</v>
       </c>
@@ -21435,7 +21450,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="358" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="358" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
         <v>370</v>
       </c>
@@ -21488,7 +21503,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="359" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="359" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
         <v>370</v>
       </c>
@@ -21541,7 +21556,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="360" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="360" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
         <v>370</v>
       </c>
@@ -21594,7 +21609,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="361" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="361" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
         <v>370</v>
       </c>
@@ -21647,7 +21662,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="362" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="362" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
         <v>370</v>
       </c>
@@ -21700,7 +21715,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="363" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="363" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
         <v>370</v>
       </c>
@@ -21753,7 +21768,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="364" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="364" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
         <v>100</v>
       </c>
@@ -21804,7 +21819,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="365" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="365" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
         <v>100</v>
       </c>
@@ -21855,7 +21870,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="366" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="366" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A366" t="s">
         <v>100</v>
       </c>
@@ -21906,7 +21921,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="367" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="367" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
         <v>100</v>
       </c>
@@ -21957,7 +21972,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="368" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="368" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A368" t="s">
         <v>100</v>
       </c>
@@ -22008,7 +22023,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="369" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="369" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A369" t="s">
         <v>100</v>
       </c>
@@ -22059,7 +22074,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="370" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="370" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A370" t="s">
         <v>100</v>
       </c>
@@ -22110,7 +22125,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="371" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="371" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A371" t="s">
         <v>100</v>
       </c>
@@ -22161,7 +22176,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="372" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="372" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A372" t="s">
         <v>191</v>
       </c>
@@ -22212,7 +22227,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="373" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="373" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A373" t="s">
         <v>191</v>
       </c>
@@ -22263,7 +22278,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="374" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="374" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A374" t="s">
         <v>191</v>
       </c>
@@ -22314,7 +22329,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="375" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="375" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A375" t="s">
         <v>191</v>
       </c>
@@ -22365,7 +22380,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="376" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="376" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
         <v>191</v>
       </c>
@@ -22414,7 +22429,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="377" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="377" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A377" t="s">
         <v>191</v>
       </c>
@@ -22465,7 +22480,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="378" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="378" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A378" t="s">
         <v>191</v>
       </c>
@@ -22516,7 +22531,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="379" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="379" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A379" t="s">
         <v>132</v>
       </c>
@@ -22569,7 +22584,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="380" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="380" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A380" t="s">
         <v>7</v>
       </c>
@@ -22622,7 +22637,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="381" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="381" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A381" t="s">
         <v>424</v>
       </c>
@@ -22675,7 +22690,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="382" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="382" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A382" t="s">
         <v>424</v>
       </c>
@@ -22728,7 +22743,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="383" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="383" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A383" t="s">
         <v>424</v>
       </c>
@@ -22781,7 +22796,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="384" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="384" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A384" t="s">
         <v>424</v>
       </c>
@@ -22834,7 +22849,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="385" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="385" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A385" s="7" t="s">
         <v>182</v>
       </c>
@@ -22885,7 +22900,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="386" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="386" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A386" s="7" t="s">
         <v>132</v>
       </c>
@@ -22938,7 +22953,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="387" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="387" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A387" s="7" t="s">
         <v>166</v>
       </c>
@@ -22989,7 +23004,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="388" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="388" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A388" s="7" t="s">
         <v>166</v>
       </c>
@@ -23040,7 +23055,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="389" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="389" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A389" s="7" t="s">
         <v>166</v>
       </c>
@@ -23091,7 +23106,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="390" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="390" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A390" s="7" t="s">
         <v>258</v>
       </c>
@@ -23142,7 +23157,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="391" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="391" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A391" s="7" t="s">
         <v>258</v>
       </c>
@@ -23195,7 +23210,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="392" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="392" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A392" s="7" t="s">
         <v>370</v>
       </c>
@@ -23248,7 +23263,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="393" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="393" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A393" s="7" t="s">
         <v>370</v>
       </c>
@@ -23301,7 +23316,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="394" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="394" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A394" s="7" t="s">
         <v>370</v>
       </c>
@@ -23354,7 +23369,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="395" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="395" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A395" s="7" t="s">
         <v>370</v>
       </c>
@@ -23399,7 +23414,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="396" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="396" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A396" s="7" t="s">
         <v>593</v>
       </c>
@@ -23448,7 +23463,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="397" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="397" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A397" s="7" t="s">
         <v>593</v>
       </c>
@@ -23497,7 +23512,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="398" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="398" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A398" t="s">
         <v>604</v>
       </c>
@@ -23550,7 +23565,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="399" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="399" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A399" t="s">
         <v>604</v>
       </c>
@@ -23599,7 +23614,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="400" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="400" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A400" t="s">
         <v>59</v>
       </c>
@@ -23650,7 +23665,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="401" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="401" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A401" t="s">
         <v>59</v>
       </c>
@@ -23701,7 +23716,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="402" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="402" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A402" t="s">
         <v>59</v>
       </c>
@@ -23752,7 +23767,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="403" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="403" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A403" t="s">
         <v>166</v>
       </c>
@@ -23803,7 +23818,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="404" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="404" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A404" t="s">
         <v>182</v>
       </c>
@@ -23854,7 +23869,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="405" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="405" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A405" t="s">
         <v>182</v>
       </c>
@@ -23907,7 +23922,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="406" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="406" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A406" t="s">
         <v>632</v>
       </c>
@@ -23956,7 +23971,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="407" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="407" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A407" s="12" t="s">
         <v>132</v>
       </c>
@@ -24009,7 +24024,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="408" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="408" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A408" s="12" t="s">
         <v>132</v>
       </c>
@@ -24062,7 +24077,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="409" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="409" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A409" s="12" t="s">
         <v>132</v>
       </c>
@@ -24115,7 +24130,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="410" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="410" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A410" s="12" t="s">
         <v>132</v>
       </c>
@@ -24168,7 +24183,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="411" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="411" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A411" s="12" t="s">
         <v>132</v>
       </c>
@@ -24221,7 +24236,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="412" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="412" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A412" s="12" t="s">
         <v>132</v>
       </c>
@@ -24274,7 +24289,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="413" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="413" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A413" s="12" t="s">
         <v>132</v>
       </c>
@@ -24327,7 +24342,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="414" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="414" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A414" s="12" t="s">
         <v>132</v>
       </c>
@@ -24380,7 +24395,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="415" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="415" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A415" s="12" t="s">
         <v>132</v>
       </c>
@@ -24433,7 +24448,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="416" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="416" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A416" s="12" t="s">
         <v>370</v>
       </c>
@@ -24484,7 +24499,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="417" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="417" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A417" t="s">
         <v>370</v>
       </c>
@@ -24535,7 +24550,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="418" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="418" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A418" t="s">
         <v>132</v>
       </c>
@@ -24588,7 +24603,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="419" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="419" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A419" t="s">
         <v>649</v>
       </c>
@@ -24637,7 +24652,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="420" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="420" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A420" t="s">
         <v>649</v>
       </c>
@@ -24683,7 +24698,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="421" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="421" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A421" s="12" t="s">
         <v>649</v>
       </c>
@@ -24727,7 +24742,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="422" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="422" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A422" t="s">
         <v>649</v>
       </c>
@@ -24773,7 +24788,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="423" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="423" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A423" t="s">
         <v>649</v>
       </c>
@@ -24819,7 +24834,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="424" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="424" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A424" t="s">
         <v>649</v>
       </c>
@@ -24865,7 +24880,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="425" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="425" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A425" t="s">
         <v>649</v>
       </c>
@@ -24909,6 +24924,57 @@
       <c r="P425" s="10"/>
       <c r="Q425">
         <v>424</v>
+      </c>
+    </row>
+    <row r="426" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A426" t="s">
+        <v>100</v>
+      </c>
+      <c r="B426" t="s">
+        <v>671</v>
+      </c>
+      <c r="C426">
+        <v>2012</v>
+      </c>
+      <c r="D426">
+        <v>1099</v>
+      </c>
+      <c r="E426">
+        <v>1150</v>
+      </c>
+      <c r="F426">
+        <v>150</v>
+      </c>
+      <c r="G426" s="8">
+        <v>79.599999999999994</v>
+      </c>
+      <c r="H426" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="I426" s="9" t="s">
+        <v>670</v>
+      </c>
+      <c r="J426" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="K426">
+        <v>1</v>
+      </c>
+      <c r="L426">
+        <v>0</v>
+      </c>
+      <c r="M426" t="s">
+        <v>278</v>
+      </c>
+      <c r="N426" t="s">
+        <v>572</v>
+      </c>
+      <c r="O426" s="12" t="s">
+        <v>616</v>
+      </c>
+      <c r="P426" s="10"/>
+      <c r="Q426">
+        <v>425</v>
       </c>
     </row>
   </sheetData>
@@ -24922,23 +24988,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.68359375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>42361</v>
       </c>
@@ -24946,7 +25012,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>42369</v>
       </c>
@@ -24954,7 +25020,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>42371</v>
       </c>
@@ -24962,7 +25028,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>42372</v>
       </c>
@@ -24970,7 +25036,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>42373</v>
       </c>
@@ -24978,7 +25044,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>42382</v>
       </c>
@@ -24986,7 +25052,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>42385</v>
       </c>
@@ -24994,7 +25060,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>42387</v>
       </c>
@@ -25002,7 +25068,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>42388</v>
       </c>
@@ -25010,7 +25076,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>42390</v>
       </c>
@@ -25018,7 +25084,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>42391</v>
       </c>
@@ -25026,7 +25092,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>42400</v>
       </c>
@@ -25034,7 +25100,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>42414</v>
       </c>
@@ -25042,7 +25108,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>42432</v>
       </c>
@@ -25053,7 +25119,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>42435</v>
       </c>
@@ -25061,7 +25127,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>42436</v>
       </c>
@@ -25069,7 +25135,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>42441</v>
       </c>
@@ -25077,7 +25143,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>42445</v>
       </c>
@@ -25085,7 +25151,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>42453</v>
       </c>
@@ -25093,7 +25159,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>42456</v>
       </c>
@@ -25101,7 +25167,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>42457</v>
       </c>
@@ -25109,7 +25175,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>42458</v>
       </c>
@@ -25117,7 +25183,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>42464</v>
       </c>
@@ -25125,7 +25191,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>42510</v>
       </c>
@@ -25133,7 +25199,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>42515</v>
       </c>
@@ -25141,7 +25207,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>42560</v>
       </c>
@@ -25149,7 +25215,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>42565</v>
       </c>
@@ -25157,7 +25223,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>42576</v>
       </c>
@@ -25165,7 +25231,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>42590</v>
       </c>
@@ -25173,7 +25239,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>42593</v>
       </c>
@@ -25181,7 +25247,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>42598</v>
       </c>
@@ -25189,7 +25255,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>42665</v>
       </c>
@@ -25197,7 +25263,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>42788</v>
       </c>
@@ -25205,7 +25271,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>42831</v>
       </c>
@@ -25213,7 +25279,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="13">
         <v>42833</v>
       </c>
@@ -25221,7 +25287,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="13">
         <v>42833</v>
       </c>
@@ -25229,7 +25295,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="13">
         <v>42874</v>
       </c>
@@ -25237,7 +25303,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="13">
         <v>42876</v>
       </c>
@@ -25245,7 +25311,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="13">
         <v>42878</v>
       </c>
@@ -25253,7 +25319,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="13">
         <v>42878</v>
       </c>
@@ -25261,7 +25327,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="13">
         <v>42879</v>
       </c>
@@ -25269,7 +25335,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="13">
         <v>42884</v>
       </c>
@@ -25277,7 +25343,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="13">
         <v>42887</v>
       </c>
@@ -25285,7 +25351,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="13">
         <v>42887</v>
       </c>
@@ -25293,7 +25359,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="13">
         <v>42891</v>
       </c>
@@ -25301,7 +25367,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="13">
         <v>42901</v>
       </c>
@@ -25309,7 +25375,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="13">
         <v>42908</v>
       </c>
@@ -25317,7 +25383,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="13">
         <v>42909</v>
       </c>
@@ -25325,7 +25391,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="13">
         <v>42910</v>
       </c>
@@ -25333,7 +25399,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="13">
         <v>42913</v>
       </c>
@@ -25341,7 +25407,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="13">
         <v>42914</v>
       </c>
@@ -25349,7 +25415,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="13">
         <v>42948</v>
       </c>
@@ -25357,12 +25423,20 @@
         <v>657</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="13">
         <v>42952</v>
       </c>
       <c r="B55" t="s">
         <v>668</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="13">
+        <v>42992</v>
+      </c>
+      <c r="B56" t="s">
+        <v>669</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
+ Sony FE 24-105
</commit_message>
<xml_diff>
--- a/BigAssTableOfLenses.xlsx
+++ b/BigAssTableOfLenses.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="444" windowWidth="23400" windowHeight="12780" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="444" windowWidth="23400" windowHeight="12780"/>
   </bookViews>
   <sheets>
     <sheet name="LensTable" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3331" uniqueCount="683">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3339" uniqueCount="685">
   <si>
     <t>Manufacture</t>
   </si>
@@ -2080,6 +2080,12 @@
   </si>
   <si>
     <t>Added Voigtlander 65mm, 40mm FE.  Added Zeiss 25/1.4.  Some sigma metadata.</t>
+  </si>
+  <si>
+    <t>Add Sony 24-105 G</t>
+  </si>
+  <si>
+    <t>FE 24-105 f/4G OSS</t>
   </si>
 </sst>
 </file>
@@ -2218,8 +2224,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q433" totalsRowShown="0">
-  <autoFilter ref="A1:Q433"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q434" totalsRowShown="0">
+  <autoFilter ref="A1:Q434"/>
   <tableColumns count="17">
     <tableColumn id="15" name="UUID"/>
     <tableColumn id="1" name="Manufacture"/>
@@ -2541,10 +2547,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q433"/>
+  <dimension ref="A1:Q434"/>
   <sheetViews>
-    <sheetView topLeftCell="A313" workbookViewId="0">
-      <selection activeCell="Q317" sqref="Q317:Q320"/>
+    <sheetView tabSelected="1" topLeftCell="A423" workbookViewId="0">
+      <selection activeCell="J441" sqref="J441"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25454,6 +25460,57 @@
         <v>610</v>
       </c>
     </row>
+    <row r="434" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A434">
+        <v>433</v>
+      </c>
+      <c r="B434" t="s">
+        <v>165</v>
+      </c>
+      <c r="C434" t="s">
+        <v>684</v>
+      </c>
+      <c r="D434">
+        <v>2017</v>
+      </c>
+      <c r="E434">
+        <v>1298</v>
+      </c>
+      <c r="F434">
+        <v>633</v>
+      </c>
+      <c r="G434">
+        <v>113</v>
+      </c>
+      <c r="H434" s="7">
+        <v>83</v>
+      </c>
+      <c r="I434" s="1">
+        <v>4</v>
+      </c>
+      <c r="J434" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="K434" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="L434">
+        <v>1</v>
+      </c>
+      <c r="M434">
+        <v>0</v>
+      </c>
+      <c r="N434" t="s">
+        <v>276</v>
+      </c>
+      <c r="O434" t="s">
+        <v>565</v>
+      </c>
+      <c r="P434" s="11" t="s">
+        <v>610</v>
+      </c>
+      <c r="Q434" s="9"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576">
@@ -25470,10 +25527,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25945,6 +26002,14 @@
         <v>682</v>
       </c>
     </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="12">
+        <v>43033</v>
+      </c>
+      <c r="B60" t="s">
+        <v>683</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
+ Panasonic/Olympus Micor 4/3
TODO: fill in some misc. info about country/type of lens
</commit_message>
<xml_diff>
--- a/BigAssTableOfLenses.xlsx
+++ b/BigAssTableOfLenses.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brand\Optics\Olaf\Software\BigAssTableOfLenses\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marro\OneDrive\Documents\GitHub\BigAssTableOfLenses\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="137" documentId="83107282411FEE9CA17C5171E68B1AD52C83904E" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{6B14FC8F-0042-45D1-9212-08D75F7784CF}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="444" windowWidth="23400" windowHeight="12780"/>
+    <workbookView xWindow="0" yWindow="444" windowWidth="23400" windowHeight="12780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LensTable" sheetId="1" r:id="rId1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3347" uniqueCount="688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3393" uniqueCount="699">
   <si>
     <t>Manufacture</t>
   </si>
@@ -2095,12 +2096,45 @@
   </si>
   <si>
     <t>Add Panasonic 200/2.8</t>
+  </si>
+  <si>
+    <t>M.Zuiko Digital 25mm f/1.8</t>
+  </si>
+  <si>
+    <t>M.Zuiko Digital ED 17mm f/1.2 PRO</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>M.Zuiko Digital ED 75mm f/1.8</t>
+  </si>
+  <si>
+    <t>M.Zuiko Digital ED 45mm f/1.2 PRO</t>
+  </si>
+  <si>
+    <t>M.Zuiko Digital 45mm f/1.8</t>
+  </si>
+  <si>
+    <t>M.Zuiko Digital 17mm f/1.8</t>
+  </si>
+  <si>
+    <t>Leica DG Summilux 25mm f/1.4 ASPH</t>
+  </si>
+  <si>
+    <t>Leica DG Summilux 12mm f/1.4 ASPH</t>
+  </si>
+  <si>
+    <t>Leica DG Nocticron 42.5mm f/1.2 ASPH POWER OIS</t>
+  </si>
+  <si>
+    <t>Added Micro 4/3 Panasonic Summilux  25, 12 mm; Nocticron 42.5mm, Olympus M.Zuiko 17/45mm f/1.2 &amp; f1.8; 25mm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2233,26 +2267,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q435" totalsRowShown="0">
-  <autoFilter ref="A1:Q435"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:Q444" totalsRowShown="0">
+  <autoFilter ref="A1:Q444" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="17">
-    <tableColumn id="15" name="UUID"/>
-    <tableColumn id="1" name="Manufacture"/>
-    <tableColumn id="2" name="Model"/>
-    <tableColumn id="3" name="Release Year"/>
-    <tableColumn id="4" name="MSRP"/>
-    <tableColumn id="5" name="Weight"/>
-    <tableColumn id="6" name="Length"/>
-    <tableColumn id="7" name="Max Diameter" dataDxfId="2"/>
-    <tableColumn id="10" name="Max Aperture"/>
-    <tableColumn id="12" name="EFL" dataDxfId="1"/>
-    <tableColumn id="11" name="Zoom" dataDxfId="0"/>
-    <tableColumn id="8" name="Stabilized"/>
-    <tableColumn id="9" name="Cinema"/>
-    <tableColumn id="13" name="Format"/>
-    <tableColumn id="14" name="Variety"/>
-    <tableColumn id="17" name="Designed In"/>
-    <tableColumn id="16" name="Made In"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="UUID"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Manufacture"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Model"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Release Year"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="MSRP"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Weight"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Length"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Max Diameter" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Max Aperture"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="EFL" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Zoom" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Stabilized"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Cinema"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Format"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Variety"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Designed In"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Made In"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2554,21 +2588,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q435"/>
+  <dimension ref="A1:Q444"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A418" workbookViewId="0">
-      <selection activeCell="C435" sqref="C435"/>
+    <sheetView tabSelected="1" topLeftCell="A425" workbookViewId="0">
+      <selection activeCell="C448" sqref="C448"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="8.109375" customWidth="1"/>
-    <col min="3" max="3" width="37.77734375" customWidth="1"/>
+    <col min="3" max="3" width="49.5546875" customWidth="1"/>
     <col min="4" max="4" width="5.44140625" customWidth="1"/>
     <col min="5" max="5" width="6.44140625" customWidth="1"/>
-    <col min="6" max="6" width="8.109375" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" customWidth="1"/>
     <col min="8" max="8" width="8.6640625" customWidth="1"/>
     <col min="9" max="9" width="12.44140625" style="1" customWidth="1"/>
     <col min="10" max="10" width="6.109375" style="3" customWidth="1"/>
@@ -25571,9 +25605,405 @@
       </c>
       <c r="Q435" s="9"/>
     </row>
+    <row r="436" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A436">
+        <v>435</v>
+      </c>
+      <c r="B436" t="s">
+        <v>426</v>
+      </c>
+      <c r="C436" t="s">
+        <v>688</v>
+      </c>
+      <c r="D436">
+        <v>2014</v>
+      </c>
+      <c r="E436">
+        <v>249</v>
+      </c>
+      <c r="F436">
+        <v>136</v>
+      </c>
+      <c r="G436">
+        <v>40.6</v>
+      </c>
+      <c r="H436" s="7">
+        <v>56</v>
+      </c>
+      <c r="I436" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="J436" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="K436" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L436">
+        <v>0</v>
+      </c>
+      <c r="M436">
+        <v>0</v>
+      </c>
+      <c r="N436" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="437" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A437">
+        <v>436</v>
+      </c>
+      <c r="B437" t="s">
+        <v>426</v>
+      </c>
+      <c r="C437" t="s">
+        <v>689</v>
+      </c>
+      <c r="D437">
+        <v>2018</v>
+      </c>
+      <c r="E437">
+        <v>1199</v>
+      </c>
+      <c r="F437">
+        <v>390</v>
+      </c>
+      <c r="G437">
+        <v>87</v>
+      </c>
+      <c r="H437" s="7">
+        <v>68.2</v>
+      </c>
+      <c r="I437" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="J437" s="8" t="s">
+        <v>690</v>
+      </c>
+      <c r="K437" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L437">
+        <v>0</v>
+      </c>
+      <c r="M437">
+        <v>0</v>
+      </c>
+      <c r="N437" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="438" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A438">
+        <v>437</v>
+      </c>
+      <c r="B438" t="s">
+        <v>426</v>
+      </c>
+      <c r="C438" t="s">
+        <v>691</v>
+      </c>
+      <c r="D438">
+        <v>2012</v>
+      </c>
+      <c r="E438">
+        <v>749</v>
+      </c>
+      <c r="F438">
+        <v>305</v>
+      </c>
+      <c r="G438">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="H438" s="7">
+        <v>64</v>
+      </c>
+      <c r="I438" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="J438" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="K438" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L438">
+        <v>0</v>
+      </c>
+      <c r="M438">
+        <v>0</v>
+      </c>
+      <c r="N438" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="439" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A439">
+        <v>438</v>
+      </c>
+      <c r="B439" t="s">
+        <v>426</v>
+      </c>
+      <c r="C439" t="s">
+        <v>692</v>
+      </c>
+      <c r="D439">
+        <v>2017</v>
+      </c>
+      <c r="E439">
+        <v>1199</v>
+      </c>
+      <c r="F439">
+        <v>410</v>
+      </c>
+      <c r="G439">
+        <v>84.9</v>
+      </c>
+      <c r="H439" s="7">
+        <v>70</v>
+      </c>
+      <c r="I439" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="J439" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="K439" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L439">
+        <v>0</v>
+      </c>
+      <c r="M439">
+        <v>0</v>
+      </c>
+      <c r="N439" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="440" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A440">
+        <v>439</v>
+      </c>
+      <c r="B440" t="s">
+        <v>426</v>
+      </c>
+      <c r="C440" t="s">
+        <v>693</v>
+      </c>
+      <c r="D440">
+        <v>2011</v>
+      </c>
+      <c r="E440">
+        <v>249</v>
+      </c>
+      <c r="F440">
+        <v>116</v>
+      </c>
+      <c r="G440">
+        <v>46</v>
+      </c>
+      <c r="H440" s="7">
+        <v>56</v>
+      </c>
+      <c r="I440" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="J440" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="K440" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L440">
+        <v>0</v>
+      </c>
+      <c r="M440">
+        <v>0</v>
+      </c>
+      <c r="N440" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="441" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A441">
+        <v>440</v>
+      </c>
+      <c r="B441" t="s">
+        <v>426</v>
+      </c>
+      <c r="C441" t="s">
+        <v>694</v>
+      </c>
+      <c r="D441">
+        <v>2013</v>
+      </c>
+      <c r="E441">
+        <v>349</v>
+      </c>
+      <c r="F441">
+        <v>120</v>
+      </c>
+      <c r="G441">
+        <v>35.5</v>
+      </c>
+      <c r="H441" s="7">
+        <v>57.5</v>
+      </c>
+      <c r="I441" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="J441" s="8" t="s">
+        <v>690</v>
+      </c>
+      <c r="K441" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L441">
+        <v>0</v>
+      </c>
+      <c r="M441">
+        <v>0</v>
+      </c>
+      <c r="N441" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="442" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A442">
+        <v>441</v>
+      </c>
+      <c r="B442" t="s">
+        <v>685</v>
+      </c>
+      <c r="C442" t="s">
+        <v>695</v>
+      </c>
+      <c r="D442">
+        <v>2011</v>
+      </c>
+      <c r="E442">
+        <v>598</v>
+      </c>
+      <c r="F442">
+        <v>200</v>
+      </c>
+      <c r="G442">
+        <v>54.5</v>
+      </c>
+      <c r="H442" s="7">
+        <v>63</v>
+      </c>
+      <c r="I442" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="J442" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="K442" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L442">
+        <v>0</v>
+      </c>
+      <c r="M442">
+        <v>0</v>
+      </c>
+      <c r="N442" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="443" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A443">
+        <v>442</v>
+      </c>
+      <c r="B443" t="s">
+        <v>685</v>
+      </c>
+      <c r="C443" t="s">
+        <v>696</v>
+      </c>
+      <c r="D443">
+        <v>2016</v>
+      </c>
+      <c r="E443">
+        <v>1298</v>
+      </c>
+      <c r="F443">
+        <v>335</v>
+      </c>
+      <c r="G443">
+        <v>70</v>
+      </c>
+      <c r="H443" s="7">
+        <v>70</v>
+      </c>
+      <c r="I443" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="J443" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="K443" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L443">
+        <v>0</v>
+      </c>
+      <c r="M443">
+        <v>0</v>
+      </c>
+      <c r="N443" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="444" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A444">
+        <v>443</v>
+      </c>
+      <c r="B444" t="s">
+        <v>685</v>
+      </c>
+      <c r="C444" t="s">
+        <v>697</v>
+      </c>
+      <c r="D444">
+        <v>2014</v>
+      </c>
+      <c r="E444">
+        <v>1598</v>
+      </c>
+      <c r="F444">
+        <v>425</v>
+      </c>
+      <c r="G444">
+        <v>76.8</v>
+      </c>
+      <c r="H444" s="7">
+        <v>74</v>
+      </c>
+      <c r="I444" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="J444" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="K444" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L444">
+        <v>1</v>
+      </c>
+      <c r="M444">
+        <v>0</v>
+      </c>
+      <c r="N444" t="s">
+        <v>284</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>COUNTIF($A:$A,A1)&lt;2</formula1>
     </dataValidation>
   </dataValidations>
@@ -25586,11 +26016,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+      <selection activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26078,6 +26508,14 @@
         <v>687</v>
       </c>
     </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="12">
+        <v>43097</v>
+      </c>
+      <c r="B62" t="s">
+        <v>698</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
+ Leica 75mm f/1.25 ASPH
</commit_message>
<xml_diff>
--- a/BigAssTableOfLenses.xlsx
+++ b/BigAssTableOfLenses.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3447" uniqueCount="706">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3456" uniqueCount="708">
   <si>
     <t>Manufacture</t>
   </si>
@@ -2149,6 +2149,12 @@
   </si>
   <si>
     <t>APO-Summicron-SL 90mm f/2 ASPH</t>
+  </si>
+  <si>
+    <t>Noctilux-M 75mm f/1.25 ASPH</t>
+  </si>
+  <si>
+    <t>Add Leica 75mm f/1.25</t>
   </si>
 </sst>
 </file>
@@ -2287,8 +2293,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q448" totalsRowShown="0">
-  <autoFilter ref="A1:Q448"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q449" totalsRowShown="0">
+  <autoFilter ref="A1:Q449"/>
   <tableColumns count="17">
     <tableColumn id="15" name="UUID"/>
     <tableColumn id="1" name="Manufacture"/>
@@ -2610,10 +2616,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q448"/>
+  <dimension ref="A1:Q449"/>
   <sheetViews>
-    <sheetView topLeftCell="A421" workbookViewId="0">
-      <selection activeCell="I448" sqref="I448"/>
+    <sheetView topLeftCell="A447" workbookViewId="0">
+      <selection activeCell="Q450" sqref="Q450"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26302,6 +26308,59 @@
         <v>613</v>
       </c>
     </row>
+    <row r="449" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A449">
+        <v>448</v>
+      </c>
+      <c r="B449" t="s">
+        <v>225</v>
+      </c>
+      <c r="C449" t="s">
+        <v>706</v>
+      </c>
+      <c r="D449">
+        <v>2017</v>
+      </c>
+      <c r="E449">
+        <v>12795</v>
+      </c>
+      <c r="F449">
+        <v>1055</v>
+      </c>
+      <c r="G449">
+        <v>91</v>
+      </c>
+      <c r="H449" s="7">
+        <v>74</v>
+      </c>
+      <c r="I449" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="J449" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="K449" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L449">
+        <v>0</v>
+      </c>
+      <c r="M449">
+        <v>0</v>
+      </c>
+      <c r="N449" t="s">
+        <v>276</v>
+      </c>
+      <c r="O449" t="s">
+        <v>567</v>
+      </c>
+      <c r="P449" s="11" t="s">
+        <v>613</v>
+      </c>
+      <c r="Q449" s="11" t="s">
+        <v>613</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576">
@@ -26318,10 +26377,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26834,6 +26893,14 @@
         <v>+ Leica 75/90 SL, +Sigma 24-105 f/4A, correct error in FE 24-105mm listing</v>
       </c>
     </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="12">
+        <v>43128</v>
+      </c>
+      <c r="B65" t="s">
+        <v>707</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
+ Sigma 14-24mm f/2.8
</commit_message>
<xml_diff>
--- a/BigAssTableOfLenses.xlsx
+++ b/BigAssTableOfLenses.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="23400" windowHeight="12780" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="23400" windowHeight="12780"/>
   </bookViews>
   <sheets>
     <sheet name="LensTable" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3456" uniqueCount="708">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3465" uniqueCount="710">
   <si>
     <t>Manufacture</t>
   </si>
@@ -2155,6 +2155,12 @@
   </si>
   <si>
     <t>Add Leica 75mm f/1.25</t>
+  </si>
+  <si>
+    <t>Add Sigma 14-24mm f/2.8</t>
+  </si>
+  <si>
+    <t>14-24mm f/2.8 DG HSM Art</t>
   </si>
 </sst>
 </file>
@@ -2293,8 +2299,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q449" totalsRowShown="0">
-  <autoFilter ref="A1:Q449"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q450" totalsRowShown="0">
+  <autoFilter ref="A1:Q450"/>
   <tableColumns count="17">
     <tableColumn id="15" name="UUID"/>
     <tableColumn id="1" name="Manufacture"/>
@@ -2616,10 +2622,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q449"/>
+  <dimension ref="A1:Q450"/>
   <sheetViews>
-    <sheetView topLeftCell="A447" workbookViewId="0">
-      <selection activeCell="Q450" sqref="Q450"/>
+    <sheetView tabSelected="1" topLeftCell="A405" workbookViewId="0">
+      <selection activeCell="E450" sqref="E450"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26361,6 +26367,57 @@
         <v>613</v>
       </c>
     </row>
+    <row r="450" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A450">
+        <v>449</v>
+      </c>
+      <c r="B450" t="s">
+        <v>100</v>
+      </c>
+      <c r="C450" t="s">
+        <v>709</v>
+      </c>
+      <c r="D450">
+        <v>2018</v>
+      </c>
+      <c r="E450" s="9"/>
+      <c r="F450">
+        <v>1150</v>
+      </c>
+      <c r="G450">
+        <v>135.1</v>
+      </c>
+      <c r="H450" s="7">
+        <v>96.4</v>
+      </c>
+      <c r="I450" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="J450" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="K450" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="L450">
+        <v>0</v>
+      </c>
+      <c r="M450">
+        <v>0</v>
+      </c>
+      <c r="N450" t="s">
+        <v>276</v>
+      </c>
+      <c r="O450" t="s">
+        <v>562</v>
+      </c>
+      <c r="P450" s="11" t="s">
+        <v>610</v>
+      </c>
+      <c r="Q450" s="11" t="s">
+        <v>610</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576">
@@ -26377,10 +26434,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26901,6 +26958,14 @@
         <v>707</v>
       </c>
     </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="12">
+        <v>43141</v>
+      </c>
+      <c r="B66" t="s">
+        <v>708</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
+ Zeiss Loxia 25mm
</commit_message>
<xml_diff>
--- a/BigAssTableOfLenses.xlsx
+++ b/BigAssTableOfLenses.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="23400" windowHeight="12780"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="23400" windowHeight="12780"/>
   </bookViews>
   <sheets>
     <sheet name="LensTable" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3465" uniqueCount="710">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3474" uniqueCount="712">
   <si>
     <t>Manufacture</t>
   </si>
@@ -2161,6 +2161,12 @@
   </si>
   <si>
     <t>14-24mm f/2.8 DG HSM Art</t>
+  </si>
+  <si>
+    <t>Loxia 25mm f/2.4</t>
+  </si>
+  <si>
+    <t>Add Loxia 25mm f/2.4</t>
   </si>
 </sst>
 </file>
@@ -2299,8 +2305,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q450" totalsRowShown="0">
-  <autoFilter ref="A1:Q450"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q451" totalsRowShown="0">
+  <autoFilter ref="A1:Q451"/>
   <tableColumns count="17">
     <tableColumn id="15" name="UUID"/>
     <tableColumn id="1" name="Manufacture"/>
@@ -2622,30 +2628,30 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q450"/>
+  <dimension ref="A1:Q451"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A405" workbookViewId="0">
-      <selection activeCell="E450" sqref="E450"/>
+    <sheetView tabSelected="1" topLeftCell="A472" workbookViewId="0">
+      <selection activeCell="G419" sqref="G419"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="8.140625" customWidth="1"/>
-    <col min="3" max="3" width="49.5703125" customWidth="1"/>
-    <col min="4" max="4" width="5.42578125" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="6.140625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="5.7109375" style="3" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="8.109375" customWidth="1"/>
+    <col min="3" max="3" width="49.5546875" customWidth="1"/>
+    <col min="4" max="4" width="5.44140625" customWidth="1"/>
+    <col min="5" max="5" width="6.44140625" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" customWidth="1"/>
+    <col min="9" max="9" width="12.44140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="6.109375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="5.6640625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" customWidth="1"/>
     <col min="13" max="13" width="9" customWidth="1"/>
-    <col min="14" max="14" width="11.7109375" customWidth="1"/>
-    <col min="16" max="17" width="8.7109375" style="11"/>
+    <col min="14" max="14" width="11.6640625" customWidth="1"/>
+    <col min="16" max="17" width="8.6640625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>673</v>
       </c>
@@ -2698,7 +2704,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -2753,7 +2759,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -2808,7 +2814,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -2863,7 +2869,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -2918,7 +2924,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -2973,7 +2979,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -3028,7 +3034,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -3083,7 +3089,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -3138,7 +3144,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -3193,7 +3199,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -3248,7 +3254,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -3303,7 +3309,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -3358,7 +3364,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -3413,7 +3419,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -3468,7 +3474,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -3523,7 +3529,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -3578,7 +3584,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -3633,7 +3639,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -3688,7 +3694,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -3743,7 +3749,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -3798,7 +3804,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -3853,7 +3859,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -3908,7 +3914,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -3963,7 +3969,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -4018,7 +4024,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -4073,7 +4079,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -4128,7 +4134,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -4183,7 +4189,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -4238,7 +4244,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -4293,7 +4299,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -4348,7 +4354,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -4403,7 +4409,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -4458,7 +4464,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -4513,7 +4519,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -4568,7 +4574,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -4623,7 +4629,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -4678,7 +4684,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -4733,7 +4739,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -4788,7 +4794,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -4843,7 +4849,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -4898,7 +4904,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -4953,7 +4959,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -5008,7 +5014,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -5061,7 +5067,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -5116,7 +5122,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -5171,7 +5177,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -5226,7 +5232,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -5281,7 +5287,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -5336,7 +5342,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -5391,7 +5397,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -5446,7 +5452,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -5501,7 +5507,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -5556,7 +5562,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -5611,7 +5617,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -5666,7 +5672,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -5721,7 +5727,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" s="5">
         <v>56</v>
       </c>
@@ -5776,7 +5782,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" s="5">
         <v>57</v>
       </c>
@@ -5831,7 +5837,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" s="5">
         <v>58</v>
       </c>
@@ -5886,7 +5892,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" s="5">
         <v>59</v>
       </c>
@@ -5941,7 +5947,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" s="5">
         <v>60</v>
       </c>
@@ -5994,7 +6000,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" s="5">
         <v>61</v>
       </c>
@@ -6049,7 +6055,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" s="5">
         <v>62</v>
       </c>
@@ -6102,7 +6108,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" s="5">
         <v>63</v>
       </c>
@@ -6155,7 +6161,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" s="5">
         <v>64</v>
       </c>
@@ -6208,7 +6214,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" s="5">
         <v>65</v>
       </c>
@@ -6261,7 +6267,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" s="5">
         <v>66</v>
       </c>
@@ -6314,7 +6320,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" s="5">
         <v>67</v>
       </c>
@@ -6367,7 +6373,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" s="5">
         <v>68</v>
       </c>
@@ -6420,7 +6426,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" s="5">
         <v>69</v>
       </c>
@@ -6473,7 +6479,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" s="5">
         <v>70</v>
       </c>
@@ -6526,7 +6532,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" s="5">
         <v>71</v>
       </c>
@@ -6579,7 +6585,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" s="5">
         <v>72</v>
       </c>
@@ -6632,7 +6638,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" s="5">
         <v>73</v>
       </c>
@@ -6685,7 +6691,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75" s="5">
         <v>74</v>
       </c>
@@ -6738,7 +6744,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76" s="5">
         <v>75</v>
       </c>
@@ -6791,7 +6797,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77" s="5">
         <v>76</v>
       </c>
@@ -6844,7 +6850,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78" s="5">
         <v>77</v>
       </c>
@@ -6897,7 +6903,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79" s="5">
         <v>78</v>
       </c>
@@ -6950,7 +6956,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A80" s="5">
         <v>79</v>
       </c>
@@ -7003,7 +7009,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A81" s="5">
         <v>80</v>
       </c>
@@ -7056,7 +7062,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A82" s="5">
         <v>81</v>
       </c>
@@ -7109,7 +7115,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A83" s="5">
         <v>82</v>
       </c>
@@ -7162,7 +7168,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A84" s="5">
         <v>83</v>
       </c>
@@ -7215,7 +7221,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A85" s="5">
         <v>84</v>
       </c>
@@ -7268,7 +7274,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A86" s="5">
         <v>85</v>
       </c>
@@ -7321,7 +7327,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A87" s="5">
         <v>86</v>
       </c>
@@ -7374,7 +7380,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A88" s="5">
         <v>87</v>
       </c>
@@ -7424,7 +7430,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A89" s="5">
         <v>88</v>
       </c>
@@ -7477,7 +7483,7 @@
       </c>
       <c r="Q89" s="9"/>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A90" s="5">
         <v>89</v>
       </c>
@@ -7526,7 +7532,7 @@
       <c r="P90" s="9"/>
       <c r="Q90" s="9"/>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A91" s="5">
         <v>90</v>
       </c>
@@ -7575,7 +7581,7 @@
       <c r="P91" s="9"/>
       <c r="Q91" s="9"/>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A92" s="5">
         <v>91</v>
       </c>
@@ -7628,7 +7634,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A93" s="5">
         <v>92</v>
       </c>
@@ -7681,7 +7687,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A94" s="5">
         <v>93</v>
       </c>
@@ -7734,7 +7740,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A95" s="5">
         <v>94</v>
       </c>
@@ -7787,7 +7793,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A96" s="5">
         <v>95</v>
       </c>
@@ -7840,7 +7846,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A97" s="5">
         <v>96</v>
       </c>
@@ -7893,7 +7899,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A98" s="5">
         <v>97</v>
       </c>
@@ -7948,7 +7954,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A99" s="5">
         <v>98</v>
       </c>
@@ -8004,7 +8010,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A100" s="5">
         <v>99</v>
       </c>
@@ -8059,7 +8065,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A101" s="5">
         <v>100</v>
       </c>
@@ -8112,7 +8118,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A102" s="5">
         <v>101</v>
       </c>
@@ -8165,7 +8171,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A103" s="5">
         <v>102</v>
       </c>
@@ -8218,7 +8224,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A104" s="5">
         <v>103</v>
       </c>
@@ -8271,7 +8277,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A105" s="5">
         <v>104</v>
       </c>
@@ -8324,7 +8330,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A106" s="5">
         <v>105</v>
       </c>
@@ -8377,7 +8383,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A107" s="5">
         <v>106</v>
       </c>
@@ -8433,7 +8439,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A108" s="5">
         <v>107</v>
       </c>
@@ -8486,7 +8492,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A109" s="5">
         <v>108</v>
       </c>
@@ -8539,7 +8545,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A110" s="5">
         <v>109</v>
       </c>
@@ -8592,7 +8598,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A111" s="5">
         <v>110</v>
       </c>
@@ -8645,7 +8651,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A112" s="5">
         <v>111</v>
       </c>
@@ -8698,7 +8704,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A113" s="5">
         <v>112</v>
       </c>
@@ -8751,7 +8757,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A114" s="5">
         <v>113</v>
       </c>
@@ -8804,7 +8810,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A115" s="5">
         <v>114</v>
       </c>
@@ -8857,7 +8863,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A116" s="5">
         <v>115</v>
       </c>
@@ -8913,7 +8919,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A117" s="5">
         <v>116</v>
       </c>
@@ -8969,7 +8975,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A118" s="5">
         <v>117</v>
       </c>
@@ -9022,7 +9028,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A119" s="5">
         <v>118</v>
       </c>
@@ -9075,7 +9081,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A120" s="5">
         <v>119</v>
       </c>
@@ -9128,7 +9134,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A121" s="5">
         <v>120</v>
       </c>
@@ -9183,7 +9189,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A122" s="5">
         <v>121</v>
       </c>
@@ -9238,7 +9244,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A123" s="5">
         <v>122</v>
       </c>
@@ -9293,7 +9299,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A124" s="5">
         <v>123</v>
       </c>
@@ -9346,7 +9352,7 @@
       </c>
       <c r="Q124" s="9"/>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A125" s="5">
         <v>124</v>
       </c>
@@ -9399,7 +9405,7 @@
       </c>
       <c r="Q125" s="9"/>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A126" s="5">
         <v>125</v>
       </c>
@@ -9452,7 +9458,7 @@
       </c>
       <c r="Q126" s="9"/>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A127" s="5">
         <v>126</v>
       </c>
@@ -9505,7 +9511,7 @@
       </c>
       <c r="Q127" s="9"/>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A128" s="5">
         <v>127</v>
       </c>
@@ -9558,7 +9564,7 @@
       </c>
       <c r="Q128" s="9"/>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A129" s="5">
         <v>128</v>
       </c>
@@ -9611,7 +9617,7 @@
       </c>
       <c r="Q129" s="9"/>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A130" s="5">
         <v>129</v>
       </c>
@@ -9664,7 +9670,7 @@
       </c>
       <c r="Q130" s="9"/>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A131" s="5">
         <v>130</v>
       </c>
@@ -9717,7 +9723,7 @@
       </c>
       <c r="Q131" s="9"/>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A132" s="5">
         <v>131</v>
       </c>
@@ -9770,7 +9776,7 @@
       </c>
       <c r="Q132" s="9"/>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A133" s="5">
         <v>132</v>
       </c>
@@ -9823,7 +9829,7 @@
       </c>
       <c r="Q133" s="9"/>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A134" s="5">
         <v>133</v>
       </c>
@@ -9876,7 +9882,7 @@
       </c>
       <c r="Q134" s="9"/>
     </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A135" s="5">
         <v>134</v>
       </c>
@@ -9929,7 +9935,7 @@
       </c>
       <c r="Q135" s="9"/>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A136" s="5">
         <v>135</v>
       </c>
@@ -9982,7 +9988,7 @@
       </c>
       <c r="Q136" s="9"/>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A137" s="5">
         <v>136</v>
       </c>
@@ -10035,7 +10041,7 @@
       </c>
       <c r="Q137" s="9"/>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A138" s="5">
         <v>137</v>
       </c>
@@ -10088,7 +10094,7 @@
       </c>
       <c r="Q138" s="9"/>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A139" s="5">
         <v>138</v>
       </c>
@@ -10142,7 +10148,7 @@
       </c>
       <c r="Q139" s="9"/>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A140" s="5">
         <v>139</v>
       </c>
@@ -10195,7 +10201,7 @@
       </c>
       <c r="Q140" s="9"/>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A141" s="5">
         <v>140</v>
       </c>
@@ -10248,7 +10254,7 @@
       </c>
       <c r="Q141" s="9"/>
     </row>
-    <row r="142" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A142" s="5">
         <v>141</v>
       </c>
@@ -10301,7 +10307,7 @@
       </c>
       <c r="Q142" s="9"/>
     </row>
-    <row r="143" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A143" s="5">
         <v>142</v>
       </c>
@@ -10354,7 +10360,7 @@
       </c>
       <c r="Q143" s="9"/>
     </row>
-    <row r="144" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A144" s="5">
         <v>143</v>
       </c>
@@ -10407,7 +10413,7 @@
       </c>
       <c r="Q144" s="9"/>
     </row>
-    <row r="145" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A145" s="5">
         <v>144</v>
       </c>
@@ -10460,7 +10466,7 @@
       </c>
       <c r="Q145" s="9"/>
     </row>
-    <row r="146" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A146" s="5">
         <v>145</v>
       </c>
@@ -10513,7 +10519,7 @@
       </c>
       <c r="Q146" s="9"/>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A147" s="5">
         <v>146</v>
       </c>
@@ -10566,7 +10572,7 @@
       </c>
       <c r="Q147" s="9"/>
     </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A148" s="5">
         <v>147</v>
       </c>
@@ -10619,7 +10625,7 @@
       </c>
       <c r="Q148" s="9"/>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A149" s="5">
         <v>148</v>
       </c>
@@ -10672,7 +10678,7 @@
       </c>
       <c r="Q149" s="9"/>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A150" s="5">
         <v>149</v>
       </c>
@@ -10725,7 +10731,7 @@
       </c>
       <c r="Q150" s="9"/>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A151" s="5">
         <v>150</v>
       </c>
@@ -10778,7 +10784,7 @@
       </c>
       <c r="Q151" s="9"/>
     </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A152" s="5">
         <v>151</v>
       </c>
@@ -10831,7 +10837,7 @@
       </c>
       <c r="Q152" s="9"/>
     </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A153" s="5">
         <v>152</v>
       </c>
@@ -10884,7 +10890,7 @@
       </c>
       <c r="Q153" s="9"/>
     </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A154" s="5">
         <v>153</v>
       </c>
@@ -10937,7 +10943,7 @@
       </c>
       <c r="Q154" s="9"/>
     </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A155" s="5">
         <v>154</v>
       </c>
@@ -10990,7 +10996,7 @@
       </c>
       <c r="Q155" s="9"/>
     </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A156" s="5">
         <v>155</v>
       </c>
@@ -11041,7 +11047,7 @@
       </c>
       <c r="Q156" s="9"/>
     </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A157" s="5">
         <v>156</v>
       </c>
@@ -11092,7 +11098,7 @@
       </c>
       <c r="Q157" s="9"/>
     </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A158" s="5">
         <v>157</v>
       </c>
@@ -11143,7 +11149,7 @@
       </c>
       <c r="Q158" s="9"/>
     </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A159" s="5">
         <v>158</v>
       </c>
@@ -11194,7 +11200,7 @@
       </c>
       <c r="Q159" s="9"/>
     </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A160" s="5">
         <v>159</v>
       </c>
@@ -11245,7 +11251,7 @@
       </c>
       <c r="Q160" s="9"/>
     </row>
-    <row r="161" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A161" s="5">
         <v>160</v>
       </c>
@@ -11296,7 +11302,7 @@
       </c>
       <c r="Q161" s="9"/>
     </row>
-    <row r="162" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A162" s="5">
         <v>161</v>
       </c>
@@ -11347,7 +11353,7 @@
       </c>
       <c r="Q162" s="9"/>
     </row>
-    <row r="163" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A163" s="5">
         <v>162</v>
       </c>
@@ -11398,7 +11404,7 @@
       </c>
       <c r="Q163" s="9"/>
     </row>
-    <row r="164" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A164" s="5">
         <v>163</v>
       </c>
@@ -11449,7 +11455,7 @@
       </c>
       <c r="Q164" s="9"/>
     </row>
-    <row r="165" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A165" s="5">
         <v>164</v>
       </c>
@@ -11500,7 +11506,7 @@
       </c>
       <c r="Q165" s="9"/>
     </row>
-    <row r="166" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A166" s="5">
         <v>165</v>
       </c>
@@ -11551,7 +11557,7 @@
       </c>
       <c r="Q166" s="9"/>
     </row>
-    <row r="167" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A167" s="5">
         <v>166</v>
       </c>
@@ -11606,7 +11612,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="168" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A168" s="5">
         <v>167</v>
       </c>
@@ -11659,7 +11665,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="169" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A169" s="5">
         <v>168</v>
       </c>
@@ -11715,7 +11721,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="170" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A170" s="5">
         <v>169</v>
       </c>
@@ -11768,7 +11774,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="171" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A171" s="5">
         <v>170</v>
       </c>
@@ -11823,7 +11829,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="172" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A172" s="5">
         <v>171</v>
       </c>
@@ -11876,7 +11882,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="173" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A173" s="5">
         <v>172</v>
       </c>
@@ -11931,7 +11937,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="174" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A174" s="5">
         <v>173</v>
       </c>
@@ -11984,7 +11990,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="175" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A175" s="5">
         <v>174</v>
       </c>
@@ -12039,7 +12045,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="176" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A176" s="5">
         <v>175</v>
       </c>
@@ -12092,7 +12098,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="177" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A177" s="5">
         <v>176</v>
       </c>
@@ -12145,7 +12151,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="178" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A178" s="5">
         <v>177</v>
       </c>
@@ -12198,7 +12204,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="179" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A179" s="5">
         <v>178</v>
       </c>
@@ -12253,7 +12259,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="180" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A180" s="5">
         <v>179</v>
       </c>
@@ -12308,7 +12314,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="181" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A181" s="5">
         <v>180</v>
       </c>
@@ -12363,7 +12369,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="182" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A182" s="5">
         <v>181</v>
       </c>
@@ -12416,7 +12422,7 @@
       </c>
       <c r="Q182" s="9"/>
     </row>
-    <row r="183" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A183" s="5">
         <v>182</v>
       </c>
@@ -12469,7 +12475,7 @@
       </c>
       <c r="Q183" s="9"/>
     </row>
-    <row r="184" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A184" s="5">
         <v>183</v>
       </c>
@@ -12522,7 +12528,7 @@
       </c>
       <c r="Q184" s="9"/>
     </row>
-    <row r="185" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A185" s="5">
         <v>184</v>
       </c>
@@ -12575,7 +12581,7 @@
       </c>
       <c r="Q185" s="9"/>
     </row>
-    <row r="186" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A186" s="5">
         <v>185</v>
       </c>
@@ -12628,7 +12634,7 @@
       </c>
       <c r="Q186" s="9"/>
     </row>
-    <row r="187" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A187" s="5">
         <v>186</v>
       </c>
@@ -12681,7 +12687,7 @@
       </c>
       <c r="Q187" s="9"/>
     </row>
-    <row r="188" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A188" s="5">
         <v>187</v>
       </c>
@@ -12734,7 +12740,7 @@
       </c>
       <c r="Q188" s="9"/>
     </row>
-    <row r="189" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A189" s="5">
         <v>188</v>
       </c>
@@ -12787,7 +12793,7 @@
       </c>
       <c r="Q189" s="9"/>
     </row>
-    <row r="190" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A190" s="5">
         <v>189</v>
       </c>
@@ -12840,7 +12846,7 @@
       </c>
       <c r="Q190" s="9"/>
     </row>
-    <row r="191" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A191" s="5">
         <v>190</v>
       </c>
@@ -12893,7 +12899,7 @@
       </c>
       <c r="Q191" s="9"/>
     </row>
-    <row r="192" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A192" s="5">
         <v>191</v>
       </c>
@@ -12946,7 +12952,7 @@
       </c>
       <c r="Q192" s="9"/>
     </row>
-    <row r="193" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A193" s="5">
         <v>192</v>
       </c>
@@ -12997,7 +13003,7 @@
       </c>
       <c r="Q193" s="9"/>
     </row>
-    <row r="194" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A194" s="5">
         <v>193</v>
       </c>
@@ -13048,7 +13054,7 @@
       </c>
       <c r="Q194" s="9"/>
     </row>
-    <row r="195" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A195" s="5">
         <v>194</v>
       </c>
@@ -13096,7 +13102,7 @@
       </c>
       <c r="Q195" s="9"/>
     </row>
-    <row r="196" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A196" s="5">
         <v>195</v>
       </c>
@@ -13147,7 +13153,7 @@
       </c>
       <c r="Q196" s="9"/>
     </row>
-    <row r="197" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A197" s="5">
         <v>196</v>
       </c>
@@ -13198,7 +13204,7 @@
       </c>
       <c r="Q197" s="9"/>
     </row>
-    <row r="198" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A198" s="5">
         <v>197</v>
       </c>
@@ -13249,7 +13255,7 @@
       </c>
       <c r="Q198" s="9"/>
     </row>
-    <row r="199" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A199" s="5">
         <v>198</v>
       </c>
@@ -13302,7 +13308,7 @@
       </c>
       <c r="Q199" s="9"/>
     </row>
-    <row r="200" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A200" s="5">
         <v>199</v>
       </c>
@@ -13355,7 +13361,7 @@
       </c>
       <c r="Q200" s="9"/>
     </row>
-    <row r="201" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A201" s="5">
         <v>200</v>
       </c>
@@ -13408,7 +13414,7 @@
       </c>
       <c r="Q201" s="9"/>
     </row>
-    <row r="202" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A202" s="5">
         <v>201</v>
       </c>
@@ -13461,7 +13467,7 @@
       </c>
       <c r="Q202" s="9"/>
     </row>
-    <row r="203" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A203" s="5">
         <v>202</v>
       </c>
@@ -13514,7 +13520,7 @@
       </c>
       <c r="Q203" s="9"/>
     </row>
-    <row r="204" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A204" s="5">
         <v>203</v>
       </c>
@@ -13567,7 +13573,7 @@
       </c>
       <c r="Q204" s="9"/>
     </row>
-    <row r="205" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A205" s="5">
         <v>204</v>
       </c>
@@ -13621,7 +13627,7 @@
       </c>
       <c r="Q205" s="9"/>
     </row>
-    <row r="206" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A206" s="5">
         <v>205</v>
       </c>
@@ -13674,7 +13680,7 @@
       </c>
       <c r="Q206" s="9"/>
     </row>
-    <row r="207" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A207" s="5">
         <v>206</v>
       </c>
@@ -13727,7 +13733,7 @@
       </c>
       <c r="Q207" s="9"/>
     </row>
-    <row r="208" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A208" s="5">
         <v>207</v>
       </c>
@@ -13780,7 +13786,7 @@
       </c>
       <c r="Q208" s="9"/>
     </row>
-    <row r="209" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A209" s="5">
         <v>208</v>
       </c>
@@ -13833,7 +13839,7 @@
       </c>
       <c r="Q209" s="9"/>
     </row>
-    <row r="210" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A210" s="5">
         <v>209</v>
       </c>
@@ -13886,7 +13892,7 @@
       </c>
       <c r="Q210" s="9"/>
     </row>
-    <row r="211" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A211" s="5">
         <v>210</v>
       </c>
@@ -13939,7 +13945,7 @@
       </c>
       <c r="Q211" s="9"/>
     </row>
-    <row r="212" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A212" s="5">
         <v>211</v>
       </c>
@@ -13992,7 +13998,7 @@
       </c>
       <c r="Q212" s="9"/>
     </row>
-    <row r="213" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A213" s="5">
         <v>212</v>
       </c>
@@ -14045,7 +14051,7 @@
       </c>
       <c r="Q213" s="9"/>
     </row>
-    <row r="214" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A214" s="5">
         <v>213</v>
       </c>
@@ -14096,7 +14102,7 @@
       </c>
       <c r="Q214" s="9"/>
     </row>
-    <row r="215" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A215" s="5">
         <v>214</v>
       </c>
@@ -14149,7 +14155,7 @@
       </c>
       <c r="Q215" s="9"/>
     </row>
-    <row r="216" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A216" s="5">
         <v>215</v>
       </c>
@@ -14202,7 +14208,7 @@
       </c>
       <c r="Q216" s="9"/>
     </row>
-    <row r="217" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A217" s="5">
         <v>216</v>
       </c>
@@ -14255,7 +14261,7 @@
       </c>
       <c r="Q217" s="9"/>
     </row>
-    <row r="218" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A218" s="5">
         <v>217</v>
       </c>
@@ -14308,7 +14314,7 @@
       </c>
       <c r="Q218" s="9"/>
     </row>
-    <row r="219" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A219" s="5">
         <v>218</v>
       </c>
@@ -14361,7 +14367,7 @@
       </c>
       <c r="Q219" s="9"/>
     </row>
-    <row r="220" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A220" s="5">
         <v>219</v>
       </c>
@@ -14414,7 +14420,7 @@
       </c>
       <c r="Q220" s="9"/>
     </row>
-    <row r="221" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A221" s="5">
         <v>220</v>
       </c>
@@ -14467,7 +14473,7 @@
       </c>
       <c r="Q221" s="9"/>
     </row>
-    <row r="222" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A222" s="5">
         <v>221</v>
       </c>
@@ -14520,7 +14526,7 @@
       </c>
       <c r="Q222" s="9"/>
     </row>
-    <row r="223" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A223" s="5">
         <v>222</v>
       </c>
@@ -14573,7 +14579,7 @@
       </c>
       <c r="Q223" s="9"/>
     </row>
-    <row r="224" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A224" s="5">
         <v>223</v>
       </c>
@@ -14624,7 +14630,7 @@
       </c>
       <c r="Q224" s="9"/>
     </row>
-    <row r="225" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A225" s="5">
         <v>224</v>
       </c>
@@ -14675,7 +14681,7 @@
       </c>
       <c r="Q225" s="9"/>
     </row>
-    <row r="226" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A226" s="5">
         <v>225</v>
       </c>
@@ -14726,7 +14732,7 @@
       </c>
       <c r="Q226" s="9"/>
     </row>
-    <row r="227" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A227" s="5">
         <v>226</v>
       </c>
@@ -14779,7 +14785,7 @@
       </c>
       <c r="Q227" s="9"/>
     </row>
-    <row r="228" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A228" s="5">
         <v>227</v>
       </c>
@@ -14832,7 +14838,7 @@
       </c>
       <c r="Q228" s="9"/>
     </row>
-    <row r="229" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A229" s="5">
         <v>228</v>
       </c>
@@ -14885,7 +14891,7 @@
       </c>
       <c r="Q229" s="9"/>
     </row>
-    <row r="230" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A230" s="5">
         <v>229</v>
       </c>
@@ -14938,7 +14944,7 @@
       </c>
       <c r="Q230" s="9"/>
     </row>
-    <row r="231" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A231" s="5">
         <v>230</v>
       </c>
@@ -14991,7 +14997,7 @@
       </c>
       <c r="Q231" s="9"/>
     </row>
-    <row r="232" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A232" s="5">
         <v>231</v>
       </c>
@@ -15042,7 +15048,7 @@
       </c>
       <c r="Q232" s="9"/>
     </row>
-    <row r="233" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A233" s="5">
         <v>232</v>
       </c>
@@ -15095,7 +15101,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="234" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A234" s="5">
         <v>233</v>
       </c>
@@ -15148,7 +15154,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="235" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A235" s="5">
         <v>234</v>
       </c>
@@ -15201,7 +15207,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="236" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A236" s="5">
         <v>235</v>
       </c>
@@ -15254,7 +15260,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="237" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A237" s="5">
         <v>236</v>
       </c>
@@ -15305,7 +15311,7 @@
       <c r="P237" s="13"/>
       <c r="Q237" s="13"/>
     </row>
-    <row r="238" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A238" s="5">
         <v>237</v>
       </c>
@@ -15354,7 +15360,7 @@
       <c r="P238" s="13"/>
       <c r="Q238" s="13"/>
     </row>
-    <row r="239" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A239" s="5">
         <v>238</v>
       </c>
@@ -15403,7 +15409,7 @@
       <c r="P239" s="13"/>
       <c r="Q239" s="13"/>
     </row>
-    <row r="240" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A240" s="5">
         <v>239</v>
       </c>
@@ -15454,7 +15460,7 @@
       <c r="P240" s="13"/>
       <c r="Q240" s="13"/>
     </row>
-    <row r="241" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A241" s="5">
         <v>240</v>
       </c>
@@ -15503,7 +15509,7 @@
       <c r="P241" s="13"/>
       <c r="Q241" s="13"/>
     </row>
-    <row r="242" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A242" s="5">
         <v>241</v>
       </c>
@@ -15552,7 +15558,7 @@
       <c r="P242" s="13"/>
       <c r="Q242" s="13"/>
     </row>
-    <row r="243" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A243" s="5">
         <v>242</v>
       </c>
@@ -15601,7 +15607,7 @@
       <c r="P243" s="13"/>
       <c r="Q243" s="13"/>
     </row>
-    <row r="244" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A244" s="5">
         <v>243</v>
       </c>
@@ -15652,7 +15658,7 @@
       <c r="P244" s="13"/>
       <c r="Q244" s="13"/>
     </row>
-    <row r="245" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A245" s="5">
         <v>244</v>
       </c>
@@ -15701,7 +15707,7 @@
       <c r="P245" s="13"/>
       <c r="Q245" s="13"/>
     </row>
-    <row r="246" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A246" s="5">
         <v>245</v>
       </c>
@@ -15750,7 +15756,7 @@
       <c r="P246" s="13"/>
       <c r="Q246" s="13"/>
     </row>
-    <row r="247" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A247" s="5">
         <v>246</v>
       </c>
@@ -15799,7 +15805,7 @@
       <c r="P247" s="13"/>
       <c r="Q247" s="13"/>
     </row>
-    <row r="248" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A248" s="5">
         <v>247</v>
       </c>
@@ -15848,7 +15854,7 @@
       <c r="P248" s="13"/>
       <c r="Q248" s="13"/>
     </row>
-    <row r="249" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A249" s="5">
         <v>248</v>
       </c>
@@ -15897,7 +15903,7 @@
       <c r="P249" s="13"/>
       <c r="Q249" s="13"/>
     </row>
-    <row r="250" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A250" s="5">
         <v>249</v>
       </c>
@@ -15948,7 +15954,7 @@
       <c r="P250" s="13"/>
       <c r="Q250" s="13"/>
     </row>
-    <row r="251" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A251" s="5">
         <v>250</v>
       </c>
@@ -15997,7 +16003,7 @@
       <c r="P251" s="13"/>
       <c r="Q251" s="13"/>
     </row>
-    <row r="252" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A252" s="5">
         <v>251</v>
       </c>
@@ -16046,7 +16052,7 @@
       <c r="P252" s="13"/>
       <c r="Q252" s="13"/>
     </row>
-    <row r="253" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A253" s="5">
         <v>252</v>
       </c>
@@ -16095,7 +16101,7 @@
       <c r="P253" s="13"/>
       <c r="Q253" s="13"/>
     </row>
-    <row r="254" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A254" s="5">
         <v>253</v>
       </c>
@@ -16150,7 +16156,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="255" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A255" s="5">
         <v>254</v>
       </c>
@@ -16203,7 +16209,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="256" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A256" s="5">
         <v>255</v>
       </c>
@@ -16256,7 +16262,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="257" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A257" s="5">
         <v>256</v>
       </c>
@@ -16311,7 +16317,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="258" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A258" s="5">
         <v>257</v>
       </c>
@@ -16364,7 +16370,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="259" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A259" s="5">
         <v>258</v>
       </c>
@@ -16417,7 +16423,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="260" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A260" s="5">
         <v>259</v>
       </c>
@@ -16472,7 +16478,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="261" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A261" s="5">
         <v>260</v>
       </c>
@@ -16527,7 +16533,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="262" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A262" s="5">
         <v>261</v>
       </c>
@@ -16582,7 +16588,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="263" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A263" s="5">
         <v>262</v>
       </c>
@@ -16635,7 +16641,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="264" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A264" s="5">
         <v>263</v>
       </c>
@@ -16688,7 +16694,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="265" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A265" s="5">
         <v>264</v>
       </c>
@@ -16741,7 +16747,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="266" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A266" s="5">
         <v>265</v>
       </c>
@@ -16796,7 +16802,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="267" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A267" s="5">
         <v>266</v>
       </c>
@@ -16851,7 +16857,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="268" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A268" s="5">
         <v>267</v>
       </c>
@@ -16906,7 +16912,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="269" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A269" s="5">
         <v>268</v>
       </c>
@@ -16959,7 +16965,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="270" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A270" s="5">
         <v>269</v>
       </c>
@@ -17012,7 +17018,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="271" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A271" s="5">
         <v>270</v>
       </c>
@@ -17067,7 +17073,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="272" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A272" s="5">
         <v>271</v>
       </c>
@@ -17122,7 +17128,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="273" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A273" s="5">
         <v>272</v>
       </c>
@@ -17175,7 +17181,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="274" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A274" s="5">
         <v>273</v>
       </c>
@@ -17228,7 +17234,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="275" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A275" s="5">
         <v>274</v>
       </c>
@@ -17283,7 +17289,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="276" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A276" s="5">
         <v>275</v>
       </c>
@@ -17338,7 +17344,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="277" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A277" s="5">
         <v>276</v>
       </c>
@@ -17393,7 +17399,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="278" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A278" s="5">
         <v>277</v>
       </c>
@@ -17448,7 +17454,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="279" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A279" s="5">
         <v>278</v>
       </c>
@@ -17501,7 +17507,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="280" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A280" s="5">
         <v>279</v>
       </c>
@@ -17554,7 +17560,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="281" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A281" s="5">
         <v>280</v>
       </c>
@@ -17607,7 +17613,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="282" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A282" s="5">
         <v>281</v>
       </c>
@@ -17660,7 +17666,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="283" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A283" s="5">
         <v>282</v>
       </c>
@@ -17713,7 +17719,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="284" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A284" s="5">
         <v>283</v>
       </c>
@@ -17768,7 +17774,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="285" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A285" s="5">
         <v>284</v>
       </c>
@@ -17823,7 +17829,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="286" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A286" s="5">
         <v>285</v>
       </c>
@@ -17878,7 +17884,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="287" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A287" s="5">
         <v>286</v>
       </c>
@@ -17933,7 +17939,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="288" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A288" s="5">
         <v>287</v>
       </c>
@@ -17988,7 +17994,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="289" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A289" s="5">
         <v>288</v>
       </c>
@@ -18041,7 +18047,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="290" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A290" s="5">
         <v>289</v>
       </c>
@@ -18094,7 +18100,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="291" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A291" s="5">
         <v>290</v>
       </c>
@@ -18147,7 +18153,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="292" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A292" s="5">
         <v>291</v>
       </c>
@@ -18200,7 +18206,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="293" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A293" s="5">
         <v>292</v>
       </c>
@@ -18253,7 +18259,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="294" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A294" s="5">
         <v>293</v>
       </c>
@@ -18308,7 +18314,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="295" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A295" s="5">
         <v>294</v>
       </c>
@@ -18363,7 +18369,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="296" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A296" s="5">
         <v>295</v>
       </c>
@@ -18418,7 +18424,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="297" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A297" s="5">
         <v>296</v>
       </c>
@@ -18473,7 +18479,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="298" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A298" s="5">
         <v>297</v>
       </c>
@@ -18528,7 +18534,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="299" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A299" s="5">
         <v>298</v>
       </c>
@@ -18581,7 +18587,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="300" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A300" s="5">
         <v>299</v>
       </c>
@@ -18634,7 +18640,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="301" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A301" s="5">
         <v>300</v>
       </c>
@@ -18687,7 +18693,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="302" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A302" s="5">
         <v>301</v>
       </c>
@@ -18742,7 +18748,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="303" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A303" s="5">
         <v>302</v>
       </c>
@@ -18797,7 +18803,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="304" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A304" s="5">
         <v>303</v>
       </c>
@@ -18850,7 +18856,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="305" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A305" s="5">
         <v>304</v>
       </c>
@@ -18905,7 +18911,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="306" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A306" s="5">
         <v>305</v>
       </c>
@@ -18958,7 +18964,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="307" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A307" s="5">
         <v>306</v>
       </c>
@@ -19011,7 +19017,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="308" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A308" s="5">
         <v>307</v>
       </c>
@@ -19064,7 +19070,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="309" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A309" s="5">
         <v>308</v>
       </c>
@@ -19117,7 +19123,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="310" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A310" s="5">
         <v>309</v>
       </c>
@@ -19170,7 +19176,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="311" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A311" s="5">
         <v>310</v>
       </c>
@@ -19223,7 +19229,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="312" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A312" s="5">
         <v>311</v>
       </c>
@@ -19276,7 +19282,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="313" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A313" s="5">
         <v>312</v>
       </c>
@@ -19329,7 +19335,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="314" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A314" s="5">
         <v>313</v>
       </c>
@@ -19382,7 +19388,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="315" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A315" s="5">
         <v>314</v>
       </c>
@@ -19435,7 +19441,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="316" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A316" s="5">
         <v>315</v>
       </c>
@@ -19488,7 +19494,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="317" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A317" s="5">
         <v>316</v>
       </c>
@@ -19541,7 +19547,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="318" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A318" s="5">
         <v>317</v>
       </c>
@@ -19594,7 +19600,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="319" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A319" s="5">
         <v>318</v>
       </c>
@@ -19647,7 +19653,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="320" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A320" s="5">
         <v>319</v>
       </c>
@@ -19700,7 +19706,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="321" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A321" s="5">
         <v>320</v>
       </c>
@@ -19753,7 +19759,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="322" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A322" s="5">
         <v>321</v>
       </c>
@@ -19804,7 +19810,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="323" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A323" s="5">
         <v>322</v>
       </c>
@@ -19855,7 +19861,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="324" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A324" s="5">
         <v>323</v>
       </c>
@@ -19906,7 +19912,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="325" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A325" s="6">
         <v>324</v>
       </c>
@@ -19957,7 +19963,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="326" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A326" s="6">
         <v>325</v>
       </c>
@@ -20008,7 +20014,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="327" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A327" s="6">
         <v>326</v>
       </c>
@@ -20057,7 +20063,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="328" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A328" s="6">
         <v>327</v>
       </c>
@@ -20110,7 +20116,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="329" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A329" s="6">
         <v>328</v>
       </c>
@@ -20163,7 +20169,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="330" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A330" s="6">
         <v>329</v>
       </c>
@@ -20216,7 +20222,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="331" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A331" s="6">
         <v>330</v>
       </c>
@@ -20269,7 +20275,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="332" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A332" s="6">
         <v>331</v>
       </c>
@@ -20320,7 +20326,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="333" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A333" s="6">
         <v>332</v>
       </c>
@@ -20371,7 +20377,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="334" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A334" s="6">
         <v>333</v>
       </c>
@@ -20422,7 +20428,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="335" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A335" s="6">
         <v>334</v>
       </c>
@@ -20473,7 +20479,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="336" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A336" s="6">
         <v>335</v>
       </c>
@@ -20524,7 +20530,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="337" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A337" s="6">
         <v>336</v>
       </c>
@@ -20575,7 +20581,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="338" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A338" s="6">
         <v>337</v>
       </c>
@@ -20628,7 +20634,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="339" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A339" s="6">
         <v>338</v>
       </c>
@@ -20679,7 +20685,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="340" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A340" s="6">
         <v>339</v>
       </c>
@@ -20730,7 +20736,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="341" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A341" s="6">
         <v>340</v>
       </c>
@@ -20781,7 +20787,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="342" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A342" s="6">
         <v>341</v>
       </c>
@@ -20832,7 +20838,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="343" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A343" s="6">
         <v>342</v>
       </c>
@@ -20883,7 +20889,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="344" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A344" s="6">
         <v>343</v>
       </c>
@@ -20934,7 +20940,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="345" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A345" s="6">
         <v>344</v>
       </c>
@@ -20985,7 +20991,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="346" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A346" s="6">
         <v>345</v>
       </c>
@@ -21036,7 +21042,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="347" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A347" s="6">
         <v>346</v>
       </c>
@@ -21087,7 +21093,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="348" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A348" s="6">
         <v>347</v>
       </c>
@@ -21138,7 +21144,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="349" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A349" s="6">
         <v>348</v>
       </c>
@@ -21189,7 +21195,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="350" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A350" s="6">
         <v>349</v>
       </c>
@@ -21240,7 +21246,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="351" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A351" s="6">
         <v>350</v>
       </c>
@@ -21291,7 +21297,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="352" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A352" s="6">
         <v>351</v>
       </c>
@@ -21342,7 +21348,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="353" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A353" s="6">
         <v>352</v>
       </c>
@@ -21393,7 +21399,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="354" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A354" s="6">
         <v>353</v>
       </c>
@@ -21444,7 +21450,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="355" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A355" s="6">
         <v>354</v>
       </c>
@@ -21497,7 +21503,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="356" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A356" s="6">
         <v>355</v>
       </c>
@@ -21550,7 +21556,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="357" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A357" s="6">
         <v>356</v>
       </c>
@@ -21603,7 +21609,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="358" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A358" s="6">
         <v>357</v>
       </c>
@@ -21656,7 +21662,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="359" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A359" s="6">
         <v>358</v>
       </c>
@@ -21709,7 +21715,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="360" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A360" s="6">
         <v>359</v>
       </c>
@@ -21762,7 +21768,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="361" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A361" s="6">
         <v>360</v>
       </c>
@@ -21815,7 +21821,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="362" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A362" s="6">
         <v>361</v>
       </c>
@@ -21868,7 +21874,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="363" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A363" s="6">
         <v>362</v>
       </c>
@@ -21921,7 +21927,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="364" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A364" s="6">
         <v>363</v>
       </c>
@@ -21974,7 +21980,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="365" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A365" s="6">
         <v>364</v>
       </c>
@@ -22027,7 +22033,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="366" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A366" s="6">
         <v>365</v>
       </c>
@@ -22080,7 +22086,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="367" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A367" s="6">
         <v>366</v>
       </c>
@@ -22133,7 +22139,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="368" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A368" s="6">
         <v>367</v>
       </c>
@@ -22186,7 +22192,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="369" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A369" s="6">
         <v>368</v>
       </c>
@@ -22239,7 +22245,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="370" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A370" s="6">
         <v>369</v>
       </c>
@@ -22292,7 +22298,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="371" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A371" s="6">
         <v>370</v>
       </c>
@@ -22345,7 +22351,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="372" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A372" s="6">
         <v>371</v>
       </c>
@@ -22396,7 +22402,7 @@
       </c>
       <c r="Q372" s="9"/>
     </row>
-    <row r="373" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A373" s="6">
         <v>372</v>
       </c>
@@ -22447,7 +22453,7 @@
       </c>
       <c r="Q373" s="9"/>
     </row>
-    <row r="374" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A374" s="6">
         <v>373</v>
       </c>
@@ -22498,7 +22504,7 @@
       </c>
       <c r="Q374" s="9"/>
     </row>
-    <row r="375" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A375" s="6">
         <v>374</v>
       </c>
@@ -22549,7 +22555,7 @@
       </c>
       <c r="Q375" s="9"/>
     </row>
-    <row r="376" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A376" s="6">
         <v>375</v>
       </c>
@@ -22598,7 +22604,7 @@
       </c>
       <c r="Q376" s="9"/>
     </row>
-    <row r="377" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A377" s="6">
         <v>376</v>
       </c>
@@ -22649,7 +22655,7 @@
       </c>
       <c r="Q377" s="9"/>
     </row>
-    <row r="378" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A378" s="6">
         <v>377</v>
       </c>
@@ -22700,7 +22706,7 @@
       </c>
       <c r="Q378" s="9"/>
     </row>
-    <row r="379" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A379" s="6">
         <v>378</v>
       </c>
@@ -22753,7 +22759,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="380" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A380" s="6">
         <v>379</v>
       </c>
@@ -22806,7 +22812,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="381" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A381" s="6">
         <v>380</v>
       </c>
@@ -22859,7 +22865,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="382" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A382" s="6">
         <v>381</v>
       </c>
@@ -22912,7 +22918,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="383" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A383" s="6">
         <v>382</v>
       </c>
@@ -22965,7 +22971,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="384" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A384" s="6">
         <v>383</v>
       </c>
@@ -23018,7 +23024,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="385" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A385" s="6">
         <v>384</v>
       </c>
@@ -23069,7 +23075,7 @@
       </c>
       <c r="Q385" s="9"/>
     </row>
-    <row r="386" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A386" s="6">
         <v>385</v>
       </c>
@@ -23122,7 +23128,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="387" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A387" s="6">
         <v>386</v>
       </c>
@@ -23173,7 +23179,7 @@
       </c>
       <c r="Q387" s="9"/>
     </row>
-    <row r="388" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A388" s="6">
         <v>387</v>
       </c>
@@ -23224,7 +23230,7 @@
       </c>
       <c r="Q388" s="9"/>
     </row>
-    <row r="389" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A389" s="6">
         <v>388</v>
       </c>
@@ -23275,7 +23281,7 @@
       </c>
       <c r="Q389" s="9"/>
     </row>
-    <row r="390" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A390" s="6">
         <v>389</v>
       </c>
@@ -23326,7 +23332,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="391" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A391" s="6">
         <v>390</v>
       </c>
@@ -23379,7 +23385,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="392" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A392" s="6">
         <v>391</v>
       </c>
@@ -23432,7 +23438,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="393" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A393" s="6">
         <v>392</v>
       </c>
@@ -23485,7 +23491,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="394" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A394" s="6">
         <v>393</v>
       </c>
@@ -23538,7 +23544,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="395" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A395" s="6">
         <v>394</v>
       </c>
@@ -23583,7 +23589,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="396" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A396" s="6">
         <v>395</v>
       </c>
@@ -23632,7 +23638,7 @@
       <c r="P396" s="9"/>
       <c r="Q396" s="9"/>
     </row>
-    <row r="397" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A397" s="6">
         <v>396</v>
       </c>
@@ -23681,7 +23687,7 @@
       <c r="P397" s="9"/>
       <c r="Q397" s="9"/>
     </row>
-    <row r="398" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A398">
         <v>397</v>
       </c>
@@ -23734,7 +23740,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="399" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A399">
         <v>398</v>
       </c>
@@ -23783,7 +23789,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="400" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A400">
         <v>399</v>
       </c>
@@ -23834,7 +23840,7 @@
       </c>
       <c r="Q400" s="9"/>
     </row>
-    <row r="401" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A401">
         <v>400</v>
       </c>
@@ -23885,7 +23891,7 @@
       </c>
       <c r="Q401" s="9"/>
     </row>
-    <row r="402" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A402">
         <v>401</v>
       </c>
@@ -23936,7 +23942,7 @@
       </c>
       <c r="Q402" s="9"/>
     </row>
-    <row r="403" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A403">
         <v>402</v>
       </c>
@@ -23987,7 +23993,7 @@
       </c>
       <c r="Q403" s="9"/>
     </row>
-    <row r="404" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A404">
         <v>403</v>
       </c>
@@ -24038,7 +24044,7 @@
       </c>
       <c r="Q404" s="9"/>
     </row>
-    <row r="405" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A405">
         <v>404</v>
       </c>
@@ -24091,7 +24097,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="406" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A406">
         <v>405</v>
       </c>
@@ -24140,7 +24146,7 @@
       <c r="P406" s="9"/>
       <c r="Q406" s="9"/>
     </row>
-    <row r="407" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A407" s="11">
         <v>406</v>
       </c>
@@ -24193,7 +24199,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="408" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A408" s="11">
         <v>407</v>
       </c>
@@ -24246,7 +24252,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="409" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A409" s="11">
         <v>408</v>
       </c>
@@ -24299,7 +24305,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="410" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A410" s="11">
         <v>409</v>
       </c>
@@ -24352,7 +24358,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="411" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A411" s="11">
         <v>410</v>
       </c>
@@ -24405,7 +24411,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="412" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A412" s="11">
         <v>411</v>
       </c>
@@ -24458,7 +24464,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="413" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A413" s="11">
         <v>412</v>
       </c>
@@ -24511,7 +24517,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="414" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A414" s="11">
         <v>413</v>
       </c>
@@ -24564,7 +24570,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="415" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A415" s="11">
         <v>414</v>
       </c>
@@ -24617,7 +24623,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="416" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A416" s="11">
         <v>415</v>
       </c>
@@ -24668,7 +24674,7 @@
       </c>
       <c r="Q416" s="9"/>
     </row>
-    <row r="417" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A417">
         <v>416</v>
       </c>
@@ -24719,7 +24725,7 @@
       </c>
       <c r="Q417" s="9"/>
     </row>
-    <row r="418" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A418">
         <v>417</v>
       </c>
@@ -24772,7 +24778,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="419" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A419">
         <v>418</v>
       </c>
@@ -24821,7 +24827,7 @@
       </c>
       <c r="Q419" s="9"/>
     </row>
-    <row r="420" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A420" s="11">
         <v>419</v>
       </c>
@@ -24870,7 +24876,7 @@
       </c>
       <c r="Q420" s="9"/>
     </row>
-    <row r="421" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A421" s="11">
         <v>420</v>
       </c>
@@ -24917,7 +24923,7 @@
       </c>
       <c r="Q421" s="9"/>
     </row>
-    <row r="422" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A422" s="11">
         <v>421</v>
       </c>
@@ -24966,7 +24972,7 @@
       </c>
       <c r="Q422" s="9"/>
     </row>
-    <row r="423" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A423" s="11">
         <v>422</v>
       </c>
@@ -25015,7 +25021,7 @@
       </c>
       <c r="Q423" s="9"/>
     </row>
-    <row r="424" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A424" s="11">
         <v>423</v>
       </c>
@@ -25064,7 +25070,7 @@
       </c>
       <c r="Q424" s="9"/>
     </row>
-    <row r="425" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A425">
         <v>424</v>
       </c>
@@ -25113,7 +25119,7 @@
       </c>
       <c r="Q425" s="9"/>
     </row>
-    <row r="426" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A426">
         <v>425</v>
       </c>
@@ -25166,7 +25172,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="427" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A427">
         <v>426</v>
       </c>
@@ -25219,7 +25225,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="428" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A428">
         <v>427</v>
       </c>
@@ -25272,7 +25278,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="429" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A429">
         <v>428</v>
       </c>
@@ -25325,7 +25331,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="430" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A430" s="18">
         <v>429</v>
       </c>
@@ -25376,7 +25382,7 @@
       </c>
       <c r="Q430" s="17"/>
     </row>
-    <row r="431" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A431">
         <v>430</v>
       </c>
@@ -25429,7 +25435,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="432" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A432">
         <v>431</v>
       </c>
@@ -25482,7 +25488,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="433" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A433">
         <v>432</v>
       </c>
@@ -25535,7 +25541,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="434" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A434">
         <v>433</v>
       </c>
@@ -25586,7 +25592,7 @@
       </c>
       <c r="Q434" s="9"/>
     </row>
-    <row r="435" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A435">
         <v>434</v>
       </c>
@@ -25637,7 +25643,7 @@
       </c>
       <c r="Q435" s="9"/>
     </row>
-    <row r="436" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A436">
         <v>435</v>
       </c>
@@ -25690,7 +25696,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="437" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A437">
         <v>436</v>
       </c>
@@ -25743,7 +25749,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="438" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A438">
         <v>437</v>
       </c>
@@ -25794,7 +25800,7 @@
       </c>
       <c r="Q438" s="9"/>
     </row>
-    <row r="439" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A439">
         <v>438</v>
       </c>
@@ -25847,7 +25853,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="440" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A440">
         <v>439</v>
       </c>
@@ -25898,7 +25904,7 @@
       </c>
       <c r="Q440" s="9"/>
     </row>
-    <row r="441" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A441">
         <v>440</v>
       </c>
@@ -25949,7 +25955,7 @@
       </c>
       <c r="Q441" s="9"/>
     </row>
-    <row r="442" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A442">
         <v>441</v>
       </c>
@@ -26000,7 +26006,7 @@
       </c>
       <c r="Q442" s="9"/>
     </row>
-    <row r="443" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A443">
         <v>442</v>
       </c>
@@ -26051,7 +26057,7 @@
       </c>
       <c r="Q443" s="9"/>
     </row>
-    <row r="444" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A444">
         <v>443</v>
       </c>
@@ -26102,7 +26108,7 @@
       </c>
       <c r="Q444" s="9"/>
     </row>
-    <row r="445" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A445">
         <v>444</v>
       </c>
@@ -26155,7 +26161,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="446" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A446">
         <v>445</v>
       </c>
@@ -26208,7 +26214,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="447" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A447">
         <v>446</v>
       </c>
@@ -26261,7 +26267,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="448" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A448">
         <v>447</v>
       </c>
@@ -26314,7 +26320,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="449" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A449">
         <v>448</v>
       </c>
@@ -26367,7 +26373,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="450" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A450">
         <v>449</v>
       </c>
@@ -26415,6 +26421,59 @@
         <v>610</v>
       </c>
       <c r="Q450" s="11" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="451" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A451">
+        <v>450</v>
+      </c>
+      <c r="B451" t="s">
+        <v>132</v>
+      </c>
+      <c r="C451" t="s">
+        <v>710</v>
+      </c>
+      <c r="D451">
+        <v>2018</v>
+      </c>
+      <c r="E451">
+        <v>1299</v>
+      </c>
+      <c r="F451">
+        <v>393</v>
+      </c>
+      <c r="G451">
+        <v>74.5</v>
+      </c>
+      <c r="H451" s="7">
+        <v>62</v>
+      </c>
+      <c r="I451" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="J451" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="K451" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L451">
+        <v>0</v>
+      </c>
+      <c r="M451">
+        <v>0</v>
+      </c>
+      <c r="N451" t="s">
+        <v>276</v>
+      </c>
+      <c r="O451" t="s">
+        <v>564</v>
+      </c>
+      <c r="P451" s="11" t="s">
+        <v>613</v>
+      </c>
+      <c r="Q451" s="11" t="s">
         <v>610</v>
       </c>
     </row>
@@ -26434,23 +26493,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G66"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
     <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="12">
         <v>42361</v>
       </c>
@@ -26458,7 +26517,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>42369</v>
       </c>
@@ -26466,7 +26525,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>42371</v>
       </c>
@@ -26474,7 +26533,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>42372</v>
       </c>
@@ -26482,7 +26541,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>42373</v>
       </c>
@@ -26490,7 +26549,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>42382</v>
       </c>
@@ -26498,7 +26557,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>42385</v>
       </c>
@@ -26506,7 +26565,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>42387</v>
       </c>
@@ -26514,7 +26573,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>42388</v>
       </c>
@@ -26522,7 +26581,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
         <v>42390</v>
       </c>
@@ -26530,7 +26589,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>42391</v>
       </c>
@@ -26538,7 +26597,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>42400</v>
       </c>
@@ -26546,7 +26605,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>42414</v>
       </c>
@@ -26554,7 +26613,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>42432</v>
       </c>
@@ -26565,7 +26624,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>42435</v>
       </c>
@@ -26573,7 +26632,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>42436</v>
       </c>
@@ -26581,7 +26640,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>42441</v>
       </c>
@@ -26589,7 +26648,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>42445</v>
       </c>
@@ -26597,7 +26656,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>42453</v>
       </c>
@@ -26605,7 +26664,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="12">
         <v>42456</v>
       </c>
@@ -26613,7 +26672,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="12">
         <v>42457</v>
       </c>
@@ -26621,7 +26680,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="12">
         <v>42458</v>
       </c>
@@ -26629,7 +26688,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="12">
         <v>42464</v>
       </c>
@@ -26637,7 +26696,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="12">
         <v>42510</v>
       </c>
@@ -26645,7 +26704,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="12">
         <v>42515</v>
       </c>
@@ -26653,7 +26712,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="12">
         <v>42560</v>
       </c>
@@ -26661,7 +26720,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="12">
         <v>42565</v>
       </c>
@@ -26669,7 +26728,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <v>42576</v>
       </c>
@@ -26677,7 +26736,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="12">
         <v>42590</v>
       </c>
@@ -26685,7 +26744,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="12">
         <v>42593</v>
       </c>
@@ -26693,7 +26752,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="12">
         <v>42598</v>
       </c>
@@ -26701,7 +26760,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="12">
         <v>42665</v>
       </c>
@@ -26709,7 +26768,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="12">
         <v>42788</v>
       </c>
@@ -26717,7 +26776,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="12">
         <v>42831</v>
       </c>
@@ -26725,7 +26784,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="12">
         <v>42833</v>
       </c>
@@ -26733,7 +26792,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="12">
         <v>42833</v>
       </c>
@@ -26741,7 +26800,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="12">
         <v>42874</v>
       </c>
@@ -26749,7 +26808,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="12">
         <v>42876</v>
       </c>
@@ -26757,7 +26816,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="12">
         <v>42878</v>
       </c>
@@ -26765,7 +26824,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="12">
         <v>42878</v>
       </c>
@@ -26773,7 +26832,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="12">
         <v>42879</v>
       </c>
@@ -26781,7 +26840,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="12">
         <v>42884</v>
       </c>
@@ -26789,7 +26848,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="12">
         <v>42887</v>
       </c>
@@ -26797,7 +26856,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="12">
         <v>42887</v>
       </c>
@@ -26805,7 +26864,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="12">
         <v>42891</v>
       </c>
@@ -26813,7 +26872,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="12">
         <v>42901</v>
       </c>
@@ -26821,7 +26880,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="12">
         <v>42908</v>
       </c>
@@ -26829,7 +26888,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="12">
         <v>42909</v>
       </c>
@@ -26837,7 +26896,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="12">
         <v>42910</v>
       </c>
@@ -26845,7 +26904,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="12">
         <v>42913</v>
       </c>
@@ -26853,7 +26912,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="12">
         <v>42914</v>
       </c>
@@ -26861,7 +26920,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="12">
         <v>42948</v>
       </c>
@@ -26869,7 +26928,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="12">
         <v>42977</v>
       </c>
@@ -26877,7 +26936,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="12">
         <v>42992</v>
       </c>
@@ -26885,7 +26944,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="12">
         <v>42996</v>
       </c>
@@ -26893,7 +26952,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="12">
         <v>42997</v>
       </c>
@@ -26901,7 +26960,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="12">
         <v>43026</v>
       </c>
@@ -26909,7 +26968,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="12">
         <v>43033</v>
       </c>
@@ -26917,7 +26976,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="12">
         <v>43047</v>
       </c>
@@ -26925,7 +26984,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="12">
         <v>43097</v>
       </c>
@@ -26933,7 +26992,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="12">
         <v>43109</v>
       </c>
@@ -26941,7 +27000,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="12">
         <v>43121</v>
       </c>
@@ -26950,7 +27009,7 @@
         <v>+ Leica 75/90 SL, +Sigma 24-105 f/4A, correct error in FE 24-105mm listing</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="12">
         <v>43128</v>
       </c>
@@ -26958,12 +27017,20 @@
         <v>707</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="12">
         <v>43141</v>
       </c>
       <c r="B66" t="s">
         <v>708</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" s="12">
+        <v>43145</v>
+      </c>
+      <c r="B67" t="s">
+        <v>711</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
+ Samyang 50mm f/1.2, + Tamron 70-210mm f/4
</commit_message>
<xml_diff>
--- a/BigAssTableOfLenses.xlsx
+++ b/BigAssTableOfLenses.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="23400" windowHeight="12780"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="23040" windowHeight="8604"/>
   </bookViews>
   <sheets>
     <sheet name="LensTable" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3474" uniqueCount="712">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3483" uniqueCount="714">
   <si>
     <t>Manufacture</t>
   </si>
@@ -2167,6 +2167,12 @@
   </si>
   <si>
     <t>Add Loxia 25mm f/2.4</t>
+  </si>
+  <si>
+    <t>XP 50mm f/1.2</t>
+  </si>
+  <si>
+    <t>Add Samyang 50mm f/1.2</t>
   </si>
 </sst>
 </file>
@@ -2305,8 +2311,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q451" totalsRowShown="0">
-  <autoFilter ref="A1:Q451"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q452" totalsRowShown="0">
+  <autoFilter ref="A1:Q452"/>
   <tableColumns count="17">
     <tableColumn id="15" name="UUID"/>
     <tableColumn id="1" name="Manufacture"/>
@@ -2628,10 +2634,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q451"/>
+  <dimension ref="A1:Q452"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A472" workbookViewId="0">
-      <selection activeCell="G419" sqref="G419"/>
+    <sheetView tabSelected="1" topLeftCell="A431" workbookViewId="0">
+      <selection activeCell="E452" sqref="E452"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26477,6 +26483,57 @@
         <v>610</v>
       </c>
     </row>
+    <row r="452" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A452">
+        <v>451</v>
+      </c>
+      <c r="B452" t="s">
+        <v>421</v>
+      </c>
+      <c r="C452" t="s">
+        <v>712</v>
+      </c>
+      <c r="D452">
+        <v>2018</v>
+      </c>
+      <c r="E452" s="9"/>
+      <c r="F452">
+        <v>1300</v>
+      </c>
+      <c r="G452">
+        <v>117.4</v>
+      </c>
+      <c r="H452" s="7">
+        <v>93</v>
+      </c>
+      <c r="I452" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="J452" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="K452" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L452">
+        <v>0</v>
+      </c>
+      <c r="M452">
+        <v>0</v>
+      </c>
+      <c r="N452" t="s">
+        <v>276</v>
+      </c>
+      <c r="O452" t="s">
+        <v>565</v>
+      </c>
+      <c r="P452" s="11" t="s">
+        <v>619</v>
+      </c>
+      <c r="Q452" s="11" t="s">
+        <v>619</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576">
@@ -26493,10 +26550,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G67"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
     <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27033,6 +27090,14 @@
         <v>711</v>
       </c>
     </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" s="12">
+        <v>43151</v>
+      </c>
+      <c r="B68" t="s">
+        <v>713</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
+ Tokina 20mm f/2 AF, correct Tamron 70-210mm model
</commit_message>
<xml_diff>
--- a/BigAssTableOfLenses.xlsx
+++ b/BigAssTableOfLenses.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3483" uniqueCount="714">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3497" uniqueCount="718">
   <si>
     <t>Manufacture</t>
   </si>
@@ -2173,6 +2173,18 @@
   </si>
   <si>
     <t>Add Samyang 50mm f/1.2</t>
+  </si>
+  <si>
+    <t>70-210mm f/4 Di VC USD</t>
+  </si>
+  <si>
+    <t>70-210</t>
+  </si>
+  <si>
+    <t>FiRIN 20mm f/2 FE AF</t>
+  </si>
+  <si>
+    <t>Add Tamron 70-210mm f/4 &amp; Add Tokina FiRIN 20mm f/2 AF</t>
   </si>
 </sst>
 </file>
@@ -2311,8 +2323,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q452" totalsRowShown="0">
-  <autoFilter ref="A1:Q452"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q454" totalsRowShown="0">
+  <autoFilter ref="A1:Q454"/>
   <tableColumns count="17">
     <tableColumn id="15" name="UUID"/>
     <tableColumn id="1" name="Manufacture"/>
@@ -2634,10 +2646,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q452"/>
+  <dimension ref="A1:Q454"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A431" workbookViewId="0">
-      <selection activeCell="E452" sqref="E452"/>
+      <selection activeCell="C448" sqref="C448"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26534,6 +26546,110 @@
         <v>619</v>
       </c>
     </row>
+    <row r="453" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A453" s="11">
+        <v>452</v>
+      </c>
+      <c r="B453" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="C453" s="11" t="s">
+        <v>714</v>
+      </c>
+      <c r="D453" s="11">
+        <v>2018</v>
+      </c>
+      <c r="E453" s="11">
+        <v>799</v>
+      </c>
+      <c r="F453" s="11">
+        <v>859</v>
+      </c>
+      <c r="G453" s="11">
+        <v>175.3</v>
+      </c>
+      <c r="H453" s="7">
+        <v>76</v>
+      </c>
+      <c r="I453" s="11">
+        <v>4</v>
+      </c>
+      <c r="J453" s="8" t="s">
+        <v>715</v>
+      </c>
+      <c r="K453" s="8">
+        <v>1</v>
+      </c>
+      <c r="L453" s="11">
+        <v>1</v>
+      </c>
+      <c r="M453" s="11">
+        <v>0</v>
+      </c>
+      <c r="N453" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="O453" s="11" t="s">
+        <v>571</v>
+      </c>
+      <c r="P453" s="11" t="s">
+        <v>610</v>
+      </c>
+      <c r="Q453" s="11" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="454" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A454" s="11">
+        <v>453</v>
+      </c>
+      <c r="B454" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="C454" s="11" t="s">
+        <v>716</v>
+      </c>
+      <c r="D454" s="11">
+        <v>2018</v>
+      </c>
+      <c r="E454" s="11"/>
+      <c r="F454" s="11">
+        <v>464</v>
+      </c>
+      <c r="G454" s="11">
+        <v>81.5</v>
+      </c>
+      <c r="H454" s="7">
+        <v>73.400000000000006</v>
+      </c>
+      <c r="I454" s="11">
+        <v>2</v>
+      </c>
+      <c r="J454" s="8">
+        <v>20</v>
+      </c>
+      <c r="K454" s="8">
+        <v>0</v>
+      </c>
+      <c r="L454" s="11">
+        <v>0</v>
+      </c>
+      <c r="M454" s="11">
+        <v>0</v>
+      </c>
+      <c r="N454" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="O454" s="11" t="s">
+        <v>562</v>
+      </c>
+      <c r="P454" s="11" t="s">
+        <v>610</v>
+      </c>
+      <c r="Q454" s="11" t="s">
+        <v>610</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576">
@@ -26550,10 +26666,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
     <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+      <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27098,6 +27214,14 @@
         <v>713</v>
       </c>
     </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" s="12">
+        <v>43153</v>
+      </c>
+      <c r="B69" t="s">
+        <v>717</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
+ sigma 14-24mm f/2.8 pricing
</commit_message>
<xml_diff>
--- a/BigAssTableOfLenses.xlsx
+++ b/BigAssTableOfLenses.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3497" uniqueCount="718">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3498" uniqueCount="719">
   <si>
     <t>Manufacture</t>
   </si>
@@ -2185,6 +2185,9 @@
   </si>
   <si>
     <t>Add Tamron 70-210mm f/4 &amp; Add Tokina FiRIN 20mm f/2 AF</t>
+  </si>
+  <si>
+    <t>Add Sigma 14-24mm f/2.8 pricing</t>
   </si>
 </sst>
 </file>
@@ -2649,7 +2652,7 @@
   <dimension ref="A1:Q454"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A431" workbookViewId="0">
-      <selection activeCell="C448" sqref="C448"/>
+      <selection activeCell="E450" sqref="E450"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26404,7 +26407,9 @@
       <c r="D450">
         <v>2018</v>
       </c>
-      <c r="E450" s="9"/>
+      <c r="E450" s="11">
+        <v>1299</v>
+      </c>
       <c r="F450">
         <v>1150</v>
       </c>
@@ -26666,10 +26671,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G69"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
     <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70"/>
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27222,6 +27227,14 @@
         <v>717</v>
       </c>
     </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" s="12">
+        <v>43155</v>
+      </c>
+      <c r="B70" t="s">
+        <v>718</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
new metadata, many new lenses
- mitakon 50, 85 speedmaster
- olympus 300, 12-40, 7-14
- panasonic 7-14, 12-35, 35-100, 50-200
- voigtlander 58, 50, 110, 21
- tokina 50
- sigma 70, 105
- venus 9, 25mm
</commit_message>
<xml_diff>
--- a/BigAssTableOfLenses.xlsx
+++ b/BigAssTableOfLenses.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3506" uniqueCount="719">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3652" uniqueCount="748">
   <si>
     <t>Manufacture</t>
   </si>
@@ -2188,6 +2188,93 @@
   </si>
   <si>
     <t>Add Sigma 14-24mm f/2.8 pricing</t>
+  </si>
+  <si>
+    <t>Speedmaster 50mm f/0.95</t>
+  </si>
+  <si>
+    <t>Speedmaster 85mm f/1.2</t>
+  </si>
+  <si>
+    <t>M.Zuiko Digital ED 300mm f/4 IS PRO</t>
+  </si>
+  <si>
+    <t>12-40</t>
+  </si>
+  <si>
+    <t>M.Zuiko Digital ED 7-14mm f/2.8 PRO</t>
+  </si>
+  <si>
+    <t>M.Zuiko Digital ED 12-40mm f/2.8 PRO</t>
+  </si>
+  <si>
+    <t>7-14</t>
+  </si>
+  <si>
+    <t>Lumix G Vario 7-14mm f/4 ASPH.</t>
+  </si>
+  <si>
+    <t>Leica DG Vario-Elmarit 8-18mm f/2.8-4 ASPH.</t>
+  </si>
+  <si>
+    <t>2.8-4</t>
+  </si>
+  <si>
+    <t>8-18</t>
+  </si>
+  <si>
+    <t>12-35</t>
+  </si>
+  <si>
+    <t>Lumix G X Vario 12-35mm f/2.8 ASPH. POWER O.I.S.</t>
+  </si>
+  <si>
+    <t>Lumix G X Vario 12-35mm f/2.8 II ASPH. POWER O.I.S.</t>
+  </si>
+  <si>
+    <t>Lumix G X Vario 35-100mm f/2.8 II Power O.I.S.</t>
+  </si>
+  <si>
+    <t>35-100</t>
+  </si>
+  <si>
+    <t>Leica DG Vario-Elmarit 50-200mm f/2.8-4 ASPH POWER O.I.S.</t>
+  </si>
+  <si>
+    <t>50-200</t>
+  </si>
+  <si>
+    <t>Nokton 58mm f/1.4 SL II S</t>
+  </si>
+  <si>
+    <t>Nokton 50mm f/1.2 Aspherical</t>
+  </si>
+  <si>
+    <t>Macro-Apo-Lanthar 110mm f/2.5</t>
+  </si>
+  <si>
+    <t>Color-Skopar 21mm f/3.5 Aspherical</t>
+  </si>
+  <si>
+    <t>Opera 50mm f/1.4 FF</t>
+  </si>
+  <si>
+    <t>70mm f/2.8 DG Macro Art</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Laowa 25mm f/2.8 Macro</t>
+  </si>
+  <si>
+    <t>Add Mitakon 50, 85 speedmaster.  Add sigma 105mm Art, 70mm Art.  Add Olympus M4/3 lineup.  Add Panasonic M4/3 lineup.  Add new Voigtlander lenses.  Add new Venus lenses.  Add new Tokina lenses. (Total: +18 lenses)</t>
+  </si>
+  <si>
+    <t>Laowa 9mm f/2.8 Zero-D</t>
   </si>
 </sst>
 </file>
@@ -2326,8 +2413,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q454" totalsRowShown="0">
-  <autoFilter ref="A1:Q454"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q473" totalsRowShown="0">
+  <autoFilter ref="A1:Q473"/>
   <tableColumns count="17">
     <tableColumn id="15" name="UUID"/>
     <tableColumn id="1" name="Manufacture"/>
@@ -2649,10 +2736,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q454"/>
+  <dimension ref="A1:Q473"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A445" workbookViewId="0">
-      <selection activeCell="B455" sqref="B455"/>
+    <sheetView tabSelected="1" topLeftCell="A450" workbookViewId="0">
+      <selection activeCell="C473" sqref="C473"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26673,8 +26760,957 @@
         <v>610</v>
       </c>
     </row>
+    <row r="455" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A455">
+        <v>454</v>
+      </c>
+      <c r="B455" t="s">
+        <v>287</v>
+      </c>
+      <c r="C455" t="s">
+        <v>719</v>
+      </c>
+      <c r="D455" s="11">
+        <v>2014</v>
+      </c>
+      <c r="E455">
+        <v>799</v>
+      </c>
+      <c r="F455">
+        <v>720</v>
+      </c>
+      <c r="G455">
+        <v>87</v>
+      </c>
+      <c r="H455" s="7">
+        <v>68.5</v>
+      </c>
+      <c r="I455" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="J455" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="K455" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L455">
+        <v>0</v>
+      </c>
+      <c r="M455">
+        <v>0</v>
+      </c>
+      <c r="N455" t="s">
+        <v>276</v>
+      </c>
+      <c r="O455" t="s">
+        <v>565</v>
+      </c>
+      <c r="P455" s="11" t="s">
+        <v>614</v>
+      </c>
+      <c r="Q455" s="11" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="456" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A456">
+        <v>455</v>
+      </c>
+      <c r="B456" t="s">
+        <v>287</v>
+      </c>
+      <c r="C456" t="s">
+        <v>720</v>
+      </c>
+      <c r="D456" s="11">
+        <v>2015</v>
+      </c>
+      <c r="E456">
+        <v>699</v>
+      </c>
+      <c r="F456">
+        <v>921</v>
+      </c>
+      <c r="G456">
+        <v>96</v>
+      </c>
+      <c r="H456" s="7">
+        <v>83</v>
+      </c>
+      <c r="I456" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="J456" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="K456" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L456">
+        <v>0</v>
+      </c>
+      <c r="M456">
+        <v>0</v>
+      </c>
+      <c r="N456" t="s">
+        <v>276</v>
+      </c>
+      <c r="O456" t="s">
+        <v>567</v>
+      </c>
+      <c r="P456" s="11" t="s">
+        <v>614</v>
+      </c>
+      <c r="Q456" s="11" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="457" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A457">
+        <v>456</v>
+      </c>
+      <c r="B457" t="s">
+        <v>426</v>
+      </c>
+      <c r="C457" t="s">
+        <v>721</v>
+      </c>
+      <c r="D457">
+        <v>2016</v>
+      </c>
+      <c r="E457">
+        <v>2499</v>
+      </c>
+      <c r="F457">
+        <v>1475</v>
+      </c>
+      <c r="G457">
+        <v>227</v>
+      </c>
+      <c r="H457" s="7">
+        <v>92.5</v>
+      </c>
+      <c r="I457" s="1">
+        <v>4</v>
+      </c>
+      <c r="J457" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="K457" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L457">
+        <v>1</v>
+      </c>
+      <c r="M457">
+        <v>0</v>
+      </c>
+      <c r="N457" t="s">
+        <v>284</v>
+      </c>
+      <c r="O457" t="s">
+        <v>700</v>
+      </c>
+      <c r="P457" s="11" t="s">
+        <v>610</v>
+      </c>
+      <c r="Q457" s="9"/>
+    </row>
+    <row r="458" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A458">
+        <v>457</v>
+      </c>
+      <c r="B458" t="s">
+        <v>426</v>
+      </c>
+      <c r="C458" t="s">
+        <v>724</v>
+      </c>
+      <c r="D458">
+        <v>2013</v>
+      </c>
+      <c r="E458">
+        <v>799</v>
+      </c>
+      <c r="F458">
+        <v>382</v>
+      </c>
+      <c r="G458">
+        <v>84</v>
+      </c>
+      <c r="H458" s="7">
+        <v>69.900000000000006</v>
+      </c>
+      <c r="I458" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="J458" s="8" t="s">
+        <v>722</v>
+      </c>
+      <c r="K458" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="L458">
+        <v>0</v>
+      </c>
+      <c r="M458">
+        <v>0</v>
+      </c>
+      <c r="N458" t="s">
+        <v>284</v>
+      </c>
+      <c r="O458" t="s">
+        <v>565</v>
+      </c>
+      <c r="P458" s="11" t="s">
+        <v>610</v>
+      </c>
+      <c r="Q458" s="9"/>
+    </row>
+    <row r="459" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A459">
+        <v>458</v>
+      </c>
+      <c r="B459" t="s">
+        <v>426</v>
+      </c>
+      <c r="C459" t="s">
+        <v>723</v>
+      </c>
+      <c r="D459">
+        <v>2015</v>
+      </c>
+      <c r="E459">
+        <v>1099</v>
+      </c>
+      <c r="F459">
+        <v>534</v>
+      </c>
+      <c r="G459">
+        <v>105.8</v>
+      </c>
+      <c r="H459" s="7">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="I459" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="J459" s="8" t="s">
+        <v>725</v>
+      </c>
+      <c r="K459" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="L459">
+        <v>0</v>
+      </c>
+      <c r="M459">
+        <v>0</v>
+      </c>
+      <c r="N459" t="s">
+        <v>284</v>
+      </c>
+      <c r="O459" t="s">
+        <v>562</v>
+      </c>
+      <c r="P459" s="11" t="s">
+        <v>610</v>
+      </c>
+      <c r="Q459" s="9"/>
+    </row>
+    <row r="460" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A460">
+        <v>459</v>
+      </c>
+      <c r="B460" t="s">
+        <v>684</v>
+      </c>
+      <c r="C460" t="s">
+        <v>726</v>
+      </c>
+      <c r="D460">
+        <v>2009</v>
+      </c>
+      <c r="E460">
+        <v>797</v>
+      </c>
+      <c r="F460">
+        <v>301</v>
+      </c>
+      <c r="G460">
+        <v>83.1</v>
+      </c>
+      <c r="H460" s="7">
+        <v>75</v>
+      </c>
+      <c r="I460" s="1">
+        <v>4</v>
+      </c>
+      <c r="J460" s="8" t="s">
+        <v>725</v>
+      </c>
+      <c r="K460" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="L460">
+        <v>0</v>
+      </c>
+      <c r="M460">
+        <v>0</v>
+      </c>
+      <c r="N460" t="s">
+        <v>284</v>
+      </c>
+      <c r="O460" t="s">
+        <v>562</v>
+      </c>
+      <c r="P460" s="11" t="s">
+        <v>610</v>
+      </c>
+      <c r="Q460" s="9"/>
+    </row>
+    <row r="461" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A461">
+        <v>460</v>
+      </c>
+      <c r="B461" t="s">
+        <v>684</v>
+      </c>
+      <c r="C461" t="s">
+        <v>727</v>
+      </c>
+      <c r="D461">
+        <v>2017</v>
+      </c>
+      <c r="E461">
+        <v>1097</v>
+      </c>
+      <c r="F461">
+        <v>315</v>
+      </c>
+      <c r="G461">
+        <v>88</v>
+      </c>
+      <c r="H461" s="7">
+        <v>73.400000000000006</v>
+      </c>
+      <c r="I461" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="J461" s="8" t="s">
+        <v>729</v>
+      </c>
+      <c r="K461" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="L461">
+        <v>0</v>
+      </c>
+      <c r="M461">
+        <v>0</v>
+      </c>
+      <c r="N461" t="s">
+        <v>284</v>
+      </c>
+      <c r="O461" t="s">
+        <v>564</v>
+      </c>
+      <c r="P461" s="11" t="s">
+        <v>610</v>
+      </c>
+      <c r="Q461" s="9"/>
+    </row>
+    <row r="462" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A462">
+        <v>461</v>
+      </c>
+      <c r="B462" t="s">
+        <v>684</v>
+      </c>
+      <c r="C462" t="s">
+        <v>731</v>
+      </c>
+      <c r="D462">
+        <v>2012</v>
+      </c>
+      <c r="E462" s="9"/>
+      <c r="F462">
+        <v>305</v>
+      </c>
+      <c r="G462">
+        <v>73.8</v>
+      </c>
+      <c r="H462">
+        <v>67.599999999999994</v>
+      </c>
+      <c r="I462" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="J462" s="8" t="s">
+        <v>730</v>
+      </c>
+      <c r="K462" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="L462">
+        <v>1</v>
+      </c>
+      <c r="M462">
+        <v>0</v>
+      </c>
+      <c r="N462" t="s">
+        <v>284</v>
+      </c>
+      <c r="O462" t="s">
+        <v>565</v>
+      </c>
+      <c r="P462" s="11" t="s">
+        <v>610</v>
+      </c>
+      <c r="Q462" s="9"/>
+    </row>
+    <row r="463" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A463">
+        <v>462</v>
+      </c>
+      <c r="B463" t="s">
+        <v>684</v>
+      </c>
+      <c r="C463" t="s">
+        <v>732</v>
+      </c>
+      <c r="D463">
+        <v>2017</v>
+      </c>
+      <c r="E463">
+        <v>898</v>
+      </c>
+      <c r="F463">
+        <v>305</v>
+      </c>
+      <c r="G463">
+        <v>73.8</v>
+      </c>
+      <c r="H463" s="7">
+        <v>67.599999999999994</v>
+      </c>
+      <c r="I463" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="J463" s="8" t="s">
+        <v>730</v>
+      </c>
+      <c r="K463" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="L463">
+        <v>1</v>
+      </c>
+      <c r="M463">
+        <v>0</v>
+      </c>
+      <c r="N463" t="s">
+        <v>284</v>
+      </c>
+      <c r="O463" t="s">
+        <v>565</v>
+      </c>
+      <c r="P463" s="11" t="s">
+        <v>610</v>
+      </c>
+      <c r="Q463" s="9"/>
+    </row>
+    <row r="464" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A464">
+        <v>463</v>
+      </c>
+      <c r="B464" t="s">
+        <v>684</v>
+      </c>
+      <c r="C464" t="s">
+        <v>733</v>
+      </c>
+      <c r="D464">
+        <v>2017</v>
+      </c>
+      <c r="E464">
+        <v>998</v>
+      </c>
+      <c r="F464">
+        <v>357</v>
+      </c>
+      <c r="G464">
+        <v>99.9</v>
+      </c>
+      <c r="H464" s="7">
+        <v>67.400000000000006</v>
+      </c>
+      <c r="I464" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="J464" s="8" t="s">
+        <v>734</v>
+      </c>
+      <c r="K464" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="L464">
+        <v>1</v>
+      </c>
+      <c r="M464">
+        <v>0</v>
+      </c>
+      <c r="N464" t="s">
+        <v>284</v>
+      </c>
+      <c r="O464" t="s">
+        <v>571</v>
+      </c>
+      <c r="P464" s="11" t="s">
+        <v>610</v>
+      </c>
+      <c r="Q464" s="9"/>
+    </row>
+    <row r="465" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A465">
+        <v>464</v>
+      </c>
+      <c r="B465" t="s">
+        <v>684</v>
+      </c>
+      <c r="C465" t="s">
+        <v>735</v>
+      </c>
+      <c r="D465">
+        <v>2018</v>
+      </c>
+      <c r="E465">
+        <v>1698</v>
+      </c>
+      <c r="F465">
+        <v>655</v>
+      </c>
+      <c r="G465">
+        <v>132</v>
+      </c>
+      <c r="H465" s="7">
+        <v>76</v>
+      </c>
+      <c r="I465" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="J465" s="8" t="s">
+        <v>736</v>
+      </c>
+      <c r="K465" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="L465">
+        <v>1</v>
+      </c>
+      <c r="M465">
+        <v>0</v>
+      </c>
+      <c r="N465" t="s">
+        <v>284</v>
+      </c>
+      <c r="O465" t="s">
+        <v>700</v>
+      </c>
+      <c r="P465" s="11" t="s">
+        <v>610</v>
+      </c>
+      <c r="Q465" s="9"/>
+    </row>
+    <row r="466" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A466">
+        <v>465</v>
+      </c>
+      <c r="B466" t="s">
+        <v>213</v>
+      </c>
+      <c r="C466" t="s">
+        <v>737</v>
+      </c>
+      <c r="D466">
+        <v>2007</v>
+      </c>
+      <c r="E466">
+        <v>599</v>
+      </c>
+      <c r="F466">
+        <v>320</v>
+      </c>
+      <c r="G466">
+        <v>45.5</v>
+      </c>
+      <c r="H466" s="7">
+        <v>67.599999999999994</v>
+      </c>
+      <c r="I466" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="J466" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="K466" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L466">
+        <v>0</v>
+      </c>
+      <c r="M466">
+        <v>0</v>
+      </c>
+      <c r="N466" t="s">
+        <v>276</v>
+      </c>
+      <c r="O466" t="s">
+        <v>565</v>
+      </c>
+      <c r="P466" s="11" t="s">
+        <v>610</v>
+      </c>
+      <c r="Q466" s="11" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="467" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A467">
+        <v>466</v>
+      </c>
+      <c r="B467" t="s">
+        <v>213</v>
+      </c>
+      <c r="C467" t="s">
+        <v>738</v>
+      </c>
+      <c r="D467">
+        <v>2018</v>
+      </c>
+      <c r="E467" s="9"/>
+      <c r="F467" s="9"/>
+      <c r="G467" s="9"/>
+      <c r="H467" s="10"/>
+      <c r="I467" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="J467" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="K467" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L467">
+        <v>0</v>
+      </c>
+      <c r="M467">
+        <v>0</v>
+      </c>
+      <c r="N467" t="s">
+        <v>276</v>
+      </c>
+      <c r="O467" t="s">
+        <v>565</v>
+      </c>
+      <c r="P467" s="11" t="s">
+        <v>610</v>
+      </c>
+      <c r="Q467" s="11" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="468" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A468">
+        <v>467</v>
+      </c>
+      <c r="B468" t="s">
+        <v>213</v>
+      </c>
+      <c r="C468" t="s">
+        <v>739</v>
+      </c>
+      <c r="D468">
+        <v>2018</v>
+      </c>
+      <c r="E468" s="9"/>
+      <c r="F468" s="9"/>
+      <c r="G468">
+        <v>99.7</v>
+      </c>
+      <c r="H468" s="7">
+        <v>78.400000000000006</v>
+      </c>
+      <c r="I468" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="J468" s="8" t="s">
+        <v>640</v>
+      </c>
+      <c r="K468" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L468">
+        <v>0</v>
+      </c>
+      <c r="M468">
+        <v>0</v>
+      </c>
+      <c r="N468" t="s">
+        <v>276</v>
+      </c>
+      <c r="O468" t="s">
+        <v>571</v>
+      </c>
+      <c r="P468" s="11" t="s">
+        <v>610</v>
+      </c>
+      <c r="Q468" s="11" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="469" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A469">
+        <v>468</v>
+      </c>
+      <c r="B469" t="s">
+        <v>213</v>
+      </c>
+      <c r="C469" t="s">
+        <v>740</v>
+      </c>
+      <c r="D469">
+        <v>2018</v>
+      </c>
+      <c r="E469" s="9"/>
+      <c r="F469" s="9"/>
+      <c r="G469">
+        <v>39.9</v>
+      </c>
+      <c r="H469" s="7">
+        <v>62.8</v>
+      </c>
+      <c r="I469" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="J469" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="K469" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L469">
+        <v>0</v>
+      </c>
+      <c r="M469">
+        <v>0</v>
+      </c>
+      <c r="N469" t="s">
+        <v>276</v>
+      </c>
+      <c r="O469" t="s">
+        <v>562</v>
+      </c>
+      <c r="P469" s="11" t="s">
+        <v>610</v>
+      </c>
+      <c r="Q469" s="11" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="470" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A470">
+        <v>469</v>
+      </c>
+      <c r="B470" t="s">
+        <v>189</v>
+      </c>
+      <c r="C470" t="s">
+        <v>741</v>
+      </c>
+      <c r="D470">
+        <v>2018</v>
+      </c>
+      <c r="E470" s="9"/>
+      <c r="F470" s="9"/>
+      <c r="G470" s="9"/>
+      <c r="H470" s="9"/>
+      <c r="I470" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="J470" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="K470" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L470">
+        <v>0</v>
+      </c>
+      <c r="M470">
+        <v>0</v>
+      </c>
+      <c r="N470" t="s">
+        <v>276</v>
+      </c>
+      <c r="O470" t="s">
+        <v>565</v>
+      </c>
+      <c r="P470" s="11" t="s">
+        <v>610</v>
+      </c>
+      <c r="Q470" s="11" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="471" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A471">
+        <v>470</v>
+      </c>
+      <c r="B471" t="s">
+        <v>100</v>
+      </c>
+      <c r="C471" t="s">
+        <v>742</v>
+      </c>
+      <c r="D471">
+        <v>2018</v>
+      </c>
+      <c r="E471" s="9"/>
+      <c r="F471">
+        <v>515</v>
+      </c>
+      <c r="G471">
+        <v>105.8</v>
+      </c>
+      <c r="H471" s="7">
+        <v>70.8</v>
+      </c>
+      <c r="I471" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="J471" s="8" t="s">
+        <v>743</v>
+      </c>
+      <c r="K471" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L471">
+        <v>0</v>
+      </c>
+      <c r="M471">
+        <v>0</v>
+      </c>
+      <c r="N471" t="s">
+        <v>276</v>
+      </c>
+      <c r="O471" t="s">
+        <v>566</v>
+      </c>
+      <c r="P471" s="11" t="s">
+        <v>610</v>
+      </c>
+      <c r="Q471" s="11" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="472" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A472">
+        <v>471</v>
+      </c>
+      <c r="B472" t="s">
+        <v>256</v>
+      </c>
+      <c r="C472" t="s">
+        <v>747</v>
+      </c>
+      <c r="D472">
+        <v>2018</v>
+      </c>
+      <c r="E472" s="9"/>
+      <c r="F472">
+        <v>215</v>
+      </c>
+      <c r="G472" s="9"/>
+      <c r="H472" s="10"/>
+      <c r="I472" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="J472" s="8" t="s">
+        <v>744</v>
+      </c>
+      <c r="K472" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L472">
+        <v>0</v>
+      </c>
+      <c r="M472">
+        <v>0</v>
+      </c>
+      <c r="N472" t="s">
+        <v>291</v>
+      </c>
+      <c r="O472" t="s">
+        <v>562</v>
+      </c>
+      <c r="P472" s="11" t="s">
+        <v>614</v>
+      </c>
+      <c r="Q472" s="11" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="473" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A473">
+        <v>472</v>
+      </c>
+      <c r="B473" t="s">
+        <v>256</v>
+      </c>
+      <c r="C473" t="s">
+        <v>745</v>
+      </c>
+      <c r="D473">
+        <v>2018</v>
+      </c>
+      <c r="E473" s="9"/>
+      <c r="F473">
+        <v>400</v>
+      </c>
+      <c r="G473" s="9"/>
+      <c r="H473" s="10"/>
+      <c r="I473" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="J473" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="K473" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L473">
+        <v>0</v>
+      </c>
+      <c r="M473">
+        <v>0</v>
+      </c>
+      <c r="N473" t="s">
+        <v>276</v>
+      </c>
+      <c r="O473" t="s">
+        <v>566</v>
+      </c>
+      <c r="P473" s="11" t="s">
+        <v>614</v>
+      </c>
+      <c r="Q473" s="11" t="s">
+        <v>614</v>
+      </c>
+    </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576">
       <formula1>COUNTIF($A:$A,A1)&lt;2</formula1>
     </dataValidation>
@@ -26689,10 +27725,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G70"/>
+  <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71"/>
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27253,6 +28289,14 @@
         <v>718</v>
       </c>
     </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" s="12">
+        <v>43164</v>
+      </c>
+      <c r="B71" t="s">
+        <v>746</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
+ Canon 20/T.5, + NiSi F3 primes, + Meyer-Optik lenses
</commit_message>
<xml_diff>
--- a/BigAssTableOfLenses.xlsx
+++ b/BigAssTableOfLenses.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3652" uniqueCount="748">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3731" uniqueCount="762">
   <si>
     <t>Manufacture</t>
   </si>
@@ -2275,6 +2275,48 @@
   </si>
   <si>
     <t>Laowa 9mm f/2.8 Zero-D</t>
+  </si>
+  <si>
+    <t>CN-E 20mm T1.5 L F</t>
+  </si>
+  <si>
+    <t>Meyer-Optik Gorlitz</t>
+  </si>
+  <si>
+    <t>Trioplan 100mm f/2.8</t>
+  </si>
+  <si>
+    <t>Trioplan 50mm f/2.9</t>
+  </si>
+  <si>
+    <t>P75 75mm f/1.9</t>
+  </si>
+  <si>
+    <t>P58 58mm f/1.9</t>
+  </si>
+  <si>
+    <t>Nocturnus III 50mm F0.95</t>
+  </si>
+  <si>
+    <t>NiSi</t>
+  </si>
+  <si>
+    <t>F3 25mm T2.1</t>
+  </si>
+  <si>
+    <t>F3 35mm T2</t>
+  </si>
+  <si>
+    <t>F3 50mm T2</t>
+  </si>
+  <si>
+    <t>F3 75mm T2</t>
+  </si>
+  <si>
+    <t>F3 100mm T2</t>
+  </si>
+  <si>
+    <t>Add Canon 20/T1.5 Cine, NiSi cine lenses, Meyer Optik lenses</t>
   </si>
 </sst>
 </file>
@@ -2413,8 +2455,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q473" totalsRowShown="0">
-  <autoFilter ref="A1:Q473"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q484" totalsRowShown="0">
+  <autoFilter ref="A1:Q484"/>
   <tableColumns count="17">
     <tableColumn id="15" name="UUID"/>
     <tableColumn id="1" name="Manufacture"/>
@@ -2736,10 +2778,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q473"/>
+  <dimension ref="A1:Q484"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A450" workbookViewId="0">
-      <selection activeCell="C473" sqref="C473"/>
+    <sheetView tabSelected="1" topLeftCell="A459" workbookViewId="0">
+      <selection activeCell="Q485" sqref="Q485"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27709,8 +27751,549 @@
         <v>614</v>
       </c>
     </row>
+    <row r="474" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A474">
+        <v>473</v>
+      </c>
+      <c r="B474" t="s">
+        <v>7</v>
+      </c>
+      <c r="C474" t="s">
+        <v>748</v>
+      </c>
+      <c r="D474">
+        <v>2018</v>
+      </c>
+      <c r="E474">
+        <v>4220</v>
+      </c>
+      <c r="F474">
+        <v>1200</v>
+      </c>
+      <c r="G474">
+        <v>118.4</v>
+      </c>
+      <c r="H474" s="7">
+        <v>118.4</v>
+      </c>
+      <c r="I474" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="J474" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="K474" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L474">
+        <v>0</v>
+      </c>
+      <c r="M474">
+        <v>1</v>
+      </c>
+      <c r="N474" t="s">
+        <v>276</v>
+      </c>
+      <c r="O474" t="s">
+        <v>562</v>
+      </c>
+      <c r="P474" s="11" t="s">
+        <v>610</v>
+      </c>
+      <c r="Q474" s="11" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="475" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A475">
+        <v>474</v>
+      </c>
+      <c r="B475" t="s">
+        <v>749</v>
+      </c>
+      <c r="C475" t="s">
+        <v>750</v>
+      </c>
+      <c r="D475" s="9">
+        <v>2015</v>
+      </c>
+      <c r="E475">
+        <v>1599</v>
+      </c>
+      <c r="F475" s="9"/>
+      <c r="G475" s="9"/>
+      <c r="H475" s="10"/>
+      <c r="I475" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="J475" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="K475" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L475">
+        <v>0</v>
+      </c>
+      <c r="M475">
+        <v>0</v>
+      </c>
+      <c r="N475" t="s">
+        <v>276</v>
+      </c>
+      <c r="O475" t="s">
+        <v>571</v>
+      </c>
+      <c r="P475" s="9"/>
+      <c r="Q475" s="9"/>
+    </row>
+    <row r="476" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A476">
+        <v>475</v>
+      </c>
+      <c r="B476" t="s">
+        <v>749</v>
+      </c>
+      <c r="C476" t="s">
+        <v>751</v>
+      </c>
+      <c r="D476">
+        <v>2016</v>
+      </c>
+      <c r="E476">
+        <v>1499</v>
+      </c>
+      <c r="F476">
+        <v>200</v>
+      </c>
+      <c r="G476" s="9"/>
+      <c r="H476" s="10"/>
+      <c r="I476" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="J476" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="K476" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L476">
+        <v>0</v>
+      </c>
+      <c r="M476">
+        <v>0</v>
+      </c>
+      <c r="N476" t="s">
+        <v>276</v>
+      </c>
+      <c r="O476" t="s">
+        <v>565</v>
+      </c>
+      <c r="P476" s="9"/>
+      <c r="Q476" s="9"/>
+    </row>
+    <row r="477" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A477">
+        <v>476</v>
+      </c>
+      <c r="B477" t="s">
+        <v>749</v>
+      </c>
+      <c r="C477" t="s">
+        <v>752</v>
+      </c>
+      <c r="D477">
+        <v>2017</v>
+      </c>
+      <c r="E477">
+        <v>1999</v>
+      </c>
+      <c r="F477">
+        <v>300</v>
+      </c>
+      <c r="G477" s="9"/>
+      <c r="H477" s="10"/>
+      <c r="I477" s="1">
+        <v>1.9</v>
+      </c>
+      <c r="J477" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="K477" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L477">
+        <v>0</v>
+      </c>
+      <c r="M477">
+        <v>0</v>
+      </c>
+      <c r="N477" t="s">
+        <v>581</v>
+      </c>
+      <c r="O477" t="s">
+        <v>565</v>
+      </c>
+      <c r="P477" s="9"/>
+      <c r="Q477" s="9"/>
+    </row>
+    <row r="478" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A478">
+        <v>477</v>
+      </c>
+      <c r="B478" t="s">
+        <v>749</v>
+      </c>
+      <c r="C478" t="s">
+        <v>753</v>
+      </c>
+      <c r="D478">
+        <v>2018</v>
+      </c>
+      <c r="E478">
+        <v>1599</v>
+      </c>
+      <c r="F478">
+        <v>200</v>
+      </c>
+      <c r="G478" s="9"/>
+      <c r="H478" s="10"/>
+      <c r="I478" s="1">
+        <v>1.9</v>
+      </c>
+      <c r="J478" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="K478" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L478">
+        <v>0</v>
+      </c>
+      <c r="M478">
+        <v>0</v>
+      </c>
+      <c r="N478" t="s">
+        <v>276</v>
+      </c>
+      <c r="O478" t="s">
+        <v>565</v>
+      </c>
+      <c r="P478" s="9"/>
+      <c r="Q478" s="9"/>
+    </row>
+    <row r="479" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A479">
+        <v>478</v>
+      </c>
+      <c r="B479" t="s">
+        <v>749</v>
+      </c>
+      <c r="C479" t="s">
+        <v>754</v>
+      </c>
+      <c r="D479">
+        <v>2018</v>
+      </c>
+      <c r="E479">
+        <v>3000</v>
+      </c>
+      <c r="F479">
+        <v>790</v>
+      </c>
+      <c r="G479" s="9"/>
+      <c r="H479" s="10"/>
+      <c r="I479" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="J479" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="K479" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L479">
+        <v>0</v>
+      </c>
+      <c r="M479">
+        <v>0</v>
+      </c>
+      <c r="N479" t="s">
+        <v>276</v>
+      </c>
+      <c r="O479" t="s">
+        <v>565</v>
+      </c>
+      <c r="P479" s="9"/>
+      <c r="Q479" s="9"/>
+    </row>
+    <row r="480" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A480">
+        <v>479</v>
+      </c>
+      <c r="B480" t="s">
+        <v>755</v>
+      </c>
+      <c r="C480" t="s">
+        <v>756</v>
+      </c>
+      <c r="D480">
+        <v>2018</v>
+      </c>
+      <c r="E480">
+        <v>3000</v>
+      </c>
+      <c r="F480">
+        <v>1330</v>
+      </c>
+      <c r="G480">
+        <v>117</v>
+      </c>
+      <c r="H480" s="7">
+        <v>95</v>
+      </c>
+      <c r="I480" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="J480" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="K480" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L480">
+        <v>0</v>
+      </c>
+      <c r="M480">
+        <v>1</v>
+      </c>
+      <c r="N480" t="s">
+        <v>276</v>
+      </c>
+      <c r="O480" t="s">
+        <v>564</v>
+      </c>
+      <c r="P480" s="11" t="s">
+        <v>614</v>
+      </c>
+      <c r="Q480" s="11" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="481" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A481">
+        <v>480</v>
+      </c>
+      <c r="B481" t="s">
+        <v>755</v>
+      </c>
+      <c r="C481" t="s">
+        <v>757</v>
+      </c>
+      <c r="D481">
+        <v>2018</v>
+      </c>
+      <c r="E481">
+        <v>2500</v>
+      </c>
+      <c r="F481">
+        <v>1280</v>
+      </c>
+      <c r="G481">
+        <v>117</v>
+      </c>
+      <c r="H481" s="7">
+        <v>95</v>
+      </c>
+      <c r="I481" s="1">
+        <v>2</v>
+      </c>
+      <c r="J481" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="K481" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L481">
+        <v>0</v>
+      </c>
+      <c r="M481">
+        <v>1</v>
+      </c>
+      <c r="N481" t="s">
+        <v>276</v>
+      </c>
+      <c r="O481" t="s">
+        <v>565</v>
+      </c>
+      <c r="P481" s="11" t="s">
+        <v>614</v>
+      </c>
+      <c r="Q481" s="11" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="482" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A482">
+        <v>481</v>
+      </c>
+      <c r="B482" t="s">
+        <v>755</v>
+      </c>
+      <c r="C482" t="s">
+        <v>758</v>
+      </c>
+      <c r="D482">
+        <v>2018</v>
+      </c>
+      <c r="E482">
+        <v>2500</v>
+      </c>
+      <c r="F482">
+        <v>1230</v>
+      </c>
+      <c r="G482">
+        <v>117</v>
+      </c>
+      <c r="H482" s="7">
+        <v>95</v>
+      </c>
+      <c r="I482" s="1">
+        <v>2</v>
+      </c>
+      <c r="J482" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="K482" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L482">
+        <v>0</v>
+      </c>
+      <c r="M482">
+        <v>1</v>
+      </c>
+      <c r="N482" t="s">
+        <v>276</v>
+      </c>
+      <c r="O482" t="s">
+        <v>565</v>
+      </c>
+      <c r="P482" s="11" t="s">
+        <v>614</v>
+      </c>
+      <c r="Q482" s="11" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="483" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A483">
+        <v>482</v>
+      </c>
+      <c r="B483" t="s">
+        <v>755</v>
+      </c>
+      <c r="C483" t="s">
+        <v>759</v>
+      </c>
+      <c r="D483">
+        <v>2018</v>
+      </c>
+      <c r="E483">
+        <v>2500</v>
+      </c>
+      <c r="F483">
+        <v>1120</v>
+      </c>
+      <c r="G483">
+        <v>117</v>
+      </c>
+      <c r="H483" s="7">
+        <v>95</v>
+      </c>
+      <c r="I483" s="1">
+        <v>2</v>
+      </c>
+      <c r="J483" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="K483" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L483">
+        <v>0</v>
+      </c>
+      <c r="M483">
+        <v>1</v>
+      </c>
+      <c r="N483" t="s">
+        <v>276</v>
+      </c>
+      <c r="O483" t="s">
+        <v>565</v>
+      </c>
+      <c r="P483" s="11" t="s">
+        <v>614</v>
+      </c>
+      <c r="Q483" s="11" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="484" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A484">
+        <v>483</v>
+      </c>
+      <c r="B484" t="s">
+        <v>755</v>
+      </c>
+      <c r="C484" t="s">
+        <v>760</v>
+      </c>
+      <c r="D484">
+        <v>2018</v>
+      </c>
+      <c r="E484">
+        <v>3000</v>
+      </c>
+      <c r="F484">
+        <v>1230</v>
+      </c>
+      <c r="G484">
+        <v>117</v>
+      </c>
+      <c r="H484" s="7">
+        <v>95</v>
+      </c>
+      <c r="I484" s="1">
+        <v>2</v>
+      </c>
+      <c r="J484" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="K484" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L484">
+        <v>0</v>
+      </c>
+      <c r="M484">
+        <v>1</v>
+      </c>
+      <c r="N484" t="s">
+        <v>276</v>
+      </c>
+      <c r="O484" t="s">
+        <v>571</v>
+      </c>
+      <c r="P484" s="11" t="s">
+        <v>614</v>
+      </c>
+      <c r="Q484" s="11" t="s">
+        <v>614</v>
+      </c>
+    </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576">
       <formula1>COUNTIF($A:$A,A1)&lt;2</formula1>
     </dataValidation>
@@ -27725,10 +28308,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G71"/>
+  <dimension ref="A1:G72"/>
   <sheetViews>
     <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+      <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28297,6 +28880,14 @@
         <v>746</v>
       </c>
     </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" s="12">
+        <v>43196</v>
+      </c>
+      <c r="B72" t="s">
+        <v>761</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
+ Leica 16-35mm SL
</commit_message>
<xml_diff>
--- a/BigAssTableOfLenses.xlsx
+++ b/BigAssTableOfLenses.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3731" uniqueCount="762">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3740" uniqueCount="764">
   <si>
     <t>Manufacture</t>
   </si>
@@ -2317,6 +2317,12 @@
   </si>
   <si>
     <t>Add Canon 20/T1.5 Cine, NiSi cine lenses, Meyer Optik lenses</t>
+  </si>
+  <si>
+    <t>Super-Vario-Elmar 16-35mm f/3.5-4.5 ASPH</t>
+  </si>
+  <si>
+    <t>Add Leica 16-35mm for SL</t>
   </si>
 </sst>
 </file>
@@ -2455,8 +2461,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q484" totalsRowShown="0">
-  <autoFilter ref="A1:Q484"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q485" totalsRowShown="0">
+  <autoFilter ref="A1:Q485"/>
   <tableColumns count="17">
     <tableColumn id="15" name="UUID"/>
     <tableColumn id="1" name="Manufacture"/>
@@ -2778,10 +2784,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q484"/>
+  <dimension ref="A1:Q485"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A459" workbookViewId="0">
-      <selection activeCell="Q485" sqref="Q485"/>
+      <selection activeCell="A486" sqref="A486"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28292,6 +28298,59 @@
         <v>614</v>
       </c>
     </row>
+    <row r="485" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A485">
+        <v>484</v>
+      </c>
+      <c r="B485" t="s">
+        <v>225</v>
+      </c>
+      <c r="C485" t="s">
+        <v>762</v>
+      </c>
+      <c r="D485">
+        <v>2018</v>
+      </c>
+      <c r="E485">
+        <v>5495</v>
+      </c>
+      <c r="F485">
+        <v>990</v>
+      </c>
+      <c r="G485">
+        <v>123</v>
+      </c>
+      <c r="H485" s="7">
+        <v>88</v>
+      </c>
+      <c r="I485" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="J485" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="K485" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="L485">
+        <v>0</v>
+      </c>
+      <c r="M485">
+        <v>0</v>
+      </c>
+      <c r="N485" t="s">
+        <v>276</v>
+      </c>
+      <c r="O485" t="s">
+        <v>562</v>
+      </c>
+      <c r="P485" s="11" t="s">
+        <v>613</v>
+      </c>
+      <c r="Q485" s="11" t="s">
+        <v>613</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576">
@@ -28308,10 +28367,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G72"/>
+  <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28888,6 +28947,14 @@
         <v>761</v>
       </c>
     </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" s="12">
+        <v>43199</v>
+      </c>
+      <c r="B73" t="s">
+        <v>763</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add Tokina FiRiN 20/2 AF price
no CSV update, minor change
</commit_message>
<xml_diff>
--- a/BigAssTableOfLenses.xlsx
+++ b/BigAssTableOfLenses.xlsx
@@ -2813,8 +2813,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Q490"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A475" workbookViewId="0">
-      <selection activeCell="E490" sqref="E490"/>
+    <sheetView tabSelected="1" topLeftCell="A440" workbookViewId="0">
+      <selection activeCell="E454" sqref="E454"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26797,7 +26797,9 @@
       <c r="D454" s="11">
         <v>2018</v>
       </c>
-      <c r="E454" s="9"/>
+      <c r="E454" s="11">
+        <v>949</v>
+      </c>
       <c r="F454" s="11">
         <v>464</v>
       </c>

</xml_diff>

<commit_message>
+ new Venus lenses, + pending Meyer lens
</commit_message>
<xml_diff>
--- a/BigAssTableOfLenses.xlsx
+++ b/BigAssTableOfLenses.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3782" uniqueCount="773">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3822" uniqueCount="782">
   <si>
     <t>Manufacture</t>
   </si>
@@ -2350,6 +2350,33 @@
   </si>
   <si>
     <t>Add Fuji 250mm GF</t>
+  </si>
+  <si>
+    <t>APO Plasmat 105mm f/2.7</t>
+  </si>
+  <si>
+    <t>Laowa 10-18mm F4.5-5.6 FE Zoom</t>
+  </si>
+  <si>
+    <t>4.5-5.6</t>
+  </si>
+  <si>
+    <t>10-18</t>
+  </si>
+  <si>
+    <t>Laowa 4mm f/2.8 Fisheye MFT</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Laowa 100mm f/2.8 2:1 Ultra-Macro APO</t>
+  </si>
+  <si>
+    <t>Laowa 17mm f/4 Zero-D GFX</t>
+  </si>
+  <si>
+    <t>Add 4 new Venus lenses as well as Meyer kickstarter lens</t>
   </si>
 </sst>
 </file>
@@ -2488,8 +2515,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q490" totalsRowShown="0">
-  <autoFilter ref="A1:Q490"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q495" totalsRowShown="0">
+  <autoFilter ref="A1:Q495"/>
   <tableColumns count="17">
     <tableColumn id="15" name="UUID"/>
     <tableColumn id="1" name="Manufacture"/>
@@ -2811,10 +2838,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q490"/>
+  <dimension ref="A1:Q495"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A440" workbookViewId="0">
-      <selection activeCell="E454" sqref="E454"/>
+    <sheetView tabSelected="1" topLeftCell="A486" workbookViewId="0">
+      <selection activeCell="C496" sqref="C496"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28637,6 +28664,251 @@
         <v>610</v>
       </c>
     </row>
+    <row r="491" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A491">
+        <v>491</v>
+      </c>
+      <c r="B491" t="s">
+        <v>749</v>
+      </c>
+      <c r="C491" t="s">
+        <v>773</v>
+      </c>
+      <c r="D491">
+        <v>2019</v>
+      </c>
+      <c r="E491" s="9"/>
+      <c r="F491" s="9"/>
+      <c r="G491" s="9"/>
+      <c r="H491" s="10"/>
+      <c r="I491" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="J491" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="K491" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L491">
+        <v>0</v>
+      </c>
+      <c r="M491">
+        <v>0</v>
+      </c>
+      <c r="N491" t="s">
+        <v>276</v>
+      </c>
+      <c r="O491" t="s">
+        <v>571</v>
+      </c>
+      <c r="P491" s="9"/>
+      <c r="Q491" s="9"/>
+    </row>
+    <row r="492" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A492">
+        <v>492</v>
+      </c>
+      <c r="B492" t="s">
+        <v>256</v>
+      </c>
+      <c r="C492" t="s">
+        <v>774</v>
+      </c>
+      <c r="D492">
+        <v>2018</v>
+      </c>
+      <c r="E492" s="9"/>
+      <c r="F492">
+        <v>496</v>
+      </c>
+      <c r="G492">
+        <v>90.9</v>
+      </c>
+      <c r="H492" s="7">
+        <v>70</v>
+      </c>
+      <c r="I492" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="J492" s="8" t="s">
+        <v>776</v>
+      </c>
+      <c r="K492" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="L492">
+        <v>0</v>
+      </c>
+      <c r="M492">
+        <v>0</v>
+      </c>
+      <c r="N492" t="s">
+        <v>276</v>
+      </c>
+      <c r="O492" t="s">
+        <v>562</v>
+      </c>
+      <c r="P492" s="11" t="s">
+        <v>614</v>
+      </c>
+      <c r="Q492" s="11" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="493" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A493">
+        <v>493</v>
+      </c>
+      <c r="B493" t="s">
+        <v>256</v>
+      </c>
+      <c r="C493" t="s">
+        <v>777</v>
+      </c>
+      <c r="D493">
+        <v>2018</v>
+      </c>
+      <c r="E493" s="13"/>
+      <c r="F493">
+        <v>135</v>
+      </c>
+      <c r="G493">
+        <v>25.5</v>
+      </c>
+      <c r="H493" s="7">
+        <v>45.2</v>
+      </c>
+      <c r="I493" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="J493" s="8" t="s">
+        <v>778</v>
+      </c>
+      <c r="K493" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L493">
+        <v>0</v>
+      </c>
+      <c r="M493">
+        <v>0</v>
+      </c>
+      <c r="N493" t="s">
+        <v>284</v>
+      </c>
+      <c r="O493" t="s">
+        <v>596</v>
+      </c>
+      <c r="P493" s="11" t="s">
+        <v>614</v>
+      </c>
+      <c r="Q493" s="11" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="494" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A494">
+        <v>494</v>
+      </c>
+      <c r="B494" t="s">
+        <v>256</v>
+      </c>
+      <c r="C494" t="s">
+        <v>779</v>
+      </c>
+      <c r="D494">
+        <v>2018</v>
+      </c>
+      <c r="E494" s="13"/>
+      <c r="F494">
+        <v>638</v>
+      </c>
+      <c r="G494">
+        <v>125</v>
+      </c>
+      <c r="H494" s="7">
+        <v>72</v>
+      </c>
+      <c r="I494" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="J494" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="K494" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L494">
+        <v>0</v>
+      </c>
+      <c r="M494">
+        <v>0</v>
+      </c>
+      <c r="N494" t="s">
+        <v>276</v>
+      </c>
+      <c r="O494" t="s">
+        <v>566</v>
+      </c>
+      <c r="P494" s="11" t="s">
+        <v>614</v>
+      </c>
+      <c r="Q494" s="11" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="495" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A495">
+        <v>495</v>
+      </c>
+      <c r="B495" t="s">
+        <v>256</v>
+      </c>
+      <c r="C495" t="s">
+        <v>780</v>
+      </c>
+      <c r="D495">
+        <v>2018</v>
+      </c>
+      <c r="E495" s="13"/>
+      <c r="F495">
+        <v>829</v>
+      </c>
+      <c r="G495">
+        <v>124.5</v>
+      </c>
+      <c r="H495" s="7">
+        <v>77.099999999999994</v>
+      </c>
+      <c r="I495" s="1">
+        <v>4</v>
+      </c>
+      <c r="J495" s="8" t="s">
+        <v>689</v>
+      </c>
+      <c r="K495" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L495">
+        <v>0</v>
+      </c>
+      <c r="M495">
+        <v>0</v>
+      </c>
+      <c r="N495" t="s">
+        <v>581</v>
+      </c>
+      <c r="O495" t="s">
+        <v>562</v>
+      </c>
+      <c r="P495" s="11" t="s">
+        <v>614</v>
+      </c>
+      <c r="Q495" s="11" t="s">
+        <v>614</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576">
@@ -28653,10 +28925,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G75"/>
+  <dimension ref="A1:G76"/>
   <sheetViews>
     <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+      <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29257,6 +29529,14 @@
         <v>772</v>
       </c>
     </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" s="12">
+        <v>43211</v>
+      </c>
+      <c r="B76" t="s">
+        <v>781</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
+ Tamron 28-75 III
</commit_message>
<xml_diff>
--- a/BigAssTableOfLenses.xlsx
+++ b/BigAssTableOfLenses.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3822" uniqueCount="782">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3830" uniqueCount="784">
   <si>
     <t>Manufacture</t>
   </si>
@@ -2377,6 +2377,12 @@
   </si>
   <si>
     <t>Add 4 new Venus lenses as well as Meyer kickstarter lens</t>
+  </si>
+  <si>
+    <t>28-75mm f/2.8 Di III RXD</t>
+  </si>
+  <si>
+    <t>Add Tamron 28-75mm III</t>
   </si>
 </sst>
 </file>
@@ -2515,8 +2521,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q495" totalsRowShown="0">
-  <autoFilter ref="A1:Q495"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q496" totalsRowShown="0">
+  <autoFilter ref="A1:Q496"/>
   <tableColumns count="17">
     <tableColumn id="15" name="UUID"/>
     <tableColumn id="1" name="Manufacture"/>
@@ -2838,10 +2844,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q495"/>
+  <dimension ref="A1:Q496"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A486" workbookViewId="0">
-      <selection activeCell="C496" sqref="C496"/>
+      <selection activeCell="Q496" sqref="Q496"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28909,6 +28915,57 @@
         <v>614</v>
       </c>
     </row>
+    <row r="496" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A496">
+        <v>496</v>
+      </c>
+      <c r="B496" t="s">
+        <v>180</v>
+      </c>
+      <c r="C496" t="s">
+        <v>782</v>
+      </c>
+      <c r="D496">
+        <v>2018</v>
+      </c>
+      <c r="E496">
+        <v>800</v>
+      </c>
+      <c r="F496">
+        <v>550</v>
+      </c>
+      <c r="G496">
+        <v>117.8</v>
+      </c>
+      <c r="H496" s="7">
+        <v>73</v>
+      </c>
+      <c r="I496" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="J496" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="K496" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="L496">
+        <v>0</v>
+      </c>
+      <c r="M496">
+        <v>0</v>
+      </c>
+      <c r="N496" t="s">
+        <v>276</v>
+      </c>
+      <c r="O496" t="s">
+        <v>565</v>
+      </c>
+      <c r="P496" s="11" t="s">
+        <v>610</v>
+      </c>
+      <c r="Q496" s="9"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576">
@@ -28925,10 +28982,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G76"/>
+  <dimension ref="A1:G77"/>
   <sheetViews>
     <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77"/>
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29537,6 +29594,14 @@
         <v>781</v>
       </c>
     </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" s="12">
+        <v>43217</v>
+      </c>
+      <c r="B77" t="s">
+        <v>783</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
+ Zeiss Supreme lenses
</commit_message>
<xml_diff>
--- a/BigAssTableOfLenses.xlsx
+++ b/BigAssTableOfLenses.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3838" uniqueCount="786">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3880" uniqueCount="794">
   <si>
     <t>Manufacture</t>
   </si>
@@ -2389,6 +2389,30 @@
   </si>
   <si>
     <t>Add Hasselblad 21/4</t>
+  </si>
+  <si>
+    <t>Add Sigma 70mm Macro Art price</t>
+  </si>
+  <si>
+    <t>Supreme Prime 25mm T1.5</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>Supreme Prime 29mm T1.5</t>
+  </si>
+  <si>
+    <t>Supreme Prime 35mm T1.5</t>
+  </si>
+  <si>
+    <t>Supreme Prime 50mm T1.5</t>
+  </si>
+  <si>
+    <t>Supreme Prime 85mm T1.5</t>
+  </si>
+  <si>
+    <t>Add Supreme Primes releasing in May '18</t>
   </si>
 </sst>
 </file>
@@ -2527,8 +2551,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q497" totalsRowShown="0">
-  <autoFilter ref="A1:Q497"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q502" totalsRowShown="0">
+  <autoFilter ref="A1:Q502"/>
   <tableColumns count="17">
     <tableColumn id="15" name="UUID"/>
     <tableColumn id="1" name="Manufacture"/>
@@ -2850,10 +2874,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q497"/>
+  <dimension ref="A1:Q502"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A486" workbookViewId="0">
-      <selection activeCell="P498" sqref="P498"/>
+    <sheetView tabSelected="1" topLeftCell="A474" workbookViewId="0">
+      <selection activeCell="R502" sqref="R502"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27693,7 +27717,9 @@
       <c r="D471">
         <v>2018</v>
       </c>
-      <c r="E471" s="9"/>
+      <c r="E471" s="11">
+        <v>570</v>
+      </c>
       <c r="F471">
         <v>515</v>
       </c>
@@ -29021,6 +29047,260 @@
       <c r="P497" s="9"/>
       <c r="Q497" s="11" t="s">
         <v>610</v>
+      </c>
+    </row>
+    <row r="498" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A498">
+        <v>498</v>
+      </c>
+      <c r="B498" t="s">
+        <v>132</v>
+      </c>
+      <c r="C498" t="s">
+        <v>787</v>
+      </c>
+      <c r="D498">
+        <v>2018</v>
+      </c>
+      <c r="E498" s="9"/>
+      <c r="F498">
+        <v>1420</v>
+      </c>
+      <c r="G498">
+        <v>119</v>
+      </c>
+      <c r="H498" s="7">
+        <v>95</v>
+      </c>
+      <c r="I498" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="J498" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="K498" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L498">
+        <v>0</v>
+      </c>
+      <c r="M498">
+        <v>1</v>
+      </c>
+      <c r="N498" t="s">
+        <v>276</v>
+      </c>
+      <c r="O498" t="s">
+        <v>564</v>
+      </c>
+      <c r="P498" s="11" t="s">
+        <v>613</v>
+      </c>
+      <c r="Q498" s="11" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="499" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A499">
+        <v>499</v>
+      </c>
+      <c r="B499" t="s">
+        <v>132</v>
+      </c>
+      <c r="C499" t="s">
+        <v>789</v>
+      </c>
+      <c r="D499">
+        <v>2018</v>
+      </c>
+      <c r="E499" s="9"/>
+      <c r="F499">
+        <v>1610</v>
+      </c>
+      <c r="G499">
+        <v>121</v>
+      </c>
+      <c r="H499" s="7">
+        <v>95</v>
+      </c>
+      <c r="I499" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="J499" s="8" t="s">
+        <v>788</v>
+      </c>
+      <c r="K499" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L499">
+        <v>0</v>
+      </c>
+      <c r="M499">
+        <v>1</v>
+      </c>
+      <c r="N499" t="s">
+        <v>276</v>
+      </c>
+      <c r="O499" t="s">
+        <v>564</v>
+      </c>
+      <c r="P499" s="11" t="s">
+        <v>613</v>
+      </c>
+      <c r="Q499" s="11" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="500" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A500">
+        <v>500</v>
+      </c>
+      <c r="B500" t="s">
+        <v>132</v>
+      </c>
+      <c r="C500" t="s">
+        <v>790</v>
+      </c>
+      <c r="D500">
+        <v>2018</v>
+      </c>
+      <c r="E500" s="9"/>
+      <c r="F500">
+        <v>1400</v>
+      </c>
+      <c r="G500">
+        <v>119</v>
+      </c>
+      <c r="H500" s="7">
+        <v>95</v>
+      </c>
+      <c r="I500" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="J500" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="K500" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L500">
+        <v>0</v>
+      </c>
+      <c r="M500">
+        <v>1</v>
+      </c>
+      <c r="N500" t="s">
+        <v>276</v>
+      </c>
+      <c r="O500" t="s">
+        <v>565</v>
+      </c>
+      <c r="P500" s="11" t="s">
+        <v>613</v>
+      </c>
+      <c r="Q500" s="11" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="501" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A501">
+        <v>501</v>
+      </c>
+      <c r="B501" t="s">
+        <v>132</v>
+      </c>
+      <c r="C501" t="s">
+        <v>791</v>
+      </c>
+      <c r="D501">
+        <v>2018</v>
+      </c>
+      <c r="E501" s="9"/>
+      <c r="F501">
+        <v>1220</v>
+      </c>
+      <c r="G501">
+        <v>119</v>
+      </c>
+      <c r="H501" s="7">
+        <v>95</v>
+      </c>
+      <c r="I501" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="J501" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="K501" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L501">
+        <v>0</v>
+      </c>
+      <c r="M501">
+        <v>1</v>
+      </c>
+      <c r="N501" t="s">
+        <v>276</v>
+      </c>
+      <c r="O501" t="s">
+        <v>565</v>
+      </c>
+      <c r="P501" s="11" t="s">
+        <v>613</v>
+      </c>
+      <c r="Q501" s="11" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="502" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A502">
+        <v>502</v>
+      </c>
+      <c r="B502" t="s">
+        <v>132</v>
+      </c>
+      <c r="C502" t="s">
+        <v>792</v>
+      </c>
+      <c r="D502">
+        <v>2018</v>
+      </c>
+      <c r="F502">
+        <v>1420</v>
+      </c>
+      <c r="G502">
+        <v>119</v>
+      </c>
+      <c r="H502" s="7">
+        <v>95</v>
+      </c>
+      <c r="I502" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="J502" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="K502" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L502">
+        <v>0</v>
+      </c>
+      <c r="M502">
+        <v>1</v>
+      </c>
+      <c r="N502" t="s">
+        <v>276</v>
+      </c>
+      <c r="O502" t="s">
+        <v>567</v>
+      </c>
+      <c r="P502" s="11" t="s">
+        <v>613</v>
+      </c>
+      <c r="Q502" s="11" t="s">
+        <v>613</v>
       </c>
     </row>
   </sheetData>
@@ -29039,10 +29319,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G78"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
     <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79"/>
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29667,6 +29947,22 @@
         <v>785</v>
       </c>
     </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="12">
+        <v>43234</v>
+      </c>
+      <c r="B79" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="12">
+        <v>43245</v>
+      </c>
+      <c r="B80" t="s">
+        <v>793</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
+ Sigma 105mm Art
</commit_message>
<xml_diff>
--- a/BigAssTableOfLenses.xlsx
+++ b/BigAssTableOfLenses.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3880" uniqueCount="794">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3889" uniqueCount="796">
   <si>
     <t>Manufacture</t>
   </si>
@@ -2413,6 +2413,12 @@
   </si>
   <si>
     <t>Add Supreme Primes releasing in May '18</t>
+  </si>
+  <si>
+    <t>105mm F1.4 HSM Art</t>
+  </si>
+  <si>
+    <t>Add Sigma 105mm Art</t>
   </si>
 </sst>
 </file>
@@ -2551,8 +2557,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q502" totalsRowShown="0">
-  <autoFilter ref="A1:Q502"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q503" totalsRowShown="0">
+  <autoFilter ref="A1:Q503"/>
   <tableColumns count="17">
     <tableColumn id="15" name="UUID"/>
     <tableColumn id="1" name="Manufacture"/>
@@ -2874,10 +2880,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q502"/>
+  <dimension ref="A1:Q503"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A474" workbookViewId="0">
-      <selection activeCell="R502" sqref="R502"/>
+    <sheetView tabSelected="1" topLeftCell="A472" workbookViewId="0">
+      <selection activeCell="C504" sqref="C504"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29303,6 +29309,59 @@
         <v>613</v>
       </c>
     </row>
+    <row r="503" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A503">
+        <v>503</v>
+      </c>
+      <c r="B503" t="s">
+        <v>100</v>
+      </c>
+      <c r="C503" t="s">
+        <v>794</v>
+      </c>
+      <c r="D503">
+        <v>2018</v>
+      </c>
+      <c r="E503">
+        <v>1599</v>
+      </c>
+      <c r="F503">
+        <v>1645</v>
+      </c>
+      <c r="G503">
+        <v>131.5</v>
+      </c>
+      <c r="H503" s="7">
+        <v>115.9</v>
+      </c>
+      <c r="I503" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="J503" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="K503" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L503">
+        <v>0</v>
+      </c>
+      <c r="M503">
+        <v>0</v>
+      </c>
+      <c r="N503" t="s">
+        <v>276</v>
+      </c>
+      <c r="O503" t="s">
+        <v>567</v>
+      </c>
+      <c r="P503" s="11" t="s">
+        <v>610</v>
+      </c>
+      <c r="Q503" s="11" t="s">
+        <v>610</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576">
@@ -29319,10 +29378,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G80"/>
+  <dimension ref="A1:G81"/>
   <sheetViews>
     <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81"/>
+      <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29963,6 +30022,14 @@
         <v>793</v>
       </c>
     </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="12">
+        <v>43245</v>
+      </c>
+      <c r="B81" t="s">
+        <v>795</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add Canon 70-200s & Samyang AF FE lenses
</commit_message>
<xml_diff>
--- a/BigAssTableOfLenses.xlsx
+++ b/BigAssTableOfLenses.xlsx
@@ -15,7 +15,7 @@
     <sheet name="LensTable" sheetId="1" r:id="rId1"/>
     <sheet name="Changelog" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3890" uniqueCount="797">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3923" uniqueCount="802">
   <si>
     <t>Manufacture</t>
   </si>
@@ -2422,6 +2422,21 @@
   </si>
   <si>
     <t>Unify f/ convention</t>
+  </si>
+  <si>
+    <t>EF 70-200mm f/2.8L IS III USM</t>
+  </si>
+  <si>
+    <t>EF 70-200mm f/4L IS II USM</t>
+  </si>
+  <si>
+    <t>AF 35mm f/2.8 FE</t>
+  </si>
+  <si>
+    <t>AF 24mm f/2.8 FE</t>
+  </si>
+  <si>
+    <t>Add Canon 70-200s, samyang 24mm f/2.8 FE &amp; 35</t>
   </si>
 </sst>
 </file>
@@ -2560,8 +2575,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q503" totalsRowShown="0">
-  <autoFilter ref="A1:Q503"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q507" totalsRowShown="0">
+  <autoFilter ref="A1:Q507"/>
   <tableColumns count="17">
     <tableColumn id="15" name="UUID"/>
     <tableColumn id="1" name="Manufacture"/>
@@ -2883,10 +2898,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q503"/>
+  <dimension ref="A1:Q507"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A466" workbookViewId="0">
-      <selection activeCell="C480" sqref="C480"/>
+    <sheetView tabSelected="1" topLeftCell="A493" workbookViewId="0">
+      <selection activeCell="A508" sqref="A508"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29365,6 +29380,218 @@
         <v>609</v>
       </c>
     </row>
+    <row r="504" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A504">
+        <v>504</v>
+      </c>
+      <c r="B504" t="s">
+        <v>7</v>
+      </c>
+      <c r="C504" t="s">
+        <v>797</v>
+      </c>
+      <c r="D504">
+        <v>2018</v>
+      </c>
+      <c r="E504">
+        <v>2099</v>
+      </c>
+      <c r="F504">
+        <v>1480</v>
+      </c>
+      <c r="G504">
+        <v>199</v>
+      </c>
+      <c r="H504" s="7">
+        <v>88.8</v>
+      </c>
+      <c r="I504" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="J504" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="K504" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="L504">
+        <v>1</v>
+      </c>
+      <c r="M504">
+        <v>0</v>
+      </c>
+      <c r="N504" t="s">
+        <v>276</v>
+      </c>
+      <c r="O504" t="s">
+        <v>570</v>
+      </c>
+      <c r="P504" s="11" t="s">
+        <v>609</v>
+      </c>
+      <c r="Q504" s="11" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="505" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A505">
+        <v>505</v>
+      </c>
+      <c r="B505" t="s">
+        <v>7</v>
+      </c>
+      <c r="C505" t="s">
+        <v>798</v>
+      </c>
+      <c r="D505">
+        <v>2018</v>
+      </c>
+      <c r="E505">
+        <v>1299</v>
+      </c>
+      <c r="F505">
+        <v>780</v>
+      </c>
+      <c r="G505">
+        <v>176</v>
+      </c>
+      <c r="H505" s="7">
+        <v>80</v>
+      </c>
+      <c r="I505" s="1">
+        <v>4</v>
+      </c>
+      <c r="J505" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="K505" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="L505">
+        <v>1</v>
+      </c>
+      <c r="M505">
+        <v>0</v>
+      </c>
+      <c r="N505" t="s">
+        <v>276</v>
+      </c>
+      <c r="O505" t="s">
+        <v>570</v>
+      </c>
+      <c r="P505" s="11" t="s">
+        <v>609</v>
+      </c>
+      <c r="Q505" s="11" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="506" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A506">
+        <v>506</v>
+      </c>
+      <c r="B506" t="s">
+        <v>420</v>
+      </c>
+      <c r="C506" t="s">
+        <v>799</v>
+      </c>
+      <c r="D506">
+        <v>2017</v>
+      </c>
+      <c r="E506">
+        <v>399</v>
+      </c>
+      <c r="F506">
+        <v>85.6</v>
+      </c>
+      <c r="G506">
+        <v>33</v>
+      </c>
+      <c r="H506" s="7">
+        <v>61.8</v>
+      </c>
+      <c r="I506" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="J506" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="K506" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L506">
+        <v>0</v>
+      </c>
+      <c r="M506">
+        <v>0</v>
+      </c>
+      <c r="N506" t="s">
+        <v>276</v>
+      </c>
+      <c r="O506" t="s">
+        <v>564</v>
+      </c>
+      <c r="P506" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="Q506" s="11" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="507" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A507">
+        <v>507</v>
+      </c>
+      <c r="B507" t="s">
+        <v>420</v>
+      </c>
+      <c r="C507" t="s">
+        <v>800</v>
+      </c>
+      <c r="D507">
+        <v>2018</v>
+      </c>
+      <c r="E507">
+        <v>399</v>
+      </c>
+      <c r="F507">
+        <v>120</v>
+      </c>
+      <c r="G507">
+        <v>37</v>
+      </c>
+      <c r="H507" s="7">
+        <v>61.8</v>
+      </c>
+      <c r="I507" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="J507" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="K507" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L507">
+        <v>0</v>
+      </c>
+      <c r="M507">
+        <v>0</v>
+      </c>
+      <c r="N507" t="s">
+        <v>276</v>
+      </c>
+      <c r="O507" t="s">
+        <v>563</v>
+      </c>
+      <c r="P507" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="Q507" s="11" t="s">
+        <v>618</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576">
@@ -29381,10 +29608,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G82"/>
+  <dimension ref="A1:G83"/>
   <sheetViews>
     <sheetView topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83"/>
+      <selection activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30041,6 +30268,14 @@
         <v>796</v>
       </c>
     </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" s="12">
+        <v>43262</v>
+      </c>
+      <c r="B83" t="s">
+        <v>801</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix model name error in Canon 85mm f/1.4 L IS
</commit_message>
<xml_diff>
--- a/BigAssTableOfLenses.xlsx
+++ b/BigAssTableOfLenses.xlsx
@@ -1989,9 +1989,6 @@
     <t>New lenses from Canon</t>
   </si>
   <si>
-    <t>85mm f/1.4L IS USM</t>
-  </si>
-  <si>
     <t>TS-E 50mm f/2.8L Macro</t>
   </si>
   <si>
@@ -2437,6 +2434,9 @@
   </si>
   <si>
     <t>Add Canon 70-200s, samyang 24mm f/2.8 FE &amp; 35</t>
+  </si>
+  <si>
+    <t>EF 85mm f/1.4L IS USM</t>
   </si>
 </sst>
 </file>
@@ -2900,8 +2900,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Q507"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A493" workbookViewId="0">
-      <selection activeCell="A508" sqref="A508"/>
+    <sheetView tabSelected="1" topLeftCell="A379" workbookViewId="0">
+      <selection activeCell="C427" sqref="C427"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2923,7 +2923,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -11890,7 +11890,7 @@
         <v>420</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="D168" s="1">
         <v>2016</v>
@@ -11999,7 +11999,7 @@
         <v>420</v>
       </c>
       <c r="C170" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="D170">
         <v>2015</v>
@@ -12107,7 +12107,7 @@
         <v>420</v>
       </c>
       <c r="C172" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D172" s="11">
         <v>2016</v>
@@ -12215,7 +12215,7 @@
         <v>420</v>
       </c>
       <c r="C174" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="D174">
         <v>2015</v>
@@ -12323,7 +12323,7 @@
         <v>420</v>
       </c>
       <c r="C176" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="D176">
         <v>2015</v>
@@ -12429,7 +12429,7 @@
         <v>420</v>
       </c>
       <c r="C178" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="D178">
         <v>2016</v>
@@ -14170,7 +14170,7 @@
         <v>165</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="D211" s="1">
         <v>2013</v>
@@ -14857,7 +14857,7 @@
         <v>180</v>
       </c>
       <c r="C224" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D224" s="1">
         <v>1992</v>
@@ -15432,7 +15432,7 @@
         <v>256</v>
       </c>
       <c r="C235" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="D235" s="1">
         <v>2016</v>
@@ -17025,7 +17025,7 @@
         <v>132</v>
       </c>
       <c r="C266" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="D266">
         <v>2011</v>
@@ -17135,7 +17135,7 @@
         <v>132</v>
       </c>
       <c r="C268" s="1" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="D268">
         <v>2015</v>
@@ -19878,7 +19878,7 @@
         <v>100</v>
       </c>
       <c r="C319" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="D319">
         <v>2017</v>
@@ -20037,7 +20037,7 @@
         <v>211</v>
       </c>
       <c r="C322" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D322" s="9"/>
       <c r="E322">
@@ -20088,7 +20088,7 @@
         <v>211</v>
       </c>
       <c r="C323" s="1" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D323" s="9"/>
       <c r="E323">
@@ -20139,7 +20139,7 @@
         <v>211</v>
       </c>
       <c r="C324" s="1" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D324" s="9"/>
       <c r="E324">
@@ -23210,7 +23210,7 @@
         <v>420</v>
       </c>
       <c r="C383" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="D383">
         <v>2015</v>
@@ -25413,7 +25413,7 @@
         <v>7</v>
       </c>
       <c r="C426" t="s">
-        <v>652</v>
+        <v>801</v>
       </c>
       <c r="D426">
         <v>2017</v>
@@ -25466,7 +25466,7 @@
         <v>7</v>
       </c>
       <c r="C427" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="D427">
         <v>2017</v>
@@ -25519,7 +25519,7 @@
         <v>7</v>
       </c>
       <c r="C428" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="D428">
         <v>2017</v>
@@ -25572,7 +25572,7 @@
         <v>7</v>
       </c>
       <c r="C429" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="D429">
         <v>2017</v>
@@ -25625,7 +25625,7 @@
         <v>100</v>
       </c>
       <c r="C430" s="14" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="D430" s="14">
         <v>2012</v>
@@ -25646,7 +25646,7 @@
         <v>2.8</v>
       </c>
       <c r="J430" s="16" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="K430" s="16" t="s">
         <v>177</v>
@@ -25676,7 +25676,7 @@
         <v>213</v>
       </c>
       <c r="C431" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="D431">
         <v>2017</v>
@@ -25697,7 +25697,7 @@
         <v>2</v>
       </c>
       <c r="J431" s="8" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="K431" s="8" t="s">
         <v>177</v>
@@ -25729,7 +25729,7 @@
         <v>213</v>
       </c>
       <c r="C432" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="D432">
         <v>2017</v>
@@ -25782,7 +25782,7 @@
         <v>132</v>
       </c>
       <c r="C433" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="D433">
         <v>2017</v>
@@ -25835,7 +25835,7 @@
         <v>165</v>
       </c>
       <c r="C434" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="D434">
         <v>2017</v>
@@ -25883,10 +25883,10 @@
         <v>434</v>
       </c>
       <c r="B435" t="s">
+        <v>682</v>
+      </c>
+      <c r="C435" t="s">
         <v>683</v>
-      </c>
-      <c r="C435" t="s">
-        <v>684</v>
       </c>
       <c r="D435">
         <v>2017</v>
@@ -25937,7 +25937,7 @@
         <v>425</v>
       </c>
       <c r="C436" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="D436">
         <v>2014</v>
@@ -25990,7 +25990,7 @@
         <v>425</v>
       </c>
       <c r="C437" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="D437">
         <v>2018</v>
@@ -26011,7 +26011,7 @@
         <v>1.2</v>
       </c>
       <c r="J437" s="8" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="K437" s="8" t="s">
         <v>177</v>
@@ -26043,7 +26043,7 @@
         <v>425</v>
       </c>
       <c r="C438" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="D438">
         <v>2012</v>
@@ -26094,7 +26094,7 @@
         <v>425</v>
       </c>
       <c r="C439" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="D439">
         <v>2017</v>
@@ -26147,7 +26147,7 @@
         <v>425</v>
       </c>
       <c r="C440" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D440">
         <v>2011</v>
@@ -26198,7 +26198,7 @@
         <v>425</v>
       </c>
       <c r="C441" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="D441">
         <v>2013</v>
@@ -26219,7 +26219,7 @@
         <v>1.8</v>
       </c>
       <c r="J441" s="8" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="K441" s="8" t="s">
         <v>177</v>
@@ -26246,10 +26246,10 @@
         <v>441</v>
       </c>
       <c r="B442" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C442" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="D442">
         <v>2011</v>
@@ -26297,10 +26297,10 @@
         <v>442</v>
       </c>
       <c r="B443" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C443" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D443">
         <v>2016</v>
@@ -26348,10 +26348,10 @@
         <v>443</v>
       </c>
       <c r="B444" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C444" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="D444">
         <v>2014</v>
@@ -26402,7 +26402,7 @@
         <v>59</v>
       </c>
       <c r="C445" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="D445">
         <v>2018</v>
@@ -26423,7 +26423,7 @@
         <v>4</v>
       </c>
       <c r="J445" s="8" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="K445" s="8" t="s">
         <v>178</v>
@@ -26438,7 +26438,7 @@
         <v>276</v>
       </c>
       <c r="O445" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="P445" s="11" t="s">
         <v>609</v>
@@ -26455,7 +26455,7 @@
         <v>100</v>
       </c>
       <c r="C446" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="D446">
         <v>2013</v>
@@ -26508,7 +26508,7 @@
         <v>225</v>
       </c>
       <c r="C447" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="D447">
         <v>2018</v>
@@ -26561,7 +26561,7 @@
         <v>225</v>
       </c>
       <c r="C448" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D448">
         <v>2018</v>
@@ -26614,7 +26614,7 @@
         <v>225</v>
       </c>
       <c r="C449" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D449">
         <v>2017</v>
@@ -26667,7 +26667,7 @@
         <v>100</v>
       </c>
       <c r="C450" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D450">
         <v>2018</v>
@@ -26720,7 +26720,7 @@
         <v>132</v>
       </c>
       <c r="C451" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="D451">
         <v>2018</v>
@@ -26773,7 +26773,7 @@
         <v>420</v>
       </c>
       <c r="C452" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D452">
         <v>2018</v>
@@ -26826,7 +26826,7 @@
         <v>180</v>
       </c>
       <c r="C453" s="11" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="D453" s="11">
         <v>2018</v>
@@ -26847,7 +26847,7 @@
         <v>4</v>
       </c>
       <c r="J453" s="8" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="K453" s="8">
         <v>1</v>
@@ -26879,7 +26879,7 @@
         <v>189</v>
       </c>
       <c r="C454" s="11" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="D454" s="11">
         <v>2018</v>
@@ -26932,7 +26932,7 @@
         <v>287</v>
       </c>
       <c r="C455" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="D455" s="11">
         <v>2014</v>
@@ -26985,7 +26985,7 @@
         <v>287</v>
       </c>
       <c r="C456" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="D456" s="11">
         <v>2015</v>
@@ -27038,7 +27038,7 @@
         <v>425</v>
       </c>
       <c r="C457" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="D457">
         <v>2016</v>
@@ -27074,7 +27074,7 @@
         <v>284</v>
       </c>
       <c r="O457" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="P457" s="11" t="s">
         <v>609</v>
@@ -27089,7 +27089,7 @@
         <v>425</v>
       </c>
       <c r="C458" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="D458">
         <v>2013</v>
@@ -27110,7 +27110,7 @@
         <v>2.8</v>
       </c>
       <c r="J458" s="8" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="K458" s="8" t="s">
         <v>178</v>
@@ -27140,7 +27140,7 @@
         <v>425</v>
       </c>
       <c r="C459" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="D459">
         <v>2015</v>
@@ -27161,7 +27161,7 @@
         <v>2.8</v>
       </c>
       <c r="J459" s="8" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="K459" s="8" t="s">
         <v>178</v>
@@ -27188,10 +27188,10 @@
         <v>459</v>
       </c>
       <c r="B460" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C460" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="D460">
         <v>2009</v>
@@ -27212,7 +27212,7 @@
         <v>4</v>
       </c>
       <c r="J460" s="8" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="K460" s="8" t="s">
         <v>178</v>
@@ -27239,10 +27239,10 @@
         <v>460</v>
       </c>
       <c r="B461" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C461" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="D461">
         <v>2017</v>
@@ -27260,10 +27260,10 @@
         <v>73.400000000000006</v>
       </c>
       <c r="I461" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="J461" s="8" t="s">
         <v>727</v>
-      </c>
-      <c r="J461" s="8" t="s">
-        <v>728</v>
       </c>
       <c r="K461" s="8" t="s">
         <v>178</v>
@@ -27290,10 +27290,10 @@
         <v>461</v>
       </c>
       <c r="B462" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C462" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="D462">
         <v>2012</v>
@@ -27312,7 +27312,7 @@
         <v>2.8</v>
       </c>
       <c r="J462" s="8" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="K462" s="8" t="s">
         <v>178</v>
@@ -27339,10 +27339,10 @@
         <v>462</v>
       </c>
       <c r="B463" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C463" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="D463">
         <v>2017</v>
@@ -27363,7 +27363,7 @@
         <v>2.8</v>
       </c>
       <c r="J463" s="8" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="K463" s="8" t="s">
         <v>178</v>
@@ -27390,10 +27390,10 @@
         <v>463</v>
       </c>
       <c r="B464" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C464" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="D464">
         <v>2017</v>
@@ -27414,7 +27414,7 @@
         <v>2.8</v>
       </c>
       <c r="J464" s="8" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="K464" s="8" t="s">
         <v>178</v>
@@ -27441,10 +27441,10 @@
         <v>464</v>
       </c>
       <c r="B465" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C465" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="D465">
         <v>2018</v>
@@ -27462,10 +27462,10 @@
         <v>76</v>
       </c>
       <c r="I465" s="1" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="J465" s="8" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="K465" s="8" t="s">
         <v>178</v>
@@ -27480,7 +27480,7 @@
         <v>284</v>
       </c>
       <c r="O465" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="P465" s="11" t="s">
         <v>609</v>
@@ -27495,7 +27495,7 @@
         <v>213</v>
       </c>
       <c r="C466" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D466">
         <v>2007</v>
@@ -27548,7 +27548,7 @@
         <v>213</v>
       </c>
       <c r="C467" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="D467">
         <v>2018</v>
@@ -27593,7 +27593,7 @@
         <v>213</v>
       </c>
       <c r="C468" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="D468">
         <v>2018</v>
@@ -27642,7 +27642,7 @@
         <v>213</v>
       </c>
       <c r="C469" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="D469">
         <v>2018</v>
@@ -27691,7 +27691,7 @@
         <v>189</v>
       </c>
       <c r="C470" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="D470">
         <v>2018</v>
@@ -27736,7 +27736,7 @@
         <v>100</v>
       </c>
       <c r="C471" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="D471">
         <v>2018</v>
@@ -27757,7 +27757,7 @@
         <v>2.8</v>
       </c>
       <c r="J471" s="8" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="K471" s="8" t="s">
         <v>177</v>
@@ -27789,7 +27789,7 @@
         <v>256</v>
       </c>
       <c r="C472" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="D472">
         <v>2018</v>
@@ -27804,7 +27804,7 @@
         <v>2.8</v>
       </c>
       <c r="J472" s="8" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="K472" s="8" t="s">
         <v>177</v>
@@ -27836,7 +27836,7 @@
         <v>256</v>
       </c>
       <c r="C473" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D473">
         <v>2018</v>
@@ -27883,7 +27883,7 @@
         <v>7</v>
       </c>
       <c r="C474" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="D474">
         <v>2018</v>
@@ -27933,10 +27933,10 @@
         <v>474</v>
       </c>
       <c r="B475" t="s">
+        <v>747</v>
+      </c>
+      <c r="C475" t="s">
         <v>748</v>
-      </c>
-      <c r="C475" t="s">
-        <v>749</v>
       </c>
       <c r="D475" s="9">
         <v>2015</v>
@@ -27976,10 +27976,10 @@
         <v>475</v>
       </c>
       <c r="B476" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C476" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="D476">
         <v>2016</v>
@@ -28021,10 +28021,10 @@
         <v>476</v>
       </c>
       <c r="B477" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C477" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="D477">
         <v>2017</v>
@@ -28066,10 +28066,10 @@
         <v>477</v>
       </c>
       <c r="B478" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C478" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="D478">
         <v>2018</v>
@@ -28111,10 +28111,10 @@
         <v>478</v>
       </c>
       <c r="B479" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C479" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="D479">
         <v>2018</v>
@@ -28156,10 +28156,10 @@
         <v>479</v>
       </c>
       <c r="B480" t="s">
+        <v>752</v>
+      </c>
+      <c r="C480" t="s">
         <v>753</v>
-      </c>
-      <c r="C480" t="s">
-        <v>754</v>
       </c>
       <c r="D480">
         <v>2018</v>
@@ -28209,10 +28209,10 @@
         <v>480</v>
       </c>
       <c r="B481" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="C481" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="D481">
         <v>2018</v>
@@ -28262,10 +28262,10 @@
         <v>481</v>
       </c>
       <c r="B482" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="C482" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="D482">
         <v>2018</v>
@@ -28315,10 +28315,10 @@
         <v>482</v>
       </c>
       <c r="B483" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="C483" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D483">
         <v>2018</v>
@@ -28368,10 +28368,10 @@
         <v>483</v>
       </c>
       <c r="B484" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="C484" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="D484">
         <v>2018</v>
@@ -28424,7 +28424,7 @@
         <v>225</v>
       </c>
       <c r="C485" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="D485">
         <v>2018</v>
@@ -28474,10 +28474,10 @@
         <v>485</v>
       </c>
       <c r="B486" t="s">
+        <v>761</v>
+      </c>
+      <c r="C486" t="s">
         <v>762</v>
-      </c>
-      <c r="C486" t="s">
-        <v>763</v>
       </c>
       <c r="D486">
         <v>2018</v>
@@ -28525,10 +28525,10 @@
         <v>486</v>
       </c>
       <c r="B487" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C487" s="11" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="D487">
         <v>2018</v>
@@ -28576,10 +28576,10 @@
         <v>487</v>
       </c>
       <c r="B488" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C488" s="11" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="D488">
         <v>2018</v>
@@ -28627,10 +28627,10 @@
         <v>489</v>
       </c>
       <c r="B489" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C489" s="11" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="D489">
         <v>2018</v>
@@ -28681,7 +28681,7 @@
         <v>366</v>
       </c>
       <c r="C490" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="D490">
         <v>2018</v>
@@ -28702,7 +28702,7 @@
         <v>4</v>
       </c>
       <c r="J490" s="8" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="K490" s="8" t="s">
         <v>177</v>
@@ -28731,10 +28731,10 @@
         <v>491</v>
       </c>
       <c r="B491" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C491" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="D491">
         <v>2019</v>
@@ -28775,7 +28775,7 @@
         <v>256</v>
       </c>
       <c r="C492" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="D492">
         <v>2018</v>
@@ -28791,10 +28791,10 @@
         <v>70</v>
       </c>
       <c r="I492" s="1" t="s">
+        <v>771</v>
+      </c>
+      <c r="J492" s="8" t="s">
         <v>772</v>
-      </c>
-      <c r="J492" s="8" t="s">
-        <v>773</v>
       </c>
       <c r="K492" s="8" t="s">
         <v>178</v>
@@ -28826,7 +28826,7 @@
         <v>256</v>
       </c>
       <c r="C493" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="D493">
         <v>2018</v>
@@ -28845,7 +28845,7 @@
         <v>2.8</v>
       </c>
       <c r="J493" s="8" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="K493" s="8" t="s">
         <v>177</v>
@@ -28877,7 +28877,7 @@
         <v>256</v>
       </c>
       <c r="C494" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="D494">
         <v>2018</v>
@@ -28928,7 +28928,7 @@
         <v>256</v>
       </c>
       <c r="C495" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="D495">
         <v>2018</v>
@@ -28947,7 +28947,7 @@
         <v>4</v>
       </c>
       <c r="J495" s="8" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="K495" s="8" t="s">
         <v>177</v>
@@ -28979,7 +28979,7 @@
         <v>180</v>
       </c>
       <c r="C496" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="D496">
         <v>2018</v>
@@ -29030,7 +29030,7 @@
         <v>586</v>
       </c>
       <c r="C497" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="D497">
         <v>2018</v>
@@ -29081,7 +29081,7 @@
         <v>132</v>
       </c>
       <c r="C498" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="D498">
         <v>2018</v>
@@ -29132,7 +29132,7 @@
         <v>132</v>
       </c>
       <c r="C499" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="D499">
         <v>2018</v>
@@ -29151,7 +29151,7 @@
         <v>1.5</v>
       </c>
       <c r="J499" s="8" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="K499" s="8" t="s">
         <v>177</v>
@@ -29183,7 +29183,7 @@
         <v>132</v>
       </c>
       <c r="C500" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="D500">
         <v>2018</v>
@@ -29234,7 +29234,7 @@
         <v>132</v>
       </c>
       <c r="C501" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="D501">
         <v>2018</v>
@@ -29285,7 +29285,7 @@
         <v>132</v>
       </c>
       <c r="C502" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="D502">
         <v>2018</v>
@@ -29335,7 +29335,7 @@
         <v>100</v>
       </c>
       <c r="C503" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="D503">
         <v>2018</v>
@@ -29388,7 +29388,7 @@
         <v>7</v>
       </c>
       <c r="C504" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="D504">
         <v>2018</v>
@@ -29441,7 +29441,7 @@
         <v>7</v>
       </c>
       <c r="C505" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="D505">
         <v>2018</v>
@@ -29494,7 +29494,7 @@
         <v>420</v>
       </c>
       <c r="C506" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="D506">
         <v>2017</v>
@@ -29547,7 +29547,7 @@
         <v>420</v>
       </c>
       <c r="C507" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="D507">
         <v>2018</v>
@@ -30056,7 +30056,7 @@
         <v>42992</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
@@ -30064,7 +30064,7 @@
         <v>42996</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
@@ -30072,7 +30072,7 @@
         <v>42997</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
@@ -30080,7 +30080,7 @@
         <v>43026</v>
       </c>
       <c r="B59" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
@@ -30088,7 +30088,7 @@
         <v>43033</v>
       </c>
       <c r="B60" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
@@ -30096,7 +30096,7 @@
         <v>43047</v>
       </c>
       <c r="B61" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
@@ -30104,7 +30104,7 @@
         <v>43097</v>
       </c>
       <c r="B62" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
@@ -30112,7 +30112,7 @@
         <v>43109</v>
       </c>
       <c r="B63" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
@@ -30129,7 +30129,7 @@
         <v>43128</v>
       </c>
       <c r="B65" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
@@ -30137,7 +30137,7 @@
         <v>43141</v>
       </c>
       <c r="B66" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
@@ -30145,7 +30145,7 @@
         <v>43145</v>
       </c>
       <c r="B67" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
@@ -30153,7 +30153,7 @@
         <v>43151</v>
       </c>
       <c r="B68" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
@@ -30161,7 +30161,7 @@
         <v>43153</v>
       </c>
       <c r="B69" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
@@ -30169,7 +30169,7 @@
         <v>43155</v>
       </c>
       <c r="B70" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
@@ -30177,7 +30177,7 @@
         <v>43164</v>
       </c>
       <c r="B71" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
@@ -30185,7 +30185,7 @@
         <v>43196</v>
       </c>
       <c r="B72" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
@@ -30193,7 +30193,7 @@
         <v>43199</v>
       </c>
       <c r="B73" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
@@ -30201,7 +30201,7 @@
         <v>43201</v>
       </c>
       <c r="B74" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
@@ -30209,7 +30209,7 @@
         <v>43202</v>
       </c>
       <c r="B75" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
@@ -30217,7 +30217,7 @@
         <v>43211</v>
       </c>
       <c r="B76" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
@@ -30225,7 +30225,7 @@
         <v>43217</v>
       </c>
       <c r="B77" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
@@ -30233,7 +30233,7 @@
         <v>43228</v>
       </c>
       <c r="B78" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
@@ -30241,7 +30241,7 @@
         <v>43234</v>
       </c>
       <c r="B79" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
@@ -30249,7 +30249,7 @@
         <v>43245</v>
       </c>
       <c r="B80" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
@@ -30257,7 +30257,7 @@
         <v>43245</v>
       </c>
       <c r="B81" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
@@ -30265,7 +30265,7 @@
         <v>43247</v>
       </c>
       <c r="B82" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
@@ -30273,7 +30273,7 @@
         <v>43262</v>
       </c>
       <c r="B83" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
+ Samyang 85mm f/1.4 EF
</commit_message>
<xml_diff>
--- a/BigAssTableOfLenses.xlsx
+++ b/BigAssTableOfLenses.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3923" uniqueCount="802">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3932" uniqueCount="804">
   <si>
     <t>Manufacture</t>
   </si>
@@ -2437,6 +2437,12 @@
   </si>
   <si>
     <t>EF 85mm f/1.4L IS USM</t>
+  </si>
+  <si>
+    <t>AF 85mm f/1.4 EF</t>
+  </si>
+  <si>
+    <t>Add Samyang 85mm f/1.4</t>
   </si>
 </sst>
 </file>
@@ -2575,8 +2581,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q507" totalsRowShown="0">
-  <autoFilter ref="A1:Q507"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q508" totalsRowShown="0">
+  <autoFilter ref="A1:Q508"/>
   <tableColumns count="17">
     <tableColumn id="15" name="UUID"/>
     <tableColumn id="1" name="Manufacture"/>
@@ -2898,10 +2904,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q507"/>
+  <dimension ref="A1:Q508"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A379" workbookViewId="0">
-      <selection activeCell="C427" sqref="C427"/>
+    <sheetView tabSelected="1" topLeftCell="A494" workbookViewId="0">
+      <selection activeCell="P509" sqref="P509"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29592,6 +29598,57 @@
         <v>618</v>
       </c>
     </row>
+    <row r="508" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A508">
+        <v>508</v>
+      </c>
+      <c r="B508" t="s">
+        <v>420</v>
+      </c>
+      <c r="C508" t="s">
+        <v>802</v>
+      </c>
+      <c r="D508">
+        <v>2018</v>
+      </c>
+      <c r="E508">
+        <v>799</v>
+      </c>
+      <c r="F508">
+        <v>485</v>
+      </c>
+      <c r="G508">
+        <v>72</v>
+      </c>
+      <c r="H508" s="10"/>
+      <c r="I508" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="J508" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="K508" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="L508">
+        <v>0</v>
+      </c>
+      <c r="M508">
+        <v>0</v>
+      </c>
+      <c r="N508" t="s">
+        <v>276</v>
+      </c>
+      <c r="O508" t="s">
+        <v>566</v>
+      </c>
+      <c r="P508" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="Q508" s="11" t="s">
+        <v>618</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576">
@@ -29608,10 +29665,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G83"/>
+  <dimension ref="A1:G84"/>
   <sheetViews>
     <sheetView topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84"/>
+      <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30276,6 +30333,14 @@
         <v>800</v>
       </c>
     </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" s="12">
+        <v>43269</v>
+      </c>
+      <c r="B84" t="s">
+        <v>803</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add Samyang 85mm f/1.8 EF diameter
</commit_message>
<xml_diff>
--- a/BigAssTableOfLenses.xlsx
+++ b/BigAssTableOfLenses.xlsx
@@ -2907,7 +2907,7 @@
   <dimension ref="A1:Q508"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A494" workbookViewId="0">
-      <selection activeCell="P509" sqref="P509"/>
+      <selection activeCell="H508" sqref="H508"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29620,7 +29620,9 @@
       <c r="G508">
         <v>72</v>
       </c>
-      <c r="H508" s="10"/>
+      <c r="H508" s="11">
+        <v>88</v>
+      </c>
       <c r="I508" s="1">
         <v>1.4</v>
       </c>

</xml_diff>